<commit_message>
Prova amb dates BDD
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D32423B1-E22D-4193-9D3D-86E18D58415F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F4A6DA-AD78-463D-8125-74CF233E9DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Dia</t>
   </si>
@@ -57,6 +46,15 @@
   </si>
   <si>
     <t>Prova</t>
+  </si>
+  <si>
+    <t>Provatina</t>
+  </si>
+  <si>
+    <t>Hola bon dia aixo es una frase exageradament llarga</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QRoWiTcO7dk</t>
   </si>
 </sst>
 </file>
@@ -418,19 +416,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H441"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="53" customWidth="1"/>
+    <col min="6" max="6" width="46.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -446,7 +448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -457,8 +459,1359 @@
         <v>6</v>
       </c>
       <c r="D2" s="2"/>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45688</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45689</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45690</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>402955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B127" s="1"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B128" s="1"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B129" s="1"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" s="1"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B136" s="1"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" s="1"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" s="1"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" s="1"/>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" s="1"/>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B142" s="1"/>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B143" s="1"/>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B144" s="1"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B146" s="1"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B147" s="1"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B148" s="1"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B149" s="1"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B150" s="1"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B151" s="1"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B152" s="1"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B153" s="1"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B154" s="1"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B155" s="1"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B156" s="1"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B157" s="1"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B158" s="1"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B159" s="1"/>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B160" s="1"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B161" s="1"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B162" s="1"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B163" s="1"/>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B164" s="1"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B165" s="1"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B166" s="1"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B167" s="1"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B168" s="1"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B169" s="1"/>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B170" s="1"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B171" s="1"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B172" s="1"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B173" s="1"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B174" s="1"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B175" s="1"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B176" s="1"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B177" s="1"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B178" s="1"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B179" s="1"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B180" s="1"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B181" s="1"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B182" s="1"/>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B183" s="1"/>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B184" s="1"/>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B185" s="1"/>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B186" s="1"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B187" s="1"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B188" s="1"/>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B189" s="1"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B190" s="1"/>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B191" s="1"/>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B192" s="1"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B193" s="1"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B194" s="1"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B195" s="1"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B196" s="1"/>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B197" s="1"/>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B198" s="1"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B199" s="1"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B200" s="1"/>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B201" s="1"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B202" s="1"/>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B203" s="1"/>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B204" s="1"/>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B205" s="1"/>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B206" s="1"/>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B207" s="1"/>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B208" s="1"/>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B209" s="1"/>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B210" s="1"/>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B211" s="1"/>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B212" s="1"/>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B213" s="1"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B214" s="1"/>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B215" s="1"/>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B216" s="1"/>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B217" s="1"/>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B218" s="1"/>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B219" s="1"/>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B220" s="1"/>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B221" s="1"/>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B222" s="1"/>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B223" s="1"/>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B224" s="1"/>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B225" s="1"/>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B226" s="1"/>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B227" s="1"/>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B228" s="1"/>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B229" s="1"/>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B230" s="1"/>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B231" s="1"/>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B232" s="1"/>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B233" s="1"/>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B234" s="1"/>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B235" s="1"/>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B236" s="1"/>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B237" s="1"/>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B238" s="1"/>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B239" s="1"/>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B240" s="1"/>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B241" s="1"/>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B242" s="1"/>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B243" s="1"/>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B244" s="1"/>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B245" s="1"/>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B246" s="1"/>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B247" s="1"/>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B248" s="1"/>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B249" s="1"/>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B250" s="1"/>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B251" s="1"/>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B252" s="1"/>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B253" s="1"/>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B254" s="1"/>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B255" s="1"/>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B256" s="1"/>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B257" s="1"/>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B258" s="1"/>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B259" s="1"/>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B260" s="1"/>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B261" s="1"/>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B262" s="1"/>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B263" s="1"/>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B264" s="1"/>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B265" s="1"/>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B266" s="1"/>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B267" s="1"/>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B268" s="1"/>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B269" s="1"/>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B270" s="1"/>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B271" s="1"/>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B272" s="1"/>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B273" s="1"/>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B274" s="1"/>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B275" s="1"/>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B276" s="1"/>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B277" s="1"/>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B278" s="1"/>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B279" s="1"/>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B280" s="1"/>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B281" s="1"/>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B282" s="1"/>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B283" s="1"/>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B284" s="1"/>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B285" s="1"/>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B286" s="1"/>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B287" s="1"/>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B288" s="1"/>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B289" s="1"/>
+    </row>
+    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B290" s="1"/>
+    </row>
+    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B291" s="1"/>
+    </row>
+    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B292" s="1"/>
+    </row>
+    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B293" s="1"/>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B294" s="1"/>
+    </row>
+    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B295" s="1"/>
+    </row>
+    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B296" s="1"/>
+    </row>
+    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B297" s="1"/>
+    </row>
+    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B298" s="1"/>
+    </row>
+    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B299" s="1"/>
+    </row>
+    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B300" s="1"/>
+    </row>
+    <row r="301" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B301" s="1"/>
+    </row>
+    <row r="302" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B302" s="1"/>
+    </row>
+    <row r="303" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B303" s="1"/>
+    </row>
+    <row r="304" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B304" s="1"/>
+    </row>
+    <row r="305" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B305" s="1"/>
+    </row>
+    <row r="306" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B306" s="1"/>
+    </row>
+    <row r="307" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B307" s="1"/>
+    </row>
+    <row r="308" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B308" s="1"/>
+    </row>
+    <row r="309" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B309" s="1"/>
+    </row>
+    <row r="310" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B310" s="1"/>
+    </row>
+    <row r="311" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B311" s="1"/>
+    </row>
+    <row r="312" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B312" s="1"/>
+    </row>
+    <row r="313" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B313" s="1"/>
+    </row>
+    <row r="314" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B314" s="1"/>
+    </row>
+    <row r="315" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B315" s="1"/>
+    </row>
+    <row r="316" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B316" s="1"/>
+    </row>
+    <row r="317" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B317" s="1"/>
+    </row>
+    <row r="318" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B318" s="1"/>
+    </row>
+    <row r="319" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B319" s="1"/>
+    </row>
+    <row r="320" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B320" s="1"/>
+    </row>
+    <row r="321" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B321" s="1"/>
+    </row>
+    <row r="322" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B322" s="1"/>
+    </row>
+    <row r="323" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B323" s="1"/>
+    </row>
+    <row r="324" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B324" s="1"/>
+    </row>
+    <row r="325" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B325" s="1"/>
+    </row>
+    <row r="326" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B326" s="1"/>
+    </row>
+    <row r="327" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B327" s="1"/>
+    </row>
+    <row r="328" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B328" s="1"/>
+    </row>
+    <row r="329" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B329" s="1"/>
+    </row>
+    <row r="330" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B330" s="1"/>
+    </row>
+    <row r="331" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B331" s="1"/>
+    </row>
+    <row r="332" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B332" s="1"/>
+    </row>
+    <row r="333" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B333" s="1"/>
+    </row>
+    <row r="334" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B334" s="1"/>
+    </row>
+    <row r="335" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B335" s="1"/>
+    </row>
+    <row r="336" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B336" s="1"/>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B337" s="1"/>
+    </row>
+    <row r="338" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B338" s="1"/>
+    </row>
+    <row r="339" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B339" s="1"/>
+    </row>
+    <row r="340" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B340" s="1"/>
+    </row>
+    <row r="341" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B341" s="1"/>
+    </row>
+    <row r="342" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B342" s="1"/>
+    </row>
+    <row r="343" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B343" s="1"/>
+    </row>
+    <row r="344" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B344" s="1"/>
+    </row>
+    <row r="345" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B345" s="1"/>
+    </row>
+    <row r="346" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B346" s="1"/>
+    </row>
+    <row r="347" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B347" s="1"/>
+    </row>
+    <row r="348" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B348" s="1"/>
+    </row>
+    <row r="349" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B349" s="1"/>
+    </row>
+    <row r="350" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B350" s="1"/>
+    </row>
+    <row r="351" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B351" s="1"/>
+    </row>
+    <row r="352" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B352" s="1"/>
+    </row>
+    <row r="353" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B353" s="1"/>
+    </row>
+    <row r="354" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B354" s="1"/>
+    </row>
+    <row r="355" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B355" s="1"/>
+    </row>
+    <row r="356" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B356" s="1"/>
+    </row>
+    <row r="357" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B357" s="1"/>
+    </row>
+    <row r="358" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B358" s="1"/>
+    </row>
+    <row r="359" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B359" s="1"/>
+    </row>
+    <row r="360" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B360" s="1"/>
+    </row>
+    <row r="361" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B361" s="1"/>
+    </row>
+    <row r="362" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B362" s="1"/>
+    </row>
+    <row r="363" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B363" s="1"/>
+    </row>
+    <row r="364" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B364" s="1"/>
+    </row>
+    <row r="365" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B365" s="1"/>
+    </row>
+    <row r="366" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B366" s="1"/>
+    </row>
+    <row r="367" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B367" s="1"/>
+    </row>
+    <row r="368" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B368" s="1"/>
+    </row>
+    <row r="369" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B369" s="1"/>
+    </row>
+    <row r="370" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B370" s="1"/>
+    </row>
+    <row r="371" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B371" s="1"/>
+    </row>
+    <row r="372" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B372" s="1"/>
+    </row>
+    <row r="373" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B373" s="1"/>
+    </row>
+    <row r="374" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B374" s="1"/>
+    </row>
+    <row r="375" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B375" s="1"/>
+    </row>
+    <row r="376" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B376" s="1"/>
+    </row>
+    <row r="377" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B377" s="1"/>
+    </row>
+    <row r="378" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B378" s="1"/>
+    </row>
+    <row r="379" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B379" s="1"/>
+    </row>
+    <row r="380" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B380" s="1"/>
+    </row>
+    <row r="381" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B381" s="1"/>
+    </row>
+    <row r="382" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B382" s="1"/>
+    </row>
+    <row r="383" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B383" s="1"/>
+    </row>
+    <row r="384" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B384" s="1"/>
+    </row>
+    <row r="385" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B385" s="1"/>
+    </row>
+    <row r="386" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B386" s="1"/>
+    </row>
+    <row r="387" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B387" s="1"/>
+    </row>
+    <row r="388" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B388" s="1"/>
+    </row>
+    <row r="389" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B389" s="1"/>
+    </row>
+    <row r="390" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B390" s="1"/>
+    </row>
+    <row r="391" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B391" s="1"/>
+    </row>
+    <row r="392" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B392" s="1"/>
+    </row>
+    <row r="393" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B393" s="1"/>
+    </row>
+    <row r="394" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B394" s="1"/>
+    </row>
+    <row r="395" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B395" s="1"/>
+    </row>
+    <row r="396" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B396" s="1"/>
+    </row>
+    <row r="397" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B397" s="1"/>
+    </row>
+    <row r="398" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B398" s="1"/>
+    </row>
+    <row r="399" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B399" s="1"/>
+    </row>
+    <row r="400" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B400" s="1"/>
+    </row>
+    <row r="401" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B401" s="1"/>
+    </row>
+    <row r="402" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B402" s="1"/>
+    </row>
+    <row r="403" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B403" s="1"/>
+    </row>
+    <row r="404" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B404" s="1"/>
+    </row>
+    <row r="405" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B405" s="1"/>
+    </row>
+    <row r="406" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B406" s="1"/>
+    </row>
+    <row r="407" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B407" s="1"/>
+    </row>
+    <row r="408" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B408" s="1"/>
+    </row>
+    <row r="409" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B409" s="1"/>
+    </row>
+    <row r="410" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B410" s="1"/>
+    </row>
+    <row r="411" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B411" s="1"/>
+    </row>
+    <row r="412" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B412" s="1"/>
+    </row>
+    <row r="413" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B413" s="1"/>
+    </row>
+    <row r="414" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B414" s="1"/>
+    </row>
+    <row r="415" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B415" s="1"/>
+    </row>
+    <row r="416" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B416" s="1"/>
+    </row>
+    <row r="417" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B417" s="1"/>
+    </row>
+    <row r="418" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B418" s="1"/>
+    </row>
+    <row r="419" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B419" s="1"/>
+    </row>
+    <row r="420" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B420" s="1"/>
+    </row>
+    <row r="421" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B421" s="1"/>
+    </row>
+    <row r="422" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B422" s="1"/>
+    </row>
+    <row r="423" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B423" s="1"/>
+    </row>
+    <row r="424" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B424" s="1"/>
+    </row>
+    <row r="425" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B425" s="1"/>
+    </row>
+    <row r="426" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B426" s="1"/>
+    </row>
+    <row r="427" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B427" s="1"/>
+    </row>
+    <row r="428" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B428" s="1"/>
+    </row>
+    <row r="429" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B429" s="1"/>
+    </row>
+    <row r="430" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B430" s="1"/>
+    </row>
+    <row r="431" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B431" s="1"/>
+    </row>
+    <row r="432" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B432" s="1"/>
+    </row>
+    <row r="433" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B433" s="1"/>
+    </row>
+    <row r="434" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B434" s="1"/>
+    </row>
+    <row r="435" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B435" s="1"/>
+    </row>
+    <row r="436" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B436" s="1"/>
+    </row>
+    <row r="437" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B437" s="1"/>
+    </row>
+    <row r="438" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B438" s="1"/>
+    </row>
+    <row r="439" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B439" s="1"/>
+    </row>
+    <row r="440" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B440" s="1"/>
+    </row>
+    <row r="441" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B441" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Prova amb fotos, countdown i hores V2
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7466F44D-3212-442A-900D-FB00720266F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE003007-66C5-410A-8D13-0A701E642BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -57,13 +57,13 @@
     <t>Perquè portem un any junts (MOOOOLT TEMPS) però se'm han passat com 4 dies al teu costat</t>
   </si>
   <si>
-    <t>./img/lola_flores</t>
-  </si>
-  <si>
     <t>Aquesta foto és de quan poravem 6 mesos. Pero segur que el somirure no l'has perdut</t>
   </si>
   <si>
     <t>Duuuurisisisisimoooo</t>
+  </si>
+  <si>
+    <t>./img/lola_flores.jpg</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:H441"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,10 +476,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -515,7 +515,7 @@
         <v>45690</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -551,6 +551,7 @@
       <c r="B9" s="4">
         <v>45694</v>
       </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">

</xml_diff>

<commit_message>
Prova amb dia d'avui mes fotos
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE003007-66C5-410A-8D13-0A701E642BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45B271F-593E-4909-BFAB-4A54C35986BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:H441"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>45639</v>
+        <v>45637</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -490,7 +490,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>45688</v>
+        <v>45638</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
App final (suposo) amb BDD de prova
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B868399-D928-4C7D-B8C7-32E993671991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A168E9-C6B7-41C2-BC07-09163E023BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -445,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
       <selection activeCell="B367" sqref="B367"/>
     </sheetView>
   </sheetViews>
@@ -482,7 +482,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>44906</v>
+        <v>45627</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -502,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>44907</v>
+        <v>45628</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -513,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>44908</v>
+        <v>45629</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -524,7 +524,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>44909</v>
+        <v>45630</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>44910</v>
+        <v>45631</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -546,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>44911</v>
+        <v>45632</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -557,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>44912</v>
+        <v>45633</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -570,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>44913</v>
+        <v>45634</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -582,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>44914</v>
+        <v>45635</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -594,7 +594,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>44915</v>
+        <v>45636</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -606,7 +606,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>44916</v>
+        <v>45637</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -617,7 +617,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>44917</v>
+        <v>45638</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -628,7 +628,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4">
-        <v>44918</v>
+        <v>45639</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -639,7 +639,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4">
-        <v>44919</v>
+        <v>45640</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -650,7 +650,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>44920</v>
+        <v>45641</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
@@ -661,7 +661,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>44921</v>
+        <v>45642</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -672,7 +672,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>44922</v>
+        <v>45643</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -683,7 +683,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4">
-        <v>44923</v>
+        <v>45644</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -694,7 +694,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4">
-        <v>44924</v>
+        <v>45645</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
@@ -705,7 +705,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4">
-        <v>44925</v>
+        <v>45646</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
@@ -716,7 +716,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4">
-        <v>44926</v>
+        <v>45647</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -727,7 +727,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4">
-        <v>44927</v>
+        <v>45648</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
@@ -738,7 +738,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4">
-        <v>44928</v>
+        <v>45649</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
@@ -749,7 +749,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4">
-        <v>44929</v>
+        <v>45650</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -760,7 +760,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4">
-        <v>44930</v>
+        <v>45651</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
@@ -771,7 +771,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4">
-        <v>44931</v>
+        <v>45652</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
@@ -782,7 +782,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4">
-        <v>44932</v>
+        <v>45653</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
@@ -793,7 +793,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4">
-        <v>44933</v>
+        <v>45654</v>
       </c>
       <c r="C29" t="s">
         <v>16</v>
@@ -804,7 +804,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4">
-        <v>44934</v>
+        <v>45655</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
@@ -815,7 +815,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <v>44935</v>
+        <v>45656</v>
       </c>
       <c r="C31" t="s">
         <v>16</v>
@@ -826,7 +826,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4">
-        <v>44936</v>
+        <v>45657</v>
       </c>
       <c r="C32" t="s">
         <v>16</v>
@@ -837,7 +837,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4">
-        <v>44937</v>
+        <v>45658</v>
       </c>
       <c r="C33" t="s">
         <v>16</v>
@@ -848,7 +848,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4">
-        <v>44938</v>
+        <v>45659</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
@@ -859,7 +859,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4">
-        <v>44939</v>
+        <v>45660</v>
       </c>
       <c r="C35" t="s">
         <v>16</v>
@@ -870,7 +870,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4">
-        <v>44940</v>
+        <v>45661</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
@@ -881,7 +881,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4">
-        <v>44941</v>
+        <v>45662</v>
       </c>
       <c r="C37" t="s">
         <v>16</v>
@@ -892,7 +892,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4">
-        <v>44942</v>
+        <v>45663</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
@@ -903,7 +903,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4">
-        <v>44943</v>
+        <v>45664</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
@@ -914,7 +914,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4">
-        <v>44944</v>
+        <v>45665</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
@@ -925,7 +925,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4">
-        <v>44945</v>
+        <v>45666</v>
       </c>
       <c r="C41" t="s">
         <v>16</v>
@@ -936,7 +936,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4">
-        <v>44946</v>
+        <v>45667</v>
       </c>
       <c r="C42" t="s">
         <v>16</v>
@@ -947,7 +947,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="4">
-        <v>44947</v>
+        <v>45668</v>
       </c>
       <c r="C43" t="s">
         <v>16</v>
@@ -958,7 +958,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4">
-        <v>44948</v>
+        <v>45669</v>
       </c>
       <c r="C44" t="s">
         <v>16</v>
@@ -969,7 +969,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="4">
-        <v>44949</v>
+        <v>45670</v>
       </c>
       <c r="C45" t="s">
         <v>16</v>
@@ -980,7 +980,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="4">
-        <v>44950</v>
+        <v>45671</v>
       </c>
       <c r="C46" t="s">
         <v>16</v>
@@ -991,7 +991,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4">
-        <v>44951</v>
+        <v>45672</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
@@ -1002,7 +1002,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="4">
-        <v>44952</v>
+        <v>45673</v>
       </c>
       <c r="C48" t="s">
         <v>16</v>
@@ -1013,7 +1013,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="4">
-        <v>44953</v>
+        <v>45674</v>
       </c>
       <c r="C49" t="s">
         <v>16</v>
@@ -1024,7 +1024,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="4">
-        <v>44954</v>
+        <v>45675</v>
       </c>
       <c r="C50" t="s">
         <v>16</v>
@@ -1035,7 +1035,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="4">
-        <v>44955</v>
+        <v>45676</v>
       </c>
       <c r="C51" t="s">
         <v>16</v>
@@ -1046,7 +1046,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="4">
-        <v>44956</v>
+        <v>45677</v>
       </c>
       <c r="C52" t="s">
         <v>16</v>
@@ -1057,7 +1057,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="4">
-        <v>44957</v>
+        <v>45678</v>
       </c>
       <c r="C53" t="s">
         <v>16</v>
@@ -1068,7 +1068,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="4">
-        <v>44958</v>
+        <v>45679</v>
       </c>
       <c r="C54" t="s">
         <v>16</v>
@@ -1079,7 +1079,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="4">
-        <v>44959</v>
+        <v>45680</v>
       </c>
       <c r="C55" t="s">
         <v>16</v>
@@ -1090,7 +1090,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="4">
-        <v>44960</v>
+        <v>45681</v>
       </c>
       <c r="C56" t="s">
         <v>16</v>
@@ -1101,7 +1101,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="4">
-        <v>44961</v>
+        <v>45682</v>
       </c>
       <c r="C57" t="s">
         <v>16</v>
@@ -1112,7 +1112,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="4">
-        <v>44962</v>
+        <v>45683</v>
       </c>
       <c r="C58" t="s">
         <v>16</v>
@@ -1123,7 +1123,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="4">
-        <v>44963</v>
+        <v>45684</v>
       </c>
       <c r="C59" t="s">
         <v>16</v>
@@ -1134,7 +1134,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="4">
-        <v>44964</v>
+        <v>45685</v>
       </c>
       <c r="C60" t="s">
         <v>16</v>
@@ -1145,7 +1145,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="4">
-        <v>44965</v>
+        <v>45686</v>
       </c>
       <c r="C61" t="s">
         <v>16</v>
@@ -1156,7 +1156,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="4">
-        <v>44966</v>
+        <v>45687</v>
       </c>
       <c r="C62" t="s">
         <v>16</v>
@@ -1167,7 +1167,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="4">
-        <v>44967</v>
+        <v>45688</v>
       </c>
       <c r="C63" t="s">
         <v>16</v>
@@ -1178,7 +1178,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="4">
-        <v>44968</v>
+        <v>45689</v>
       </c>
       <c r="C64" t="s">
         <v>16</v>
@@ -1189,7 +1189,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="4">
-        <v>44969</v>
+        <v>45690</v>
       </c>
       <c r="C65" t="s">
         <v>16</v>
@@ -1200,7 +1200,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="4">
-        <v>44970</v>
+        <v>45691</v>
       </c>
       <c r="C66" t="s">
         <v>16</v>
@@ -1211,7 +1211,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="4">
-        <v>44971</v>
+        <v>45692</v>
       </c>
       <c r="C67" t="s">
         <v>16</v>
@@ -1222,7 +1222,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="4">
-        <v>44972</v>
+        <v>45693</v>
       </c>
       <c r="C68" t="s">
         <v>16</v>
@@ -1233,7 +1233,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="4">
-        <v>44973</v>
+        <v>45694</v>
       </c>
       <c r="C69" t="s">
         <v>16</v>
@@ -1244,7 +1244,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="4">
-        <v>44974</v>
+        <v>45695</v>
       </c>
       <c r="C70" t="s">
         <v>16</v>
@@ -1255,7 +1255,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="4">
-        <v>44975</v>
+        <v>45696</v>
       </c>
       <c r="C71" t="s">
         <v>16</v>
@@ -1266,7 +1266,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="4">
-        <v>44976</v>
+        <v>45697</v>
       </c>
       <c r="C72" t="s">
         <v>16</v>
@@ -1277,7 +1277,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="4">
-        <v>44977</v>
+        <v>45698</v>
       </c>
       <c r="C73" t="s">
         <v>16</v>
@@ -1288,7 +1288,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="4">
-        <v>44978</v>
+        <v>45699</v>
       </c>
       <c r="C74" t="s">
         <v>16</v>
@@ -1299,7 +1299,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="4">
-        <v>44979</v>
+        <v>45700</v>
       </c>
       <c r="C75" t="s">
         <v>16</v>
@@ -1310,7 +1310,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="4">
-        <v>44980</v>
+        <v>45701</v>
       </c>
       <c r="C76" t="s">
         <v>16</v>
@@ -1321,7 +1321,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="4">
-        <v>44981</v>
+        <v>45702</v>
       </c>
       <c r="C77" t="s">
         <v>16</v>
@@ -1332,7 +1332,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="4">
-        <v>44982</v>
+        <v>45703</v>
       </c>
       <c r="C78" t="s">
         <v>16</v>
@@ -1343,7 +1343,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="4">
-        <v>44983</v>
+        <v>45704</v>
       </c>
       <c r="C79" t="s">
         <v>16</v>
@@ -1354,7 +1354,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="4">
-        <v>44984</v>
+        <v>45705</v>
       </c>
       <c r="C80" t="s">
         <v>16</v>
@@ -1365,7 +1365,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="4">
-        <v>44985</v>
+        <v>45706</v>
       </c>
       <c r="C81" t="s">
         <v>16</v>
@@ -1376,7 +1376,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="4">
-        <v>44986</v>
+        <v>45707</v>
       </c>
       <c r="C82" t="s">
         <v>16</v>
@@ -1387,7 +1387,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="4">
-        <v>44987</v>
+        <v>45708</v>
       </c>
       <c r="C83" t="s">
         <v>16</v>
@@ -1398,7 +1398,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="4">
-        <v>44988</v>
+        <v>45709</v>
       </c>
       <c r="C84" t="s">
         <v>16</v>
@@ -1409,7 +1409,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="4">
-        <v>44989</v>
+        <v>45710</v>
       </c>
       <c r="C85" t="s">
         <v>16</v>
@@ -1420,7 +1420,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="4">
-        <v>44990</v>
+        <v>45711</v>
       </c>
       <c r="C86" t="s">
         <v>16</v>
@@ -1431,7 +1431,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="4">
-        <v>44991</v>
+        <v>45712</v>
       </c>
       <c r="C87" t="s">
         <v>16</v>
@@ -1442,7 +1442,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="4">
-        <v>44992</v>
+        <v>45713</v>
       </c>
       <c r="C88" t="s">
         <v>16</v>
@@ -1453,7 +1453,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="4">
-        <v>44993</v>
+        <v>45714</v>
       </c>
       <c r="C89" t="s">
         <v>16</v>
@@ -1464,7 +1464,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="4">
-        <v>44994</v>
+        <v>45715</v>
       </c>
       <c r="C90" t="s">
         <v>16</v>
@@ -1475,7 +1475,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="4">
-        <v>44995</v>
+        <v>45716</v>
       </c>
       <c r="C91" t="s">
         <v>16</v>
@@ -1486,7 +1486,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="4">
-        <v>44996</v>
+        <v>45717</v>
       </c>
       <c r="C92" t="s">
         <v>16</v>
@@ -1497,7 +1497,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="4">
-        <v>44997</v>
+        <v>45718</v>
       </c>
       <c r="C93" t="s">
         <v>16</v>
@@ -1508,7 +1508,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="4">
-        <v>44998</v>
+        <v>45719</v>
       </c>
       <c r="C94" t="s">
         <v>16</v>
@@ -1519,7 +1519,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="4">
-        <v>44999</v>
+        <v>45720</v>
       </c>
       <c r="C95" t="s">
         <v>16</v>
@@ -1530,7 +1530,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="4">
-        <v>45000</v>
+        <v>45721</v>
       </c>
       <c r="C96" t="s">
         <v>16</v>
@@ -1541,7 +1541,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="4">
-        <v>45001</v>
+        <v>45722</v>
       </c>
       <c r="C97" t="s">
         <v>16</v>
@@ -1552,7 +1552,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="4">
-        <v>45002</v>
+        <v>45723</v>
       </c>
       <c r="C98" t="s">
         <v>16</v>
@@ -1563,7 +1563,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="4">
-        <v>45003</v>
+        <v>45724</v>
       </c>
       <c r="C99" t="s">
         <v>16</v>
@@ -1574,7 +1574,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="4">
-        <v>45004</v>
+        <v>45725</v>
       </c>
       <c r="C100" t="s">
         <v>16</v>
@@ -1585,7 +1585,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="4">
-        <v>45005</v>
+        <v>45726</v>
       </c>
       <c r="C101" t="s">
         <v>16</v>
@@ -1596,7 +1596,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="4">
-        <v>45006</v>
+        <v>45727</v>
       </c>
       <c r="C102" t="s">
         <v>16</v>
@@ -1607,7 +1607,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="4">
-        <v>45007</v>
+        <v>45728</v>
       </c>
       <c r="C103" t="s">
         <v>16</v>
@@ -1618,7 +1618,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="4">
-        <v>45008</v>
+        <v>45729</v>
       </c>
       <c r="C104" t="s">
         <v>16</v>
@@ -1629,7 +1629,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="4">
-        <v>45009</v>
+        <v>45730</v>
       </c>
       <c r="C105" t="s">
         <v>16</v>
@@ -1640,7 +1640,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="4">
-        <v>45010</v>
+        <v>45731</v>
       </c>
       <c r="C106" t="s">
         <v>16</v>
@@ -1651,7 +1651,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="4">
-        <v>45011</v>
+        <v>45732</v>
       </c>
       <c r="C107" t="s">
         <v>16</v>
@@ -1662,7 +1662,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="4">
-        <v>45012</v>
+        <v>45733</v>
       </c>
       <c r="C108" t="s">
         <v>16</v>
@@ -1673,7 +1673,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="4">
-        <v>45013</v>
+        <v>45734</v>
       </c>
       <c r="C109" t="s">
         <v>16</v>
@@ -1684,7 +1684,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="4">
-        <v>45014</v>
+        <v>45735</v>
       </c>
       <c r="C110" t="s">
         <v>16</v>
@@ -1695,7 +1695,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="4">
-        <v>45015</v>
+        <v>45736</v>
       </c>
       <c r="C111" t="s">
         <v>16</v>
@@ -1706,7 +1706,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="4">
-        <v>45016</v>
+        <v>45737</v>
       </c>
       <c r="C112" t="s">
         <v>16</v>
@@ -1717,7 +1717,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="4">
-        <v>45017</v>
+        <v>45738</v>
       </c>
       <c r="C113" t="s">
         <v>16</v>
@@ -1728,7 +1728,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="4">
-        <v>45018</v>
+        <v>45739</v>
       </c>
       <c r="C114" t="s">
         <v>16</v>
@@ -1739,7 +1739,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="4">
-        <v>45019</v>
+        <v>45740</v>
       </c>
       <c r="C115" t="s">
         <v>16</v>
@@ -1750,7 +1750,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="4">
-        <v>45020</v>
+        <v>45741</v>
       </c>
       <c r="C116" t="s">
         <v>16</v>
@@ -1761,7 +1761,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="4">
-        <v>45021</v>
+        <v>45742</v>
       </c>
       <c r="C117" t="s">
         <v>16</v>
@@ -1772,7 +1772,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="4">
-        <v>45022</v>
+        <v>45743</v>
       </c>
       <c r="C118" t="s">
         <v>16</v>
@@ -1783,7 +1783,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="4">
-        <v>45023</v>
+        <v>45744</v>
       </c>
       <c r="C119" t="s">
         <v>16</v>
@@ -1794,7 +1794,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="4">
-        <v>45024</v>
+        <v>45745</v>
       </c>
       <c r="C120" t="s">
         <v>16</v>
@@ -1805,7 +1805,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="4">
-        <v>45025</v>
+        <v>45746</v>
       </c>
       <c r="C121" t="s">
         <v>16</v>
@@ -1816,7 +1816,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="4">
-        <v>45026</v>
+        <v>45747</v>
       </c>
       <c r="C122" t="s">
         <v>16</v>
@@ -1827,7 +1827,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="4">
-        <v>45027</v>
+        <v>45748</v>
       </c>
       <c r="C123" t="s">
         <v>16</v>
@@ -1838,7 +1838,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="4">
-        <v>45028</v>
+        <v>45749</v>
       </c>
       <c r="C124" t="s">
         <v>16</v>
@@ -1849,7 +1849,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="4">
-        <v>45029</v>
+        <v>45750</v>
       </c>
       <c r="C125" t="s">
         <v>16</v>
@@ -1860,7 +1860,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="4">
-        <v>45030</v>
+        <v>45751</v>
       </c>
       <c r="C126" t="s">
         <v>16</v>
@@ -1871,7 +1871,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="4">
-        <v>45031</v>
+        <v>45752</v>
       </c>
       <c r="C127" t="s">
         <v>16</v>
@@ -1882,7 +1882,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="4">
-        <v>45032</v>
+        <v>45753</v>
       </c>
       <c r="C128" t="s">
         <v>16</v>
@@ -1893,7 +1893,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="4">
-        <v>45033</v>
+        <v>45754</v>
       </c>
       <c r="C129" t="s">
         <v>16</v>
@@ -1904,7 +1904,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="4">
-        <v>45034</v>
+        <v>45755</v>
       </c>
       <c r="C130" t="s">
         <v>16</v>
@@ -1915,7 +1915,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="4">
-        <v>45035</v>
+        <v>45756</v>
       </c>
       <c r="C131" t="s">
         <v>16</v>
@@ -1926,7 +1926,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="4">
-        <v>45036</v>
+        <v>45757</v>
       </c>
       <c r="C132" t="s">
         <v>16</v>
@@ -1937,7 +1937,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="4">
-        <v>45037</v>
+        <v>45758</v>
       </c>
       <c r="C133" t="s">
         <v>16</v>
@@ -1948,7 +1948,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="4">
-        <v>45038</v>
+        <v>45759</v>
       </c>
       <c r="C134" t="s">
         <v>16</v>
@@ -1959,7 +1959,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="4">
-        <v>45039</v>
+        <v>45760</v>
       </c>
       <c r="C135" t="s">
         <v>16</v>
@@ -1970,7 +1970,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="4">
-        <v>45040</v>
+        <v>45761</v>
       </c>
       <c r="C136" t="s">
         <v>16</v>
@@ -1981,7 +1981,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="4">
-        <v>45041</v>
+        <v>45762</v>
       </c>
       <c r="C137" t="s">
         <v>16</v>
@@ -1992,7 +1992,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="4">
-        <v>45042</v>
+        <v>45763</v>
       </c>
       <c r="C138" t="s">
         <v>16</v>
@@ -2003,7 +2003,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="4">
-        <v>45043</v>
+        <v>45764</v>
       </c>
       <c r="C139" t="s">
         <v>16</v>
@@ -2014,7 +2014,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="4">
-        <v>45044</v>
+        <v>45765</v>
       </c>
       <c r="C140" t="s">
         <v>16</v>
@@ -2025,7 +2025,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="4">
-        <v>45045</v>
+        <v>45766</v>
       </c>
       <c r="C141" t="s">
         <v>16</v>
@@ -2036,7 +2036,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="4">
-        <v>45046</v>
+        <v>45767</v>
       </c>
       <c r="C142" t="s">
         <v>16</v>
@@ -2047,7 +2047,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="4">
-        <v>45047</v>
+        <v>45768</v>
       </c>
       <c r="C143" t="s">
         <v>16</v>
@@ -2058,7 +2058,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="4">
-        <v>45048</v>
+        <v>45769</v>
       </c>
       <c r="C144" t="s">
         <v>16</v>
@@ -2069,7 +2069,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="4">
-        <v>45049</v>
+        <v>45770</v>
       </c>
       <c r="C145" t="s">
         <v>16</v>
@@ -2080,7 +2080,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="4">
-        <v>45050</v>
+        <v>45771</v>
       </c>
       <c r="C146" t="s">
         <v>16</v>
@@ -2091,7 +2091,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="4">
-        <v>45051</v>
+        <v>45772</v>
       </c>
       <c r="C147" t="s">
         <v>16</v>
@@ -2102,7 +2102,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="4">
-        <v>45052</v>
+        <v>45773</v>
       </c>
       <c r="C148" t="s">
         <v>16</v>
@@ -2113,7 +2113,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="4">
-        <v>45053</v>
+        <v>45774</v>
       </c>
       <c r="C149" t="s">
         <v>16</v>
@@ -2124,7 +2124,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="4">
-        <v>45054</v>
+        <v>45775</v>
       </c>
       <c r="C150" t="s">
         <v>16</v>
@@ -2135,7 +2135,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="4">
-        <v>45055</v>
+        <v>45776</v>
       </c>
       <c r="C151" t="s">
         <v>16</v>
@@ -2146,7 +2146,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="4">
-        <v>45056</v>
+        <v>45777</v>
       </c>
       <c r="C152" t="s">
         <v>16</v>
@@ -2157,7 +2157,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="4">
-        <v>45057</v>
+        <v>45778</v>
       </c>
       <c r="C153" t="s">
         <v>16</v>
@@ -2168,7 +2168,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="4">
-        <v>45058</v>
+        <v>45779</v>
       </c>
       <c r="C154" t="s">
         <v>16</v>
@@ -2179,7 +2179,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="4">
-        <v>45059</v>
+        <v>45780</v>
       </c>
       <c r="C155" t="s">
         <v>16</v>
@@ -2190,7 +2190,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="4">
-        <v>45060</v>
+        <v>45781</v>
       </c>
       <c r="C156" t="s">
         <v>16</v>
@@ -2201,7 +2201,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="4">
-        <v>45061</v>
+        <v>45782</v>
       </c>
       <c r="C157" t="s">
         <v>16</v>
@@ -2212,7 +2212,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="4">
-        <v>45062</v>
+        <v>45783</v>
       </c>
       <c r="C158" t="s">
         <v>16</v>
@@ -2223,7 +2223,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="4">
-        <v>45063</v>
+        <v>45784</v>
       </c>
       <c r="C159" t="s">
         <v>16</v>
@@ -2234,7 +2234,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="4">
-        <v>45064</v>
+        <v>45785</v>
       </c>
       <c r="C160" t="s">
         <v>16</v>
@@ -2245,7 +2245,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="4">
-        <v>45065</v>
+        <v>45786</v>
       </c>
       <c r="C161" t="s">
         <v>16</v>
@@ -2256,7 +2256,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="4">
-        <v>45066</v>
+        <v>45787</v>
       </c>
       <c r="C162" t="s">
         <v>16</v>
@@ -2267,7 +2267,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="4">
-        <v>45067</v>
+        <v>45788</v>
       </c>
       <c r="C163" t="s">
         <v>16</v>
@@ -2278,7 +2278,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="4">
-        <v>45068</v>
+        <v>45789</v>
       </c>
       <c r="C164" t="s">
         <v>16</v>
@@ -2289,7 +2289,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="4">
-        <v>45069</v>
+        <v>45790</v>
       </c>
       <c r="C165" t="s">
         <v>16</v>
@@ -2300,7 +2300,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="4">
-        <v>45070</v>
+        <v>45791</v>
       </c>
       <c r="C166" t="s">
         <v>16</v>
@@ -2311,7 +2311,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="4">
-        <v>45071</v>
+        <v>45792</v>
       </c>
       <c r="C167" t="s">
         <v>16</v>
@@ -2322,7 +2322,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="4">
-        <v>45072</v>
+        <v>45793</v>
       </c>
       <c r="C168" t="s">
         <v>16</v>
@@ -2333,7 +2333,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="4">
-        <v>45073</v>
+        <v>45794</v>
       </c>
       <c r="C169" t="s">
         <v>16</v>
@@ -2344,7 +2344,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="4">
-        <v>45074</v>
+        <v>45795</v>
       </c>
       <c r="C170" t="s">
         <v>16</v>
@@ -2355,7 +2355,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="4">
-        <v>45075</v>
+        <v>45796</v>
       </c>
       <c r="C171" t="s">
         <v>16</v>
@@ -2366,7 +2366,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="4">
-        <v>45076</v>
+        <v>45797</v>
       </c>
       <c r="C172" t="s">
         <v>16</v>
@@ -2377,7 +2377,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="4">
-        <v>45077</v>
+        <v>45798</v>
       </c>
       <c r="C173" t="s">
         <v>16</v>
@@ -2388,7 +2388,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="4">
-        <v>45078</v>
+        <v>45799</v>
       </c>
       <c r="C174" t="s">
         <v>16</v>
@@ -2399,7 +2399,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="4">
-        <v>45079</v>
+        <v>45800</v>
       </c>
       <c r="C175" t="s">
         <v>16</v>
@@ -2410,7 +2410,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="4">
-        <v>45080</v>
+        <v>45801</v>
       </c>
       <c r="C176" t="s">
         <v>16</v>
@@ -2421,7 +2421,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="4">
-        <v>45081</v>
+        <v>45802</v>
       </c>
       <c r="C177" t="s">
         <v>16</v>
@@ -2432,7 +2432,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="4">
-        <v>45082</v>
+        <v>45803</v>
       </c>
       <c r="C178" t="s">
         <v>16</v>
@@ -2443,7 +2443,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="4">
-        <v>45083</v>
+        <v>45804</v>
       </c>
       <c r="C179" t="s">
         <v>16</v>
@@ -2454,7 +2454,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="4">
-        <v>45084</v>
+        <v>45805</v>
       </c>
       <c r="C180" t="s">
         <v>16</v>
@@ -2465,7 +2465,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="4">
-        <v>45085</v>
+        <v>45806</v>
       </c>
       <c r="C181" t="s">
         <v>16</v>
@@ -2476,7 +2476,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="4">
-        <v>45086</v>
+        <v>45807</v>
       </c>
       <c r="C182" t="s">
         <v>16</v>
@@ -2487,7 +2487,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="4">
-        <v>45087</v>
+        <v>45808</v>
       </c>
       <c r="C183" t="s">
         <v>16</v>
@@ -2498,7 +2498,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="4">
-        <v>45088</v>
+        <v>45809</v>
       </c>
       <c r="C184" t="s">
         <v>16</v>
@@ -2509,7 +2509,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="4">
-        <v>45089</v>
+        <v>45810</v>
       </c>
       <c r="C185" t="s">
         <v>16</v>
@@ -2520,7 +2520,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="4">
-        <v>45090</v>
+        <v>45811</v>
       </c>
       <c r="C186" t="s">
         <v>16</v>
@@ -2531,7 +2531,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="4">
-        <v>45091</v>
+        <v>45812</v>
       </c>
       <c r="C187" t="s">
         <v>16</v>
@@ -2542,7 +2542,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="4">
-        <v>45092</v>
+        <v>45813</v>
       </c>
       <c r="C188" t="s">
         <v>16</v>
@@ -2553,7 +2553,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="4">
-        <v>45093</v>
+        <v>45814</v>
       </c>
       <c r="C189" t="s">
         <v>16</v>
@@ -2564,7 +2564,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="4">
-        <v>45094</v>
+        <v>45815</v>
       </c>
       <c r="C190" t="s">
         <v>16</v>
@@ -2575,7 +2575,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="4">
-        <v>45095</v>
+        <v>45816</v>
       </c>
       <c r="C191" t="s">
         <v>16</v>
@@ -2586,7 +2586,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="4">
-        <v>45096</v>
+        <v>45817</v>
       </c>
       <c r="C192" t="s">
         <v>16</v>
@@ -2597,7 +2597,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="4">
-        <v>45097</v>
+        <v>45818</v>
       </c>
       <c r="C193" t="s">
         <v>16</v>
@@ -2608,7 +2608,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="4">
-        <v>45098</v>
+        <v>45819</v>
       </c>
       <c r="C194" t="s">
         <v>16</v>
@@ -2619,7 +2619,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="4">
-        <v>45099</v>
+        <v>45820</v>
       </c>
       <c r="C195" t="s">
         <v>16</v>
@@ -2630,7 +2630,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="4">
-        <v>45100</v>
+        <v>45821</v>
       </c>
       <c r="C196" t="s">
         <v>16</v>
@@ -2641,7 +2641,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="4">
-        <v>45101</v>
+        <v>45822</v>
       </c>
       <c r="C197" t="s">
         <v>16</v>
@@ -2652,7 +2652,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="4">
-        <v>45102</v>
+        <v>45823</v>
       </c>
       <c r="C198" t="s">
         <v>16</v>
@@ -2663,7 +2663,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="4">
-        <v>45103</v>
+        <v>45824</v>
       </c>
       <c r="C199" t="s">
         <v>16</v>
@@ -2674,7 +2674,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="4">
-        <v>45104</v>
+        <v>45825</v>
       </c>
       <c r="C200" t="s">
         <v>16</v>
@@ -2685,7 +2685,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="4">
-        <v>45105</v>
+        <v>45826</v>
       </c>
       <c r="C201" t="s">
         <v>16</v>
@@ -2696,7 +2696,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="4">
-        <v>45106</v>
+        <v>45827</v>
       </c>
       <c r="C202" t="s">
         <v>16</v>
@@ -2707,7 +2707,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="4">
-        <v>45107</v>
+        <v>45828</v>
       </c>
       <c r="C203" t="s">
         <v>16</v>
@@ -2718,7 +2718,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="4">
-        <v>45108</v>
+        <v>45829</v>
       </c>
       <c r="C204" t="s">
         <v>16</v>
@@ -2729,7 +2729,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="4">
-        <v>45109</v>
+        <v>45830</v>
       </c>
       <c r="C205" t="s">
         <v>16</v>
@@ -2740,7 +2740,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="4">
-        <v>45110</v>
+        <v>45831</v>
       </c>
       <c r="C206" t="s">
         <v>16</v>
@@ -2751,7 +2751,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="4">
-        <v>45111</v>
+        <v>45832</v>
       </c>
       <c r="C207" t="s">
         <v>16</v>
@@ -2762,7 +2762,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="4">
-        <v>45112</v>
+        <v>45833</v>
       </c>
       <c r="C208" t="s">
         <v>16</v>
@@ -2773,7 +2773,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="4">
-        <v>45113</v>
+        <v>45834</v>
       </c>
       <c r="C209" t="s">
         <v>16</v>
@@ -2784,7 +2784,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="4">
-        <v>45114</v>
+        <v>45835</v>
       </c>
       <c r="C210" t="s">
         <v>16</v>
@@ -2795,7 +2795,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="4">
-        <v>45115</v>
+        <v>45836</v>
       </c>
       <c r="C211" t="s">
         <v>16</v>
@@ -2806,7 +2806,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="4">
-        <v>45116</v>
+        <v>45837</v>
       </c>
       <c r="C212" t="s">
         <v>16</v>
@@ -2817,7 +2817,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="4">
-        <v>45117</v>
+        <v>45838</v>
       </c>
       <c r="C213" t="s">
         <v>16</v>
@@ -2828,7 +2828,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="4">
-        <v>45118</v>
+        <v>45839</v>
       </c>
       <c r="C214" t="s">
         <v>16</v>
@@ -2839,7 +2839,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="4">
-        <v>45119</v>
+        <v>45840</v>
       </c>
       <c r="C215" t="s">
         <v>16</v>
@@ -2850,7 +2850,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="4">
-        <v>45120</v>
+        <v>45841</v>
       </c>
       <c r="C216" t="s">
         <v>16</v>
@@ -2861,7 +2861,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="4">
-        <v>45121</v>
+        <v>45842</v>
       </c>
       <c r="C217" t="s">
         <v>16</v>
@@ -2872,7 +2872,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="4">
-        <v>45122</v>
+        <v>45843</v>
       </c>
       <c r="C218" t="s">
         <v>16</v>
@@ -2883,7 +2883,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="4">
-        <v>45123</v>
+        <v>45844</v>
       </c>
       <c r="C219" t="s">
         <v>16</v>
@@ -2894,7 +2894,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="4">
-        <v>45124</v>
+        <v>45845</v>
       </c>
       <c r="C220" t="s">
         <v>16</v>
@@ -2905,7 +2905,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="4">
-        <v>45125</v>
+        <v>45846</v>
       </c>
       <c r="C221" t="s">
         <v>16</v>
@@ -2916,7 +2916,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="4">
-        <v>45126</v>
+        <v>45847</v>
       </c>
       <c r="C222" t="s">
         <v>16</v>
@@ -2927,7 +2927,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="4">
-        <v>45127</v>
+        <v>45848</v>
       </c>
       <c r="C223" t="s">
         <v>16</v>
@@ -2938,7 +2938,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="4">
-        <v>45128</v>
+        <v>45849</v>
       </c>
       <c r="C224" t="s">
         <v>16</v>
@@ -2949,7 +2949,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="4">
-        <v>45129</v>
+        <v>45850</v>
       </c>
       <c r="C225" t="s">
         <v>16</v>
@@ -2960,7 +2960,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="4">
-        <v>45130</v>
+        <v>45851</v>
       </c>
       <c r="C226" t="s">
         <v>16</v>
@@ -2971,7 +2971,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="4">
-        <v>45131</v>
+        <v>45852</v>
       </c>
       <c r="C227" t="s">
         <v>16</v>
@@ -2982,7 +2982,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="4">
-        <v>45132</v>
+        <v>45853</v>
       </c>
       <c r="C228" t="s">
         <v>16</v>
@@ -2993,7 +2993,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="4">
-        <v>45133</v>
+        <v>45854</v>
       </c>
       <c r="C229" t="s">
         <v>16</v>
@@ -3004,7 +3004,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="4">
-        <v>45134</v>
+        <v>45855</v>
       </c>
       <c r="C230" t="s">
         <v>16</v>
@@ -3015,7 +3015,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="4">
-        <v>45135</v>
+        <v>45856</v>
       </c>
       <c r="C231" t="s">
         <v>16</v>
@@ -3026,7 +3026,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="4">
-        <v>45136</v>
+        <v>45857</v>
       </c>
       <c r="C232" t="s">
         <v>16</v>
@@ -3037,7 +3037,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="4">
-        <v>45137</v>
+        <v>45858</v>
       </c>
       <c r="C233" t="s">
         <v>16</v>
@@ -3048,7 +3048,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="4">
-        <v>45138</v>
+        <v>45859</v>
       </c>
       <c r="C234" t="s">
         <v>16</v>
@@ -3059,7 +3059,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="4">
-        <v>45139</v>
+        <v>45860</v>
       </c>
       <c r="C235" t="s">
         <v>16</v>
@@ -3070,7 +3070,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="4">
-        <v>45140</v>
+        <v>45861</v>
       </c>
       <c r="C236" t="s">
         <v>16</v>
@@ -3081,7 +3081,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="4">
-        <v>45141</v>
+        <v>45862</v>
       </c>
       <c r="C237" t="s">
         <v>16</v>
@@ -3092,7 +3092,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="4">
-        <v>45142</v>
+        <v>45863</v>
       </c>
       <c r="C238" t="s">
         <v>16</v>
@@ -3103,7 +3103,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="4">
-        <v>45143</v>
+        <v>45864</v>
       </c>
       <c r="C239" t="s">
         <v>16</v>
@@ -3114,7 +3114,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="4">
-        <v>45144</v>
+        <v>45865</v>
       </c>
       <c r="C240" t="s">
         <v>16</v>
@@ -3125,7 +3125,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="4">
-        <v>45145</v>
+        <v>45866</v>
       </c>
       <c r="C241" t="s">
         <v>16</v>
@@ -3136,7 +3136,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="4">
-        <v>45146</v>
+        <v>45867</v>
       </c>
       <c r="C242" t="s">
         <v>16</v>
@@ -3147,7 +3147,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="4">
-        <v>45147</v>
+        <v>45868</v>
       </c>
       <c r="C243" t="s">
         <v>16</v>
@@ -3158,7 +3158,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="4">
-        <v>45148</v>
+        <v>45869</v>
       </c>
       <c r="C244" t="s">
         <v>16</v>
@@ -3169,7 +3169,7 @@
         <v>244</v>
       </c>
       <c r="B245" s="4">
-        <v>45149</v>
+        <v>45870</v>
       </c>
       <c r="C245" t="s">
         <v>16</v>
@@ -3180,7 +3180,7 @@
         <v>245</v>
       </c>
       <c r="B246" s="4">
-        <v>45150</v>
+        <v>45871</v>
       </c>
       <c r="C246" t="s">
         <v>16</v>
@@ -3191,7 +3191,7 @@
         <v>246</v>
       </c>
       <c r="B247" s="4">
-        <v>45151</v>
+        <v>45872</v>
       </c>
       <c r="C247" t="s">
         <v>16</v>
@@ -3202,7 +3202,7 @@
         <v>247</v>
       </c>
       <c r="B248" s="4">
-        <v>45152</v>
+        <v>45873</v>
       </c>
       <c r="C248" t="s">
         <v>16</v>
@@ -3213,7 +3213,7 @@
         <v>248</v>
       </c>
       <c r="B249" s="4">
-        <v>45153</v>
+        <v>45874</v>
       </c>
       <c r="C249" t="s">
         <v>16</v>
@@ -3224,7 +3224,7 @@
         <v>249</v>
       </c>
       <c r="B250" s="4">
-        <v>45154</v>
+        <v>45875</v>
       </c>
       <c r="C250" t="s">
         <v>16</v>
@@ -3235,7 +3235,7 @@
         <v>250</v>
       </c>
       <c r="B251" s="4">
-        <v>45155</v>
+        <v>45876</v>
       </c>
       <c r="C251" t="s">
         <v>16</v>
@@ -3246,7 +3246,7 @@
         <v>251</v>
       </c>
       <c r="B252" s="4">
-        <v>45156</v>
+        <v>45877</v>
       </c>
       <c r="C252" t="s">
         <v>16</v>
@@ -3257,7 +3257,7 @@
         <v>252</v>
       </c>
       <c r="B253" s="4">
-        <v>45157</v>
+        <v>45878</v>
       </c>
       <c r="C253" t="s">
         <v>16</v>
@@ -3268,7 +3268,7 @@
         <v>253</v>
       </c>
       <c r="B254" s="4">
-        <v>45158</v>
+        <v>45879</v>
       </c>
       <c r="C254" t="s">
         <v>16</v>
@@ -3279,7 +3279,7 @@
         <v>254</v>
       </c>
       <c r="B255" s="4">
-        <v>45159</v>
+        <v>45880</v>
       </c>
       <c r="C255" t="s">
         <v>16</v>
@@ -3290,7 +3290,7 @@
         <v>255</v>
       </c>
       <c r="B256" s="4">
-        <v>45160</v>
+        <v>45881</v>
       </c>
       <c r="C256" t="s">
         <v>16</v>
@@ -3301,7 +3301,7 @@
         <v>256</v>
       </c>
       <c r="B257" s="4">
-        <v>45161</v>
+        <v>45882</v>
       </c>
       <c r="C257" t="s">
         <v>16</v>
@@ -3312,7 +3312,7 @@
         <v>257</v>
       </c>
       <c r="B258" s="4">
-        <v>45162</v>
+        <v>45883</v>
       </c>
       <c r="C258" t="s">
         <v>16</v>
@@ -3323,7 +3323,7 @@
         <v>258</v>
       </c>
       <c r="B259" s="4">
-        <v>45163</v>
+        <v>45884</v>
       </c>
       <c r="C259" t="s">
         <v>16</v>
@@ -3334,7 +3334,7 @@
         <v>259</v>
       </c>
       <c r="B260" s="4">
-        <v>45164</v>
+        <v>45885</v>
       </c>
       <c r="C260" t="s">
         <v>16</v>
@@ -3345,7 +3345,7 @@
         <v>260</v>
       </c>
       <c r="B261" s="4">
-        <v>45165</v>
+        <v>45886</v>
       </c>
       <c r="C261" t="s">
         <v>16</v>
@@ -3356,7 +3356,7 @@
         <v>261</v>
       </c>
       <c r="B262" s="4">
-        <v>45166</v>
+        <v>45887</v>
       </c>
       <c r="C262" t="s">
         <v>16</v>
@@ -3367,7 +3367,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="4">
-        <v>45167</v>
+        <v>45888</v>
       </c>
       <c r="C263" t="s">
         <v>16</v>
@@ -3378,7 +3378,7 @@
         <v>263</v>
       </c>
       <c r="B264" s="4">
-        <v>45168</v>
+        <v>45889</v>
       </c>
       <c r="C264" t="s">
         <v>16</v>
@@ -3389,7 +3389,7 @@
         <v>264</v>
       </c>
       <c r="B265" s="4">
-        <v>45169</v>
+        <v>45890</v>
       </c>
       <c r="C265" t="s">
         <v>16</v>
@@ -3400,7 +3400,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="4">
-        <v>45170</v>
+        <v>45891</v>
       </c>
       <c r="C266" t="s">
         <v>16</v>
@@ -3411,7 +3411,7 @@
         <v>266</v>
       </c>
       <c r="B267" s="4">
-        <v>45171</v>
+        <v>45892</v>
       </c>
       <c r="C267" t="s">
         <v>16</v>
@@ -3422,7 +3422,7 @@
         <v>267</v>
       </c>
       <c r="B268" s="4">
-        <v>45172</v>
+        <v>45893</v>
       </c>
       <c r="C268" t="s">
         <v>16</v>
@@ -3433,7 +3433,7 @@
         <v>268</v>
       </c>
       <c r="B269" s="4">
-        <v>45173</v>
+        <v>45894</v>
       </c>
       <c r="C269" t="s">
         <v>16</v>
@@ -3444,7 +3444,7 @@
         <v>269</v>
       </c>
       <c r="B270" s="4">
-        <v>45174</v>
+        <v>45895</v>
       </c>
       <c r="C270" t="s">
         <v>16</v>
@@ -3455,7 +3455,7 @@
         <v>270</v>
       </c>
       <c r="B271" s="4">
-        <v>45175</v>
+        <v>45896</v>
       </c>
       <c r="C271" t="s">
         <v>16</v>
@@ -3466,7 +3466,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="4">
-        <v>45176</v>
+        <v>45897</v>
       </c>
       <c r="C272" t="s">
         <v>16</v>
@@ -3477,7 +3477,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="4">
-        <v>45177</v>
+        <v>45898</v>
       </c>
       <c r="C273" t="s">
         <v>16</v>
@@ -3488,7 +3488,7 @@
         <v>273</v>
       </c>
       <c r="B274" s="4">
-        <v>45178</v>
+        <v>45899</v>
       </c>
       <c r="C274" t="s">
         <v>16</v>
@@ -3499,7 +3499,7 @@
         <v>274</v>
       </c>
       <c r="B275" s="4">
-        <v>45179</v>
+        <v>45900</v>
       </c>
       <c r="C275" t="s">
         <v>16</v>
@@ -3510,7 +3510,7 @@
         <v>275</v>
       </c>
       <c r="B276" s="4">
-        <v>45180</v>
+        <v>45901</v>
       </c>
       <c r="C276" t="s">
         <v>16</v>
@@ -3521,7 +3521,7 @@
         <v>276</v>
       </c>
       <c r="B277" s="4">
-        <v>45181</v>
+        <v>45902</v>
       </c>
       <c r="C277" t="s">
         <v>16</v>
@@ -3532,7 +3532,7 @@
         <v>277</v>
       </c>
       <c r="B278" s="4">
-        <v>45182</v>
+        <v>45903</v>
       </c>
       <c r="C278" t="s">
         <v>16</v>
@@ -3543,7 +3543,7 @@
         <v>278</v>
       </c>
       <c r="B279" s="4">
-        <v>45183</v>
+        <v>45904</v>
       </c>
       <c r="C279" t="s">
         <v>16</v>
@@ -3554,7 +3554,7 @@
         <v>279</v>
       </c>
       <c r="B280" s="4">
-        <v>45184</v>
+        <v>45905</v>
       </c>
       <c r="C280" t="s">
         <v>16</v>
@@ -3565,7 +3565,7 @@
         <v>280</v>
       </c>
       <c r="B281" s="4">
-        <v>45185</v>
+        <v>45906</v>
       </c>
       <c r="C281" t="s">
         <v>16</v>
@@ -3576,7 +3576,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="4">
-        <v>45186</v>
+        <v>45907</v>
       </c>
       <c r="C282" t="s">
         <v>16</v>
@@ -3587,7 +3587,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="4">
-        <v>45187</v>
+        <v>45908</v>
       </c>
       <c r="C283" t="s">
         <v>16</v>
@@ -3598,7 +3598,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="4">
-        <v>45188</v>
+        <v>45909</v>
       </c>
       <c r="C284" t="s">
         <v>16</v>
@@ -3609,7 +3609,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="4">
-        <v>45189</v>
+        <v>45910</v>
       </c>
       <c r="C285" t="s">
         <v>16</v>
@@ -3620,7 +3620,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="4">
-        <v>45190</v>
+        <v>45911</v>
       </c>
       <c r="C286" t="s">
         <v>16</v>
@@ -3631,7 +3631,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="4">
-        <v>45191</v>
+        <v>45912</v>
       </c>
       <c r="C287" t="s">
         <v>16</v>
@@ -3642,7 +3642,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="4">
-        <v>45192</v>
+        <v>45913</v>
       </c>
       <c r="C288" t="s">
         <v>16</v>
@@ -3653,7 +3653,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="4">
-        <v>45193</v>
+        <v>45914</v>
       </c>
       <c r="C289" t="s">
         <v>16</v>
@@ -3664,7 +3664,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="4">
-        <v>45194</v>
+        <v>45915</v>
       </c>
       <c r="C290" t="s">
         <v>16</v>
@@ -3675,7 +3675,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="4">
-        <v>45195</v>
+        <v>45916</v>
       </c>
       <c r="C291" t="s">
         <v>16</v>
@@ -3686,7 +3686,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="4">
-        <v>45196</v>
+        <v>45917</v>
       </c>
       <c r="C292" t="s">
         <v>16</v>
@@ -3697,7 +3697,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="4">
-        <v>45197</v>
+        <v>45918</v>
       </c>
       <c r="C293" t="s">
         <v>16</v>
@@ -3708,7 +3708,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="4">
-        <v>45198</v>
+        <v>45919</v>
       </c>
       <c r="C294" t="s">
         <v>16</v>
@@ -3719,7 +3719,7 @@
         <v>294</v>
       </c>
       <c r="B295" s="4">
-        <v>45199</v>
+        <v>45920</v>
       </c>
       <c r="C295" t="s">
         <v>16</v>
@@ -3730,7 +3730,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="4">
-        <v>45200</v>
+        <v>45921</v>
       </c>
       <c r="C296" t="s">
         <v>16</v>
@@ -3741,7 +3741,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="4">
-        <v>45201</v>
+        <v>45922</v>
       </c>
       <c r="C297" t="s">
         <v>16</v>
@@ -3752,7 +3752,7 @@
         <v>297</v>
       </c>
       <c r="B298" s="4">
-        <v>45202</v>
+        <v>45923</v>
       </c>
       <c r="C298" t="s">
         <v>16</v>
@@ -3763,7 +3763,7 @@
         <v>298</v>
       </c>
       <c r="B299" s="4">
-        <v>45203</v>
+        <v>45924</v>
       </c>
       <c r="C299" t="s">
         <v>16</v>
@@ -3774,7 +3774,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="4">
-        <v>45204</v>
+        <v>45925</v>
       </c>
       <c r="C300" t="s">
         <v>16</v>
@@ -3785,7 +3785,7 @@
         <v>300</v>
       </c>
       <c r="B301" s="4">
-        <v>45205</v>
+        <v>45926</v>
       </c>
       <c r="C301" t="s">
         <v>16</v>
@@ -3796,7 +3796,7 @@
         <v>301</v>
       </c>
       <c r="B302" s="4">
-        <v>45206</v>
+        <v>45927</v>
       </c>
       <c r="C302" t="s">
         <v>16</v>
@@ -3807,7 +3807,7 @@
         <v>302</v>
       </c>
       <c r="B303" s="4">
-        <v>45207</v>
+        <v>45928</v>
       </c>
       <c r="C303" t="s">
         <v>16</v>
@@ -3818,7 +3818,7 @@
         <v>303</v>
       </c>
       <c r="B304" s="4">
-        <v>45208</v>
+        <v>45929</v>
       </c>
       <c r="C304" t="s">
         <v>16</v>
@@ -3829,7 +3829,7 @@
         <v>304</v>
       </c>
       <c r="B305" s="4">
-        <v>45209</v>
+        <v>45930</v>
       </c>
       <c r="C305" t="s">
         <v>16</v>
@@ -3840,7 +3840,7 @@
         <v>305</v>
       </c>
       <c r="B306" s="4">
-        <v>45210</v>
+        <v>45931</v>
       </c>
       <c r="C306" t="s">
         <v>16</v>
@@ -3851,7 +3851,7 @@
         <v>306</v>
       </c>
       <c r="B307" s="4">
-        <v>45211</v>
+        <v>45932</v>
       </c>
       <c r="C307" t="s">
         <v>16</v>
@@ -3862,7 +3862,7 @@
         <v>307</v>
       </c>
       <c r="B308" s="4">
-        <v>45212</v>
+        <v>45933</v>
       </c>
       <c r="C308" t="s">
         <v>16</v>
@@ -3873,7 +3873,7 @@
         <v>308</v>
       </c>
       <c r="B309" s="4">
-        <v>45213</v>
+        <v>45934</v>
       </c>
       <c r="C309" t="s">
         <v>16</v>
@@ -3884,7 +3884,7 @@
         <v>309</v>
       </c>
       <c r="B310" s="4">
-        <v>45214</v>
+        <v>45935</v>
       </c>
       <c r="C310" t="s">
         <v>16</v>
@@ -3895,7 +3895,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="4">
-        <v>45215</v>
+        <v>45936</v>
       </c>
       <c r="C311" t="s">
         <v>16</v>
@@ -3906,7 +3906,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="4">
-        <v>45216</v>
+        <v>45937</v>
       </c>
       <c r="C312" t="s">
         <v>16</v>
@@ -3917,7 +3917,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="4">
-        <v>45217</v>
+        <v>45938</v>
       </c>
       <c r="C313" t="s">
         <v>16</v>
@@ -3928,7 +3928,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="4">
-        <v>45218</v>
+        <v>45939</v>
       </c>
       <c r="C314" t="s">
         <v>16</v>
@@ -3939,7 +3939,7 @@
         <v>314</v>
       </c>
       <c r="B315" s="4">
-        <v>45219</v>
+        <v>45940</v>
       </c>
       <c r="C315" t="s">
         <v>16</v>
@@ -3950,7 +3950,7 @@
         <v>315</v>
       </c>
       <c r="B316" s="4">
-        <v>45220</v>
+        <v>45941</v>
       </c>
       <c r="C316" t="s">
         <v>16</v>
@@ -3961,7 +3961,7 @@
         <v>316</v>
       </c>
       <c r="B317" s="4">
-        <v>45221</v>
+        <v>45942</v>
       </c>
       <c r="C317" t="s">
         <v>16</v>
@@ -3972,7 +3972,7 @@
         <v>317</v>
       </c>
       <c r="B318" s="4">
-        <v>45222</v>
+        <v>45943</v>
       </c>
       <c r="C318" t="s">
         <v>16</v>
@@ -3983,7 +3983,7 @@
         <v>318</v>
       </c>
       <c r="B319" s="4">
-        <v>45223</v>
+        <v>45944</v>
       </c>
       <c r="C319" t="s">
         <v>16</v>
@@ -3994,7 +3994,7 @@
         <v>319</v>
       </c>
       <c r="B320" s="4">
-        <v>45224</v>
+        <v>45945</v>
       </c>
       <c r="C320" t="s">
         <v>16</v>
@@ -4005,7 +4005,7 @@
         <v>320</v>
       </c>
       <c r="B321" s="4">
-        <v>45225</v>
+        <v>45946</v>
       </c>
       <c r="C321" t="s">
         <v>16</v>
@@ -4016,7 +4016,7 @@
         <v>321</v>
       </c>
       <c r="B322" s="4">
-        <v>45226</v>
+        <v>45947</v>
       </c>
       <c r="C322" t="s">
         <v>16</v>
@@ -4027,7 +4027,7 @@
         <v>322</v>
       </c>
       <c r="B323" s="4">
-        <v>45227</v>
+        <v>45948</v>
       </c>
       <c r="C323" t="s">
         <v>16</v>
@@ -4038,7 +4038,7 @@
         <v>323</v>
       </c>
       <c r="B324" s="4">
-        <v>45228</v>
+        <v>45949</v>
       </c>
       <c r="C324" t="s">
         <v>16</v>
@@ -4049,7 +4049,7 @@
         <v>324</v>
       </c>
       <c r="B325" s="4">
-        <v>45229</v>
+        <v>45950</v>
       </c>
       <c r="C325" t="s">
         <v>16</v>
@@ -4060,7 +4060,7 @@
         <v>325</v>
       </c>
       <c r="B326" s="4">
-        <v>45230</v>
+        <v>45951</v>
       </c>
       <c r="C326" t="s">
         <v>16</v>
@@ -4071,7 +4071,7 @@
         <v>326</v>
       </c>
       <c r="B327" s="4">
-        <v>45231</v>
+        <v>45952</v>
       </c>
       <c r="C327" t="s">
         <v>16</v>
@@ -4082,7 +4082,7 @@
         <v>327</v>
       </c>
       <c r="B328" s="4">
-        <v>45232</v>
+        <v>45953</v>
       </c>
       <c r="C328" t="s">
         <v>16</v>
@@ -4093,7 +4093,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="4">
-        <v>45233</v>
+        <v>45954</v>
       </c>
       <c r="C329" t="s">
         <v>16</v>
@@ -4104,7 +4104,7 @@
         <v>329</v>
       </c>
       <c r="B330" s="4">
-        <v>45234</v>
+        <v>45955</v>
       </c>
       <c r="C330" t="s">
         <v>16</v>
@@ -4115,7 +4115,7 @@
         <v>330</v>
       </c>
       <c r="B331" s="4">
-        <v>45235</v>
+        <v>45956</v>
       </c>
       <c r="C331" t="s">
         <v>16</v>
@@ -4126,7 +4126,7 @@
         <v>331</v>
       </c>
       <c r="B332" s="4">
-        <v>45236</v>
+        <v>45957</v>
       </c>
       <c r="C332" t="s">
         <v>16</v>
@@ -4137,7 +4137,7 @@
         <v>332</v>
       </c>
       <c r="B333" s="4">
-        <v>45237</v>
+        <v>45958</v>
       </c>
       <c r="C333" t="s">
         <v>16</v>
@@ -4148,7 +4148,7 @@
         <v>333</v>
       </c>
       <c r="B334" s="4">
-        <v>45238</v>
+        <v>45959</v>
       </c>
       <c r="C334" t="s">
         <v>16</v>
@@ -4159,7 +4159,7 @@
         <v>334</v>
       </c>
       <c r="B335" s="4">
-        <v>45239</v>
+        <v>45960</v>
       </c>
       <c r="C335" t="s">
         <v>16</v>
@@ -4170,7 +4170,7 @@
         <v>335</v>
       </c>
       <c r="B336" s="4">
-        <v>45240</v>
+        <v>45961</v>
       </c>
       <c r="C336" t="s">
         <v>16</v>
@@ -4181,7 +4181,7 @@
         <v>336</v>
       </c>
       <c r="B337" s="4">
-        <v>45241</v>
+        <v>45962</v>
       </c>
       <c r="C337" t="s">
         <v>16</v>
@@ -4192,7 +4192,7 @@
         <v>337</v>
       </c>
       <c r="B338" s="4">
-        <v>45242</v>
+        <v>45963</v>
       </c>
       <c r="C338" t="s">
         <v>16</v>
@@ -4203,7 +4203,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="4">
-        <v>45243</v>
+        <v>45964</v>
       </c>
       <c r="C339" t="s">
         <v>16</v>
@@ -4214,7 +4214,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="4">
-        <v>45244</v>
+        <v>45965</v>
       </c>
       <c r="C340" t="s">
         <v>16</v>
@@ -4225,7 +4225,7 @@
         <v>340</v>
       </c>
       <c r="B341" s="4">
-        <v>45245</v>
+        <v>45966</v>
       </c>
       <c r="C341" t="s">
         <v>16</v>
@@ -4236,7 +4236,7 @@
         <v>341</v>
       </c>
       <c r="B342" s="4">
-        <v>45246</v>
+        <v>45967</v>
       </c>
       <c r="C342" t="s">
         <v>16</v>
@@ -4247,7 +4247,7 @@
         <v>342</v>
       </c>
       <c r="B343" s="4">
-        <v>45247</v>
+        <v>45968</v>
       </c>
       <c r="C343" t="s">
         <v>16</v>
@@ -4258,7 +4258,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="4">
-        <v>45248</v>
+        <v>45969</v>
       </c>
       <c r="C344" t="s">
         <v>16</v>
@@ -4269,7 +4269,7 @@
         <v>344</v>
       </c>
       <c r="B345" s="4">
-        <v>45249</v>
+        <v>45970</v>
       </c>
       <c r="C345" t="s">
         <v>16</v>
@@ -4280,7 +4280,7 @@
         <v>345</v>
       </c>
       <c r="B346" s="4">
-        <v>45250</v>
+        <v>45971</v>
       </c>
       <c r="C346" t="s">
         <v>16</v>
@@ -4291,7 +4291,7 @@
         <v>346</v>
       </c>
       <c r="B347" s="4">
-        <v>45251</v>
+        <v>45972</v>
       </c>
       <c r="C347" t="s">
         <v>16</v>
@@ -4302,7 +4302,7 @@
         <v>347</v>
       </c>
       <c r="B348" s="4">
-        <v>45252</v>
+        <v>45973</v>
       </c>
       <c r="C348" t="s">
         <v>16</v>
@@ -4313,7 +4313,7 @@
         <v>348</v>
       </c>
       <c r="B349" s="4">
-        <v>45253</v>
+        <v>45974</v>
       </c>
       <c r="C349" t="s">
         <v>16</v>
@@ -4324,7 +4324,7 @@
         <v>349</v>
       </c>
       <c r="B350" s="4">
-        <v>45254</v>
+        <v>45975</v>
       </c>
       <c r="C350" t="s">
         <v>16</v>
@@ -4335,7 +4335,7 @@
         <v>350</v>
       </c>
       <c r="B351" s="4">
-        <v>45255</v>
+        <v>45976</v>
       </c>
       <c r="C351" t="s">
         <v>16</v>
@@ -4346,7 +4346,7 @@
         <v>351</v>
       </c>
       <c r="B352" s="4">
-        <v>45256</v>
+        <v>45977</v>
       </c>
       <c r="C352" t="s">
         <v>16</v>
@@ -4357,7 +4357,7 @@
         <v>352</v>
       </c>
       <c r="B353" s="4">
-        <v>45257</v>
+        <v>45978</v>
       </c>
       <c r="C353" t="s">
         <v>16</v>
@@ -4368,7 +4368,7 @@
         <v>353</v>
       </c>
       <c r="B354" s="4">
-        <v>45258</v>
+        <v>45979</v>
       </c>
       <c r="C354" t="s">
         <v>16</v>
@@ -4379,7 +4379,7 @@
         <v>354</v>
       </c>
       <c r="B355" s="4">
-        <v>45259</v>
+        <v>45980</v>
       </c>
       <c r="C355" t="s">
         <v>16</v>
@@ -4390,7 +4390,7 @@
         <v>355</v>
       </c>
       <c r="B356" s="4">
-        <v>45260</v>
+        <v>45981</v>
       </c>
       <c r="C356" t="s">
         <v>16</v>
@@ -4401,7 +4401,7 @@
         <v>356</v>
       </c>
       <c r="B357" s="4">
-        <v>45261</v>
+        <v>45982</v>
       </c>
       <c r="C357" t="s">
         <v>16</v>
@@ -4412,7 +4412,7 @@
         <v>357</v>
       </c>
       <c r="B358" s="4">
-        <v>45262</v>
+        <v>45983</v>
       </c>
       <c r="C358" t="s">
         <v>16</v>
@@ -4423,7 +4423,7 @@
         <v>358</v>
       </c>
       <c r="B359" s="4">
-        <v>45263</v>
+        <v>45984</v>
       </c>
       <c r="C359" t="s">
         <v>16</v>
@@ -4434,7 +4434,7 @@
         <v>359</v>
       </c>
       <c r="B360" s="4">
-        <v>45264</v>
+        <v>45985</v>
       </c>
       <c r="C360" t="s">
         <v>16</v>
@@ -4445,7 +4445,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="4">
-        <v>45265</v>
+        <v>45986</v>
       </c>
       <c r="C361" t="s">
         <v>16</v>
@@ -4456,7 +4456,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="4">
-        <v>45266</v>
+        <v>45987</v>
       </c>
       <c r="C362" t="s">
         <v>16</v>
@@ -4468,7 +4468,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="4">
-        <v>45267</v>
+        <v>45988</v>
       </c>
       <c r="C363" t="s">
         <v>16</v>
@@ -4479,7 +4479,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="4">
-        <v>45268</v>
+        <v>45989</v>
       </c>
       <c r="C364" t="s">
         <v>16</v>
@@ -4490,7 +4490,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="4">
-        <v>45269</v>
+        <v>45990</v>
       </c>
       <c r="C365" t="s">
         <v>16</v>
@@ -4501,7 +4501,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="4">
-        <v>45270</v>
+        <v>45991</v>
       </c>
       <c r="C366" t="s">
         <v>16</v>
@@ -4512,7 +4512,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="4">
-        <v>45271</v>
+        <v>45992</v>
       </c>
       <c r="C367" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Prova videos i captar el dia d'avui
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2E7E84-3F19-45AC-AB93-2E2E722FFBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C65066A-A4FF-4F25-BC49-72210F668DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="142">
   <si>
     <t>Dia</t>
   </si>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C74" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,7 +858,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>44591</v>
+        <v>45641</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -875,7 +875,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>44592</v>
+        <v>45642</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -889,10 +889,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>44593</v>
+        <v>45643</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -900,7 +903,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>44594</v>
+        <v>45644</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -911,7 +914,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>44595</v>
+        <v>45645</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -922,7 +925,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>44596</v>
+        <v>45646</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -933,7 +936,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>44597</v>
+        <v>45647</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -952,7 +955,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>44598</v>
+        <v>45648</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -964,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>44599</v>
+        <v>45649</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -976,7 +979,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>44600</v>
+        <v>45650</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -988,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>44601</v>
+        <v>45651</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -1005,7 +1008,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>44602</v>
+        <v>45652</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
@@ -1016,7 +1019,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4">
-        <v>44603</v>
+        <v>45653</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -1027,7 +1030,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4">
-        <v>44604</v>
+        <v>45654</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -1038,7 +1041,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>44605</v>
+        <v>45655</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1049,7 +1052,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>44606</v>
+        <v>45656</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
@@ -1060,7 +1063,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>44607</v>
+        <v>45657</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
@@ -1071,7 +1074,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4">
-        <v>44608</v>
+        <v>45658</v>
       </c>
       <c r="C19" t="s">
         <v>30</v>
@@ -1088,7 +1091,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4">
-        <v>44609</v>
+        <v>45659</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
@@ -1099,7 +1102,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4">
-        <v>44610</v>
+        <v>45660</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
@@ -1111,7 +1114,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4">
-        <v>44611</v>
+        <v>45661</v>
       </c>
       <c r="C22" t="s">
         <v>36</v>
@@ -1122,7 +1125,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4">
-        <v>44612</v>
+        <v>45662</v>
       </c>
       <c r="C23" t="s">
         <v>37</v>
@@ -1133,7 +1136,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4">
-        <v>44613</v>
+        <v>45663</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -1144,7 +1147,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4">
-        <v>44614</v>
+        <v>45664</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
@@ -1155,7 +1158,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4">
-        <v>44615</v>
+        <v>45665</v>
       </c>
       <c r="C26" t="s">
         <v>40</v>
@@ -1166,7 +1169,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4">
-        <v>44616</v>
+        <v>45666</v>
       </c>
       <c r="C27" t="s">
         <v>41</v>
@@ -1177,7 +1180,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4">
-        <v>44617</v>
+        <v>45667</v>
       </c>
       <c r="C28" t="s">
         <v>42</v>
@@ -1191,7 +1194,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4">
-        <v>44618</v>
+        <v>45668</v>
       </c>
       <c r="C29" t="s">
         <v>44</v>
@@ -1202,7 +1205,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4">
-        <v>44619</v>
+        <v>45669</v>
       </c>
       <c r="C30" t="s">
         <v>56</v>
@@ -1213,7 +1216,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <v>44620</v>
+        <v>45670</v>
       </c>
       <c r="C31" t="s">
         <v>57</v>
@@ -1224,7 +1227,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4">
-        <v>44621</v>
+        <v>45671</v>
       </c>
       <c r="C32" t="s">
         <v>58</v>
@@ -1241,7 +1244,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4">
-        <v>44622</v>
+        <v>45672</v>
       </c>
       <c r="C33" t="s">
         <v>61</v>
@@ -1252,7 +1255,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4">
-        <v>44623</v>
+        <v>45673</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -1263,7 +1266,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4">
-        <v>44624</v>
+        <v>45674</v>
       </c>
       <c r="C35" t="s">
         <v>63</v>
@@ -1274,7 +1277,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4">
-        <v>44625</v>
+        <v>45675</v>
       </c>
       <c r="C36" t="s">
         <v>64</v>
@@ -1285,7 +1288,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4">
-        <v>44626</v>
+        <v>45676</v>
       </c>
       <c r="C37" t="s">
         <v>65</v>
@@ -1296,7 +1299,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4">
-        <v>44627</v>
+        <v>45677</v>
       </c>
       <c r="C38" t="s">
         <v>66</v>
@@ -1307,7 +1310,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4">
-        <v>44628</v>
+        <v>45678</v>
       </c>
       <c r="C39" t="s">
         <v>67</v>
@@ -1318,7 +1321,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4">
-        <v>44629</v>
+        <v>45679</v>
       </c>
       <c r="C40" t="s">
         <v>68</v>
@@ -1329,7 +1332,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4">
-        <v>44630</v>
+        <v>45680</v>
       </c>
       <c r="C41" t="s">
         <v>69</v>
@@ -1340,7 +1343,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4">
-        <v>44631</v>
+        <v>45681</v>
       </c>
       <c r="C42" t="s">
         <v>70</v>
@@ -1351,7 +1354,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="4">
-        <v>44632</v>
+        <v>45682</v>
       </c>
       <c r="C43" t="s">
         <v>71</v>
@@ -1362,7 +1365,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4">
-        <v>44633</v>
+        <v>45683</v>
       </c>
       <c r="C44" t="s">
         <v>72</v>
@@ -1373,7 +1376,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="4">
-        <v>44634</v>
+        <v>45684</v>
       </c>
       <c r="C45" t="s">
         <v>73</v>
@@ -1387,7 +1390,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="4">
-        <v>44635</v>
+        <v>45685</v>
       </c>
       <c r="C46" t="s">
         <v>75</v>
@@ -1398,7 +1401,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4">
-        <v>44636</v>
+        <v>45686</v>
       </c>
       <c r="C47" t="s">
         <v>76</v>
@@ -1409,7 +1412,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="4">
-        <v>44637</v>
+        <v>45687</v>
       </c>
       <c r="C48" t="s">
         <v>77</v>
@@ -1420,7 +1423,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="4">
-        <v>44638</v>
+        <v>45688</v>
       </c>
       <c r="C49" t="s">
         <v>78</v>
@@ -1431,7 +1434,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="4">
-        <v>44639</v>
+        <v>45689</v>
       </c>
       <c r="C50" t="s">
         <v>79</v>
@@ -1442,7 +1445,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="4">
-        <v>44640</v>
+        <v>45690</v>
       </c>
       <c r="C51" t="s">
         <v>80</v>
@@ -1453,7 +1456,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="4">
-        <v>44641</v>
+        <v>45691</v>
       </c>
       <c r="C52" t="s">
         <v>81</v>
@@ -1464,7 +1467,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="4">
-        <v>44642</v>
+        <v>45692</v>
       </c>
       <c r="C53" t="s">
         <v>82</v>
@@ -1475,7 +1478,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="4">
-        <v>44643</v>
+        <v>45693</v>
       </c>
       <c r="C54" t="s">
         <v>83</v>
@@ -1486,7 +1489,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="4">
-        <v>44644</v>
+        <v>45694</v>
       </c>
       <c r="C55" t="s">
         <v>84</v>
@@ -1497,7 +1500,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="4">
-        <v>44645</v>
+        <v>45695</v>
       </c>
       <c r="C56" t="s">
         <v>85</v>
@@ -1508,7 +1511,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="4">
-        <v>44646</v>
+        <v>45696</v>
       </c>
       <c r="C57" t="s">
         <v>45</v>
@@ -1519,7 +1522,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="4">
-        <v>44647</v>
+        <v>45697</v>
       </c>
       <c r="C58" t="s">
         <v>86</v>
@@ -1536,7 +1539,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="4">
-        <v>44648</v>
+        <v>45698</v>
       </c>
       <c r="C59" t="s">
         <v>89</v>
@@ -1547,7 +1550,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="4">
-        <v>44649</v>
+        <v>45699</v>
       </c>
       <c r="C60" t="s">
         <v>90</v>
@@ -1558,7 +1561,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="4">
-        <v>44650</v>
+        <v>45700</v>
       </c>
       <c r="C61" t="s">
         <v>91</v>
@@ -1569,7 +1572,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="4">
-        <v>44651</v>
+        <v>45701</v>
       </c>
       <c r="C62" t="s">
         <v>102</v>
@@ -1580,7 +1583,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="4">
-        <v>44652</v>
+        <v>45702</v>
       </c>
       <c r="C63" t="s">
         <v>103</v>
@@ -1591,7 +1594,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="4">
-        <v>44653</v>
+        <v>45703</v>
       </c>
       <c r="C64" t="s">
         <v>104</v>
@@ -1602,7 +1605,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="4">
-        <v>44654</v>
+        <v>45704</v>
       </c>
       <c r="C65" t="s">
         <v>105</v>
@@ -1616,7 +1619,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="4">
-        <v>44655</v>
+        <v>45705</v>
       </c>
       <c r="C66" t="s">
         <v>110</v>
@@ -1627,7 +1630,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="4">
-        <v>44656</v>
+        <v>45706</v>
       </c>
       <c r="C67" t="s">
         <v>109</v>
@@ -1638,7 +1641,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="4">
-        <v>44657</v>
+        <v>45707</v>
       </c>
       <c r="C68" t="s">
         <v>108</v>
@@ -1649,7 +1652,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="4">
-        <v>44658</v>
+        <v>45708</v>
       </c>
       <c r="C69" t="s">
         <v>107</v>
@@ -1660,7 +1663,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="4">
-        <v>44659</v>
+        <v>45709</v>
       </c>
       <c r="C70" t="s">
         <v>111</v>
@@ -1671,7 +1674,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="4">
-        <v>44660</v>
+        <v>45710</v>
       </c>
       <c r="C71" t="s">
         <v>112</v>
@@ -1688,7 +1691,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="4">
-        <v>44661</v>
+        <v>45711</v>
       </c>
       <c r="C72" t="s">
         <v>115</v>
@@ -1699,7 +1702,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="4">
-        <v>44662</v>
+        <v>45712</v>
       </c>
       <c r="C73" t="s">
         <v>116</v>
@@ -1710,7 +1713,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="4">
-        <v>44663</v>
+        <v>45713</v>
       </c>
       <c r="C74" t="s">
         <v>117</v>
@@ -1721,7 +1724,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="4">
-        <v>44664</v>
+        <v>45714</v>
       </c>
       <c r="C75" t="s">
         <v>118</v>
@@ -1732,7 +1735,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="4">
-        <v>44665</v>
+        <v>45715</v>
       </c>
       <c r="C76" t="s">
         <v>119</v>
@@ -1743,7 +1746,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="4">
-        <v>44666</v>
+        <v>45716</v>
       </c>
       <c r="C77" t="s">
         <v>120</v>
@@ -1754,7 +1757,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="4">
-        <v>44667</v>
+        <v>45717</v>
       </c>
       <c r="C78" t="s">
         <v>121</v>
@@ -1765,7 +1768,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="4">
-        <v>44668</v>
+        <v>45718</v>
       </c>
       <c r="C79" t="s">
         <v>127</v>
@@ -1776,7 +1779,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="4">
-        <v>44669</v>
+        <v>45719</v>
       </c>
       <c r="C80" t="s">
         <v>123</v>
@@ -1790,7 +1793,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="4">
-        <v>44670</v>
+        <v>45720</v>
       </c>
       <c r="C81" t="s">
         <v>124</v>
@@ -1801,7 +1804,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="4">
-        <v>44671</v>
+        <v>45721</v>
       </c>
       <c r="C82" t="s">
         <v>126</v>
@@ -1812,7 +1815,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="4">
-        <v>44672</v>
+        <v>45722</v>
       </c>
       <c r="C83" t="s">
         <v>125</v>
@@ -1829,7 +1832,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="4">
-        <v>44673</v>
+        <v>45723</v>
       </c>
       <c r="C84" t="s">
         <v>130</v>
@@ -1840,7 +1843,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="4">
-        <v>44674</v>
+        <v>45724</v>
       </c>
       <c r="C85" t="s">
         <v>131</v>
@@ -1857,7 +1860,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="4">
-        <v>44675</v>
+        <v>45725</v>
       </c>
       <c r="C86" t="s">
         <v>134</v>
@@ -1868,7 +1871,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="4">
-        <v>44676</v>
+        <v>45726</v>
       </c>
       <c r="C87" t="s">
         <v>135</v>
@@ -1879,7 +1882,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="4">
-        <v>44677</v>
+        <v>45727</v>
       </c>
       <c r="C88" t="s">
         <v>46</v>
@@ -1890,7 +1893,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="4">
-        <v>44678</v>
+        <v>45728</v>
       </c>
       <c r="C89" t="s">
         <v>136</v>
@@ -1901,7 +1904,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="4">
-        <v>44679</v>
+        <v>45729</v>
       </c>
       <c r="C90" t="s">
         <v>137</v>
@@ -1912,7 +1915,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="4">
-        <v>44680</v>
+        <v>45730</v>
       </c>
       <c r="C91" t="s">
         <v>138</v>
@@ -1923,7 +1926,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="4">
-        <v>44681</v>
+        <v>45731</v>
       </c>
       <c r="C92" t="s">
         <v>92</v>
@@ -1934,7 +1937,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="4">
-        <v>44682</v>
+        <v>45732</v>
       </c>
       <c r="C93" t="s">
         <v>139</v>
@@ -1945,7 +1948,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="4">
-        <v>44683</v>
+        <v>45733</v>
       </c>
       <c r="C94" t="s">
         <v>140</v>
@@ -1959,7 +1962,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="4">
-        <v>44684</v>
+        <v>45734</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -1970,7 +1973,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="4">
-        <v>44685</v>
+        <v>45735</v>
       </c>
       <c r="C96" t="s">
         <v>8</v>
@@ -1981,7 +1984,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="4">
-        <v>44686</v>
+        <v>45736</v>
       </c>
       <c r="C97" t="s">
         <v>8</v>
@@ -1992,7 +1995,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="4">
-        <v>44687</v>
+        <v>45737</v>
       </c>
       <c r="C98" t="s">
         <v>8</v>
@@ -2003,7 +2006,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="4">
-        <v>44688</v>
+        <v>45738</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -2014,7 +2017,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="4">
-        <v>44689</v>
+        <v>45739</v>
       </c>
       <c r="C100" t="s">
         <v>8</v>
@@ -2025,7 +2028,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="4">
-        <v>44690</v>
+        <v>45740</v>
       </c>
       <c r="C101" t="s">
         <v>8</v>
@@ -2036,7 +2039,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="4">
-        <v>44691</v>
+        <v>45741</v>
       </c>
       <c r="C102" t="s">
         <v>8</v>
@@ -2047,7 +2050,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="4">
-        <v>44692</v>
+        <v>45742</v>
       </c>
       <c r="C103" t="s">
         <v>8</v>
@@ -2058,7 +2061,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="4">
-        <v>44693</v>
+        <v>45743</v>
       </c>
       <c r="C104" t="s">
         <v>8</v>
@@ -2069,7 +2072,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="4">
-        <v>44694</v>
+        <v>45744</v>
       </c>
       <c r="C105" t="s">
         <v>8</v>
@@ -2080,7 +2083,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="4">
-        <v>44695</v>
+        <v>45745</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -2091,7 +2094,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="4">
-        <v>44696</v>
+        <v>45746</v>
       </c>
       <c r="C107" t="s">
         <v>8</v>
@@ -2102,7 +2105,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="4">
-        <v>44697</v>
+        <v>45747</v>
       </c>
       <c r="C108" t="s">
         <v>8</v>
@@ -2113,7 +2116,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="4">
-        <v>44698</v>
+        <v>45748</v>
       </c>
       <c r="C109" t="s">
         <v>8</v>
@@ -2124,7 +2127,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="4">
-        <v>44699</v>
+        <v>45749</v>
       </c>
       <c r="C110" t="s">
         <v>8</v>
@@ -2135,7 +2138,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="4">
-        <v>44700</v>
+        <v>45750</v>
       </c>
       <c r="C111" t="s">
         <v>8</v>
@@ -2146,7 +2149,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="4">
-        <v>44701</v>
+        <v>45751</v>
       </c>
       <c r="C112" t="s">
         <v>8</v>
@@ -2157,7 +2160,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="4">
-        <v>44702</v>
+        <v>45752</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -2168,7 +2171,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="4">
-        <v>44703</v>
+        <v>45753</v>
       </c>
       <c r="C114" t="s">
         <v>8</v>
@@ -2179,7 +2182,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="4">
-        <v>44704</v>
+        <v>45754</v>
       </c>
       <c r="C115" t="s">
         <v>8</v>
@@ -2190,7 +2193,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="4">
-        <v>44705</v>
+        <v>45755</v>
       </c>
       <c r="C116" t="s">
         <v>8</v>
@@ -2201,7 +2204,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="4">
-        <v>44706</v>
+        <v>45756</v>
       </c>
       <c r="C117" t="s">
         <v>8</v>
@@ -2212,7 +2215,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="4">
-        <v>44707</v>
+        <v>45757</v>
       </c>
       <c r="C118" t="s">
         <v>47</v>
@@ -2223,7 +2226,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="4">
-        <v>44708</v>
+        <v>45758</v>
       </c>
       <c r="C119" t="s">
         <v>8</v>
@@ -2234,7 +2237,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="4">
-        <v>44709</v>
+        <v>45759</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -2245,7 +2248,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="4">
-        <v>44710</v>
+        <v>45760</v>
       </c>
       <c r="C121" t="s">
         <v>8</v>
@@ -2256,7 +2259,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="4">
-        <v>44711</v>
+        <v>45761</v>
       </c>
       <c r="C122" t="s">
         <v>93</v>
@@ -2267,7 +2270,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="4">
-        <v>44712</v>
+        <v>45762</v>
       </c>
       <c r="C123" t="s">
         <v>8</v>
@@ -2278,7 +2281,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="4">
-        <v>44713</v>
+        <v>45763</v>
       </c>
       <c r="C124" t="s">
         <v>8</v>
@@ -2289,7 +2292,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="4">
-        <v>44714</v>
+        <v>45764</v>
       </c>
       <c r="C125" t="s">
         <v>8</v>
@@ -2300,7 +2303,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="4">
-        <v>44715</v>
+        <v>45765</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
@@ -2311,7 +2314,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="4">
-        <v>44716</v>
+        <v>45766</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -2322,7 +2325,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="4">
-        <v>44717</v>
+        <v>45767</v>
       </c>
       <c r="C128" t="s">
         <v>8</v>
@@ -2333,7 +2336,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="4">
-        <v>44718</v>
+        <v>45768</v>
       </c>
       <c r="C129" t="s">
         <v>8</v>
@@ -2344,7 +2347,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="4">
-        <v>44719</v>
+        <v>45769</v>
       </c>
       <c r="C130" t="s">
         <v>8</v>
@@ -2355,7 +2358,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="4">
-        <v>44720</v>
+        <v>45770</v>
       </c>
       <c r="C131" t="s">
         <v>8</v>
@@ -2366,7 +2369,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="4">
-        <v>44721</v>
+        <v>45771</v>
       </c>
       <c r="C132" t="s">
         <v>8</v>
@@ -2377,7 +2380,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="4">
-        <v>44722</v>
+        <v>45772</v>
       </c>
       <c r="C133" t="s">
         <v>8</v>
@@ -2388,7 +2391,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="4">
-        <v>44723</v>
+        <v>45773</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -2399,7 +2402,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="4">
-        <v>44724</v>
+        <v>45774</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
@@ -2410,7 +2413,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="4">
-        <v>44725</v>
+        <v>45775</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
@@ -2421,7 +2424,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="4">
-        <v>44726</v>
+        <v>45776</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
@@ -2432,7 +2435,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="4">
-        <v>44727</v>
+        <v>45777</v>
       </c>
       <c r="C138" t="s">
         <v>8</v>
@@ -2443,7 +2446,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="4">
-        <v>44728</v>
+        <v>45778</v>
       </c>
       <c r="C139" t="s">
         <v>8</v>
@@ -2454,7 +2457,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="4">
-        <v>44729</v>
+        <v>45779</v>
       </c>
       <c r="C140" t="s">
         <v>8</v>
@@ -2465,7 +2468,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="4">
-        <v>44730</v>
+        <v>45780</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -2476,7 +2479,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="4">
-        <v>44731</v>
+        <v>45781</v>
       </c>
       <c r="C142" t="s">
         <v>8</v>
@@ -2487,7 +2490,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="4">
-        <v>44732</v>
+        <v>45782</v>
       </c>
       <c r="C143" t="s">
         <v>8</v>
@@ -2498,7 +2501,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="4">
-        <v>44733</v>
+        <v>45783</v>
       </c>
       <c r="C144" t="s">
         <v>8</v>
@@ -2509,7 +2512,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="4">
-        <v>44734</v>
+        <v>45784</v>
       </c>
       <c r="C145" t="s">
         <v>8</v>
@@ -2520,7 +2523,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="4">
-        <v>44735</v>
+        <v>45785</v>
       </c>
       <c r="C146" t="s">
         <v>8</v>
@@ -2531,7 +2534,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="4">
-        <v>44736</v>
+        <v>45786</v>
       </c>
       <c r="C147" t="s">
         <v>8</v>
@@ -2542,7 +2545,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="4">
-        <v>44737</v>
+        <v>45787</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -2553,7 +2556,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="4">
-        <v>44738</v>
+        <v>45788</v>
       </c>
       <c r="C149" t="s">
         <v>48</v>
@@ -2564,7 +2567,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="4">
-        <v>44739</v>
+        <v>45789</v>
       </c>
       <c r="C150" t="s">
         <v>8</v>
@@ -2575,7 +2578,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="4">
-        <v>44740</v>
+        <v>45790</v>
       </c>
       <c r="C151" t="s">
         <v>8</v>
@@ -2586,7 +2589,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="4">
-        <v>44741</v>
+        <v>45791</v>
       </c>
       <c r="C152" t="s">
         <v>8</v>
@@ -2597,7 +2600,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="4">
-        <v>44742</v>
+        <v>45792</v>
       </c>
       <c r="C153" t="s">
         <v>94</v>
@@ -2608,7 +2611,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="4">
-        <v>44743</v>
+        <v>45793</v>
       </c>
       <c r="C154" t="s">
         <v>8</v>
@@ -2619,7 +2622,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="4">
-        <v>44744</v>
+        <v>45794</v>
       </c>
       <c r="C155" t="s">
         <v>8</v>
@@ -2630,7 +2633,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="4">
-        <v>44745</v>
+        <v>45795</v>
       </c>
       <c r="C156" t="s">
         <v>8</v>
@@ -2641,7 +2644,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="4">
-        <v>44746</v>
+        <v>45796</v>
       </c>
       <c r="C157" t="s">
         <v>8</v>
@@ -2652,7 +2655,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="4">
-        <v>44747</v>
+        <v>45797</v>
       </c>
       <c r="C158" t="s">
         <v>8</v>
@@ -2663,7 +2666,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="4">
-        <v>44748</v>
+        <v>45798</v>
       </c>
       <c r="C159" t="s">
         <v>8</v>
@@ -2674,7 +2677,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="4">
-        <v>44749</v>
+        <v>45799</v>
       </c>
       <c r="C160" t="s">
         <v>8</v>
@@ -2685,7 +2688,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="4">
-        <v>44750</v>
+        <v>45800</v>
       </c>
       <c r="C161" t="s">
         <v>8</v>
@@ -2696,7 +2699,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="4">
-        <v>44751</v>
+        <v>45801</v>
       </c>
       <c r="C162" t="s">
         <v>8</v>
@@ -2707,7 +2710,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="4">
-        <v>44752</v>
+        <v>45802</v>
       </c>
       <c r="C163" t="s">
         <v>8</v>
@@ -2718,7 +2721,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="4">
-        <v>44753</v>
+        <v>45803</v>
       </c>
       <c r="C164" t="s">
         <v>8</v>
@@ -2729,7 +2732,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="4">
-        <v>44754</v>
+        <v>45804</v>
       </c>
       <c r="C165" t="s">
         <v>8</v>
@@ -2740,7 +2743,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="4">
-        <v>44755</v>
+        <v>45805</v>
       </c>
       <c r="C166" t="s">
         <v>8</v>
@@ -2751,7 +2754,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="4">
-        <v>44756</v>
+        <v>45806</v>
       </c>
       <c r="C167" t="s">
         <v>8</v>
@@ -2762,7 +2765,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="4">
-        <v>44757</v>
+        <v>45807</v>
       </c>
       <c r="C168" t="s">
         <v>8</v>
@@ -2773,7 +2776,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="4">
-        <v>44758</v>
+        <v>45808</v>
       </c>
       <c r="C169" t="s">
         <v>8</v>
@@ -2784,7 +2787,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="4">
-        <v>44759</v>
+        <v>45809</v>
       </c>
       <c r="C170" t="s">
         <v>8</v>
@@ -2795,7 +2798,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="4">
-        <v>44760</v>
+        <v>45810</v>
       </c>
       <c r="C171" t="s">
         <v>8</v>
@@ -2806,7 +2809,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="4">
-        <v>44761</v>
+        <v>45811</v>
       </c>
       <c r="C172" t="s">
         <v>8</v>
@@ -2817,7 +2820,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="4">
-        <v>44762</v>
+        <v>45812</v>
       </c>
       <c r="C173" t="s">
         <v>8</v>
@@ -2828,7 +2831,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="4">
-        <v>44763</v>
+        <v>45813</v>
       </c>
       <c r="C174" t="s">
         <v>8</v>
@@ -2839,7 +2842,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="4">
-        <v>44764</v>
+        <v>45814</v>
       </c>
       <c r="C175" t="s">
         <v>8</v>
@@ -2850,7 +2853,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="4">
-        <v>44765</v>
+        <v>45815</v>
       </c>
       <c r="C176" t="s">
         <v>8</v>
@@ -2861,7 +2864,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="4">
-        <v>44766</v>
+        <v>45816</v>
       </c>
       <c r="C177" t="s">
         <v>8</v>
@@ -2872,7 +2875,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="4">
-        <v>44767</v>
+        <v>45817</v>
       </c>
       <c r="C178" t="s">
         <v>8</v>
@@ -2883,7 +2886,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="4">
-        <v>44768</v>
+        <v>45818</v>
       </c>
       <c r="C179" t="s">
         <v>49</v>
@@ -2894,7 +2897,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="4">
-        <v>44769</v>
+        <v>45819</v>
       </c>
       <c r="C180" t="s">
         <v>8</v>
@@ -2905,7 +2908,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="4">
-        <v>44770</v>
+        <v>45820</v>
       </c>
       <c r="C181" t="s">
         <v>8</v>
@@ -2916,7 +2919,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="4">
-        <v>44771</v>
+        <v>45821</v>
       </c>
       <c r="C182" t="s">
         <v>8</v>
@@ -2927,7 +2930,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="4">
-        <v>44772</v>
+        <v>45822</v>
       </c>
       <c r="C183" t="s">
         <v>95</v>
@@ -2938,7 +2941,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="4">
-        <v>44773</v>
+        <v>45823</v>
       </c>
       <c r="C184" t="s">
         <v>8</v>
@@ -2949,7 +2952,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="4">
-        <v>44774</v>
+        <v>45824</v>
       </c>
       <c r="C185" t="s">
         <v>8</v>
@@ -2960,7 +2963,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="4">
-        <v>44775</v>
+        <v>45825</v>
       </c>
       <c r="C186" t="s">
         <v>8</v>
@@ -2971,7 +2974,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="4">
-        <v>44776</v>
+        <v>45826</v>
       </c>
       <c r="C187" t="s">
         <v>8</v>
@@ -2982,7 +2985,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="4">
-        <v>44777</v>
+        <v>45827</v>
       </c>
       <c r="C188" t="s">
         <v>8</v>
@@ -2993,7 +2996,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="4">
-        <v>44778</v>
+        <v>45828</v>
       </c>
       <c r="C189" t="s">
         <v>8</v>
@@ -3004,7 +3007,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="4">
-        <v>44779</v>
+        <v>45829</v>
       </c>
       <c r="C190" t="s">
         <v>8</v>
@@ -3015,7 +3018,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="4">
-        <v>44780</v>
+        <v>45830</v>
       </c>
       <c r="C191" t="s">
         <v>8</v>
@@ -3026,7 +3029,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="4">
-        <v>44781</v>
+        <v>45831</v>
       </c>
       <c r="C192" t="s">
         <v>8</v>
@@ -3037,7 +3040,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="4">
-        <v>44782</v>
+        <v>45832</v>
       </c>
       <c r="C193" t="s">
         <v>8</v>
@@ -3048,7 +3051,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="4">
-        <v>44783</v>
+        <v>45833</v>
       </c>
       <c r="C194" t="s">
         <v>8</v>
@@ -3059,7 +3062,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="4">
-        <v>44784</v>
+        <v>45834</v>
       </c>
       <c r="C195" t="s">
         <v>8</v>
@@ -3070,7 +3073,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="4">
-        <v>44785</v>
+        <v>45835</v>
       </c>
       <c r="C196" t="s">
         <v>8</v>
@@ -3081,7 +3084,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="4">
-        <v>44786</v>
+        <v>45836</v>
       </c>
       <c r="C197" t="s">
         <v>8</v>
@@ -3092,7 +3095,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="4">
-        <v>44787</v>
+        <v>45837</v>
       </c>
       <c r="C198" t="s">
         <v>8</v>
@@ -3103,7 +3106,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="4">
-        <v>44788</v>
+        <v>45838</v>
       </c>
       <c r="C199" t="s">
         <v>8</v>
@@ -3114,7 +3117,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="4">
-        <v>44789</v>
+        <v>45839</v>
       </c>
       <c r="C200" t="s">
         <v>8</v>
@@ -3125,7 +3128,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="4">
-        <v>44790</v>
+        <v>45840</v>
       </c>
       <c r="C201" t="s">
         <v>8</v>
@@ -3136,7 +3139,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="4">
-        <v>44791</v>
+        <v>45841</v>
       </c>
       <c r="C202" t="s">
         <v>8</v>
@@ -3147,7 +3150,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="4">
-        <v>44792</v>
+        <v>45842</v>
       </c>
       <c r="C203" t="s">
         <v>8</v>
@@ -3158,7 +3161,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="4">
-        <v>44793</v>
+        <v>45843</v>
       </c>
       <c r="C204" t="s">
         <v>8</v>
@@ -3169,7 +3172,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="4">
-        <v>44794</v>
+        <v>45844</v>
       </c>
       <c r="C205" t="s">
         <v>8</v>
@@ -3180,7 +3183,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="4">
-        <v>44795</v>
+        <v>45845</v>
       </c>
       <c r="C206" t="s">
         <v>8</v>
@@ -3191,7 +3194,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="4">
-        <v>44796</v>
+        <v>45846</v>
       </c>
       <c r="C207" t="s">
         <v>8</v>
@@ -3202,7 +3205,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="4">
-        <v>44797</v>
+        <v>45847</v>
       </c>
       <c r="C208" t="s">
         <v>8</v>
@@ -3213,7 +3216,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="4">
-        <v>44798</v>
+        <v>45848</v>
       </c>
       <c r="C209" t="s">
         <v>8</v>
@@ -3224,7 +3227,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="4">
-        <v>44799</v>
+        <v>45849</v>
       </c>
       <c r="C210" t="s">
         <v>50</v>
@@ -3235,7 +3238,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="4">
-        <v>44800</v>
+        <v>45850</v>
       </c>
       <c r="C211" t="s">
         <v>8</v>
@@ -3246,7 +3249,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="4">
-        <v>44801</v>
+        <v>45851</v>
       </c>
       <c r="C212" t="s">
         <v>8</v>
@@ -3257,7 +3260,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="4">
-        <v>44802</v>
+        <v>45852</v>
       </c>
       <c r="C213" t="s">
         <v>8</v>
@@ -3268,7 +3271,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="4">
-        <v>44803</v>
+        <v>45853</v>
       </c>
       <c r="C214" t="s">
         <v>96</v>
@@ -3279,7 +3282,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="4">
-        <v>44804</v>
+        <v>45854</v>
       </c>
       <c r="C215" t="s">
         <v>8</v>
@@ -3290,7 +3293,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="4">
-        <v>44805</v>
+        <v>45855</v>
       </c>
       <c r="C216" t="s">
         <v>8</v>
@@ -3301,7 +3304,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="4">
-        <v>44806</v>
+        <v>45856</v>
       </c>
       <c r="C217" t="s">
         <v>8</v>
@@ -3312,7 +3315,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="4">
-        <v>44807</v>
+        <v>45857</v>
       </c>
       <c r="C218" t="s">
         <v>8</v>
@@ -3323,7 +3326,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="4">
-        <v>44808</v>
+        <v>45858</v>
       </c>
       <c r="C219" t="s">
         <v>8</v>
@@ -3334,7 +3337,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="4">
-        <v>44809</v>
+        <v>45859</v>
       </c>
       <c r="C220" t="s">
         <v>8</v>
@@ -3345,7 +3348,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="4">
-        <v>44810</v>
+        <v>45860</v>
       </c>
       <c r="C221" t="s">
         <v>8</v>
@@ -3356,7 +3359,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="4">
-        <v>44811</v>
+        <v>45861</v>
       </c>
       <c r="C222" t="s">
         <v>8</v>
@@ -3367,7 +3370,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="4">
-        <v>44812</v>
+        <v>45862</v>
       </c>
       <c r="C223" t="s">
         <v>8</v>
@@ -3378,7 +3381,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="4">
-        <v>44813</v>
+        <v>45863</v>
       </c>
       <c r="C224" t="s">
         <v>8</v>
@@ -3389,7 +3392,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="4">
-        <v>44814</v>
+        <v>45864</v>
       </c>
       <c r="C225" t="s">
         <v>8</v>
@@ -3400,7 +3403,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="4">
-        <v>44815</v>
+        <v>45865</v>
       </c>
       <c r="C226" t="s">
         <v>8</v>
@@ -3411,7 +3414,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="4">
-        <v>44816</v>
+        <v>45866</v>
       </c>
       <c r="C227" t="s">
         <v>8</v>
@@ -3422,7 +3425,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="4">
-        <v>44817</v>
+        <v>45867</v>
       </c>
       <c r="C228" t="s">
         <v>8</v>
@@ -3433,7 +3436,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="4">
-        <v>44818</v>
+        <v>45868</v>
       </c>
       <c r="C229" t="s">
         <v>8</v>
@@ -3444,7 +3447,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="4">
-        <v>44819</v>
+        <v>45869</v>
       </c>
       <c r="C230" t="s">
         <v>8</v>
@@ -3455,7 +3458,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="4">
-        <v>44820</v>
+        <v>45870</v>
       </c>
       <c r="C231" t="s">
         <v>8</v>
@@ -3466,7 +3469,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="4">
-        <v>44821</v>
+        <v>45871</v>
       </c>
       <c r="C232" t="s">
         <v>8</v>
@@ -3477,7 +3480,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="4">
-        <v>44822</v>
+        <v>45872</v>
       </c>
       <c r="C233" t="s">
         <v>8</v>
@@ -3488,7 +3491,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="4">
-        <v>44823</v>
+        <v>45873</v>
       </c>
       <c r="C234" t="s">
         <v>8</v>
@@ -3499,7 +3502,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="4">
-        <v>44824</v>
+        <v>45874</v>
       </c>
       <c r="C235" t="s">
         <v>8</v>
@@ -3510,7 +3513,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="4">
-        <v>44825</v>
+        <v>45875</v>
       </c>
       <c r="C236" t="s">
         <v>8</v>
@@ -3521,7 +3524,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="4">
-        <v>44826</v>
+        <v>45876</v>
       </c>
       <c r="C237" t="s">
         <v>8</v>
@@ -3532,7 +3535,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="4">
-        <v>44827</v>
+        <v>45877</v>
       </c>
       <c r="C238" t="s">
         <v>8</v>
@@ -3543,7 +3546,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="4">
-        <v>44828</v>
+        <v>45878</v>
       </c>
       <c r="C239" t="s">
         <v>8</v>
@@ -3554,7 +3557,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="4">
-        <v>44829</v>
+        <v>45879</v>
       </c>
       <c r="C240" t="s">
         <v>8</v>
@@ -3565,7 +3568,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="4">
-        <v>44830</v>
+        <v>45880</v>
       </c>
       <c r="C241" t="s">
         <v>51</v>
@@ -3576,7 +3579,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="4">
-        <v>44831</v>
+        <v>45881</v>
       </c>
       <c r="C242" t="s">
         <v>8</v>
@@ -3587,7 +3590,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="4">
-        <v>44832</v>
+        <v>45882</v>
       </c>
       <c r="C243" t="s">
         <v>8</v>
@@ -3598,7 +3601,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="4">
-        <v>44833</v>
+        <v>45883</v>
       </c>
       <c r="C244" t="s">
         <v>8</v>
@@ -3609,7 +3612,7 @@
         <v>244</v>
       </c>
       <c r="B245" s="4">
-        <v>44834</v>
+        <v>45884</v>
       </c>
       <c r="C245" t="s">
         <v>97</v>
@@ -3620,7 +3623,7 @@
         <v>245</v>
       </c>
       <c r="B246" s="4">
-        <v>44835</v>
+        <v>45885</v>
       </c>
       <c r="C246" t="s">
         <v>8</v>
@@ -3631,7 +3634,7 @@
         <v>246</v>
       </c>
       <c r="B247" s="4">
-        <v>44836</v>
+        <v>45886</v>
       </c>
       <c r="C247" t="s">
         <v>8</v>
@@ -3642,7 +3645,7 @@
         <v>247</v>
       </c>
       <c r="B248" s="4">
-        <v>44837</v>
+        <v>45887</v>
       </c>
       <c r="C248" t="s">
         <v>8</v>
@@ -3653,7 +3656,7 @@
         <v>248</v>
       </c>
       <c r="B249" s="4">
-        <v>44838</v>
+        <v>45888</v>
       </c>
       <c r="C249" t="s">
         <v>8</v>
@@ -3664,7 +3667,7 @@
         <v>249</v>
       </c>
       <c r="B250" s="4">
-        <v>44839</v>
+        <v>45889</v>
       </c>
       <c r="C250" t="s">
         <v>8</v>
@@ -3675,7 +3678,7 @@
         <v>250</v>
       </c>
       <c r="B251" s="4">
-        <v>44840</v>
+        <v>45890</v>
       </c>
       <c r="C251" t="s">
         <v>8</v>
@@ -3686,7 +3689,7 @@
         <v>251</v>
       </c>
       <c r="B252" s="4">
-        <v>44841</v>
+        <v>45891</v>
       </c>
       <c r="C252" t="s">
         <v>8</v>
@@ -3697,7 +3700,7 @@
         <v>252</v>
       </c>
       <c r="B253" s="4">
-        <v>44842</v>
+        <v>45892</v>
       </c>
       <c r="C253" t="s">
         <v>8</v>
@@ -3708,7 +3711,7 @@
         <v>253</v>
       </c>
       <c r="B254" s="4">
-        <v>44843</v>
+        <v>45893</v>
       </c>
       <c r="C254" t="s">
         <v>8</v>
@@ -3719,7 +3722,7 @@
         <v>254</v>
       </c>
       <c r="B255" s="4">
-        <v>44844</v>
+        <v>45894</v>
       </c>
       <c r="C255" t="s">
         <v>8</v>
@@ -3730,7 +3733,7 @@
         <v>255</v>
       </c>
       <c r="B256" s="4">
-        <v>44845</v>
+        <v>45895</v>
       </c>
       <c r="C256" t="s">
         <v>8</v>
@@ -3741,7 +3744,7 @@
         <v>256</v>
       </c>
       <c r="B257" s="4">
-        <v>44846</v>
+        <v>45896</v>
       </c>
       <c r="C257" t="s">
         <v>8</v>
@@ -3752,7 +3755,7 @@
         <v>257</v>
       </c>
       <c r="B258" s="4">
-        <v>44847</v>
+        <v>45897</v>
       </c>
       <c r="C258" t="s">
         <v>8</v>
@@ -3763,7 +3766,7 @@
         <v>258</v>
       </c>
       <c r="B259" s="4">
-        <v>44848</v>
+        <v>45898</v>
       </c>
       <c r="C259" t="s">
         <v>8</v>
@@ -3774,7 +3777,7 @@
         <v>259</v>
       </c>
       <c r="B260" s="4">
-        <v>44849</v>
+        <v>45899</v>
       </c>
       <c r="C260" t="s">
         <v>8</v>
@@ -3785,7 +3788,7 @@
         <v>260</v>
       </c>
       <c r="B261" s="4">
-        <v>44850</v>
+        <v>45900</v>
       </c>
       <c r="C261" t="s">
         <v>8</v>
@@ -3796,7 +3799,7 @@
         <v>261</v>
       </c>
       <c r="B262" s="4">
-        <v>44851</v>
+        <v>45901</v>
       </c>
       <c r="C262" t="s">
         <v>8</v>
@@ -3807,7 +3810,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="4">
-        <v>44852</v>
+        <v>45902</v>
       </c>
       <c r="C263" t="s">
         <v>8</v>
@@ -3818,7 +3821,7 @@
         <v>263</v>
       </c>
       <c r="B264" s="4">
-        <v>44853</v>
+        <v>45903</v>
       </c>
       <c r="C264" t="s">
         <v>8</v>
@@ -3829,7 +3832,7 @@
         <v>264</v>
       </c>
       <c r="B265" s="4">
-        <v>44854</v>
+        <v>45904</v>
       </c>
       <c r="C265" t="s">
         <v>8</v>
@@ -3840,7 +3843,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="4">
-        <v>44855</v>
+        <v>45905</v>
       </c>
       <c r="C266" t="s">
         <v>8</v>
@@ -3851,7 +3854,7 @@
         <v>266</v>
       </c>
       <c r="B267" s="4">
-        <v>44856</v>
+        <v>45906</v>
       </c>
       <c r="C267" t="s">
         <v>8</v>
@@ -3862,7 +3865,7 @@
         <v>267</v>
       </c>
       <c r="B268" s="4">
-        <v>44857</v>
+        <v>45907</v>
       </c>
       <c r="C268" t="s">
         <v>8</v>
@@ -3873,7 +3876,7 @@
         <v>268</v>
       </c>
       <c r="B269" s="4">
-        <v>44858</v>
+        <v>45908</v>
       </c>
       <c r="C269" t="s">
         <v>8</v>
@@ -3884,7 +3887,7 @@
         <v>269</v>
       </c>
       <c r="B270" s="4">
-        <v>44859</v>
+        <v>45909</v>
       </c>
       <c r="C270" t="s">
         <v>8</v>
@@ -3895,7 +3898,7 @@
         <v>270</v>
       </c>
       <c r="B271" s="4">
-        <v>44860</v>
+        <v>45910</v>
       </c>
       <c r="C271" t="s">
         <v>52</v>
@@ -3906,7 +3909,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="4">
-        <v>44861</v>
+        <v>45911</v>
       </c>
       <c r="C272" t="s">
         <v>8</v>
@@ -3917,7 +3920,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="4">
-        <v>44862</v>
+        <v>45912</v>
       </c>
       <c r="C273" t="s">
         <v>8</v>
@@ -3928,7 +3931,7 @@
         <v>273</v>
       </c>
       <c r="B274" s="4">
-        <v>44863</v>
+        <v>45913</v>
       </c>
       <c r="C274" t="s">
         <v>8</v>
@@ -3939,7 +3942,7 @@
         <v>274</v>
       </c>
       <c r="B275" s="4">
-        <v>44864</v>
+        <v>45914</v>
       </c>
       <c r="C275" t="s">
         <v>98</v>
@@ -3950,7 +3953,7 @@
         <v>275</v>
       </c>
       <c r="B276" s="4">
-        <v>44865</v>
+        <v>45915</v>
       </c>
       <c r="C276" t="s">
         <v>8</v>
@@ -3961,7 +3964,7 @@
         <v>276</v>
       </c>
       <c r="B277" s="4">
-        <v>44866</v>
+        <v>45916</v>
       </c>
       <c r="C277" t="s">
         <v>8</v>
@@ -3972,7 +3975,7 @@
         <v>277</v>
       </c>
       <c r="B278" s="4">
-        <v>44867</v>
+        <v>45917</v>
       </c>
       <c r="C278" t="s">
         <v>8</v>
@@ -3983,7 +3986,7 @@
         <v>278</v>
       </c>
       <c r="B279" s="4">
-        <v>44868</v>
+        <v>45918</v>
       </c>
       <c r="C279" t="s">
         <v>8</v>
@@ -3994,7 +3997,7 @@
         <v>279</v>
       </c>
       <c r="B280" s="4">
-        <v>44869</v>
+        <v>45919</v>
       </c>
       <c r="C280" t="s">
         <v>8</v>
@@ -4005,7 +4008,7 @@
         <v>280</v>
       </c>
       <c r="B281" s="4">
-        <v>44870</v>
+        <v>45920</v>
       </c>
       <c r="C281" t="s">
         <v>8</v>
@@ -4016,7 +4019,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="4">
-        <v>44871</v>
+        <v>45921</v>
       </c>
       <c r="C282" t="s">
         <v>8</v>
@@ -4027,7 +4030,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="4">
-        <v>44872</v>
+        <v>45922</v>
       </c>
       <c r="C283" t="s">
         <v>8</v>
@@ -4038,7 +4041,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="4">
-        <v>44873</v>
+        <v>45923</v>
       </c>
       <c r="C284" t="s">
         <v>8</v>
@@ -4049,7 +4052,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="4">
-        <v>44874</v>
+        <v>45924</v>
       </c>
       <c r="C285" t="s">
         <v>8</v>
@@ -4060,7 +4063,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="4">
-        <v>44875</v>
+        <v>45925</v>
       </c>
       <c r="C286" t="s">
         <v>8</v>
@@ -4071,7 +4074,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="4">
-        <v>44876</v>
+        <v>45926</v>
       </c>
       <c r="C287" t="s">
         <v>8</v>
@@ -4082,7 +4085,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="4">
-        <v>44877</v>
+        <v>45927</v>
       </c>
       <c r="C288" t="s">
         <v>8</v>
@@ -4093,7 +4096,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="4">
-        <v>44878</v>
+        <v>45928</v>
       </c>
       <c r="C289" t="s">
         <v>8</v>
@@ -4104,7 +4107,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="4">
-        <v>44879</v>
+        <v>45929</v>
       </c>
       <c r="C290" t="s">
         <v>8</v>
@@ -4115,7 +4118,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="4">
-        <v>44880</v>
+        <v>45930</v>
       </c>
       <c r="C291" t="s">
         <v>8</v>
@@ -4126,7 +4129,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="4">
-        <v>44881</v>
+        <v>45931</v>
       </c>
       <c r="C292" t="s">
         <v>8</v>
@@ -4137,7 +4140,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="4">
-        <v>44882</v>
+        <v>45932</v>
       </c>
       <c r="C293" t="s">
         <v>8</v>
@@ -4148,7 +4151,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="4">
-        <v>44883</v>
+        <v>45933</v>
       </c>
       <c r="C294" t="s">
         <v>8</v>
@@ -4159,7 +4162,7 @@
         <v>294</v>
       </c>
       <c r="B295" s="4">
-        <v>44884</v>
+        <v>45934</v>
       </c>
       <c r="C295" t="s">
         <v>8</v>
@@ -4170,7 +4173,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="4">
-        <v>44885</v>
+        <v>45935</v>
       </c>
       <c r="C296" t="s">
         <v>8</v>
@@ -4181,7 +4184,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="4">
-        <v>44886</v>
+        <v>45936</v>
       </c>
       <c r="C297" t="s">
         <v>8</v>
@@ -4192,7 +4195,7 @@
         <v>297</v>
       </c>
       <c r="B298" s="4">
-        <v>44887</v>
+        <v>45937</v>
       </c>
       <c r="C298" t="s">
         <v>8</v>
@@ -4203,7 +4206,7 @@
         <v>298</v>
       </c>
       <c r="B299" s="4">
-        <v>44888</v>
+        <v>45938</v>
       </c>
       <c r="C299" t="s">
         <v>8</v>
@@ -4214,7 +4217,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="4">
-        <v>44889</v>
+        <v>45939</v>
       </c>
       <c r="C300" t="s">
         <v>8</v>
@@ -4225,7 +4228,7 @@
         <v>300</v>
       </c>
       <c r="B301" s="4">
-        <v>44890</v>
+        <v>45940</v>
       </c>
       <c r="C301" t="s">
         <v>8</v>
@@ -4236,7 +4239,7 @@
         <v>301</v>
       </c>
       <c r="B302" s="4">
-        <v>44891</v>
+        <v>45941</v>
       </c>
       <c r="C302" t="s">
         <v>53</v>
@@ -4247,7 +4250,7 @@
         <v>302</v>
       </c>
       <c r="B303" s="4">
-        <v>44892</v>
+        <v>45942</v>
       </c>
       <c r="C303" t="s">
         <v>8</v>
@@ -4258,7 +4261,7 @@
         <v>303</v>
       </c>
       <c r="B304" s="4">
-        <v>44893</v>
+        <v>45943</v>
       </c>
       <c r="C304" t="s">
         <v>8</v>
@@ -4269,7 +4272,7 @@
         <v>304</v>
       </c>
       <c r="B305" s="4">
-        <v>44894</v>
+        <v>45944</v>
       </c>
       <c r="C305" t="s">
         <v>8</v>
@@ -4280,7 +4283,7 @@
         <v>305</v>
       </c>
       <c r="B306" s="4">
-        <v>44895</v>
+        <v>45945</v>
       </c>
       <c r="C306" t="s">
         <v>99</v>
@@ -4291,7 +4294,7 @@
         <v>306</v>
       </c>
       <c r="B307" s="4">
-        <v>44896</v>
+        <v>45946</v>
       </c>
       <c r="C307" t="s">
         <v>8</v>
@@ -4302,7 +4305,7 @@
         <v>307</v>
       </c>
       <c r="B308" s="4">
-        <v>44897</v>
+        <v>45947</v>
       </c>
       <c r="C308" t="s">
         <v>8</v>
@@ -4313,7 +4316,7 @@
         <v>308</v>
       </c>
       <c r="B309" s="4">
-        <v>44898</v>
+        <v>45948</v>
       </c>
       <c r="C309" t="s">
         <v>8</v>
@@ -4324,7 +4327,7 @@
         <v>309</v>
       </c>
       <c r="B310" s="4">
-        <v>44899</v>
+        <v>45949</v>
       </c>
       <c r="C310" t="s">
         <v>8</v>
@@ -4335,7 +4338,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="4">
-        <v>44900</v>
+        <v>45950</v>
       </c>
       <c r="C311" t="s">
         <v>8</v>
@@ -4346,7 +4349,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="4">
-        <v>44901</v>
+        <v>45951</v>
       </c>
       <c r="C312" t="s">
         <v>8</v>
@@ -4357,7 +4360,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="4">
-        <v>44902</v>
+        <v>45952</v>
       </c>
       <c r="C313" t="s">
         <v>8</v>
@@ -4368,7 +4371,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="4">
-        <v>44903</v>
+        <v>45953</v>
       </c>
       <c r="C314" t="s">
         <v>8</v>
@@ -4379,7 +4382,7 @@
         <v>314</v>
       </c>
       <c r="B315" s="4">
-        <v>44904</v>
+        <v>45954</v>
       </c>
       <c r="C315" t="s">
         <v>8</v>
@@ -4390,7 +4393,7 @@
         <v>315</v>
       </c>
       <c r="B316" s="4">
-        <v>44905</v>
+        <v>45955</v>
       </c>
       <c r="C316" t="s">
         <v>8</v>
@@ -4401,7 +4404,7 @@
         <v>316</v>
       </c>
       <c r="B317" s="4">
-        <v>44906</v>
+        <v>45956</v>
       </c>
       <c r="C317" t="s">
         <v>8</v>
@@ -4412,7 +4415,7 @@
         <v>317</v>
       </c>
       <c r="B318" s="4">
-        <v>44907</v>
+        <v>45957</v>
       </c>
       <c r="C318" t="s">
         <v>8</v>
@@ -4423,7 +4426,7 @@
         <v>318</v>
       </c>
       <c r="B319" s="4">
-        <v>44908</v>
+        <v>45958</v>
       </c>
       <c r="C319" t="s">
         <v>8</v>
@@ -4434,7 +4437,7 @@
         <v>319</v>
       </c>
       <c r="B320" s="4">
-        <v>44909</v>
+        <v>45959</v>
       </c>
       <c r="C320" t="s">
         <v>8</v>
@@ -4445,7 +4448,7 @@
         <v>320</v>
       </c>
       <c r="B321" s="4">
-        <v>44910</v>
+        <v>45960</v>
       </c>
       <c r="C321" t="s">
         <v>8</v>
@@ -4456,7 +4459,7 @@
         <v>321</v>
       </c>
       <c r="B322" s="4">
-        <v>44911</v>
+        <v>45961</v>
       </c>
       <c r="C322" t="s">
         <v>8</v>
@@ -4467,7 +4470,7 @@
         <v>322</v>
       </c>
       <c r="B323" s="4">
-        <v>44912</v>
+        <v>45962</v>
       </c>
       <c r="C323" t="s">
         <v>8</v>
@@ -4478,7 +4481,7 @@
         <v>323</v>
       </c>
       <c r="B324" s="4">
-        <v>44913</v>
+        <v>45963</v>
       </c>
       <c r="C324" t="s">
         <v>8</v>
@@ -4489,7 +4492,7 @@
         <v>324</v>
       </c>
       <c r="B325" s="4">
-        <v>44914</v>
+        <v>45964</v>
       </c>
       <c r="C325" t="s">
         <v>8</v>
@@ -4500,7 +4503,7 @@
         <v>325</v>
       </c>
       <c r="B326" s="4">
-        <v>44915</v>
+        <v>45965</v>
       </c>
       <c r="C326" t="s">
         <v>8</v>
@@ -4511,7 +4514,7 @@
         <v>326</v>
       </c>
       <c r="B327" s="4">
-        <v>44916</v>
+        <v>45966</v>
       </c>
       <c r="C327" t="s">
         <v>8</v>
@@ -4522,7 +4525,7 @@
         <v>327</v>
       </c>
       <c r="B328" s="4">
-        <v>44917</v>
+        <v>45967</v>
       </c>
       <c r="C328" t="s">
         <v>8</v>
@@ -4533,7 +4536,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="4">
-        <v>44918</v>
+        <v>45968</v>
       </c>
       <c r="C329" t="s">
         <v>8</v>
@@ -4544,7 +4547,7 @@
         <v>329</v>
       </c>
       <c r="B330" s="4">
-        <v>44919</v>
+        <v>45969</v>
       </c>
       <c r="C330" t="s">
         <v>8</v>
@@ -4555,7 +4558,7 @@
         <v>330</v>
       </c>
       <c r="B331" s="4">
-        <v>44920</v>
+        <v>45970</v>
       </c>
       <c r="C331" t="s">
         <v>8</v>
@@ -4566,7 +4569,7 @@
         <v>331</v>
       </c>
       <c r="B332" s="4">
-        <v>44921</v>
+        <v>45971</v>
       </c>
       <c r="C332" t="s">
         <v>54</v>
@@ -4577,7 +4580,7 @@
         <v>332</v>
       </c>
       <c r="B333" s="4">
-        <v>44922</v>
+        <v>45972</v>
       </c>
       <c r="C333" t="s">
         <v>8</v>
@@ -4588,7 +4591,7 @@
         <v>333</v>
       </c>
       <c r="B334" s="4">
-        <v>44923</v>
+        <v>45973</v>
       </c>
       <c r="C334" t="s">
         <v>8</v>
@@ -4599,7 +4602,7 @@
         <v>334</v>
       </c>
       <c r="B335" s="4">
-        <v>44924</v>
+        <v>45974</v>
       </c>
       <c r="C335" t="s">
         <v>8</v>
@@ -4610,7 +4613,7 @@
         <v>335</v>
       </c>
       <c r="B336" s="4">
-        <v>44925</v>
+        <v>45975</v>
       </c>
       <c r="C336" t="s">
         <v>100</v>
@@ -4621,7 +4624,7 @@
         <v>336</v>
       </c>
       <c r="B337" s="4">
-        <v>44926</v>
+        <v>45976</v>
       </c>
       <c r="C337" t="s">
         <v>8</v>
@@ -4632,7 +4635,7 @@
         <v>337</v>
       </c>
       <c r="B338" s="4">
-        <v>44927</v>
+        <v>45977</v>
       </c>
       <c r="C338" t="s">
         <v>8</v>
@@ -4643,7 +4646,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="4">
-        <v>44928</v>
+        <v>45978</v>
       </c>
       <c r="C339" t="s">
         <v>8</v>
@@ -4654,7 +4657,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="4">
-        <v>44929</v>
+        <v>45979</v>
       </c>
       <c r="C340" t="s">
         <v>8</v>
@@ -4665,7 +4668,7 @@
         <v>340</v>
       </c>
       <c r="B341" s="4">
-        <v>44930</v>
+        <v>45980</v>
       </c>
       <c r="C341" t="s">
         <v>8</v>
@@ -4676,7 +4679,7 @@
         <v>341</v>
       </c>
       <c r="B342" s="4">
-        <v>44931</v>
+        <v>45981</v>
       </c>
       <c r="C342" t="s">
         <v>8</v>
@@ -4687,7 +4690,7 @@
         <v>342</v>
       </c>
       <c r="B343" s="4">
-        <v>44932</v>
+        <v>45982</v>
       </c>
       <c r="C343" t="s">
         <v>8</v>
@@ -4698,7 +4701,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="4">
-        <v>44933</v>
+        <v>45983</v>
       </c>
       <c r="C344" t="s">
         <v>8</v>
@@ -4709,7 +4712,7 @@
         <v>344</v>
       </c>
       <c r="B345" s="4">
-        <v>44934</v>
+        <v>45984</v>
       </c>
       <c r="C345" t="s">
         <v>8</v>
@@ -4720,7 +4723,7 @@
         <v>345</v>
       </c>
       <c r="B346" s="4">
-        <v>44935</v>
+        <v>45985</v>
       </c>
       <c r="C346" t="s">
         <v>8</v>
@@ -4731,7 +4734,7 @@
         <v>346</v>
       </c>
       <c r="B347" s="4">
-        <v>44936</v>
+        <v>45986</v>
       </c>
       <c r="C347" t="s">
         <v>8</v>
@@ -4742,7 +4745,7 @@
         <v>347</v>
       </c>
       <c r="B348" s="4">
-        <v>44937</v>
+        <v>45987</v>
       </c>
       <c r="C348" t="s">
         <v>8</v>
@@ -4753,7 +4756,7 @@
         <v>348</v>
       </c>
       <c r="B349" s="4">
-        <v>44938</v>
+        <v>45988</v>
       </c>
       <c r="C349" t="s">
         <v>8</v>
@@ -4764,7 +4767,7 @@
         <v>349</v>
       </c>
       <c r="B350" s="4">
-        <v>44939</v>
+        <v>45989</v>
       </c>
       <c r="C350" t="s">
         <v>8</v>
@@ -4775,7 +4778,7 @@
         <v>350</v>
       </c>
       <c r="B351" s="4">
-        <v>44940</v>
+        <v>45990</v>
       </c>
       <c r="C351" t="s">
         <v>8</v>
@@ -4786,7 +4789,7 @@
         <v>351</v>
       </c>
       <c r="B352" s="4">
-        <v>44941</v>
+        <v>45991</v>
       </c>
       <c r="C352" t="s">
         <v>8</v>
@@ -4797,7 +4800,7 @@
         <v>352</v>
       </c>
       <c r="B353" s="4">
-        <v>44942</v>
+        <v>45992</v>
       </c>
       <c r="C353" t="s">
         <v>8</v>
@@ -4808,7 +4811,7 @@
         <v>353</v>
       </c>
       <c r="B354" s="4">
-        <v>44943</v>
+        <v>45993</v>
       </c>
       <c r="C354" t="s">
         <v>8</v>
@@ -4819,7 +4822,7 @@
         <v>354</v>
       </c>
       <c r="B355" s="4">
-        <v>44944</v>
+        <v>45994</v>
       </c>
       <c r="C355" t="s">
         <v>8</v>
@@ -4830,7 +4833,7 @@
         <v>355</v>
       </c>
       <c r="B356" s="4">
-        <v>44945</v>
+        <v>45995</v>
       </c>
       <c r="C356" t="s">
         <v>8</v>
@@ -4841,7 +4844,7 @@
         <v>356</v>
       </c>
       <c r="B357" s="4">
-        <v>44946</v>
+        <v>45996</v>
       </c>
       <c r="C357" t="s">
         <v>8</v>
@@ -4852,7 +4855,7 @@
         <v>357</v>
       </c>
       <c r="B358" s="4">
-        <v>44947</v>
+        <v>45997</v>
       </c>
       <c r="C358" t="s">
         <v>8</v>
@@ -4863,7 +4866,7 @@
         <v>358</v>
       </c>
       <c r="B359" s="4">
-        <v>44948</v>
+        <v>45998</v>
       </c>
       <c r="C359" t="s">
         <v>8</v>
@@ -4874,7 +4877,7 @@
         <v>359</v>
       </c>
       <c r="B360" s="4">
-        <v>44949</v>
+        <v>45999</v>
       </c>
       <c r="C360" t="s">
         <v>8</v>
@@ -4885,7 +4888,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="4">
-        <v>44950</v>
+        <v>46000</v>
       </c>
       <c r="C361" t="s">
         <v>8</v>
@@ -4896,7 +4899,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="4">
-        <v>44951</v>
+        <v>46001</v>
       </c>
       <c r="C362" t="s">
         <v>8</v>
@@ -4908,7 +4911,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="4">
-        <v>44952</v>
+        <v>46002</v>
       </c>
       <c r="C363" t="s">
         <v>55</v>
@@ -4919,7 +4922,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="4">
-        <v>44953</v>
+        <v>46003</v>
       </c>
       <c r="C364" t="s">
         <v>8</v>
@@ -4930,7 +4933,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="4">
-        <v>44954</v>
+        <v>46004</v>
       </c>
       <c r="C365" t="s">
         <v>8</v>
@@ -4941,7 +4944,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="4">
-        <v>44955</v>
+        <v>46005</v>
       </c>
       <c r="C366" t="s">
         <v>8</v>
@@ -4952,7 +4955,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="4">
-        <v>44956</v>
+        <v>46006</v>
       </c>
       <c r="C367" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Noves fotos i fins dia 100
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A60A94D-10E2-4E77-AA69-09DCA8DE6B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B603CB-3F34-40C3-912F-8B71EF9EC2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="171">
   <si>
     <t>Dia</t>
   </si>
@@ -270,9 +270,6 @@
     <t>Aquesta foto és de quan vam anar a Barcelona a veure BARBIEEE</t>
   </si>
   <si>
-    <t>Perquè t'encanta el sushi i algun dia m'ensenyaràs a fer servir els palillos</t>
-  </si>
-  <si>
     <t>Perquè ets molt sincera i transparent</t>
   </si>
   <si>
@@ -342,18 +339,12 @@
     <t>./img/bereal_macarro.jpeg</t>
   </si>
   <si>
-    <t>No sé quant em vas regalar aquest collaret però m'encantaa!</t>
-  </si>
-  <si>
     <t>Perquè fas les millors bromes del món</t>
   </si>
   <si>
     <t>Perquè hem perdones inclús quan et molesto MOOOLT (això no passa mai però bueno)</t>
   </si>
   <si>
-    <t>Perquè fem apostes sobre altres parelles (shhhht però em debs un sopaaar!)</t>
-  </si>
-  <si>
     <t>Perquè em dones pau i em fas sentir a casa, sempre</t>
   </si>
   <si>
@@ -381,9 +372,6 @@
     <t>Perquè  coneixes als meus amics i saps ser amiga dels meus amics</t>
   </si>
   <si>
-    <t>Perquè el teu amor és el meu refugi i la meva força</t>
-  </si>
-  <si>
     <t>./img/colonies.jpeg</t>
   </si>
   <si>
@@ -495,7 +483,61 @@
     <t>Et posso una foto maca de nosaltres dos perquè no t'enfadis (porfa)</t>
   </si>
   <si>
-    <t>./img/cor.png</t>
+    <t>Perquè t'encanta el sushi i algun dia m'ensenyaràs a fer servir els palillos, MENTIDA JA U HAS FET. Això ho pots veure en el vídeo</t>
+  </si>
+  <si>
+    <t>./video/sushi.aprenent.mp4</t>
+  </si>
+  <si>
+    <t>No sé quan em vas regalar aquest collaret però m'encantaa!</t>
+  </si>
+  <si>
+    <t>Perquè fem apostes sobre altres parelles (no t'ho dic molt però em debs un sopaaar!)</t>
+  </si>
+  <si>
+    <t>Perquè ets literalment la MEGAN FOX</t>
+  </si>
+  <si>
+    <t>Perquè sempre ens ho passem bé junts</t>
+  </si>
+  <si>
+    <t>Perquè la teva família m'ha acollit molt</t>
+  </si>
+  <si>
+    <t>Perquè fem viatges MOOOOLT guais (ANDORRAAA)</t>
+  </si>
+  <si>
+    <t>Perquè ets perfecte</t>
+  </si>
+  <si>
+    <t>Perquè juges als meus jocs de mòbil</t>
+  </si>
+  <si>
+    <t>Perquè m'escoltes</t>
+  </si>
+  <si>
+    <t>Perquè vam anar a un concert de JOAN DAUSÀ (no hi ha fotos :( )</t>
+  </si>
+  <si>
+    <t>Perquè ets molt elegant</t>
+  </si>
+  <si>
+    <t>Perquè saps que dir en els moments imprtants</t>
+  </si>
+  <si>
+    <t>El missatge d'ahir era mentida!! Quan et vaig dir t'estimo per primera vegada TU NO VAS DIR JO TAMBÉ T'ESTIMO</t>
+  </si>
+  <si>
+    <t>Perquè ets fàcil de perdonar (per exemple, el missatge d'ahir ja te'l he perdonat)</t>
+  </si>
+  <si>
+    <t>Perquè tens molta memòria, no se si encara et faig jugar al My Singuin Monsters però erets MASSA bona al memory!</t>
+  </si>
+  <si>
+    <t>./img/singuing_monsters.jpeg</t>
+  </si>
+  <si>
+    <t>./img/mirall_andorra1.jpeg</t>
   </si>
 </sst>
 </file>
@@ -543,13 +585,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,7 +908,7 @@
   <dimension ref="A1:H441"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C353" sqref="C353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,10 +945,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>45669</v>
+        <v>45687</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -916,7 +957,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -924,10 +965,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>45670</v>
+        <v>45688</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -938,13 +979,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>45671</v>
+        <v>45689</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -953,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>45672</v>
+        <v>45690</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -964,19 +1002,18 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>45673</v>
+        <v>45691</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>143</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>45674</v>
+        <v>45692</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -987,10 +1024,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>45675</v>
+        <v>45693</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1006,7 +1043,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>45676</v>
+        <v>45694</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -1018,7 +1055,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>45677</v>
+        <v>45695</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -1030,7 +1067,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>45678</v>
+        <v>45696</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -1042,7 +1079,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>45679</v>
+        <v>45697</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1059,7 +1096,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>45680</v>
+        <v>45698</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -1070,7 +1107,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4">
-        <v>45681</v>
+        <v>45699</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -1083,7 +1120,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4">
-        <v>45682</v>
+        <v>45700</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
@@ -1094,7 +1131,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>45683</v>
+        <v>45701</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -1106,16 +1143,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>45684</v>
+        <v>45702</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1123,7 +1160,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>45685</v>
+        <v>45703</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -1134,7 +1171,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4">
-        <v>45686</v>
+        <v>45704</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
@@ -1152,7 +1189,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4">
-        <v>45687</v>
+        <v>45705</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1163,7 +1200,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4">
-        <v>45688</v>
+        <v>45706</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
@@ -1175,7 +1212,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4">
-        <v>45689</v>
+        <v>45707</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
@@ -1186,7 +1223,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4">
-        <v>45690</v>
+        <v>45708</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
@@ -1197,10 +1234,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="4">
-        <v>45691</v>
+        <v>45709</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1208,7 +1245,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4">
-        <v>45692</v>
+        <v>45710</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
@@ -1219,13 +1256,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="4">
-        <v>45693</v>
+        <v>45711</v>
       </c>
       <c r="C26" t="s">
         <v>33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1233,7 +1267,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4">
-        <v>45694</v>
+        <v>45712</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
@@ -1244,7 +1278,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4">
-        <v>45695</v>
+        <v>45713</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
@@ -1258,7 +1292,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4">
-        <v>45696</v>
+        <v>45714</v>
       </c>
       <c r="C29" t="s">
         <v>37</v>
@@ -1269,7 +1303,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4">
-        <v>45697</v>
+        <v>45715</v>
       </c>
       <c r="C30" t="s">
         <v>49</v>
@@ -1280,7 +1314,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4">
-        <v>45698</v>
+        <v>45716</v>
       </c>
       <c r="C31" t="s">
         <v>50</v>
@@ -1291,10 +1325,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="4">
-        <v>45699</v>
+        <v>45717</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1302,7 +1336,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4">
-        <v>45700</v>
+        <v>45718</v>
       </c>
       <c r="C33" t="s">
         <v>54</v>
@@ -1313,10 +1347,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="4">
-        <v>45701</v>
+        <v>45719</v>
       </c>
       <c r="C34" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1324,7 +1358,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4">
-        <v>45702</v>
+        <v>45720</v>
       </c>
       <c r="C35" t="s">
         <v>55</v>
@@ -1335,7 +1369,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4">
-        <v>45703</v>
+        <v>45721</v>
       </c>
       <c r="C36" t="s">
         <v>56</v>
@@ -1346,7 +1380,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4">
-        <v>45704</v>
+        <v>45722</v>
       </c>
       <c r="C37" t="s">
         <v>57</v>
@@ -1357,7 +1391,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4">
-        <v>45705</v>
+        <v>45723</v>
       </c>
       <c r="C38" t="s">
         <v>58</v>
@@ -1368,7 +1402,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4">
-        <v>45706</v>
+        <v>45724</v>
       </c>
       <c r="C39" t="s">
         <v>59</v>
@@ -1379,7 +1413,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4">
-        <v>45707</v>
+        <v>45725</v>
       </c>
       <c r="C40" t="s">
         <v>60</v>
@@ -1390,7 +1424,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4">
-        <v>45708</v>
+        <v>45726</v>
       </c>
       <c r="C41" t="s">
         <v>61</v>
@@ -1401,7 +1435,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4">
-        <v>45709</v>
+        <v>45727</v>
       </c>
       <c r="C42" t="s">
         <v>62</v>
@@ -1412,16 +1446,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="4">
-        <v>45710</v>
+        <v>45728</v>
       </c>
       <c r="C43" t="s">
         <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E43" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1429,7 +1463,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4">
-        <v>45711</v>
+        <v>45729</v>
       </c>
       <c r="C44" t="s">
         <v>64</v>
@@ -1440,7 +1474,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="4">
-        <v>45712</v>
+        <v>45730</v>
       </c>
       <c r="C45" t="s">
         <v>65</v>
@@ -1454,7 +1488,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="4">
-        <v>45713</v>
+        <v>45731</v>
       </c>
       <c r="C46" t="s">
         <v>67</v>
@@ -1465,7 +1499,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4">
-        <v>45714</v>
+        <v>45732</v>
       </c>
       <c r="C47" t="s">
         <v>68</v>
@@ -1476,117 +1510,117 @@
         <v>47</v>
       </c>
       <c r="B48" s="4">
-        <v>45715</v>
+        <v>45733</v>
       </c>
       <c r="C48" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="4">
-        <v>45716</v>
+        <v>45734</v>
       </c>
       <c r="C49" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="4">
-        <v>45717</v>
+        <v>45735</v>
       </c>
       <c r="C50" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="4">
-        <v>45718</v>
+        <v>45736</v>
       </c>
       <c r="C51" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="4">
-        <v>45719</v>
+        <v>45737</v>
       </c>
       <c r="C52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="4">
-        <v>45720</v>
+        <v>45738</v>
       </c>
       <c r="C53" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="4">
-        <v>45721</v>
+        <v>45739</v>
       </c>
       <c r="C54" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="4">
-        <v>45722</v>
+        <v>45740</v>
       </c>
       <c r="C55" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="4">
-        <v>45723</v>
+        <v>45741</v>
       </c>
       <c r="C56" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="4">
-        <v>45724</v>
+        <v>45742</v>
       </c>
       <c r="C57" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="4">
-        <v>45725</v>
+        <v>45743</v>
       </c>
       <c r="C58" t="s">
         <v>78</v>
@@ -1598,70 +1632,73 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="4">
-        <v>45726</v>
+        <v>45744</v>
       </c>
       <c r="C59" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="F59" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="4">
-        <v>45727</v>
+        <v>45745</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="4">
-        <v>45728</v>
+        <v>45746</v>
       </c>
       <c r="C61" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="4">
-        <v>45729</v>
+        <v>45747</v>
       </c>
       <c r="C62" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="4">
-        <v>45730</v>
+        <v>45748</v>
       </c>
       <c r="C63" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" s="4">
-        <v>45731</v>
+        <v>45749</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1669,13 +1706,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="4">
-        <v>45732</v>
+        <v>45750</v>
       </c>
       <c r="C65" t="s">
+        <v>95</v>
+      </c>
+      <c r="F65" t="s">
         <v>96</v>
-      </c>
-      <c r="F65" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1683,10 +1720,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="4">
-        <v>45733</v>
+        <v>45751</v>
       </c>
       <c r="C66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1694,10 +1731,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="4">
-        <v>45734</v>
+        <v>45752</v>
       </c>
       <c r="C67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1705,10 +1742,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="4">
-        <v>45735</v>
+        <v>45753</v>
       </c>
       <c r="C68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -1716,10 +1753,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="4">
-        <v>45736</v>
+        <v>45754</v>
       </c>
       <c r="C69" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -1727,10 +1764,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="4">
-        <v>45737</v>
+        <v>45755</v>
       </c>
       <c r="C70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -1738,16 +1775,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="4">
-        <v>45738</v>
+        <v>45756</v>
       </c>
       <c r="C71" t="s">
+        <v>102</v>
+      </c>
+      <c r="D71" t="s">
         <v>103</v>
       </c>
-      <c r="D71" t="s">
-        <v>104</v>
-      </c>
       <c r="E71" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -1755,10 +1792,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="4">
-        <v>45739</v>
+        <v>45757</v>
       </c>
       <c r="C72" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -1766,10 +1803,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="4">
-        <v>45740</v>
+        <v>45758</v>
       </c>
       <c r="C73" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -1777,10 +1814,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="4">
-        <v>45741</v>
+        <v>45759</v>
       </c>
       <c r="C74" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -1788,10 +1825,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="4">
-        <v>45742</v>
+        <v>45760</v>
       </c>
       <c r="C75" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -1799,10 +1836,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="4">
-        <v>45743</v>
+        <v>45761</v>
       </c>
       <c r="C76" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -1810,10 +1847,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="4">
-        <v>45744</v>
+        <v>45762</v>
       </c>
       <c r="C77" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -1821,10 +1858,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="4">
-        <v>45745</v>
+        <v>45763</v>
       </c>
       <c r="C78" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -1832,10 +1869,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="4">
-        <v>45746</v>
+        <v>45764</v>
       </c>
       <c r="C79" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -1843,13 +1880,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="4">
-        <v>45747</v>
+        <v>45765</v>
       </c>
       <c r="C80" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F80" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -1857,10 +1894,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="4">
-        <v>45748</v>
+        <v>45766</v>
       </c>
       <c r="C81" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -1868,10 +1905,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="4">
-        <v>45749</v>
+        <v>45767</v>
       </c>
       <c r="C82" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -1879,16 +1916,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="4">
-        <v>45750</v>
+        <v>45768</v>
       </c>
       <c r="C83" t="s">
+        <v>113</v>
+      </c>
+      <c r="D83" t="s">
+        <v>115</v>
+      </c>
+      <c r="E83" t="s">
         <v>116</v>
-      </c>
-      <c r="D83" t="s">
-        <v>119</v>
-      </c>
-      <c r="E83" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -1896,10 +1933,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="4">
-        <v>45751</v>
+        <v>45769</v>
       </c>
       <c r="C84" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -1907,16 +1944,16 @@
         <v>84</v>
       </c>
       <c r="B85" s="4">
-        <v>45752</v>
+        <v>45770</v>
       </c>
       <c r="C85" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D85" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E85" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -1924,10 +1961,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="4">
-        <v>45753</v>
+        <v>45771</v>
       </c>
       <c r="C86" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -1935,10 +1972,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="4">
-        <v>45754</v>
+        <v>45772</v>
       </c>
       <c r="C87" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -1946,7 +1983,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="4">
-        <v>45755</v>
+        <v>45773</v>
       </c>
       <c r="C88" t="s">
         <v>39</v>
@@ -1957,10 +1994,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="4">
-        <v>45756</v>
+        <v>45774</v>
       </c>
       <c r="C89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -1968,10 +2005,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="4">
-        <v>45757</v>
+        <v>45775</v>
       </c>
       <c r="C90" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -1979,10 +2016,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="4">
-        <v>45758</v>
+        <v>45776</v>
       </c>
       <c r="C91" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -1990,10 +2027,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="4">
-        <v>45759</v>
+        <v>45777</v>
       </c>
       <c r="C92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2001,10 +2038,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="4">
-        <v>45760</v>
+        <v>45778</v>
       </c>
       <c r="C93" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2012,13 +2049,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="4">
-        <v>45761</v>
+        <v>45779</v>
       </c>
       <c r="C94" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F94" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2026,7 +2063,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="4">
-        <v>45762</v>
+        <v>45780</v>
       </c>
       <c r="C95" t="s">
         <v>51</v>
@@ -2043,183 +2080,189 @@
         <v>95</v>
       </c>
       <c r="B96" s="4">
-        <v>45763</v>
+        <v>45781</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" s="4">
-        <v>45764</v>
+        <v>45782</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" s="4">
-        <v>45765</v>
+        <v>45783</v>
       </c>
       <c r="C98" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+      <c r="D98" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" s="4">
-        <v>45766</v>
+        <v>45784</v>
       </c>
       <c r="C99" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" s="4">
-        <v>45767</v>
+        <v>45785</v>
       </c>
       <c r="C100" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" s="4">
-        <v>45768</v>
+        <v>45786</v>
       </c>
       <c r="C101" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" s="4">
-        <v>45769</v>
+        <v>45787</v>
       </c>
       <c r="C102" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" s="4">
-        <v>45770</v>
+        <v>45788</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104" s="4">
-        <v>45771</v>
+        <v>45789</v>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" s="4">
-        <v>45772</v>
+        <v>45790</v>
       </c>
       <c r="C105" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106" s="4">
-        <v>45773</v>
+        <v>45791</v>
       </c>
       <c r="C106" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107" s="4">
-        <v>45774</v>
+        <v>45792</v>
       </c>
       <c r="C107" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="D107" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108" s="4">
-        <v>45775</v>
+        <v>45793</v>
       </c>
       <c r="C108" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109" s="4">
-        <v>45776</v>
+        <v>45794</v>
       </c>
       <c r="C109" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
       <c r="B110" s="4">
-        <v>45777</v>
+        <v>45795</v>
       </c>
       <c r="C110" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
       <c r="B111" s="4">
-        <v>45778</v>
+        <v>45796</v>
       </c>
       <c r="C111" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
       <c r="B112" s="4">
-        <v>45779</v>
+        <v>45797</v>
       </c>
       <c r="C112" t="s">
         <v>8</v>
@@ -2230,7 +2273,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="4">
-        <v>45780</v>
+        <v>45798</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -2241,7 +2284,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="4">
-        <v>45781</v>
+        <v>45799</v>
       </c>
       <c r="C114" t="s">
         <v>8</v>
@@ -2252,7 +2295,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="4">
-        <v>45782</v>
+        <v>45800</v>
       </c>
       <c r="C115" t="s">
         <v>8</v>
@@ -2263,7 +2306,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="4">
-        <v>45783</v>
+        <v>45801</v>
       </c>
       <c r="C116" t="s">
         <v>8</v>
@@ -2274,7 +2317,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="4">
-        <v>45784</v>
+        <v>45802</v>
       </c>
       <c r="C117" t="s">
         <v>8</v>
@@ -2285,7 +2328,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="4">
-        <v>45785</v>
+        <v>45803</v>
       </c>
       <c r="C118" t="s">
         <v>40</v>
@@ -2296,7 +2339,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="4">
-        <v>45786</v>
+        <v>45804</v>
       </c>
       <c r="C119" t="s">
         <v>8</v>
@@ -2307,7 +2350,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="4">
-        <v>45787</v>
+        <v>45805</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -2318,7 +2361,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="4">
-        <v>45788</v>
+        <v>45806</v>
       </c>
       <c r="C121" t="s">
         <v>8</v>
@@ -2329,10 +2372,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="4">
-        <v>45789</v>
+        <v>45807</v>
       </c>
       <c r="C122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -2340,7 +2383,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="4">
-        <v>45790</v>
+        <v>45808</v>
       </c>
       <c r="C123" t="s">
         <v>8</v>
@@ -2351,10 +2394,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="4">
-        <v>45791</v>
+        <v>45809</v>
       </c>
       <c r="C124" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -2362,7 +2405,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="4">
-        <v>45792</v>
+        <v>45810</v>
       </c>
       <c r="C125" t="s">
         <v>8</v>
@@ -2373,7 +2416,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="4">
-        <v>45793</v>
+        <v>45811</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
@@ -2384,7 +2427,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="4">
-        <v>45794</v>
+        <v>45812</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -2395,7 +2438,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="4">
-        <v>45795</v>
+        <v>45813</v>
       </c>
       <c r="C128" t="s">
         <v>8</v>
@@ -2406,7 +2449,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="4">
-        <v>45796</v>
+        <v>45814</v>
       </c>
       <c r="C129" t="s">
         <v>8</v>
@@ -2417,7 +2460,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="4">
-        <v>45797</v>
+        <v>45815</v>
       </c>
       <c r="C130" t="s">
         <v>8</v>
@@ -2428,7 +2471,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="4">
-        <v>45798</v>
+        <v>45816</v>
       </c>
       <c r="C131" t="s">
         <v>8</v>
@@ -2439,7 +2482,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="4">
-        <v>45799</v>
+        <v>45817</v>
       </c>
       <c r="C132" t="s">
         <v>8</v>
@@ -2450,7 +2493,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="4">
-        <v>45800</v>
+        <v>45818</v>
       </c>
       <c r="C133" t="s">
         <v>8</v>
@@ -2461,7 +2504,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="4">
-        <v>45801</v>
+        <v>45819</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -2472,7 +2515,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="4">
-        <v>45802</v>
+        <v>45820</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
@@ -2483,7 +2526,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="4">
-        <v>45803</v>
+        <v>45821</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
@@ -2494,7 +2537,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="4">
-        <v>45804</v>
+        <v>45822</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
@@ -2505,7 +2548,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="4">
-        <v>45805</v>
+        <v>45823</v>
       </c>
       <c r="C138" t="s">
         <v>8</v>
@@ -2516,7 +2559,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="4">
-        <v>45806</v>
+        <v>45824</v>
       </c>
       <c r="C139" t="s">
         <v>8</v>
@@ -2527,7 +2570,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="4">
-        <v>45807</v>
+        <v>45825</v>
       </c>
       <c r="C140" t="s">
         <v>8</v>
@@ -2538,7 +2581,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="4">
-        <v>45808</v>
+        <v>45826</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -2549,7 +2592,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="4">
-        <v>45809</v>
+        <v>45827</v>
       </c>
       <c r="C142" t="s">
         <v>8</v>
@@ -2560,7 +2603,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="4">
-        <v>45810</v>
+        <v>45828</v>
       </c>
       <c r="C143" t="s">
         <v>8</v>
@@ -2571,7 +2614,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="4">
-        <v>45811</v>
+        <v>45829</v>
       </c>
       <c r="C144" t="s">
         <v>8</v>
@@ -2582,7 +2625,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="4">
-        <v>45812</v>
+        <v>45830</v>
       </c>
       <c r="C145" t="s">
         <v>8</v>
@@ -2593,7 +2636,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="4">
-        <v>45813</v>
+        <v>45831</v>
       </c>
       <c r="C146" t="s">
         <v>8</v>
@@ -2604,7 +2647,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="4">
-        <v>45814</v>
+        <v>45832</v>
       </c>
       <c r="C147" t="s">
         <v>8</v>
@@ -2615,7 +2658,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="4">
-        <v>45815</v>
+        <v>45833</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -2626,7 +2669,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="4">
-        <v>45816</v>
+        <v>45834</v>
       </c>
       <c r="C149" t="s">
         <v>41</v>
@@ -2637,7 +2680,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="4">
-        <v>45817</v>
+        <v>45835</v>
       </c>
       <c r="C150" t="s">
         <v>8</v>
@@ -2648,7 +2691,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="4">
-        <v>45818</v>
+        <v>45836</v>
       </c>
       <c r="C151" t="s">
         <v>8</v>
@@ -2659,7 +2702,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="4">
-        <v>45819</v>
+        <v>45837</v>
       </c>
       <c r="C152" t="s">
         <v>8</v>
@@ -2670,10 +2713,10 @@
         <v>152</v>
       </c>
       <c r="B153" s="4">
-        <v>45820</v>
+        <v>45838</v>
       </c>
       <c r="C153" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -2681,10 +2724,10 @@
         <v>153</v>
       </c>
       <c r="B154" s="4">
-        <v>45821</v>
+        <v>45839</v>
       </c>
       <c r="C154" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -2692,7 +2735,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="4">
-        <v>45822</v>
+        <v>45840</v>
       </c>
       <c r="C155" t="s">
         <v>8</v>
@@ -2703,7 +2746,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="4">
-        <v>45823</v>
+        <v>45841</v>
       </c>
       <c r="C156" t="s">
         <v>8</v>
@@ -2714,7 +2757,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="4">
-        <v>45824</v>
+        <v>45842</v>
       </c>
       <c r="C157" t="s">
         <v>8</v>
@@ -2725,7 +2768,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="4">
-        <v>45825</v>
+        <v>45843</v>
       </c>
       <c r="C158" t="s">
         <v>8</v>
@@ -2736,7 +2779,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="4">
-        <v>45826</v>
+        <v>45844</v>
       </c>
       <c r="C159" t="s">
         <v>8</v>
@@ -2747,7 +2790,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="4">
-        <v>45827</v>
+        <v>45845</v>
       </c>
       <c r="C160" t="s">
         <v>8</v>
@@ -2758,7 +2801,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="4">
-        <v>45828</v>
+        <v>45846</v>
       </c>
       <c r="C161" t="s">
         <v>8</v>
@@ -2769,7 +2812,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="4">
-        <v>45829</v>
+        <v>45847</v>
       </c>
       <c r="C162" t="s">
         <v>8</v>
@@ -2780,7 +2823,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="4">
-        <v>45830</v>
+        <v>45848</v>
       </c>
       <c r="C163" t="s">
         <v>8</v>
@@ -2791,7 +2834,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="4">
-        <v>45831</v>
+        <v>45849</v>
       </c>
       <c r="C164" t="s">
         <v>8</v>
@@ -2802,7 +2845,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="4">
-        <v>45832</v>
+        <v>45850</v>
       </c>
       <c r="C165" t="s">
         <v>8</v>
@@ -2813,7 +2856,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="4">
-        <v>45833</v>
+        <v>45851</v>
       </c>
       <c r="C166" t="s">
         <v>8</v>
@@ -2824,7 +2867,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="4">
-        <v>45834</v>
+        <v>45852</v>
       </c>
       <c r="C167" t="s">
         <v>8</v>
@@ -2835,7 +2878,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="4">
-        <v>45835</v>
+        <v>45853</v>
       </c>
       <c r="C168" t="s">
         <v>8</v>
@@ -2846,7 +2889,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="4">
-        <v>45836</v>
+        <v>45854</v>
       </c>
       <c r="C169" t="s">
         <v>8</v>
@@ -2857,7 +2900,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="4">
-        <v>45837</v>
+        <v>45855</v>
       </c>
       <c r="C170" t="s">
         <v>8</v>
@@ -2868,7 +2911,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="4">
-        <v>45838</v>
+        <v>45856</v>
       </c>
       <c r="C171" t="s">
         <v>8</v>
@@ -2879,7 +2922,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="4">
-        <v>45839</v>
+        <v>45857</v>
       </c>
       <c r="C172" t="s">
         <v>8</v>
@@ -2890,7 +2933,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="4">
-        <v>45840</v>
+        <v>45858</v>
       </c>
       <c r="C173" t="s">
         <v>8</v>
@@ -2901,7 +2944,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="4">
-        <v>45841</v>
+        <v>45859</v>
       </c>
       <c r="C174" t="s">
         <v>8</v>
@@ -2912,7 +2955,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="4">
-        <v>45842</v>
+        <v>45860</v>
       </c>
       <c r="C175" t="s">
         <v>8</v>
@@ -2923,7 +2966,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="4">
-        <v>45843</v>
+        <v>45861</v>
       </c>
       <c r="C176" t="s">
         <v>8</v>
@@ -2934,7 +2977,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="4">
-        <v>45844</v>
+        <v>45862</v>
       </c>
       <c r="C177" t="s">
         <v>8</v>
@@ -2945,7 +2988,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="4">
-        <v>45845</v>
+        <v>45863</v>
       </c>
       <c r="C178" t="s">
         <v>8</v>
@@ -2956,7 +2999,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="4">
-        <v>45846</v>
+        <v>45864</v>
       </c>
       <c r="C179" t="s">
         <v>42</v>
@@ -2967,7 +3010,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="4">
-        <v>45847</v>
+        <v>45865</v>
       </c>
       <c r="C180" t="s">
         <v>8</v>
@@ -2978,7 +3021,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="4">
-        <v>45848</v>
+        <v>45866</v>
       </c>
       <c r="C181" t="s">
         <v>8</v>
@@ -2989,7 +3032,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="4">
-        <v>45849</v>
+        <v>45867</v>
       </c>
       <c r="C182" t="s">
         <v>8</v>
@@ -3000,10 +3043,10 @@
         <v>182</v>
       </c>
       <c r="B183" s="4">
-        <v>45850</v>
+        <v>45868</v>
       </c>
       <c r="C183" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -3011,7 +3054,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="4">
-        <v>45851</v>
+        <v>45869</v>
       </c>
       <c r="C184" t="s">
         <v>8</v>
@@ -3022,10 +3065,10 @@
         <v>184</v>
       </c>
       <c r="B185" s="4">
-        <v>45852</v>
+        <v>45870</v>
       </c>
       <c r="C185" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -3033,7 +3076,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="4">
-        <v>45853</v>
+        <v>45871</v>
       </c>
       <c r="C186" t="s">
         <v>8</v>
@@ -3044,7 +3087,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="4">
-        <v>45854</v>
+        <v>45872</v>
       </c>
       <c r="C187" t="s">
         <v>8</v>
@@ -3055,7 +3098,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="4">
-        <v>45855</v>
+        <v>45873</v>
       </c>
       <c r="C188" t="s">
         <v>8</v>
@@ -3066,7 +3109,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="4">
-        <v>45856</v>
+        <v>45874</v>
       </c>
       <c r="C189" t="s">
         <v>8</v>
@@ -3077,7 +3120,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="4">
-        <v>45857</v>
+        <v>45875</v>
       </c>
       <c r="C190" t="s">
         <v>8</v>
@@ -3088,7 +3131,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="4">
-        <v>45858</v>
+        <v>45876</v>
       </c>
       <c r="C191" t="s">
         <v>8</v>
@@ -3099,7 +3142,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="4">
-        <v>45859</v>
+        <v>45877</v>
       </c>
       <c r="C192" t="s">
         <v>8</v>
@@ -3110,7 +3153,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="4">
-        <v>45860</v>
+        <v>45878</v>
       </c>
       <c r="C193" t="s">
         <v>8</v>
@@ -3121,7 +3164,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="4">
-        <v>45861</v>
+        <v>45879</v>
       </c>
       <c r="C194" t="s">
         <v>8</v>
@@ -3132,7 +3175,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="4">
-        <v>45862</v>
+        <v>45880</v>
       </c>
       <c r="C195" t="s">
         <v>8</v>
@@ -3143,7 +3186,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="4">
-        <v>45863</v>
+        <v>45881</v>
       </c>
       <c r="C196" t="s">
         <v>8</v>
@@ -3154,7 +3197,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="4">
-        <v>45864</v>
+        <v>45882</v>
       </c>
       <c r="C197" t="s">
         <v>8</v>
@@ -3165,7 +3208,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="4">
-        <v>45865</v>
+        <v>45883</v>
       </c>
       <c r="C198" t="s">
         <v>8</v>
@@ -3176,7 +3219,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="4">
-        <v>45866</v>
+        <v>45884</v>
       </c>
       <c r="C199" t="s">
         <v>8</v>
@@ -3187,7 +3230,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="4">
-        <v>45867</v>
+        <v>45885</v>
       </c>
       <c r="C200" t="s">
         <v>8</v>
@@ -3198,7 +3241,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="4">
-        <v>45868</v>
+        <v>45886</v>
       </c>
       <c r="C201" t="s">
         <v>8</v>
@@ -3209,7 +3252,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="4">
-        <v>45869</v>
+        <v>45887</v>
       </c>
       <c r="C202" t="s">
         <v>8</v>
@@ -3220,7 +3263,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="4">
-        <v>45870</v>
+        <v>45888</v>
       </c>
       <c r="C203" t="s">
         <v>8</v>
@@ -3231,7 +3274,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="4">
-        <v>45871</v>
+        <v>45889</v>
       </c>
       <c r="C204" t="s">
         <v>8</v>
@@ -3242,7 +3285,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="4">
-        <v>45872</v>
+        <v>45890</v>
       </c>
       <c r="C205" t="s">
         <v>8</v>
@@ -3253,7 +3296,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="4">
-        <v>45873</v>
+        <v>45891</v>
       </c>
       <c r="C206" t="s">
         <v>8</v>
@@ -3264,7 +3307,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="4">
-        <v>45874</v>
+        <v>45892</v>
       </c>
       <c r="C207" t="s">
         <v>8</v>
@@ -3275,7 +3318,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="4">
-        <v>45875</v>
+        <v>45893</v>
       </c>
       <c r="C208" t="s">
         <v>8</v>
@@ -3286,7 +3329,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="4">
-        <v>45876</v>
+        <v>45894</v>
       </c>
       <c r="C209" t="s">
         <v>8</v>
@@ -3297,7 +3340,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="4">
-        <v>45877</v>
+        <v>45895</v>
       </c>
       <c r="C210" t="s">
         <v>43</v>
@@ -3308,7 +3351,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="4">
-        <v>45878</v>
+        <v>45896</v>
       </c>
       <c r="C211" t="s">
         <v>8</v>
@@ -3319,7 +3362,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="4">
-        <v>45879</v>
+        <v>45897</v>
       </c>
       <c r="C212" t="s">
         <v>8</v>
@@ -3330,7 +3373,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="4">
-        <v>45880</v>
+        <v>45898</v>
       </c>
       <c r="C213" t="s">
         <v>8</v>
@@ -3341,10 +3384,10 @@
         <v>213</v>
       </c>
       <c r="B214" s="4">
-        <v>45881</v>
+        <v>45899</v>
       </c>
       <c r="C214" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
@@ -3352,7 +3395,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="4">
-        <v>45882</v>
+        <v>45900</v>
       </c>
       <c r="C215" t="s">
         <v>8</v>
@@ -3363,10 +3406,10 @@
         <v>215</v>
       </c>
       <c r="B216" s="4">
-        <v>45883</v>
+        <v>45901</v>
       </c>
       <c r="C216" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
@@ -3374,7 +3417,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="4">
-        <v>45884</v>
+        <v>45902</v>
       </c>
       <c r="C217" t="s">
         <v>8</v>
@@ -3385,7 +3428,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="4">
-        <v>45885</v>
+        <v>45903</v>
       </c>
       <c r="C218" t="s">
         <v>8</v>
@@ -3396,7 +3439,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="4">
-        <v>45886</v>
+        <v>45904</v>
       </c>
       <c r="C219" t="s">
         <v>8</v>
@@ -3407,7 +3450,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="4">
-        <v>45887</v>
+        <v>45905</v>
       </c>
       <c r="C220" t="s">
         <v>8</v>
@@ -3418,7 +3461,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="4">
-        <v>45888</v>
+        <v>45906</v>
       </c>
       <c r="C221" t="s">
         <v>8</v>
@@ -3429,7 +3472,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="4">
-        <v>45889</v>
+        <v>45907</v>
       </c>
       <c r="C222" t="s">
         <v>8</v>
@@ -3440,7 +3483,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="4">
-        <v>45890</v>
+        <v>45908</v>
       </c>
       <c r="C223" t="s">
         <v>8</v>
@@ -3451,7 +3494,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="4">
-        <v>45891</v>
+        <v>45909</v>
       </c>
       <c r="C224" t="s">
         <v>8</v>
@@ -3462,7 +3505,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="4">
-        <v>45892</v>
+        <v>45910</v>
       </c>
       <c r="C225" t="s">
         <v>8</v>
@@ -3473,7 +3516,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="4">
-        <v>45893</v>
+        <v>45911</v>
       </c>
       <c r="C226" t="s">
         <v>8</v>
@@ -3484,7 +3527,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="4">
-        <v>45894</v>
+        <v>45912</v>
       </c>
       <c r="C227" t="s">
         <v>8</v>
@@ -3495,7 +3538,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="4">
-        <v>45895</v>
+        <v>45913</v>
       </c>
       <c r="C228" t="s">
         <v>8</v>
@@ -3506,7 +3549,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="4">
-        <v>45896</v>
+        <v>45914</v>
       </c>
       <c r="C229" t="s">
         <v>8</v>
@@ -3517,7 +3560,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="4">
-        <v>45897</v>
+        <v>45915</v>
       </c>
       <c r="C230" t="s">
         <v>8</v>
@@ -3528,7 +3571,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="4">
-        <v>45898</v>
+        <v>45916</v>
       </c>
       <c r="C231" t="s">
         <v>8</v>
@@ -3539,7 +3582,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="4">
-        <v>45899</v>
+        <v>45917</v>
       </c>
       <c r="C232" t="s">
         <v>8</v>
@@ -3550,7 +3593,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="4">
-        <v>45900</v>
+        <v>45918</v>
       </c>
       <c r="C233" t="s">
         <v>8</v>
@@ -3561,7 +3604,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="4">
-        <v>45901</v>
+        <v>45919</v>
       </c>
       <c r="C234" t="s">
         <v>8</v>
@@ -3572,7 +3615,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="4">
-        <v>45902</v>
+        <v>45920</v>
       </c>
       <c r="C235" t="s">
         <v>8</v>
@@ -3583,7 +3626,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="4">
-        <v>45903</v>
+        <v>45921</v>
       </c>
       <c r="C236" t="s">
         <v>8</v>
@@ -3594,7 +3637,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="4">
-        <v>45904</v>
+        <v>45922</v>
       </c>
       <c r="C237" t="s">
         <v>8</v>
@@ -3605,7 +3648,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="4">
-        <v>45905</v>
+        <v>45923</v>
       </c>
       <c r="C238" t="s">
         <v>8</v>
@@ -3616,7 +3659,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="4">
-        <v>45906</v>
+        <v>45924</v>
       </c>
       <c r="C239" t="s">
         <v>8</v>
@@ -3627,7 +3670,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="4">
-        <v>45907</v>
+        <v>45925</v>
       </c>
       <c r="C240" t="s">
         <v>8</v>
@@ -3638,7 +3681,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="4">
-        <v>45908</v>
+        <v>45926</v>
       </c>
       <c r="C241" t="s">
         <v>44</v>
@@ -3649,7 +3692,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="4">
-        <v>45909</v>
+        <v>45927</v>
       </c>
       <c r="C242" t="s">
         <v>8</v>
@@ -3660,7 +3703,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="4">
-        <v>45910</v>
+        <v>45928</v>
       </c>
       <c r="C243" t="s">
         <v>8</v>
@@ -3671,7 +3714,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="4">
-        <v>45911</v>
+        <v>45929</v>
       </c>
       <c r="C244" t="s">
         <v>8</v>
@@ -3682,10 +3725,10 @@
         <v>244</v>
       </c>
       <c r="B245" s="4">
-        <v>45912</v>
+        <v>45930</v>
       </c>
       <c r="C245" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
@@ -3693,10 +3736,10 @@
         <v>245</v>
       </c>
       <c r="B246" s="4">
-        <v>45913</v>
+        <v>45931</v>
       </c>
       <c r="C246" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
@@ -3704,7 +3747,7 @@
         <v>246</v>
       </c>
       <c r="B247" s="4">
-        <v>45914</v>
+        <v>45932</v>
       </c>
       <c r="C247" t="s">
         <v>8</v>
@@ -3715,7 +3758,7 @@
         <v>247</v>
       </c>
       <c r="B248" s="4">
-        <v>45915</v>
+        <v>45933</v>
       </c>
       <c r="C248" t="s">
         <v>8</v>
@@ -3726,7 +3769,7 @@
         <v>248</v>
       </c>
       <c r="B249" s="4">
-        <v>45916</v>
+        <v>45934</v>
       </c>
       <c r="C249" t="s">
         <v>8</v>
@@ -3737,7 +3780,7 @@
         <v>249</v>
       </c>
       <c r="B250" s="4">
-        <v>45917</v>
+        <v>45935</v>
       </c>
       <c r="C250" t="s">
         <v>8</v>
@@ -3748,7 +3791,7 @@
         <v>250</v>
       </c>
       <c r="B251" s="4">
-        <v>45918</v>
+        <v>45936</v>
       </c>
       <c r="C251" t="s">
         <v>8</v>
@@ -3759,7 +3802,7 @@
         <v>251</v>
       </c>
       <c r="B252" s="4">
-        <v>45919</v>
+        <v>45937</v>
       </c>
       <c r="C252" t="s">
         <v>8</v>
@@ -3770,7 +3813,7 @@
         <v>252</v>
       </c>
       <c r="B253" s="4">
-        <v>45920</v>
+        <v>45938</v>
       </c>
       <c r="C253" t="s">
         <v>8</v>
@@ -3781,7 +3824,7 @@
         <v>253</v>
       </c>
       <c r="B254" s="4">
-        <v>45921</v>
+        <v>45939</v>
       </c>
       <c r="C254" t="s">
         <v>8</v>
@@ -3792,7 +3835,7 @@
         <v>254</v>
       </c>
       <c r="B255" s="4">
-        <v>45922</v>
+        <v>45940</v>
       </c>
       <c r="C255" t="s">
         <v>8</v>
@@ -3803,7 +3846,7 @@
         <v>255</v>
       </c>
       <c r="B256" s="4">
-        <v>45923</v>
+        <v>45941</v>
       </c>
       <c r="C256" t="s">
         <v>8</v>
@@ -3814,7 +3857,7 @@
         <v>256</v>
       </c>
       <c r="B257" s="4">
-        <v>45924</v>
+        <v>45942</v>
       </c>
       <c r="C257" t="s">
         <v>8</v>
@@ -3825,7 +3868,7 @@
         <v>257</v>
       </c>
       <c r="B258" s="4">
-        <v>45925</v>
+        <v>45943</v>
       </c>
       <c r="C258" t="s">
         <v>8</v>
@@ -3836,7 +3879,7 @@
         <v>258</v>
       </c>
       <c r="B259" s="4">
-        <v>45926</v>
+        <v>45944</v>
       </c>
       <c r="C259" t="s">
         <v>8</v>
@@ -3847,7 +3890,7 @@
         <v>259</v>
       </c>
       <c r="B260" s="4">
-        <v>45927</v>
+        <v>45945</v>
       </c>
       <c r="C260" t="s">
         <v>8</v>
@@ -3858,7 +3901,7 @@
         <v>260</v>
       </c>
       <c r="B261" s="4">
-        <v>45928</v>
+        <v>45946</v>
       </c>
       <c r="C261" t="s">
         <v>8</v>
@@ -3869,7 +3912,7 @@
         <v>261</v>
       </c>
       <c r="B262" s="4">
-        <v>45929</v>
+        <v>45947</v>
       </c>
       <c r="C262" t="s">
         <v>8</v>
@@ -3880,7 +3923,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="4">
-        <v>45930</v>
+        <v>45948</v>
       </c>
       <c r="C263" t="s">
         <v>8</v>
@@ -3891,7 +3934,7 @@
         <v>263</v>
       </c>
       <c r="B264" s="4">
-        <v>45931</v>
+        <v>45949</v>
       </c>
       <c r="C264" t="s">
         <v>8</v>
@@ -3902,7 +3945,7 @@
         <v>264</v>
       </c>
       <c r="B265" s="4">
-        <v>45932</v>
+        <v>45950</v>
       </c>
       <c r="C265" t="s">
         <v>8</v>
@@ -3913,7 +3956,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="4">
-        <v>45933</v>
+        <v>45951</v>
       </c>
       <c r="C266" t="s">
         <v>8</v>
@@ -3924,7 +3967,7 @@
         <v>266</v>
       </c>
       <c r="B267" s="4">
-        <v>45934</v>
+        <v>45952</v>
       </c>
       <c r="C267" t="s">
         <v>8</v>
@@ -3935,7 +3978,7 @@
         <v>267</v>
       </c>
       <c r="B268" s="4">
-        <v>45935</v>
+        <v>45953</v>
       </c>
       <c r="C268" t="s">
         <v>8</v>
@@ -3946,7 +3989,7 @@
         <v>268</v>
       </c>
       <c r="B269" s="4">
-        <v>45936</v>
+        <v>45954</v>
       </c>
       <c r="C269" t="s">
         <v>8</v>
@@ -3957,7 +4000,7 @@
         <v>269</v>
       </c>
       <c r="B270" s="4">
-        <v>45937</v>
+        <v>45955</v>
       </c>
       <c r="C270" t="s">
         <v>8</v>
@@ -3968,7 +4011,7 @@
         <v>270</v>
       </c>
       <c r="B271" s="4">
-        <v>45938</v>
+        <v>45956</v>
       </c>
       <c r="C271" t="s">
         <v>45</v>
@@ -3979,7 +4022,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="4">
-        <v>45939</v>
+        <v>45957</v>
       </c>
       <c r="C272" t="s">
         <v>8</v>
@@ -3990,7 +4033,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="4">
-        <v>45940</v>
+        <v>45958</v>
       </c>
       <c r="C273" t="s">
         <v>8</v>
@@ -4001,7 +4044,7 @@
         <v>273</v>
       </c>
       <c r="B274" s="4">
-        <v>45941</v>
+        <v>45959</v>
       </c>
       <c r="C274" t="s">
         <v>8</v>
@@ -4012,10 +4055,10 @@
         <v>274</v>
       </c>
       <c r="B275" s="4">
-        <v>45942</v>
+        <v>45960</v>
       </c>
       <c r="C275" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
@@ -4023,7 +4066,7 @@
         <v>275</v>
       </c>
       <c r="B276" s="4">
-        <v>45943</v>
+        <v>45961</v>
       </c>
       <c r="C276" t="s">
         <v>8</v>
@@ -4034,10 +4077,10 @@
         <v>276</v>
       </c>
       <c r="B277" s="4">
-        <v>45944</v>
+        <v>45962</v>
       </c>
       <c r="C277" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
@@ -4045,7 +4088,7 @@
         <v>277</v>
       </c>
       <c r="B278" s="4">
-        <v>45945</v>
+        <v>45963</v>
       </c>
       <c r="C278" t="s">
         <v>8</v>
@@ -4056,7 +4099,7 @@
         <v>278</v>
       </c>
       <c r="B279" s="4">
-        <v>45946</v>
+        <v>45964</v>
       </c>
       <c r="C279" t="s">
         <v>8</v>
@@ -4067,7 +4110,7 @@
         <v>279</v>
       </c>
       <c r="B280" s="4">
-        <v>45947</v>
+        <v>45965</v>
       </c>
       <c r="C280" t="s">
         <v>8</v>
@@ -4078,7 +4121,7 @@
         <v>280</v>
       </c>
       <c r="B281" s="4">
-        <v>45948</v>
+        <v>45966</v>
       </c>
       <c r="C281" t="s">
         <v>8</v>
@@ -4089,7 +4132,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="4">
-        <v>45949</v>
+        <v>45967</v>
       </c>
       <c r="C282" t="s">
         <v>8</v>
@@ -4100,7 +4143,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="4">
-        <v>45950</v>
+        <v>45968</v>
       </c>
       <c r="C283" t="s">
         <v>8</v>
@@ -4111,7 +4154,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="4">
-        <v>45951</v>
+        <v>45969</v>
       </c>
       <c r="C284" t="s">
         <v>8</v>
@@ -4122,7 +4165,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="4">
-        <v>45952</v>
+        <v>45970</v>
       </c>
       <c r="C285" t="s">
         <v>8</v>
@@ -4133,7 +4176,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="4">
-        <v>45953</v>
+        <v>45971</v>
       </c>
       <c r="C286" t="s">
         <v>8</v>
@@ -4144,7 +4187,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="4">
-        <v>45954</v>
+        <v>45972</v>
       </c>
       <c r="C287" t="s">
         <v>8</v>
@@ -4155,7 +4198,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="4">
-        <v>45955</v>
+        <v>45973</v>
       </c>
       <c r="C288" t="s">
         <v>8</v>
@@ -4166,7 +4209,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="4">
-        <v>45956</v>
+        <v>45974</v>
       </c>
       <c r="C289" t="s">
         <v>8</v>
@@ -4177,7 +4220,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="4">
-        <v>45957</v>
+        <v>45975</v>
       </c>
       <c r="C290" t="s">
         <v>8</v>
@@ -4188,7 +4231,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="4">
-        <v>45958</v>
+        <v>45976</v>
       </c>
       <c r="C291" t="s">
         <v>8</v>
@@ -4199,7 +4242,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="4">
-        <v>45959</v>
+        <v>45977</v>
       </c>
       <c r="C292" t="s">
         <v>8</v>
@@ -4210,7 +4253,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="4">
-        <v>45960</v>
+        <v>45978</v>
       </c>
       <c r="C293" t="s">
         <v>8</v>
@@ -4221,7 +4264,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="4">
-        <v>45961</v>
+        <v>45979</v>
       </c>
       <c r="C294" t="s">
         <v>8</v>
@@ -4232,7 +4275,7 @@
         <v>294</v>
       </c>
       <c r="B295" s="4">
-        <v>45962</v>
+        <v>45980</v>
       </c>
       <c r="C295" t="s">
         <v>8</v>
@@ -4243,7 +4286,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="4">
-        <v>45963</v>
+        <v>45981</v>
       </c>
       <c r="C296" t="s">
         <v>8</v>
@@ -4254,7 +4297,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="4">
-        <v>45964</v>
+        <v>45982</v>
       </c>
       <c r="C297" t="s">
         <v>8</v>
@@ -4265,7 +4308,7 @@
         <v>297</v>
       </c>
       <c r="B298" s="4">
-        <v>45965</v>
+        <v>45983</v>
       </c>
       <c r="C298" t="s">
         <v>8</v>
@@ -4276,7 +4319,7 @@
         <v>298</v>
       </c>
       <c r="B299" s="4">
-        <v>45966</v>
+        <v>45984</v>
       </c>
       <c r="C299" t="s">
         <v>8</v>
@@ -4287,7 +4330,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="4">
-        <v>45967</v>
+        <v>45985</v>
       </c>
       <c r="C300" t="s">
         <v>8</v>
@@ -4298,7 +4341,7 @@
         <v>300</v>
       </c>
       <c r="B301" s="4">
-        <v>45968</v>
+        <v>45986</v>
       </c>
       <c r="C301" t="s">
         <v>8</v>
@@ -4309,7 +4352,7 @@
         <v>301</v>
       </c>
       <c r="B302" s="4">
-        <v>45969</v>
+        <v>45987</v>
       </c>
       <c r="C302" t="s">
         <v>46</v>
@@ -4320,7 +4363,7 @@
         <v>302</v>
       </c>
       <c r="B303" s="4">
-        <v>45970</v>
+        <v>45988</v>
       </c>
       <c r="C303" t="s">
         <v>8</v>
@@ -4331,7 +4374,7 @@
         <v>303</v>
       </c>
       <c r="B304" s="4">
-        <v>45971</v>
+        <v>45989</v>
       </c>
       <c r="C304" t="s">
         <v>8</v>
@@ -4342,7 +4385,7 @@
         <v>304</v>
       </c>
       <c r="B305" s="4">
-        <v>45972</v>
+        <v>45990</v>
       </c>
       <c r="C305" t="s">
         <v>8</v>
@@ -4353,10 +4396,10 @@
         <v>305</v>
       </c>
       <c r="B306" s="4">
-        <v>45973</v>
+        <v>45991</v>
       </c>
       <c r="C306" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
@@ -4364,10 +4407,10 @@
         <v>306</v>
       </c>
       <c r="B307" s="4">
-        <v>45974</v>
+        <v>45992</v>
       </c>
       <c r="C307" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
@@ -4375,7 +4418,7 @@
         <v>307</v>
       </c>
       <c r="B308" s="4">
-        <v>45975</v>
+        <v>45993</v>
       </c>
       <c r="C308" t="s">
         <v>8</v>
@@ -4386,7 +4429,7 @@
         <v>308</v>
       </c>
       <c r="B309" s="4">
-        <v>45976</v>
+        <v>45994</v>
       </c>
       <c r="C309" t="s">
         <v>8</v>
@@ -4397,7 +4440,7 @@
         <v>309</v>
       </c>
       <c r="B310" s="4">
-        <v>45977</v>
+        <v>45995</v>
       </c>
       <c r="C310" t="s">
         <v>8</v>
@@ -4408,7 +4451,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="4">
-        <v>45978</v>
+        <v>45996</v>
       </c>
       <c r="C311" t="s">
         <v>8</v>
@@ -4419,7 +4462,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="4">
-        <v>45979</v>
+        <v>45997</v>
       </c>
       <c r="C312" t="s">
         <v>8</v>
@@ -4430,7 +4473,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="4">
-        <v>45980</v>
+        <v>45998</v>
       </c>
       <c r="C313" t="s">
         <v>8</v>
@@ -4441,7 +4484,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="4">
-        <v>45981</v>
+        <v>45999</v>
       </c>
       <c r="C314" t="s">
         <v>8</v>
@@ -4452,7 +4495,7 @@
         <v>314</v>
       </c>
       <c r="B315" s="4">
-        <v>45982</v>
+        <v>46000</v>
       </c>
       <c r="C315" t="s">
         <v>8</v>
@@ -4463,7 +4506,7 @@
         <v>315</v>
       </c>
       <c r="B316" s="4">
-        <v>45983</v>
+        <v>46001</v>
       </c>
       <c r="C316" t="s">
         <v>8</v>
@@ -4474,7 +4517,7 @@
         <v>316</v>
       </c>
       <c r="B317" s="4">
-        <v>45984</v>
+        <v>46002</v>
       </c>
       <c r="C317" t="s">
         <v>8</v>
@@ -4485,7 +4528,7 @@
         <v>317</v>
       </c>
       <c r="B318" s="4">
-        <v>45985</v>
+        <v>46003</v>
       </c>
       <c r="C318" t="s">
         <v>8</v>
@@ -4496,7 +4539,7 @@
         <v>318</v>
       </c>
       <c r="B319" s="4">
-        <v>45986</v>
+        <v>46004</v>
       </c>
       <c r="C319" t="s">
         <v>8</v>
@@ -4507,7 +4550,7 @@
         <v>319</v>
       </c>
       <c r="B320" s="4">
-        <v>45987</v>
+        <v>46005</v>
       </c>
       <c r="C320" t="s">
         <v>8</v>
@@ -4518,7 +4561,7 @@
         <v>320</v>
       </c>
       <c r="B321" s="4">
-        <v>45988</v>
+        <v>46006</v>
       </c>
       <c r="C321" t="s">
         <v>8</v>
@@ -4529,7 +4572,7 @@
         <v>321</v>
       </c>
       <c r="B322" s="4">
-        <v>45989</v>
+        <v>46007</v>
       </c>
       <c r="C322" t="s">
         <v>8</v>
@@ -4540,7 +4583,7 @@
         <v>322</v>
       </c>
       <c r="B323" s="4">
-        <v>45990</v>
+        <v>46008</v>
       </c>
       <c r="C323" t="s">
         <v>8</v>
@@ -4551,7 +4594,7 @@
         <v>323</v>
       </c>
       <c r="B324" s="4">
-        <v>45991</v>
+        <v>46009</v>
       </c>
       <c r="C324" t="s">
         <v>8</v>
@@ -4562,7 +4605,7 @@
         <v>324</v>
       </c>
       <c r="B325" s="4">
-        <v>45992</v>
+        <v>46010</v>
       </c>
       <c r="C325" t="s">
         <v>8</v>
@@ -4573,7 +4616,7 @@
         <v>325</v>
       </c>
       <c r="B326" s="4">
-        <v>45993</v>
+        <v>46011</v>
       </c>
       <c r="C326" t="s">
         <v>8</v>
@@ -4584,7 +4627,7 @@
         <v>326</v>
       </c>
       <c r="B327" s="4">
-        <v>45994</v>
+        <v>46012</v>
       </c>
       <c r="C327" t="s">
         <v>8</v>
@@ -4595,7 +4638,7 @@
         <v>327</v>
       </c>
       <c r="B328" s="4">
-        <v>45995</v>
+        <v>46013</v>
       </c>
       <c r="C328" t="s">
         <v>8</v>
@@ -4606,7 +4649,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="4">
-        <v>45996</v>
+        <v>46014</v>
       </c>
       <c r="C329" t="s">
         <v>8</v>
@@ -4617,7 +4660,7 @@
         <v>329</v>
       </c>
       <c r="B330" s="4">
-        <v>45997</v>
+        <v>46015</v>
       </c>
       <c r="C330" t="s">
         <v>8</v>
@@ -4628,7 +4671,7 @@
         <v>330</v>
       </c>
       <c r="B331" s="4">
-        <v>45998</v>
+        <v>46016</v>
       </c>
       <c r="C331" t="s">
         <v>8</v>
@@ -4639,7 +4682,7 @@
         <v>331</v>
       </c>
       <c r="B332" s="4">
-        <v>45999</v>
+        <v>46017</v>
       </c>
       <c r="C332" t="s">
         <v>47</v>
@@ -4650,7 +4693,7 @@
         <v>332</v>
       </c>
       <c r="B333" s="4">
-        <v>46000</v>
+        <v>46018</v>
       </c>
       <c r="C333" t="s">
         <v>8</v>
@@ -4661,7 +4704,7 @@
         <v>333</v>
       </c>
       <c r="B334" s="4">
-        <v>46001</v>
+        <v>46019</v>
       </c>
       <c r="C334" t="s">
         <v>8</v>
@@ -4672,7 +4715,7 @@
         <v>334</v>
       </c>
       <c r="B335" s="4">
-        <v>46002</v>
+        <v>46020</v>
       </c>
       <c r="C335" t="s">
         <v>8</v>
@@ -4683,10 +4726,10 @@
         <v>335</v>
       </c>
       <c r="B336" s="4">
-        <v>46003</v>
+        <v>46021</v>
       </c>
       <c r="C336" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
@@ -4694,7 +4737,7 @@
         <v>336</v>
       </c>
       <c r="B337" s="4">
-        <v>46004</v>
+        <v>46022</v>
       </c>
       <c r="C337" t="s">
         <v>8</v>
@@ -4705,10 +4748,10 @@
         <v>337</v>
       </c>
       <c r="B338" s="4">
-        <v>46005</v>
+        <v>46023</v>
       </c>
       <c r="C338" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
@@ -4716,7 +4759,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="4">
-        <v>46006</v>
+        <v>46024</v>
       </c>
       <c r="C339" t="s">
         <v>8</v>
@@ -4727,7 +4770,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="4">
-        <v>46007</v>
+        <v>46025</v>
       </c>
       <c r="C340" t="s">
         <v>8</v>
@@ -4738,7 +4781,7 @@
         <v>340</v>
       </c>
       <c r="B341" s="4">
-        <v>46008</v>
+        <v>46026</v>
       </c>
       <c r="C341" t="s">
         <v>8</v>
@@ -4749,7 +4792,7 @@
         <v>341</v>
       </c>
       <c r="B342" s="4">
-        <v>46009</v>
+        <v>46027</v>
       </c>
       <c r="C342" t="s">
         <v>8</v>
@@ -4760,7 +4803,7 @@
         <v>342</v>
       </c>
       <c r="B343" s="4">
-        <v>46010</v>
+        <v>46028</v>
       </c>
       <c r="C343" t="s">
         <v>8</v>
@@ -4771,7 +4814,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="4">
-        <v>46011</v>
+        <v>46029</v>
       </c>
       <c r="C344" t="s">
         <v>8</v>
@@ -4782,7 +4825,7 @@
         <v>344</v>
       </c>
       <c r="B345" s="4">
-        <v>46012</v>
+        <v>46030</v>
       </c>
       <c r="C345" t="s">
         <v>8</v>
@@ -4793,7 +4836,7 @@
         <v>345</v>
       </c>
       <c r="B346" s="4">
-        <v>46013</v>
+        <v>46031</v>
       </c>
       <c r="C346" t="s">
         <v>8</v>
@@ -4804,7 +4847,7 @@
         <v>346</v>
       </c>
       <c r="B347" s="4">
-        <v>46014</v>
+        <v>46032</v>
       </c>
       <c r="C347" t="s">
         <v>8</v>
@@ -4815,7 +4858,7 @@
         <v>347</v>
       </c>
       <c r="B348" s="4">
-        <v>46015</v>
+        <v>46033</v>
       </c>
       <c r="C348" t="s">
         <v>8</v>
@@ -4826,7 +4869,7 @@
         <v>348</v>
       </c>
       <c r="B349" s="4">
-        <v>46016</v>
+        <v>46034</v>
       </c>
       <c r="C349" t="s">
         <v>8</v>
@@ -4837,7 +4880,7 @@
         <v>349</v>
       </c>
       <c r="B350" s="4">
-        <v>46017</v>
+        <v>46035</v>
       </c>
       <c r="C350" t="s">
         <v>8</v>
@@ -4848,7 +4891,7 @@
         <v>350</v>
       </c>
       <c r="B351" s="4">
-        <v>46018</v>
+        <v>46036</v>
       </c>
       <c r="C351" t="s">
         <v>8</v>
@@ -4859,7 +4902,7 @@
         <v>351</v>
       </c>
       <c r="B352" s="4">
-        <v>46019</v>
+        <v>46037</v>
       </c>
       <c r="C352" t="s">
         <v>8</v>
@@ -4870,7 +4913,7 @@
         <v>352</v>
       </c>
       <c r="B353" s="4">
-        <v>46020</v>
+        <v>46038</v>
       </c>
       <c r="C353" t="s">
         <v>8</v>
@@ -4881,7 +4924,7 @@
         <v>353</v>
       </c>
       <c r="B354" s="4">
-        <v>46021</v>
+        <v>46039</v>
       </c>
       <c r="C354" t="s">
         <v>8</v>
@@ -4892,7 +4935,7 @@
         <v>354</v>
       </c>
       <c r="B355" s="4">
-        <v>46022</v>
+        <v>46040</v>
       </c>
       <c r="C355" t="s">
         <v>8</v>
@@ -4903,7 +4946,7 @@
         <v>355</v>
       </c>
       <c r="B356" s="4">
-        <v>46023</v>
+        <v>46041</v>
       </c>
       <c r="C356" t="s">
         <v>8</v>
@@ -4914,7 +4957,7 @@
         <v>356</v>
       </c>
       <c r="B357" s="4">
-        <v>46024</v>
+        <v>46042</v>
       </c>
       <c r="C357" t="s">
         <v>8</v>
@@ -4925,7 +4968,7 @@
         <v>357</v>
       </c>
       <c r="B358" s="4">
-        <v>46025</v>
+        <v>46043</v>
       </c>
       <c r="C358" t="s">
         <v>8</v>
@@ -4936,7 +4979,7 @@
         <v>358</v>
       </c>
       <c r="B359" s="4">
-        <v>46026</v>
+        <v>46044</v>
       </c>
       <c r="C359" t="s">
         <v>8</v>
@@ -4947,7 +4990,7 @@
         <v>359</v>
       </c>
       <c r="B360" s="4">
-        <v>46027</v>
+        <v>46045</v>
       </c>
       <c r="C360" t="s">
         <v>8</v>
@@ -4958,7 +5001,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="4">
-        <v>46028</v>
+        <v>46046</v>
       </c>
       <c r="C361" t="s">
         <v>8</v>
@@ -4969,7 +5012,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="4">
-        <v>46029</v>
+        <v>46047</v>
       </c>
       <c r="C362" t="s">
         <v>8</v>
@@ -4981,7 +5024,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="4">
-        <v>46030</v>
+        <v>46048</v>
       </c>
       <c r="C363" t="s">
         <v>48</v>
@@ -4992,7 +5035,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="4">
-        <v>46031</v>
+        <v>46049</v>
       </c>
       <c r="C364" t="s">
         <v>8</v>
@@ -5003,7 +5046,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="4">
-        <v>46032</v>
+        <v>46050</v>
       </c>
       <c r="C365" t="s">
         <v>8</v>
@@ -5014,7 +5057,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="4">
-        <v>46033</v>
+        <v>46051</v>
       </c>
       <c r="C366" t="s">
         <v>8</v>
@@ -5025,10 +5068,10 @@
         <v>366</v>
       </c>
       <c r="B367" s="4">
-        <v>46034</v>
+        <v>46052</v>
       </c>
       <c r="C367" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Noves fotus, idea de pelis
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B603CB-3F34-40C3-912F-8B71EF9EC2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2403B18E-C0AB-4CF7-8BA6-95150E98951C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="192">
   <si>
     <t>Dia</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Perquè tens el somriure més maco del món sencer</t>
   </si>
   <si>
-    <t>Perquè ets una persona molt treballadora.</t>
-  </si>
-  <si>
     <t>./img/lady_bug.jpeg</t>
   </si>
   <si>
@@ -519,9 +516,6 @@
     <t>Perquè vam anar a un concert de JOAN DAUSÀ (no hi ha fotos :( )</t>
   </si>
   <si>
-    <t>Perquè ets molt elegant</t>
-  </si>
-  <si>
     <t>Perquè saps que dir en els moments imprtants</t>
   </si>
   <si>
@@ -531,13 +525,82 @@
     <t>Perquè ets fàcil de perdonar (per exemple, el missatge d'ahir ja te'l he perdonat)</t>
   </si>
   <si>
-    <t>Perquè tens molta memòria, no se si encara et faig jugar al My Singuin Monsters però erets MASSA bona al memory!</t>
-  </si>
-  <si>
     <t>./img/singuing_monsters.jpeg</t>
   </si>
   <si>
     <t>./img/mirall_andorra1.jpeg</t>
+  </si>
+  <si>
+    <t>Perquè tens molta memòria, no se si encara et faig jugar al My Singuing Monsters però erets MASSA bona al memory!</t>
+  </si>
+  <si>
+    <t>Perquè ets una persona molt treballadora. (Enhorabona pel teu examen de psicoo!!!)</t>
+  </si>
+  <si>
+    <t>Perquè ets molt elegant ;)</t>
+  </si>
+  <si>
+    <t>Perquè saps com fer-me riure</t>
+  </si>
+  <si>
+    <t>Perquè les teves inseguretats son coses que jo adoro de tú</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè ets LA MILLOR MONITORA QUE HA TINGUT LA MEVA COSINA </t>
+  </si>
+  <si>
+    <t>Perquè hem vist pel·lícules MOLT XULES JUNTS. Et deixo el tràiler de la PRIMERA PELI que vam veure junts! Quins nervis.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RDE6Uz73A7g</t>
+  </si>
+  <si>
+    <t>Perquè ets una noia atenta</t>
+  </si>
+  <si>
+    <t>Perquè em cuides quan estic MOOOLT MALALT (sempre)</t>
+  </si>
+  <si>
+    <t>./img/malito.jpg</t>
+  </si>
+  <si>
+    <t>Perquè ets molt endreçada (almenys quan he de venir a casa teva)</t>
+  </si>
+  <si>
+    <t>Perquè no em deixes entrar a la teva habitació si no està neta</t>
+  </si>
+  <si>
+    <t>Perquè ets divertida</t>
+  </si>
+  <si>
+    <t>Perquè ets detallista</t>
+  </si>
+  <si>
+    <t>Perquè quan és nadal compres amb mi la figuerta al mercat de Santa Llucia</t>
+  </si>
+  <si>
+    <t>Perquè soc el teu XOFER PERSONAL i m'encanta encara que em queixi (molt poques vegades, però)</t>
+  </si>
+  <si>
+    <t>Perquè em fas riure molt quan et fas la xula</t>
+  </si>
+  <si>
+    <t>Perquè m'has deixat descobrir la teva manera de riure</t>
+  </si>
+  <si>
+    <t>Perquè m'encanta que m'expliquis els teus problemes</t>
+  </si>
+  <si>
+    <t>Perquè sempre m'escoltes quan t'explico els meus problemes</t>
+  </si>
+  <si>
+    <t>Perquè m'has fet descobrir LA ISLA DE LAS TENTACIONES (tot i que al principi ho criticava molt)</t>
+  </si>
+  <si>
+    <t>./img/isla.jpg</t>
+  </si>
+  <si>
+    <t>M'ha ENCANTAT criticar a aquesta noia amb tu :)</t>
   </si>
 </sst>
 </file>
@@ -585,12 +648,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C353" sqref="C353"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="95" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,7 +1012,7 @@
         <v>45687</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -957,7 +1021,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -968,7 +1032,7 @@
         <v>45688</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -982,7 +1046,7 @@
         <v>45689</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1005,7 +1069,7 @@
         <v>45691</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1016,7 +1080,7 @@
         <v>45692</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1026,14 +1090,14 @@
       <c r="B8" s="4">
         <v>45693</v>
       </c>
-      <c r="C8" t="s">
-        <v>144</v>
+      <c r="C8" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
         <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
@@ -1046,7 +1110,7 @@
         <v>45694</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -1058,7 +1122,7 @@
         <v>45695</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -1070,7 +1134,7 @@
         <v>45696</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1082,13 +1146,13 @@
         <v>45697</v>
       </c>
       <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
         <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1099,7 +1163,7 @@
         <v>45698</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1110,7 +1174,7 @@
         <v>45699</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1123,7 +1187,7 @@
         <v>45700</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1134,7 +1198,7 @@
         <v>45701</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -1146,13 +1210,13 @@
         <v>45702</v>
       </c>
       <c r="C17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" t="s">
         <v>145</v>
-      </c>
-      <c r="D17" t="s">
-        <v>147</v>
-      </c>
-      <c r="E17" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1163,7 +1227,7 @@
         <v>45703</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1174,13 +1238,13 @@
         <v>45704</v>
       </c>
       <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
         <v>24</v>
       </c>
-      <c r="D19" t="s">
-        <v>25</v>
-      </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1192,7 +1256,7 @@
         <v>45705</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1203,7 +1267,7 @@
         <v>45706</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="2"/>
     </row>
@@ -1215,7 +1279,7 @@
         <v>45707</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1226,7 +1290,7 @@
         <v>45708</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1237,7 +1301,7 @@
         <v>45709</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1248,7 +1312,7 @@
         <v>45710</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1259,7 +1323,7 @@
         <v>45711</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1270,7 +1334,7 @@
         <v>45712</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1281,10 +1345,10 @@
         <v>45713</v>
       </c>
       <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" t="s">
         <v>35</v>
-      </c>
-      <c r="F28" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1295,7 +1359,7 @@
         <v>45714</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1306,7 +1370,7 @@
         <v>45715</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1317,7 +1381,7 @@
         <v>45716</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1328,7 +1392,7 @@
         <v>45717</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1339,7 +1403,7 @@
         <v>45718</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1350,7 +1414,7 @@
         <v>45719</v>
       </c>
       <c r="C34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1361,7 +1425,7 @@
         <v>45720</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1372,7 +1436,13 @@
         <v>45721</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>189</v>
+      </c>
+      <c r="D36" t="s">
+        <v>190</v>
+      </c>
+      <c r="E36" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1383,7 +1453,7 @@
         <v>45722</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1394,7 +1464,7 @@
         <v>45723</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1405,7 +1475,7 @@
         <v>45724</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1416,7 +1486,7 @@
         <v>45725</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1427,7 +1497,7 @@
         <v>45726</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1438,7 +1508,7 @@
         <v>45727</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1449,13 +1519,13 @@
         <v>45728</v>
       </c>
       <c r="C43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D43" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" t="s">
         <v>150</v>
-      </c>
-      <c r="E43" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1466,7 +1536,7 @@
         <v>45729</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1477,10 +1547,10 @@
         <v>45730</v>
       </c>
       <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" t="s">
         <v>65</v>
-      </c>
-      <c r="F45" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1491,7 +1561,7 @@
         <v>45731</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1502,7 +1572,7 @@
         <v>45732</v>
       </c>
       <c r="C47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,7 +1583,7 @@
         <v>45733</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1524,7 +1594,7 @@
         <v>45734</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1535,7 +1605,7 @@
         <v>45735</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1546,7 +1616,7 @@
         <v>45736</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1557,7 +1627,7 @@
         <v>45737</v>
       </c>
       <c r="C52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1568,7 +1638,7 @@
         <v>45738</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1579,7 +1649,7 @@
         <v>45739</v>
       </c>
       <c r="C54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1590,7 +1660,7 @@
         <v>45740</v>
       </c>
       <c r="C55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1601,7 +1671,7 @@
         <v>45741</v>
       </c>
       <c r="C56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1612,7 +1682,7 @@
         <v>45742</v>
       </c>
       <c r="C57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1623,13 +1693,13 @@
         <v>45743</v>
       </c>
       <c r="C58" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" t="s">
         <v>78</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>79</v>
-      </c>
-      <c r="E58" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1640,10 +1710,10 @@
         <v>45744</v>
       </c>
       <c r="C59" t="s">
+        <v>151</v>
+      </c>
+      <c r="F59" t="s">
         <v>152</v>
-      </c>
-      <c r="F59" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1654,7 +1724,7 @@
         <v>45745</v>
       </c>
       <c r="C60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1665,7 +1735,7 @@
         <v>45746</v>
       </c>
       <c r="C61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1676,7 +1746,7 @@
         <v>45747</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1687,7 +1757,7 @@
         <v>45748</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1698,7 +1768,7 @@
         <v>45749</v>
       </c>
       <c r="C64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1709,10 +1779,10 @@
         <v>45750</v>
       </c>
       <c r="C65" t="s">
+        <v>94</v>
+      </c>
+      <c r="F65" t="s">
         <v>95</v>
-      </c>
-      <c r="F65" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1723,7 +1793,7 @@
         <v>45751</v>
       </c>
       <c r="C66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1734,7 +1804,7 @@
         <v>45752</v>
       </c>
       <c r="C67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1745,7 +1815,7 @@
         <v>45753</v>
       </c>
       <c r="C68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -1756,7 +1826,7 @@
         <v>45754</v>
       </c>
       <c r="C69" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -1767,7 +1837,7 @@
         <v>45755</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -1778,13 +1848,13 @@
         <v>45756</v>
       </c>
       <c r="C71" t="s">
+        <v>101</v>
+      </c>
+      <c r="D71" t="s">
         <v>102</v>
       </c>
-      <c r="D71" t="s">
-        <v>103</v>
-      </c>
       <c r="E71" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -1795,7 +1865,7 @@
         <v>45757</v>
       </c>
       <c r="C72" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -1806,7 +1876,7 @@
         <v>45758</v>
       </c>
       <c r="C73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -1817,7 +1887,7 @@
         <v>45759</v>
       </c>
       <c r="C74" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -1828,7 +1898,7 @@
         <v>45760</v>
       </c>
       <c r="C75" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -1839,7 +1909,7 @@
         <v>45761</v>
       </c>
       <c r="C76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -1850,7 +1920,7 @@
         <v>45762</v>
       </c>
       <c r="C77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -1861,7 +1931,7 @@
         <v>45763</v>
       </c>
       <c r="C78" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -1872,7 +1942,7 @@
         <v>45764</v>
       </c>
       <c r="C79" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -1883,10 +1953,10 @@
         <v>45765</v>
       </c>
       <c r="C80" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -1897,7 +1967,7 @@
         <v>45766</v>
       </c>
       <c r="C81" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -1908,7 +1978,7 @@
         <v>45767</v>
       </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -1919,13 +1989,13 @@
         <v>45768</v>
       </c>
       <c r="C83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D83" t="s">
+        <v>114</v>
+      </c>
+      <c r="E83" t="s">
         <v>115</v>
-      </c>
-      <c r="E83" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -1936,7 +2006,7 @@
         <v>45769</v>
       </c>
       <c r="C84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -1947,13 +2017,13 @@
         <v>45770</v>
       </c>
       <c r="C85" t="s">
+        <v>117</v>
+      </c>
+      <c r="D85" t="s">
         <v>118</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>119</v>
-      </c>
-      <c r="E85" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -1964,7 +2034,7 @@
         <v>45771</v>
       </c>
       <c r="C86" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -1975,7 +2045,7 @@
         <v>45772</v>
       </c>
       <c r="C87" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -1986,7 +2056,7 @@
         <v>45773</v>
       </c>
       <c r="C88" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -1997,7 +2067,7 @@
         <v>45774</v>
       </c>
       <c r="C89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2008,7 +2078,7 @@
         <v>45775</v>
       </c>
       <c r="C90" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2019,7 +2089,7 @@
         <v>45776</v>
       </c>
       <c r="C91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2030,7 +2100,7 @@
         <v>45777</v>
       </c>
       <c r="C92" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2041,7 +2111,7 @@
         <v>45778</v>
       </c>
       <c r="C93" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2052,10 +2122,10 @@
         <v>45779</v>
       </c>
       <c r="C94" t="s">
+        <v>125</v>
+      </c>
+      <c r="F94" t="s">
         <v>126</v>
-      </c>
-      <c r="F94" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2066,13 +2136,13 @@
         <v>45780</v>
       </c>
       <c r="C95" t="s">
+        <v>50</v>
+      </c>
+      <c r="D95" t="s">
         <v>51</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>52</v>
-      </c>
-      <c r="E95" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2083,10 +2153,10 @@
         <v>45781</v>
       </c>
       <c r="C96" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2094,10 +2164,10 @@
         <v>45782</v>
       </c>
       <c r="C97" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2105,13 +2175,13 @@
         <v>45783</v>
       </c>
       <c r="C98" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D98" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2119,10 +2189,10 @@
         <v>45784</v>
       </c>
       <c r="C99" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2130,10 +2200,10 @@
         <v>45785</v>
       </c>
       <c r="C100" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2141,10 +2211,10 @@
         <v>45786</v>
       </c>
       <c r="C101" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2152,10 +2222,10 @@
         <v>45787</v>
       </c>
       <c r="C102" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2163,10 +2233,10 @@
         <v>45788</v>
       </c>
       <c r="C103" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2174,10 +2244,10 @@
         <v>45789</v>
       </c>
       <c r="C104" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2185,10 +2255,10 @@
         <v>45790</v>
       </c>
       <c r="C105" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2196,10 +2266,10 @@
         <v>45791</v>
       </c>
       <c r="C106" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2210,10 +2280,10 @@
         <v>168</v>
       </c>
       <c r="D107" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2221,10 +2291,10 @@
         <v>45793</v>
       </c>
       <c r="C108" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2232,10 +2302,10 @@
         <v>45794</v>
       </c>
       <c r="C109" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2243,10 +2313,10 @@
         <v>45795</v>
       </c>
       <c r="C110" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2254,10 +2324,13 @@
         <v>45796</v>
       </c>
       <c r="C111" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+      <c r="F111" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2265,10 +2338,10 @@
         <v>45797</v>
       </c>
       <c r="C112" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2276,10 +2349,13 @@
         <v>45798</v>
       </c>
       <c r="C113" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+      <c r="D113" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2287,10 +2363,10 @@
         <v>45799</v>
       </c>
       <c r="C114" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2298,10 +2374,10 @@
         <v>45800</v>
       </c>
       <c r="C115" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2309,10 +2385,10 @@
         <v>45801</v>
       </c>
       <c r="C116" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2320,10 +2396,10 @@
         <v>45802</v>
       </c>
       <c r="C117" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2331,10 +2407,10 @@
         <v>45803</v>
       </c>
       <c r="C118" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2342,10 +2418,10 @@
         <v>45804</v>
       </c>
       <c r="C119" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2353,10 +2429,10 @@
         <v>45805</v>
       </c>
       <c r="C120" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2364,10 +2440,10 @@
         <v>45806</v>
       </c>
       <c r="C121" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2375,10 +2451,10 @@
         <v>45807</v>
       </c>
       <c r="C122" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2386,10 +2462,10 @@
         <v>45808</v>
       </c>
       <c r="C123" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2397,10 +2473,10 @@
         <v>45809</v>
       </c>
       <c r="C124" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2408,10 +2484,10 @@
         <v>45810</v>
       </c>
       <c r="C125" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2419,10 +2495,10 @@
         <v>45811</v>
       </c>
       <c r="C126" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2430,10 +2506,10 @@
         <v>45812</v>
       </c>
       <c r="C127" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -2444,7 +2520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -2455,7 +2531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -2466,7 +2542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -2477,7 +2553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -2488,7 +2564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -2499,7 +2575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -2510,7 +2586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -2521,7 +2597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -2532,7 +2608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -2542,8 +2618,9 @@
       <c r="C137" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D137" s="2"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -2554,7 +2631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -2565,7 +2642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -2576,7 +2653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -2587,7 +2664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -2598,7 +2675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -2609,7 +2686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -2672,7 +2749,7 @@
         <v>45834</v>
       </c>
       <c r="C149" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -2716,7 +2793,7 @@
         <v>45838</v>
       </c>
       <c r="C153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -2727,7 +2804,7 @@
         <v>45839</v>
       </c>
       <c r="C154" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -3002,7 +3079,7 @@
         <v>45864</v>
       </c>
       <c r="C179" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -3046,7 +3123,7 @@
         <v>45868</v>
       </c>
       <c r="C183" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -3068,7 +3145,7 @@
         <v>45870</v>
       </c>
       <c r="C185" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -3343,7 +3420,7 @@
         <v>45895</v>
       </c>
       <c r="C210" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
@@ -3387,7 +3464,7 @@
         <v>45899</v>
       </c>
       <c r="C214" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
@@ -3409,7 +3486,7 @@
         <v>45901</v>
       </c>
       <c r="C216" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
@@ -3684,7 +3761,7 @@
         <v>45926</v>
       </c>
       <c r="C241" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
@@ -3728,7 +3805,7 @@
         <v>45930</v>
       </c>
       <c r="C245" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
@@ -3739,7 +3816,7 @@
         <v>45931</v>
       </c>
       <c r="C246" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
@@ -4014,7 +4091,7 @@
         <v>45956</v>
       </c>
       <c r="C271" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
@@ -4058,7 +4135,7 @@
         <v>45960</v>
       </c>
       <c r="C275" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
@@ -4080,7 +4157,7 @@
         <v>45962</v>
       </c>
       <c r="C277" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
@@ -4355,7 +4432,7 @@
         <v>45987</v>
       </c>
       <c r="C302" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
@@ -4399,7 +4476,7 @@
         <v>45991</v>
       </c>
       <c r="C306" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
@@ -4410,7 +4487,7 @@
         <v>45992</v>
       </c>
       <c r="C307" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
@@ -4685,7 +4762,7 @@
         <v>46017</v>
       </c>
       <c r="C332" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
@@ -4729,7 +4806,7 @@
         <v>46021</v>
       </c>
       <c r="C336" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
@@ -4751,7 +4828,7 @@
         <v>46023</v>
       </c>
       <c r="C338" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
@@ -5027,7 +5104,7 @@
         <v>46048</v>
       </c>
       <c r="C363" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.3">
@@ -5071,7 +5148,7 @@
         <v>46052</v>
       </c>
       <c r="C367" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Noves fotos i idea no estas guapa
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2403B18E-C0AB-4CF7-8BA6-95150E98951C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF23269F-42FE-4E90-A81E-DB120B462993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="209">
   <si>
     <t>Dia</t>
   </si>
@@ -585,9 +585,6 @@
     <t>Perquè em fas riure molt quan et fas la xula</t>
   </si>
   <si>
-    <t>Perquè m'has deixat descobrir la teva manera de riure</t>
-  </si>
-  <si>
     <t>Perquè m'encanta que m'expliquis els teus problemes</t>
   </si>
   <si>
@@ -601,6 +598,60 @@
   </si>
   <si>
     <t>M'ha ENCANTAT criticar a aquesta noia amb tu :)</t>
+  </si>
+  <si>
+    <t>Perquè m'has deixat descobrir la teva manera de riure, percert, tu podries anar al concurs que et passo en el vídeo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=jNOwkKfCLaU</t>
+  </si>
+  <si>
+    <t>Perquè ets LA MILLOR fent memes</t>
+  </si>
+  <si>
+    <t>./img/make_it_meme.jpg</t>
+  </si>
+  <si>
+    <t>Aquest joc (espero que t'enrecordis) vam jugar un dia al trèvol i erets MASSA BONA!</t>
+  </si>
+  <si>
+    <t>Perquè em saps apujar els anims quan ho necessito</t>
+  </si>
+  <si>
+    <t>Perquè TU LA PARTES BOY</t>
+  </si>
+  <si>
+    <t>./img/la_partes_boy.jpg</t>
+  </si>
+  <si>
+    <t>BOMBOCLAT (no se si encara està de moda això)</t>
+  </si>
+  <si>
+    <t>Perquè encara que tu diguis que no surts PERFECTE a totes les fotos (part 1)</t>
+  </si>
+  <si>
+    <t>./img/no_be1.jpeg</t>
+  </si>
+  <si>
+    <t>La foto quan va haver-hi el DESASTRE de inundació a Tarragona</t>
+  </si>
+  <si>
+    <t>Perquè encara que tu diguis que no surts PERFECTE a totes les fotos (part 2)</t>
+  </si>
+  <si>
+    <t>./img/no_be2.jpeg</t>
+  </si>
+  <si>
+    <t>Una foto on estàs PRECIOSA de quan ens vam fer els regals d'un any junts</t>
+  </si>
+  <si>
+    <t>Perquè encara que tu diguis que no surts PERFECTE a totes les fotos (part 3)</t>
+  </si>
+  <si>
+    <t>./img/no_be3.jpeg</t>
+  </si>
+  <si>
+    <t>La MEVA FOTO PREFERIDA de tu, encara que tú vas dir que la borrés :(</t>
   </si>
 </sst>
 </file>
@@ -648,13 +699,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="95" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="95" workbookViewId="0">
+      <selection activeCell="E196" sqref="E196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,7 +1140,7 @@
       <c r="B8" s="4">
         <v>45693</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" t="s">
         <v>143</v>
       </c>
       <c r="D8" t="s">
@@ -1436,13 +1486,13 @@
         <v>45721</v>
       </c>
       <c r="C36" t="s">
+        <v>188</v>
+      </c>
+      <c r="D36" t="s">
         <v>189</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>190</v>
-      </c>
-      <c r="E36" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2341,7 +2391,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2355,7 +2405,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2366,7 +2416,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2377,7 +2427,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2388,7 +2438,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2399,7 +2449,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2410,7 +2460,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2421,7 +2471,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2432,7 +2482,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2443,7 +2493,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2454,7 +2504,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2462,10 +2512,13 @@
         <v>45808</v>
       </c>
       <c r="C123" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+      <c r="F123" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2476,7 +2529,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2484,10 +2537,10 @@
         <v>45810</v>
       </c>
       <c r="C125" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2495,10 +2548,10 @@
         <v>45811</v>
       </c>
       <c r="C126" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2509,7 +2562,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -2517,10 +2570,16 @@
         <v>45813</v>
       </c>
       <c r="C128" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+      <c r="D128" t="s">
+        <v>194</v>
+      </c>
+      <c r="E128" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -2528,10 +2587,10 @@
         <v>45814</v>
       </c>
       <c r="C129" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -2539,10 +2598,16 @@
         <v>45815</v>
       </c>
       <c r="C130" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+      <c r="D130" t="s">
+        <v>198</v>
+      </c>
+      <c r="E130" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -2553,7 +2618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -2564,7 +2629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -2575,7 +2640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -2586,7 +2651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -2597,7 +2662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -2608,7 +2673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -2620,7 +2685,7 @@
       </c>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -2628,10 +2693,16 @@
         <v>45823</v>
       </c>
       <c r="C138" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+      <c r="D138" t="s">
+        <v>201</v>
+      </c>
+      <c r="E138" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -2642,7 +2713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -2653,7 +2724,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -2664,7 +2735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -2675,7 +2746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -2686,7 +2757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -2873,7 +2944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -2884,7 +2955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -2895,7 +2966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -2906,7 +2977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -2917,7 +2988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -2925,10 +2996,16 @@
         <v>45850</v>
       </c>
       <c r="C165" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="D165" t="s">
+        <v>204</v>
+      </c>
+      <c r="E165" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -2939,7 +3016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -2950,7 +3027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -2961,7 +3038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -2972,7 +3049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -2983,7 +3060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -2994,7 +3071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -3005,7 +3082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -3016,7 +3093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -3027,7 +3104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -3038,7 +3115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -3225,7 +3302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>192</v>
       </c>
@@ -3236,7 +3313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>193</v>
       </c>
@@ -3247,7 +3324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>194</v>
       </c>
@@ -3258,7 +3335,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>195</v>
       </c>
@@ -3266,10 +3343,16 @@
         <v>45881</v>
       </c>
       <c r="C196" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="D196" t="s">
+        <v>207</v>
+      </c>
+      <c r="E196" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>196</v>
       </c>
@@ -3280,7 +3363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>197</v>
       </c>
@@ -3291,7 +3374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>198</v>
       </c>
@@ -3302,7 +3385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>199</v>
       </c>
@@ -3313,7 +3396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>200</v>
       </c>
@@ -3324,7 +3407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>201</v>
       </c>
@@ -3335,7 +3418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>202</v>
       </c>
@@ -3346,7 +3429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>203</v>
       </c>
@@ -3357,7 +3440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>204</v>
       </c>
@@ -3368,7 +3451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>205</v>
       </c>
@@ -3379,7 +3462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>206</v>
       </c>
@@ -3390,7 +3473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>207</v>
       </c>

</xml_diff>

<commit_message>
Noves fotos i videos
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0536B6D5-B046-4DAC-8D7D-D4FC5658081F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE9BF5C-EE00-4615-8A91-22D7F571EA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="285">
   <si>
     <t>Dia</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Perquè ets la meva trois-tête preferida (fixa't com de bé escric en Francès!!)</t>
   </si>
   <si>
-    <t>Perquè ets una persona atenta</t>
-  </si>
-  <si>
     <t>Perquè cada dia que passa estic més enamorat de tú</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>https://www.youtube.com/watch?v=n2igjYFojUo</t>
   </si>
   <si>
-    <t>Perquè fa 1 ANY I MIG que quedem (sí t'ho recordare cada més)</t>
-  </si>
-  <si>
     <t>Perquè fa 1 ANY I SET MESOS QUE QUEDEM</t>
   </si>
   <si>
@@ -219,9 +213,6 @@
     <t>Perquè fas veure que t'interesses per les coses de la meva carrera</t>
   </si>
   <si>
-    <t>Perquè em dius friki i m'encanta (encara que faig veure que no.) Si apretes el link podràs veure que vol dir ser un friki i potser ti sents identificada</t>
-  </si>
-  <si>
     <t>https://ca.wikipedia.org/wiki/Friqui</t>
   </si>
   <si>
@@ -456,9 +447,6 @@
     <t>Perquè sempre em demostres el teu amor, inclús quan és el dia dels enamoraaaats!! (AVUIIIII) I per celebrar-ho…</t>
   </si>
   <si>
-    <t>Aquí veuràs un espòiler de què farem avui!! (Espero que puguis)</t>
-  </si>
-  <si>
     <t>./img/impro_show.jpeg</t>
   </si>
   <si>
@@ -748,6 +736,150 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Perquè quan ens enfadem ho sabem solucionar.</t>
+  </si>
+  <si>
+    <t>Perquè ets una persona atenta i que sap parlar amb mi quan tenim qualsevol problema.</t>
+  </si>
+  <si>
+    <t>Perquè hem vist pel·lícules MOLT XULES JUNTS AL CINE. La segona que vam veure junts és segurament la teva preferida per raons que no conec, però et deixo el tràiler.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zUFt9_WOoPc</t>
+  </si>
+  <si>
+    <t>Perquè hem vist pel·lícules MOLT XULES JUNTS AL CINE. La tercera que vam veure junts em vas dir que no t'agradaria perquè era d'animació, però tu vas acabar plorant perquè era MOOOLT xula (sempre tinc raò)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8-_4gvrHAys</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=t06RUxPbp_c</t>
+  </si>
+  <si>
+    <t>Perquè hem vist pel·lícules MOLT XULES JUNTS AL CINE. La quarta que vam veure junts va ser al cine de Tarragona, quan vam anar-hi amb els meus pares. Va d'un superheroi que és BASTANT guai, però no tant com jo</t>
+  </si>
+  <si>
+    <t>Perquè hem vist pel·lícules MOLT XULES JUNTS AL CINE. La cinquena que vam veure junts tu vas dir que et va agradar, a mi també però era MASSA rara i feia MOLT fàstic. Et deixo el tràiler (jo no l'he pogut tornar a mirar)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LL7-o30o9ec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè hem vist pel·lícules MOLT XULES JUNTS AL CINE. La sisena que vam veure junts va ser BASTANT xula, però tú vas dir que molt avorrida. Ens van possar un curt i van fer un col·loqui abans de la peli. Et deixo el tràiler. </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Hoh3SiB5Lmo</t>
+  </si>
+  <si>
+    <t>Perquè hem vist pel·lícules MOLT XULES JUNTS AL CINE. La setena que vam veure junts va ser molt guai, però la voliem veure en versió original per escoltar les cançons i no vam poder :(. Et deixo el tràiler</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UNHQgy3jawI</t>
+  </si>
+  <si>
+    <t>Perquè m'encanta quan obres els meus regals.</t>
+  </si>
+  <si>
+    <t>./img/any1.jpeg</t>
+  </si>
+  <si>
+    <t>Aquesta foto, encara que una mica borrosa, surt com de guapa estaves quan vas obrir les pistes per accedir a aquesta FANTÀSTICA web</t>
+  </si>
+  <si>
+    <t>Perquè em dones calma</t>
+  </si>
+  <si>
+    <t>Perquè m'expliques com funcionen les teves assignatures de la universitat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè em prioritzes (NO SEMPRE I U HAURIES DE FER SEMPRE) </t>
+  </si>
+  <si>
+    <t>Perquè no ets envejosa</t>
+  </si>
+  <si>
+    <t>Perquè rius de les bromes que faig quan et dic que hauries de ser MEGA TOXICA (tinc raò, ho has de ser més)</t>
+  </si>
+  <si>
+    <t>Perquè tot i que no coincidim molt en gustos musicals, sempre ets LA MILLOR DJ quan et porto en cotxe. (Per cert, espero que ja tinguis el carnet!)</t>
+  </si>
+  <si>
+    <t>Perquè no t'enfades amb mi tot i que alguns cops faig molt el tonto (siusplau no t'enfadis per posar la foto d'ahir)</t>
+  </si>
+  <si>
+    <t>Perquè som una parella SUPER GUAPA</t>
+  </si>
+  <si>
+    <t>./img/mirall_altre.jpeg</t>
+  </si>
+  <si>
+    <t>Una foto que vaig fer jo encara que no tinc una gran habilitat amb el mòbil</t>
+  </si>
+  <si>
+    <t>Perquè m'encanta quan poguem anem agafats de la mà tot i que al principi no ho feiem</t>
+  </si>
+  <si>
+    <t>Perquè m'has fet descobrir-te i descorir-me més a mi mateix</t>
+  </si>
+  <si>
+    <t>Perquè et poses MOLT vermella quan et poses nerviosa</t>
+  </si>
+  <si>
+    <t>Perquè t'encanta queixar-te</t>
+  </si>
+  <si>
+    <t>Perquè t'agrada molt (potser massa) fer-me enfadar</t>
+  </si>
+  <si>
+    <t>Aquí tens un espòiler de què farem avui!! (Potser mengem una mica de sushi també!)</t>
+  </si>
+  <si>
+    <t>Perquè fa 1 ANY I MIG que quedem (sí t'ho recordare cada mes). Aquest, però, és moooolt especial perquè 1 any i mig es un MONTON de temps!</t>
+  </si>
+  <si>
+    <t>Perquè em dius friki i m'encanta (encara que faig veure que no.) Si apretes el link podràs veure que vol dir ser un friki i potser t'hi sents identificada</t>
+  </si>
+  <si>
+    <t>Perquè el primer viatje que vam fer ja em va fer veure que t'estimare sempre</t>
+  </si>
+  <si>
+    <t>./img/foto_riu.jpeg</t>
+  </si>
+  <si>
+    <t>Vam anar a Andorra la Vella, ens ho vam passar mooolt be</t>
+  </si>
+  <si>
+    <t>Perquè tens uns ulls preciosos (això ja t'ho havia dit però és veritat)</t>
+  </si>
+  <si>
+    <t>./img/ulls_macos.jpg</t>
+  </si>
+  <si>
+    <t>En aquesta foto que vam fer a Andorra la Vella se't veuen uns ulls preciosos. Ets la noia més guapa del món.</t>
+  </si>
+  <si>
+    <t>Perquè quan dormim junts sempre em dius que tens fred o calor (MOOOLT PESADA)</t>
+  </si>
+  <si>
+    <t>Perquè sempre hem demanes pijama</t>
+  </si>
+  <si>
+    <t>Perquè la meva roba et queda millor que a mi</t>
+  </si>
+  <si>
+    <t>Perquè em fas regals MOLT XULOS (alguns cops robats de l'Eloi)</t>
+  </si>
+  <si>
+    <t>Perquè m'ajudes a netejar</t>
+  </si>
+  <si>
+    <t>./img/netejant_cotxe.jpg</t>
+  </si>
+  <si>
+    <t>Aquí està la netejadora MÉS GUAPA de cotxes ajudant al xòfer a que la LIMUSINA en la que va estigui neta</t>
   </si>
 </sst>
 </file>
@@ -758,7 +890,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -770,6 +902,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -792,17 +932,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1117,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="95" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="81" workbookViewId="0">
+      <selection activeCell="E183" sqref="E183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1158,7 +1301,7 @@
         <v>45687</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -1167,7 +1310,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1178,7 +1321,7 @@
         <v>45688</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -1192,7 +1335,7 @@
         <v>45689</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1215,7 +1358,7 @@
         <v>45691</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1226,7 +1369,7 @@
         <v>45692</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1237,7 +1380,7 @@
         <v>45693</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1295,7 +1438,7 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
@@ -1333,7 +1476,7 @@
         <v>45700</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1344,7 +1487,7 @@
         <v>45701</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -1356,13 +1499,13 @@
         <v>45702</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1373,7 +1516,7 @@
         <v>45703</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1384,13 +1527,13 @@
         <v>45704</v>
       </c>
       <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" t="s">
-        <v>24</v>
-      </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1402,7 +1545,7 @@
         <v>45705</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1413,7 +1556,7 @@
         <v>45706</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="2"/>
     </row>
@@ -1425,7 +1568,7 @@
         <v>45707</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1436,7 +1579,7 @@
         <v>45708</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1447,7 +1590,7 @@
         <v>45709</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1458,7 +1601,7 @@
         <v>45710</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1469,7 +1612,7 @@
         <v>45711</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1480,7 +1623,7 @@
         <v>45712</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1491,10 +1634,10 @@
         <v>45713</v>
       </c>
       <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
         <v>34</v>
-      </c>
-      <c r="F28" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1505,7 +1648,7 @@
         <v>45714</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1516,7 +1659,7 @@
         <v>45715</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1527,7 +1670,7 @@
         <v>45716</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1538,7 +1681,7 @@
         <v>45717</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1549,7 +1692,7 @@
         <v>45718</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1560,7 +1703,7 @@
         <v>45719</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1571,7 +1714,7 @@
         <v>45720</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1582,13 +1725,13 @@
         <v>45721</v>
       </c>
       <c r="C36" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D36" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E36" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1599,7 +1742,7 @@
         <v>45722</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1610,7 +1753,7 @@
         <v>45723</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1621,7 +1764,7 @@
         <v>45724</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1632,7 +1775,7 @@
         <v>45725</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1643,7 +1786,7 @@
         <v>45726</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1654,7 +1797,7 @@
         <v>45727</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1665,13 +1808,13 @@
         <v>45728</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E43" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1682,7 +1825,7 @@
         <v>45729</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1693,10 +1836,10 @@
         <v>45730</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>271</v>
       </c>
       <c r="F45" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1707,7 +1850,7 @@
         <v>45731</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1718,7 +1861,7 @@
         <v>45732</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1729,7 +1872,7 @@
         <v>45733</v>
       </c>
       <c r="C48" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1740,7 +1883,7 @@
         <v>45734</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1751,7 +1894,7 @@
         <v>45735</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1762,7 +1905,7 @@
         <v>45736</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1773,7 +1916,7 @@
         <v>45737</v>
       </c>
       <c r="C52" t="s">
-        <v>72</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1784,7 +1927,7 @@
         <v>45738</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1795,7 +1938,7 @@
         <v>45739</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1806,7 +1949,7 @@
         <v>45740</v>
       </c>
       <c r="C55" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1817,7 +1960,7 @@
         <v>45741</v>
       </c>
       <c r="C56" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1828,7 +1971,7 @@
         <v>45742</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1839,13 +1982,13 @@
         <v>45743</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D58" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E58" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1856,10 +1999,10 @@
         <v>45744</v>
       </c>
       <c r="C59" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F59" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1870,7 +2013,7 @@
         <v>45745</v>
       </c>
       <c r="C60" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1881,7 +2024,7 @@
         <v>45746</v>
       </c>
       <c r="C61" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1892,7 +2035,7 @@
         <v>45747</v>
       </c>
       <c r="C62" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1903,7 +2046,7 @@
         <v>45748</v>
       </c>
       <c r="C63" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1914,7 +2057,7 @@
         <v>45749</v>
       </c>
       <c r="C64" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1925,10 +2068,10 @@
         <v>45750</v>
       </c>
       <c r="C65" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F65" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1939,7 +2082,7 @@
         <v>45751</v>
       </c>
       <c r="C66" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1950,7 +2093,7 @@
         <v>45752</v>
       </c>
       <c r="C67" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1961,7 +2104,7 @@
         <v>45753</v>
       </c>
       <c r="C68" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -1972,7 +2115,7 @@
         <v>45754</v>
       </c>
       <c r="C69" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -1983,7 +2126,7 @@
         <v>45755</v>
       </c>
       <c r="C70" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -1994,13 +2137,13 @@
         <v>45756</v>
       </c>
       <c r="C71" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D71" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E71" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2011,7 +2154,7 @@
         <v>45757</v>
       </c>
       <c r="C72" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2022,7 +2165,7 @@
         <v>45758</v>
       </c>
       <c r="C73" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2033,7 +2176,7 @@
         <v>45759</v>
       </c>
       <c r="C74" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2044,7 +2187,7 @@
         <v>45760</v>
       </c>
       <c r="C75" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2055,7 +2198,7 @@
         <v>45761</v>
       </c>
       <c r="C76" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2066,7 +2209,7 @@
         <v>45762</v>
       </c>
       <c r="C77" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2077,7 +2220,7 @@
         <v>45763</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2088,7 +2231,7 @@
         <v>45764</v>
       </c>
       <c r="C79" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2099,10 +2242,10 @@
         <v>45765</v>
       </c>
       <c r="C80" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F80" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2113,7 +2256,7 @@
         <v>45766</v>
       </c>
       <c r="C81" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2124,7 +2267,7 @@
         <v>45767</v>
       </c>
       <c r="C82" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2135,13 +2278,13 @@
         <v>45768</v>
       </c>
       <c r="C83" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" t="s">
+        <v>109</v>
+      </c>
+      <c r="E83" t="s">
         <v>110</v>
-      </c>
-      <c r="D83" t="s">
-        <v>112</v>
-      </c>
-      <c r="E83" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2152,7 +2295,7 @@
         <v>45769</v>
       </c>
       <c r="C84" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2163,13 +2306,13 @@
         <v>45770</v>
       </c>
       <c r="C85" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D85" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E85" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2180,7 +2323,7 @@
         <v>45771</v>
       </c>
       <c r="C86" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2191,7 +2334,7 @@
         <v>45772</v>
       </c>
       <c r="C87" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2202,7 +2345,7 @@
         <v>45773</v>
       </c>
       <c r="C88" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2213,7 +2356,7 @@
         <v>45774</v>
       </c>
       <c r="C89" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2224,7 +2367,7 @@
         <v>45775</v>
       </c>
       <c r="C90" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2235,7 +2378,7 @@
         <v>45776</v>
       </c>
       <c r="C91" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2246,7 +2389,7 @@
         <v>45777</v>
       </c>
       <c r="C92" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2257,7 +2400,7 @@
         <v>45778</v>
       </c>
       <c r="C93" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2268,10 +2411,10 @@
         <v>45779</v>
       </c>
       <c r="C94" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F94" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2282,13 +2425,13 @@
         <v>45780</v>
       </c>
       <c r="C95" t="s">
+        <v>48</v>
+      </c>
+      <c r="D95" t="s">
+        <v>49</v>
+      </c>
+      <c r="E95" t="s">
         <v>50</v>
-      </c>
-      <c r="D95" t="s">
-        <v>51</v>
-      </c>
-      <c r="E95" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2299,7 +2442,7 @@
         <v>45781</v>
       </c>
       <c r="C96" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2310,7 +2453,7 @@
         <v>45782</v>
       </c>
       <c r="C97" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2321,10 +2464,10 @@
         <v>45783</v>
       </c>
       <c r="C98" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D98" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2335,7 +2478,7 @@
         <v>45784</v>
       </c>
       <c r="C99" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2346,7 +2489,7 @@
         <v>45785</v>
       </c>
       <c r="C100" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2357,7 +2500,7 @@
         <v>45786</v>
       </c>
       <c r="C101" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2368,7 +2511,7 @@
         <v>45787</v>
       </c>
       <c r="C102" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2379,7 +2522,7 @@
         <v>45788</v>
       </c>
       <c r="C103" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2390,7 +2533,7 @@
         <v>45789</v>
       </c>
       <c r="C104" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2401,7 +2544,7 @@
         <v>45790</v>
       </c>
       <c r="C105" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2412,7 +2555,7 @@
         <v>45791</v>
       </c>
       <c r="C106" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2423,10 +2566,10 @@
         <v>45792</v>
       </c>
       <c r="C107" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D107" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2437,7 +2580,7 @@
         <v>45793</v>
       </c>
       <c r="C108" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2448,7 +2591,7 @@
         <v>45794</v>
       </c>
       <c r="C109" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,7 +2602,7 @@
         <v>45795</v>
       </c>
       <c r="C110" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2470,10 +2613,10 @@
         <v>45796</v>
       </c>
       <c r="C111" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F111" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -2484,7 +2627,7 @@
         <v>45797</v>
       </c>
       <c r="C112" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -2495,10 +2638,10 @@
         <v>45798</v>
       </c>
       <c r="C113" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D113" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -2509,7 +2652,7 @@
         <v>45799</v>
       </c>
       <c r="C114" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -2520,7 +2663,7 @@
         <v>45800</v>
       </c>
       <c r="C115" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -2531,7 +2674,7 @@
         <v>45801</v>
       </c>
       <c r="C116" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -2542,7 +2685,7 @@
         <v>45802</v>
       </c>
       <c r="C117" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -2553,7 +2696,7 @@
         <v>45803</v>
       </c>
       <c r="C118" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -2564,7 +2707,7 @@
         <v>45804</v>
       </c>
       <c r="C119" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -2575,7 +2718,7 @@
         <v>45805</v>
       </c>
       <c r="C120" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -2586,7 +2729,7 @@
         <v>45806</v>
       </c>
       <c r="C121" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -2597,7 +2740,7 @@
         <v>45807</v>
       </c>
       <c r="C122" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -2608,10 +2751,10 @@
         <v>45808</v>
       </c>
       <c r="C123" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F123" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -2622,7 +2765,7 @@
         <v>45809</v>
       </c>
       <c r="C124" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -2633,7 +2776,7 @@
         <v>45810</v>
       </c>
       <c r="C125" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -2644,7 +2787,7 @@
         <v>45811</v>
       </c>
       <c r="C126" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -2655,7 +2798,7 @@
         <v>45812</v>
       </c>
       <c r="C127" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -2666,13 +2809,13 @@
         <v>45813</v>
       </c>
       <c r="C128" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D128" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E128" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2683,7 +2826,7 @@
         <v>45814</v>
       </c>
       <c r="C129" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2694,13 +2837,13 @@
         <v>45815</v>
       </c>
       <c r="C130" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D130" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E130" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2711,7 +2854,7 @@
         <v>45816</v>
       </c>
       <c r="C131" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -2722,7 +2865,7 @@
         <v>45817</v>
       </c>
       <c r="C132" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -2733,7 +2876,7 @@
         <v>45818</v>
       </c>
       <c r="C133" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -2744,7 +2887,7 @@
         <v>45819</v>
       </c>
       <c r="C134" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -2755,7 +2898,7 @@
         <v>45820</v>
       </c>
       <c r="C135" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -2766,7 +2909,7 @@
         <v>45821</v>
       </c>
       <c r="C136" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -2777,13 +2920,13 @@
         <v>45822</v>
       </c>
       <c r="C137" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E137" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -2794,13 +2937,13 @@
         <v>45823</v>
       </c>
       <c r="C138" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D138" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E138" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -2811,7 +2954,7 @@
         <v>45824</v>
       </c>
       <c r="C139" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -2822,7 +2965,7 @@
         <v>45825</v>
       </c>
       <c r="C140" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -2833,7 +2976,7 @@
         <v>45826</v>
       </c>
       <c r="C141" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -2844,7 +2987,7 @@
         <v>45827</v>
       </c>
       <c r="C142" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -2855,7 +2998,7 @@
         <v>45828</v>
       </c>
       <c r="C143" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -2866,7 +3009,7 @@
         <v>45829</v>
       </c>
       <c r="C144" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
@@ -2877,7 +3020,7 @@
         <v>45830</v>
       </c>
       <c r="C145" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -2888,13 +3031,13 @@
         <v>45831</v>
       </c>
       <c r="C146" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D146" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E146" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
@@ -2905,7 +3048,7 @@
         <v>45832</v>
       </c>
       <c r="C147" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -2916,10 +3059,10 @@
         <v>45833</v>
       </c>
       <c r="C148" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D148" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
@@ -2930,7 +3073,7 @@
         <v>45834</v>
       </c>
       <c r="C149" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
@@ -2941,7 +3084,7 @@
         <v>45835</v>
       </c>
       <c r="C150" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
@@ -2952,7 +3095,7 @@
         <v>45836</v>
       </c>
       <c r="C151" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
@@ -2963,7 +3106,7 @@
         <v>45837</v>
       </c>
       <c r="C152" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
@@ -2974,7 +3117,7 @@
         <v>45838</v>
       </c>
       <c r="C153" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
@@ -2985,7 +3128,7 @@
         <v>45839</v>
       </c>
       <c r="C154" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
@@ -2996,10 +3139,10 @@
         <v>45840</v>
       </c>
       <c r="C155" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F155" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
@@ -3010,7 +3153,7 @@
         <v>45841</v>
       </c>
       <c r="C156" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
@@ -3021,7 +3164,10 @@
         <v>45842</v>
       </c>
       <c r="C157" t="s">
-        <v>8</v>
+        <v>239</v>
+      </c>
+      <c r="F157" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
@@ -3032,7 +3178,13 @@
         <v>45843</v>
       </c>
       <c r="C158" t="s">
-        <v>8</v>
+        <v>251</v>
+      </c>
+      <c r="D158" t="s">
+        <v>252</v>
+      </c>
+      <c r="E158" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
@@ -3043,19 +3195,19 @@
         <v>45844</v>
       </c>
       <c r="C159" t="s">
-        <v>8</v>
+        <v>254</v>
       </c>
       <c r="E159" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F159" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G159" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H159" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
@@ -3066,10 +3218,10 @@
         <v>45845</v>
       </c>
       <c r="C160" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -3077,10 +3229,10 @@
         <v>45846</v>
       </c>
       <c r="C161" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -3088,10 +3240,10 @@
         <v>45847</v>
       </c>
       <c r="C162" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -3099,10 +3251,10 @@
         <v>45848</v>
       </c>
       <c r="C163" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -3110,10 +3262,10 @@
         <v>45849</v>
       </c>
       <c r="C164" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -3121,16 +3273,16 @@
         <v>45850</v>
       </c>
       <c r="C165" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D165" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E165" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -3138,10 +3290,10 @@
         <v>45851</v>
       </c>
       <c r="C166" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -3149,10 +3301,16 @@
         <v>45852</v>
       </c>
       <c r="C167" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+      <c r="D167" t="s">
+        <v>262</v>
+      </c>
+      <c r="E167" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -3160,10 +3318,10 @@
         <v>45853</v>
       </c>
       <c r="C168" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -3171,10 +3329,10 @@
         <v>45854</v>
       </c>
       <c r="C169" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -3182,10 +3340,10 @@
         <v>45855</v>
       </c>
       <c r="C170" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -3193,10 +3351,13 @@
         <v>45856</v>
       </c>
       <c r="C171" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+      <c r="F171" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -3204,10 +3365,10 @@
         <v>45857</v>
       </c>
       <c r="C172" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -3215,10 +3376,10 @@
         <v>45858</v>
       </c>
       <c r="C173" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -3226,10 +3387,16 @@
         <v>45859</v>
       </c>
       <c r="C174" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+      <c r="D174" t="s">
+        <v>273</v>
+      </c>
+      <c r="E174" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -3237,10 +3404,10 @@
         <v>45860</v>
       </c>
       <c r="C175" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -3248,10 +3415,10 @@
         <v>45861</v>
       </c>
       <c r="C176" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
@@ -3259,10 +3426,10 @@
         <v>45862</v>
       </c>
       <c r="C177" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
@@ -3270,10 +3437,10 @@
         <v>45863</v>
       </c>
       <c r="C178" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
@@ -3281,10 +3448,10 @@
         <v>45864</v>
       </c>
       <c r="C179" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -3292,10 +3459,16 @@
         <v>45865</v>
       </c>
       <c r="C180" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+      <c r="D180" t="s">
+        <v>283</v>
+      </c>
+      <c r="E180" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -3306,7 +3479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -3317,7 +3490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -3325,10 +3498,10 @@
         <v>45868</v>
       </c>
       <c r="C183" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -3339,7 +3512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
@@ -3347,10 +3520,10 @@
         <v>45870</v>
       </c>
       <c r="C185" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
@@ -3361,7 +3534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
@@ -3372,7 +3545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
@@ -3383,7 +3556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
@@ -3394,7 +3567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
@@ -3402,10 +3575,13 @@
         <v>45875</v>
       </c>
       <c r="C190" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="F190" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
@@ -3416,7 +3592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
@@ -3468,13 +3644,13 @@
         <v>45881</v>
       </c>
       <c r="C196" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D196" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E196" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
@@ -3562,7 +3738,13 @@
         <v>45889</v>
       </c>
       <c r="C204" t="s">
-        <v>8</v>
+        <v>275</v>
+      </c>
+      <c r="D204" t="s">
+        <v>276</v>
+      </c>
+      <c r="E204" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
@@ -3628,7 +3810,7 @@
         <v>45895</v>
       </c>
       <c r="C210" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
@@ -3661,7 +3843,7 @@
         <v>45898</v>
       </c>
       <c r="C213" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
@@ -3672,7 +3854,7 @@
         <v>45899</v>
       </c>
       <c r="C214" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
@@ -3694,7 +3876,7 @@
         <v>45901</v>
       </c>
       <c r="C216" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
@@ -3785,7 +3967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>224</v>
       </c>
@@ -3796,7 +3978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>225</v>
       </c>
@@ -3807,7 +3989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>226</v>
       </c>
@@ -3818,7 +4000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>227</v>
       </c>
@@ -3826,16 +4008,16 @@
         <v>45913</v>
       </c>
       <c r="C228" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D228" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E228" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>228</v>
       </c>
@@ -3846,7 +4028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>229</v>
       </c>
@@ -3857,7 +4039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>230</v>
       </c>
@@ -3868,7 +4050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>231</v>
       </c>
@@ -3879,7 +4061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>232</v>
       </c>
@@ -3890,7 +4072,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>233</v>
       </c>
@@ -3901,7 +4083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>234</v>
       </c>
@@ -3909,10 +4091,13 @@
         <v>45920</v>
       </c>
       <c r="C235" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+      <c r="F235" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>235</v>
       </c>
@@ -3923,7 +4108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>236</v>
       </c>
@@ -3934,7 +4119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>237</v>
       </c>
@@ -3945,7 +4130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>238</v>
       </c>
@@ -3956,7 +4141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>239</v>
       </c>
@@ -3967,7 +4152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>240</v>
       </c>
@@ -3975,10 +4160,10 @@
         <v>45926</v>
       </c>
       <c r="C241" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>241</v>
       </c>
@@ -3989,7 +4174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>242</v>
       </c>
@@ -4000,7 +4185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>243</v>
       </c>
@@ -4011,7 +4196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>244</v>
       </c>
@@ -4019,10 +4204,10 @@
         <v>45930</v>
       </c>
       <c r="C245" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>245</v>
       </c>
@@ -4030,10 +4215,10 @@
         <v>45931</v>
       </c>
       <c r="C246" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>246</v>
       </c>
@@ -4044,7 +4229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>247</v>
       </c>
@@ -4055,7 +4240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>248</v>
       </c>
@@ -4066,7 +4251,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>249</v>
       </c>
@@ -4077,7 +4262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>250</v>
       </c>
@@ -4088,7 +4273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>251</v>
       </c>
@@ -4099,7 +4284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>252</v>
       </c>
@@ -4110,7 +4295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>253</v>
       </c>
@@ -4118,10 +4303,13 @@
         <v>45939</v>
       </c>
       <c r="C254" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+      <c r="F254" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>254</v>
       </c>
@@ -4132,7 +4320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>255</v>
       </c>
@@ -4305,7 +4493,7 @@
         <v>45956</v>
       </c>
       <c r="C271" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
@@ -4349,7 +4537,7 @@
         <v>45960</v>
       </c>
       <c r="C275" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
@@ -4371,7 +4559,7 @@
         <v>45962</v>
       </c>
       <c r="C277" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
@@ -4495,7 +4683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>288</v>
       </c>
@@ -4506,7 +4694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>289</v>
       </c>
@@ -4517,7 +4705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>290</v>
       </c>
@@ -4528,7 +4716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>291</v>
       </c>
@@ -4539,7 +4727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>292</v>
       </c>
@@ -4550,7 +4738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>293</v>
       </c>
@@ -4558,10 +4746,13 @@
         <v>45979</v>
       </c>
       <c r="C294" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+      <c r="F294" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>294</v>
       </c>
@@ -4572,7 +4763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>295</v>
       </c>
@@ -4583,7 +4774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>296</v>
       </c>
@@ -4594,7 +4785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>297</v>
       </c>
@@ -4605,7 +4796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>298</v>
       </c>
@@ -4616,7 +4807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>299</v>
       </c>
@@ -4627,7 +4818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>300</v>
       </c>
@@ -4638,7 +4829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>301</v>
       </c>
@@ -4646,10 +4837,10 @@
         <v>45987</v>
       </c>
       <c r="C302" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>302</v>
       </c>
@@ -4660,7 +4851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>303</v>
       </c>
@@ -4690,7 +4881,7 @@
         <v>45991</v>
       </c>
       <c r="C306" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
@@ -4701,7 +4892,7 @@
         <v>45992</v>
       </c>
       <c r="C307" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
@@ -4976,7 +5167,7 @@
         <v>46017</v>
       </c>
       <c r="C332" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
@@ -5020,7 +5211,7 @@
         <v>46021</v>
       </c>
       <c r="C336" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
@@ -5042,7 +5233,7 @@
         <v>46023</v>
       </c>
       <c r="C338" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
@@ -5318,7 +5509,7 @@
         <v>46048</v>
       </c>
       <c r="C363" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.3">
@@ -5362,7 +5553,7 @@
         <v>46052</v>
       </c>
       <c r="C367" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.3">
@@ -5588,7 +5779,13 @@
       <c r="B441" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F190" r:id="rId1" xr:uid="{6D4FC811-6F80-41BA-BC76-E6909C6FBFED}"/>
+    <hyperlink ref="F235" r:id="rId2" xr:uid="{E998A04B-268C-4A7C-86EE-C9B5716C1BC9}"/>
+    <hyperlink ref="F254" r:id="rId3" xr:uid="{51FDD2BC-91D1-44BE-BA56-F7AD31A6FBFA}"/>
+    <hyperlink ref="F294" r:id="rId4" xr:uid="{C7FA78CD-BCFE-450E-A87C-940CB730F7A6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fotos de Bereal tots fets menys Lola
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE9BF5C-EE00-4615-8A91-22D7F571EA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DCB5B4-1287-4808-8B84-E806C9F6F1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="317">
   <si>
     <t>Dia</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Perquè els teus ulls brillen d'una manera especial</t>
   </si>
   <si>
-    <t>Perquè tens una màgia especial per lligar. Sempre recordarè quan vas dir la frase que em va enamorar: Jo si que tinc bones vistes...</t>
-  </si>
-  <si>
     <t>Perquè ets una noia experta en TOT</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>Perquè ets molt empàtica</t>
   </si>
   <si>
-    <t xml:space="preserve">Perquè ets la primera persona així d'especial que he tingut </t>
-  </si>
-  <si>
     <t>Perquè el teu riure és brutal</t>
   </si>
   <si>
@@ -880,6 +874,108 @@
   </si>
   <si>
     <t>Aquí està la netejadora MÉS GUAPA de cotxes ajudant al xòfer a que la LIMUSINA en la que va estigui neta</t>
+  </si>
+  <si>
+    <t>Perquè em deixis que fagi els MILLORS BEREALS</t>
+  </si>
+  <si>
+    <t>./img/bereal1.jpeg</t>
+  </si>
+  <si>
+    <t>Aquesta és LA PRIMERA FOTO QUE TENIM JUNTS. Ens vam amagar una mica perquè erem tímids encara</t>
+  </si>
+  <si>
+    <t>Perquè em deixes penjar els MILLORS BERALS amb tu</t>
+  </si>
+  <si>
+    <t>./img/bereal2.jpeg</t>
+  </si>
+  <si>
+    <t>./img/bereal3.jpeg</t>
+  </si>
+  <si>
+    <t>./img/bereal4.jpeg</t>
+  </si>
+  <si>
+    <t>Aquest Bereal és de tancada amb la NAVARROSSA (aquell dia la Bufona va triunfar)</t>
+  </si>
+  <si>
+    <t>Perquè em deixes penjar els MILLORS BEREALS amb tuu</t>
+  </si>
+  <si>
+    <t>Vaig penjar aquest Bereal un dia que ens vam trobar amb tots, va ser una mica raro però estaves GUAPISSIMA!</t>
+  </si>
+  <si>
+    <t>Perquè em deixes penar els MILLORS BEREALS amb tu</t>
+  </si>
+  <si>
+    <t>En aquest Bereal estàvem menjant un BONÍSSIM plat de pasta (amb quesitooos)</t>
+  </si>
+  <si>
+    <t>Perquè tens una màgia especial per lligar. Sempre recordarè quan vas dir la frase que em va enamorar: Jo si que tinc bones vistes…</t>
+  </si>
+  <si>
+    <t>./img/bereal5.jpeg</t>
+  </si>
+  <si>
+    <t>En aquest Bereal TORNEM A MENJAR PASTA. Aquest cop, però, amb el teu DELICIÓS Mc and Cheese (encara que alguns cops digui que no està tant bo)</t>
+  </si>
+  <si>
+    <t>Perquè ets la primera persona així d'especial que he conegut</t>
+  </si>
+  <si>
+    <t>Perqupe em deixes penajr els MILLORS BEREALS amb tuu</t>
+  </si>
+  <si>
+    <t>./img/bereal6.jpeg</t>
+  </si>
+  <si>
+    <t>En aquest Bereal ja començes amb la teva mania de tapar-te la cara, t'ho perdono perquè estàvem veient SUPER MARIO</t>
+  </si>
+  <si>
+    <t>./img/bereal7.jpeg</t>
+  </si>
+  <si>
+    <t>En aquest Bereal surts ajudant me a netejar la limusina. No està malament perquè d'alguna manera s'ha de pagar el taxi.</t>
+  </si>
+  <si>
+    <t>./img/bereal8.jpeg</t>
+  </si>
+  <si>
+    <t>Un Beral molt xulo de quan vam anar a Manlleu, vem veure VACAAAS!</t>
+  </si>
+  <si>
+    <t>./img/bereal9.jpeg</t>
+  </si>
+  <si>
+    <t>En aquest BeReal veiem com em deixes sense res de menjar per poder cruspir-te tu TOTA la pizza</t>
+  </si>
+  <si>
+    <t>./img/bereal10.jpeg</t>
+  </si>
+  <si>
+    <t>Un Beral de quan vam anar a veure BARBIE junts</t>
+  </si>
+  <si>
+    <t>./img/bereal11.jpeg</t>
+  </si>
+  <si>
+    <t>En aquesta Beral surts fent la teva activitat preferida</t>
+  </si>
+  <si>
+    <t>Perquè em deixies penjar ELS MILLORS BERALS amb tuu</t>
+  </si>
+  <si>
+    <t>./img/bereal12.jpeg</t>
+  </si>
+  <si>
+    <t>Un beral amb les TREMENDAS mascarillas que vam fer després de Caldea a Andorra</t>
+  </si>
+  <si>
+    <t>./img/bereal13.jpeg</t>
+  </si>
+  <si>
+    <t>En aquest Beral podem veure com, CLARISSIMAMENT, sóc moolt millor que tú a bolos (i no només a la Wii)</t>
   </si>
 </sst>
 </file>
@@ -1260,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="81" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183"/>
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D277" sqref="D277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1301,7 +1397,7 @@
         <v>45687</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -1310,7 +1406,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1321,7 +1417,7 @@
         <v>45688</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -1335,7 +1431,7 @@
         <v>45689</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1358,7 +1454,7 @@
         <v>45691</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1369,7 +1465,7 @@
         <v>45692</v>
       </c>
       <c r="C7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1380,7 +1476,7 @@
         <v>45693</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1476,7 +1572,7 @@
         <v>45700</v>
       </c>
       <c r="C15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1499,13 +1595,13 @@
         <v>45702</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1579,7 +1675,13 @@
         <v>45708</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>286</v>
+      </c>
+      <c r="D23" t="s">
+        <v>287</v>
+      </c>
+      <c r="E23" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1590,7 +1692,7 @@
         <v>45709</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1648,7 +1750,7 @@
         <v>45714</v>
       </c>
       <c r="C29" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1681,7 +1783,7 @@
         <v>45717</v>
       </c>
       <c r="C32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1692,7 +1794,13 @@
         <v>45718</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>291</v>
+      </c>
+      <c r="D33" t="s">
+        <v>288</v>
+      </c>
+      <c r="E33" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1703,7 +1811,7 @@
         <v>45719</v>
       </c>
       <c r="C34" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1725,13 +1833,13 @@
         <v>45721</v>
       </c>
       <c r="C36" t="s">
+        <v>180</v>
+      </c>
+      <c r="D36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" t="s">
         <v>182</v>
-      </c>
-      <c r="D36" t="s">
-        <v>183</v>
-      </c>
-      <c r="E36" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1775,7 +1883,13 @@
         <v>45725</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>293</v>
+      </c>
+      <c r="D40" t="s">
+        <v>289</v>
+      </c>
+      <c r="E40" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1811,10 +1925,10 @@
         <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E43" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1836,7 +1950,7 @@
         <v>45730</v>
       </c>
       <c r="C45" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F45" t="s">
         <v>62</v>
@@ -1872,7 +1986,13 @@
         <v>45733</v>
       </c>
       <c r="C48" t="s">
-        <v>65</v>
+        <v>291</v>
+      </c>
+      <c r="D48" t="s">
+        <v>296</v>
+      </c>
+      <c r="E48" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1883,7 +2003,7 @@
         <v>45734</v>
       </c>
       <c r="C49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1894,7 +2014,7 @@
         <v>45735</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1905,7 +2025,7 @@
         <v>45736</v>
       </c>
       <c r="C51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1916,7 +2036,7 @@
         <v>45737</v>
       </c>
       <c r="C52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1927,7 +2047,7 @@
         <v>45738</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1938,7 +2058,13 @@
         <v>45739</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>299</v>
+      </c>
+      <c r="D54" t="s">
+        <v>300</v>
+      </c>
+      <c r="E54" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1949,7 +2075,7 @@
         <v>45740</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1960,7 +2086,7 @@
         <v>45741</v>
       </c>
       <c r="C56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1982,13 +2108,13 @@
         <v>45743</v>
       </c>
       <c r="C58" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" t="s">
         <v>74</v>
-      </c>
-      <c r="D58" t="s">
-        <v>75</v>
-      </c>
-      <c r="E58" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1999,10 +2125,10 @@
         <v>45744</v>
       </c>
       <c r="C59" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F59" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2013,7 +2139,7 @@
         <v>45745</v>
       </c>
       <c r="C60" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2024,7 +2150,7 @@
         <v>45746</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2035,7 +2161,7 @@
         <v>45747</v>
       </c>
       <c r="C62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2046,7 +2172,7 @@
         <v>45748</v>
       </c>
       <c r="C63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2057,7 +2183,7 @@
         <v>45749</v>
       </c>
       <c r="C64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2068,10 +2194,10 @@
         <v>45750</v>
       </c>
       <c r="C65" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2082,7 +2208,7 @@
         <v>45751</v>
       </c>
       <c r="C66" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2093,7 +2219,7 @@
         <v>45752</v>
       </c>
       <c r="C67" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2104,7 +2230,13 @@
         <v>45753</v>
       </c>
       <c r="C68" t="s">
-        <v>93</v>
+        <v>291</v>
+      </c>
+      <c r="D68" t="s">
+        <v>302</v>
+      </c>
+      <c r="E68" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2115,7 +2247,7 @@
         <v>45754</v>
       </c>
       <c r="C69" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2126,7 +2258,7 @@
         <v>45755</v>
       </c>
       <c r="C70" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2137,13 +2269,13 @@
         <v>45756</v>
       </c>
       <c r="C71" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D71" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E71" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2154,7 +2286,7 @@
         <v>45757</v>
       </c>
       <c r="C72" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2165,7 +2297,7 @@
         <v>45758</v>
       </c>
       <c r="C73" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2176,7 +2308,7 @@
         <v>45759</v>
       </c>
       <c r="C74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2187,7 +2319,7 @@
         <v>45760</v>
       </c>
       <c r="C75" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2198,7 +2330,7 @@
         <v>45761</v>
       </c>
       <c r="C76" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2209,7 +2341,13 @@
         <v>45762</v>
       </c>
       <c r="C77" t="s">
-        <v>102</v>
+        <v>291</v>
+      </c>
+      <c r="D77" t="s">
+        <v>304</v>
+      </c>
+      <c r="E77" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2220,7 +2358,7 @@
         <v>45763</v>
       </c>
       <c r="C78" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2231,7 +2369,7 @@
         <v>45764</v>
       </c>
       <c r="C79" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2242,10 +2380,10 @@
         <v>45765</v>
       </c>
       <c r="C80" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F80" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2256,7 +2394,7 @@
         <v>45766</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2267,7 +2405,7 @@
         <v>45767</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2278,13 +2416,13 @@
         <v>45768</v>
       </c>
       <c r="C83" t="s">
+        <v>105</v>
+      </c>
+      <c r="D83" t="s">
         <v>107</v>
       </c>
-      <c r="D83" t="s">
-        <v>109</v>
-      </c>
       <c r="E83" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2295,7 +2433,7 @@
         <v>45769</v>
       </c>
       <c r="C84" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2306,13 +2444,13 @@
         <v>45770</v>
       </c>
       <c r="C85" t="s">
+        <v>110</v>
+      </c>
+      <c r="D85" t="s">
+        <v>111</v>
+      </c>
+      <c r="E85" t="s">
         <v>112</v>
-      </c>
-      <c r="D85" t="s">
-        <v>113</v>
-      </c>
-      <c r="E85" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2323,7 +2461,7 @@
         <v>45771</v>
       </c>
       <c r="C86" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2334,7 +2472,7 @@
         <v>45772</v>
       </c>
       <c r="C87" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2356,7 +2494,7 @@
         <v>45774</v>
       </c>
       <c r="C89" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2367,7 +2505,7 @@
         <v>45775</v>
       </c>
       <c r="C90" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2378,7 +2516,7 @@
         <v>45776</v>
       </c>
       <c r="C91" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2389,7 +2527,7 @@
         <v>45777</v>
       </c>
       <c r="C92" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2400,7 +2538,7 @@
         <v>45778</v>
       </c>
       <c r="C93" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2411,10 +2549,10 @@
         <v>45779</v>
       </c>
       <c r="C94" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F94" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2442,7 +2580,7 @@
         <v>45781</v>
       </c>
       <c r="C96" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2453,7 +2591,7 @@
         <v>45782</v>
       </c>
       <c r="C97" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2464,10 +2602,10 @@
         <v>45783</v>
       </c>
       <c r="C98" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D98" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2478,7 +2616,7 @@
         <v>45784</v>
       </c>
       <c r="C99" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2489,7 +2627,7 @@
         <v>45785</v>
       </c>
       <c r="C100" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2500,7 +2638,7 @@
         <v>45786</v>
       </c>
       <c r="C101" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2511,7 +2649,7 @@
         <v>45787</v>
       </c>
       <c r="C102" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2522,7 +2660,13 @@
         <v>45788</v>
       </c>
       <c r="C103" t="s">
-        <v>164</v>
+        <v>291</v>
+      </c>
+      <c r="D103" t="s">
+        <v>308</v>
+      </c>
+      <c r="E103" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2533,7 +2677,7 @@
         <v>45789</v>
       </c>
       <c r="C104" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2544,7 +2688,7 @@
         <v>45790</v>
       </c>
       <c r="C105" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2555,7 +2699,7 @@
         <v>45791</v>
       </c>
       <c r="C106" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2566,10 +2710,10 @@
         <v>45792</v>
       </c>
       <c r="C107" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D107" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2580,7 +2724,7 @@
         <v>45793</v>
       </c>
       <c r="C108" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2591,7 +2735,7 @@
         <v>45794</v>
       </c>
       <c r="C109" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2602,7 +2746,7 @@
         <v>45795</v>
       </c>
       <c r="C110" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2613,10 +2757,10 @@
         <v>45796</v>
       </c>
       <c r="C111" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F111" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -2627,7 +2771,7 @@
         <v>45797</v>
       </c>
       <c r="C112" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -2638,10 +2782,10 @@
         <v>45798</v>
       </c>
       <c r="C113" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D113" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -2652,7 +2796,7 @@
         <v>45799</v>
       </c>
       <c r="C114" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -2663,7 +2807,7 @@
         <v>45800</v>
       </c>
       <c r="C115" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -2674,7 +2818,7 @@
         <v>45801</v>
       </c>
       <c r="C116" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -2685,7 +2829,7 @@
         <v>45802</v>
       </c>
       <c r="C117" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -2707,7 +2851,7 @@
         <v>45804</v>
       </c>
       <c r="C119" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -2718,7 +2862,13 @@
         <v>45805</v>
       </c>
       <c r="C120" t="s">
-        <v>178</v>
+        <v>283</v>
+      </c>
+      <c r="D120" t="s">
+        <v>284</v>
+      </c>
+      <c r="E120" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -2729,7 +2879,7 @@
         <v>45806</v>
       </c>
       <c r="C121" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -2740,7 +2890,7 @@
         <v>45807</v>
       </c>
       <c r="C122" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -2751,10 +2901,10 @@
         <v>45808</v>
       </c>
       <c r="C123" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F123" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -2765,7 +2915,7 @@
         <v>45809</v>
       </c>
       <c r="C124" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -2776,7 +2926,7 @@
         <v>45810</v>
       </c>
       <c r="C125" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -2787,7 +2937,7 @@
         <v>45811</v>
       </c>
       <c r="C126" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -2809,13 +2959,13 @@
         <v>45813</v>
       </c>
       <c r="C128" t="s">
+        <v>185</v>
+      </c>
+      <c r="D128" t="s">
+        <v>186</v>
+      </c>
+      <c r="E128" t="s">
         <v>187</v>
-      </c>
-      <c r="D128" t="s">
-        <v>188</v>
-      </c>
-      <c r="E128" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2826,7 +2976,7 @@
         <v>45814</v>
       </c>
       <c r="C129" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2837,13 +2987,13 @@
         <v>45815</v>
       </c>
       <c r="C130" t="s">
+        <v>189</v>
+      </c>
+      <c r="D130" t="s">
+        <v>190</v>
+      </c>
+      <c r="E130" t="s">
         <v>191</v>
-      </c>
-      <c r="D130" t="s">
-        <v>192</v>
-      </c>
-      <c r="E130" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2854,7 +3004,7 @@
         <v>45816</v>
       </c>
       <c r="C131" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -2865,7 +3015,7 @@
         <v>45817</v>
       </c>
       <c r="C132" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -2876,7 +3026,7 @@
         <v>45818</v>
       </c>
       <c r="C133" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -2887,7 +3037,7 @@
         <v>45819</v>
       </c>
       <c r="C134" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -2898,7 +3048,7 @@
         <v>45820</v>
       </c>
       <c r="C135" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -2909,7 +3059,7 @@
         <v>45821</v>
       </c>
       <c r="C136" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -2920,13 +3070,13 @@
         <v>45822</v>
       </c>
       <c r="C137" t="s">
+        <v>213</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E137" t="s">
         <v>215</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E137" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -2937,13 +3087,13 @@
         <v>45823</v>
       </c>
       <c r="C138" t="s">
+        <v>192</v>
+      </c>
+      <c r="D138" t="s">
+        <v>193</v>
+      </c>
+      <c r="E138" t="s">
         <v>194</v>
-      </c>
-      <c r="D138" t="s">
-        <v>195</v>
-      </c>
-      <c r="E138" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -2954,7 +3104,7 @@
         <v>45824</v>
       </c>
       <c r="C139" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -2965,7 +3115,7 @@
         <v>45825</v>
       </c>
       <c r="C140" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -2976,7 +3126,7 @@
         <v>45826</v>
       </c>
       <c r="C141" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -2987,7 +3137,7 @@
         <v>45827</v>
       </c>
       <c r="C142" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -2998,7 +3148,7 @@
         <v>45828</v>
       </c>
       <c r="C143" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -3009,7 +3159,7 @@
         <v>45829</v>
       </c>
       <c r="C144" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
@@ -3020,7 +3170,7 @@
         <v>45830</v>
       </c>
       <c r="C145" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -3031,13 +3181,13 @@
         <v>45831</v>
       </c>
       <c r="C146" t="s">
+        <v>223</v>
+      </c>
+      <c r="D146" t="s">
+        <v>224</v>
+      </c>
+      <c r="E146" t="s">
         <v>225</v>
-      </c>
-      <c r="D146" t="s">
-        <v>226</v>
-      </c>
-      <c r="E146" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
@@ -3048,7 +3198,7 @@
         <v>45832</v>
       </c>
       <c r="C147" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -3059,10 +3209,10 @@
         <v>45833</v>
       </c>
       <c r="C148" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D148" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
@@ -3084,7 +3234,7 @@
         <v>45835</v>
       </c>
       <c r="C150" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
@@ -3095,7 +3245,7 @@
         <v>45836</v>
       </c>
       <c r="C151" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
@@ -3106,7 +3256,7 @@
         <v>45837</v>
       </c>
       <c r="C152" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
@@ -3117,7 +3267,7 @@
         <v>45838</v>
       </c>
       <c r="C153" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
@@ -3128,7 +3278,7 @@
         <v>45839</v>
       </c>
       <c r="C154" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
@@ -3139,10 +3289,10 @@
         <v>45840</v>
       </c>
       <c r="C155" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F155" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
@@ -3153,7 +3303,7 @@
         <v>45841</v>
       </c>
       <c r="C156" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
@@ -3164,10 +3314,10 @@
         <v>45842</v>
       </c>
       <c r="C157" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F157" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
@@ -3178,13 +3328,13 @@
         <v>45843</v>
       </c>
       <c r="C158" t="s">
+        <v>249</v>
+      </c>
+      <c r="D158" t="s">
+        <v>250</v>
+      </c>
+      <c r="E158" t="s">
         <v>251</v>
-      </c>
-      <c r="D158" t="s">
-        <v>252</v>
-      </c>
-      <c r="E158" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
@@ -3195,19 +3345,19 @@
         <v>45844</v>
       </c>
       <c r="C159" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E159" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F159" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G159" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H159" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
@@ -3218,7 +3368,7 @@
         <v>45845</v>
       </c>
       <c r="C160" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -3229,7 +3379,7 @@
         <v>45846</v>
       </c>
       <c r="C161" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,7 +3390,7 @@
         <v>45847</v>
       </c>
       <c r="C162" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -3251,7 +3401,7 @@
         <v>45848</v>
       </c>
       <c r="C163" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
@@ -3262,7 +3412,7 @@
         <v>45849</v>
       </c>
       <c r="C164" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
@@ -3273,13 +3423,13 @@
         <v>45850</v>
       </c>
       <c r="C165" t="s">
+        <v>195</v>
+      </c>
+      <c r="D165" t="s">
+        <v>196</v>
+      </c>
+      <c r="E165" t="s">
         <v>197</v>
-      </c>
-      <c r="D165" t="s">
-        <v>198</v>
-      </c>
-      <c r="E165" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
@@ -3290,7 +3440,7 @@
         <v>45851</v>
       </c>
       <c r="C166" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
@@ -3301,13 +3451,13 @@
         <v>45852</v>
       </c>
       <c r="C167" t="s">
+        <v>259</v>
+      </c>
+      <c r="D167" t="s">
+        <v>260</v>
+      </c>
+      <c r="E167" t="s">
         <v>261</v>
-      </c>
-      <c r="D167" t="s">
-        <v>262</v>
-      </c>
-      <c r="E167" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
@@ -3318,7 +3468,7 @@
         <v>45853</v>
       </c>
       <c r="C168" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
@@ -3329,7 +3479,7 @@
         <v>45854</v>
       </c>
       <c r="C169" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
@@ -3340,7 +3490,7 @@
         <v>45855</v>
       </c>
       <c r="C170" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
@@ -3351,10 +3501,10 @@
         <v>45856</v>
       </c>
       <c r="C171" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F171" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
@@ -3365,7 +3515,7 @@
         <v>45857</v>
       </c>
       <c r="C172" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
@@ -3376,7 +3526,7 @@
         <v>45858</v>
       </c>
       <c r="C173" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
@@ -3387,13 +3537,13 @@
         <v>45859</v>
       </c>
       <c r="C174" t="s">
+        <v>270</v>
+      </c>
+      <c r="D174" t="s">
+        <v>271</v>
+      </c>
+      <c r="E174" t="s">
         <v>272</v>
-      </c>
-      <c r="D174" t="s">
-        <v>273</v>
-      </c>
-      <c r="E174" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
@@ -3404,7 +3554,7 @@
         <v>45860</v>
       </c>
       <c r="C175" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
@@ -3415,7 +3565,7 @@
         <v>45861</v>
       </c>
       <c r="C176" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
@@ -3426,7 +3576,7 @@
         <v>45862</v>
       </c>
       <c r="C177" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
@@ -3437,7 +3587,7 @@
         <v>45863</v>
       </c>
       <c r="C178" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
@@ -3459,13 +3609,13 @@
         <v>45865</v>
       </c>
       <c r="C180" t="s">
+        <v>280</v>
+      </c>
+      <c r="D180" t="s">
+        <v>281</v>
+      </c>
+      <c r="E180" t="s">
         <v>282</v>
-      </c>
-      <c r="D180" t="s">
-        <v>283</v>
-      </c>
-      <c r="E180" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
@@ -3476,7 +3626,7 @@
         <v>45866</v>
       </c>
       <c r="C181" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
@@ -3487,7 +3637,7 @@
         <v>45867</v>
       </c>
       <c r="C182" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
@@ -3498,7 +3648,7 @@
         <v>45868</v>
       </c>
       <c r="C183" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
@@ -3509,7 +3659,7 @@
         <v>45869</v>
       </c>
       <c r="C184" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
@@ -3520,7 +3670,7 @@
         <v>45870</v>
       </c>
       <c r="C185" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
@@ -3531,7 +3681,13 @@
         <v>45871</v>
       </c>
       <c r="C186" t="s">
-        <v>8</v>
+        <v>291</v>
+      </c>
+      <c r="D186" t="s">
+        <v>306</v>
+      </c>
+      <c r="E186" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
@@ -3542,7 +3698,7 @@
         <v>45872</v>
       </c>
       <c r="C187" t="s">
-        <v>8</v>
+        <v>295</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
@@ -3553,7 +3709,7 @@
         <v>45873</v>
       </c>
       <c r="C188" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
@@ -3564,7 +3720,7 @@
         <v>45874</v>
       </c>
       <c r="C189" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
@@ -3575,10 +3731,10 @@
         <v>45875</v>
       </c>
       <c r="C190" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
@@ -3589,7 +3745,7 @@
         <v>45876</v>
       </c>
       <c r="C191" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
@@ -3600,7 +3756,7 @@
         <v>45877</v>
       </c>
       <c r="C192" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
@@ -3611,7 +3767,7 @@
         <v>45878</v>
       </c>
       <c r="C193" t="s">
-        <v>8</v>
+        <v>162</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
@@ -3622,7 +3778,13 @@
         <v>45879</v>
       </c>
       <c r="C194" t="s">
-        <v>8</v>
+        <v>286</v>
+      </c>
+      <c r="D194" t="s">
+        <v>310</v>
+      </c>
+      <c r="E194" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
@@ -3644,13 +3806,13 @@
         <v>45881</v>
       </c>
       <c r="C196" t="s">
+        <v>198</v>
+      </c>
+      <c r="D196" t="s">
+        <v>199</v>
+      </c>
+      <c r="E196" t="s">
         <v>200</v>
-      </c>
-      <c r="D196" t="s">
-        <v>201</v>
-      </c>
-      <c r="E196" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
@@ -3738,13 +3900,13 @@
         <v>45889</v>
       </c>
       <c r="C204" t="s">
+        <v>273</v>
+      </c>
+      <c r="D204" t="s">
+        <v>274</v>
+      </c>
+      <c r="E204" t="s">
         <v>275</v>
-      </c>
-      <c r="D204" t="s">
-        <v>276</v>
-      </c>
-      <c r="E204" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
@@ -3791,7 +3953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
@@ -3802,7 +3964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
@@ -3813,7 +3975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
@@ -3824,7 +3986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
@@ -3835,7 +3997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
@@ -3843,10 +4005,10 @@
         <v>45898</v>
       </c>
       <c r="C213" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
@@ -3854,10 +4016,10 @@
         <v>45899</v>
       </c>
       <c r="C214" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
@@ -3868,7 +4030,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
@@ -3876,10 +4038,10 @@
         <v>45901</v>
       </c>
       <c r="C216" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
@@ -3890,7 +4052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
@@ -3901,7 +4063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
@@ -3912,7 +4074,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
@@ -3923,7 +4085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
@@ -3934,7 +4096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
@@ -3942,10 +4104,10 @@
         <v>45907</v>
       </c>
       <c r="C222" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
@@ -3955,8 +4117,14 @@
       <c r="C223" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D223" t="s">
+        <v>313</v>
+      </c>
+      <c r="E223" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
@@ -4008,13 +4176,13 @@
         <v>45913</v>
       </c>
       <c r="C228" t="s">
+        <v>201</v>
+      </c>
+      <c r="D228" t="s">
+        <v>202</v>
+      </c>
+      <c r="E228" t="s">
         <v>203</v>
-      </c>
-      <c r="D228" t="s">
-        <v>204</v>
-      </c>
-      <c r="E228" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
@@ -4091,10 +4259,10 @@
         <v>45920</v>
       </c>
       <c r="C235" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.3">
@@ -4204,7 +4372,7 @@
         <v>45930</v>
       </c>
       <c r="C245" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.3">
@@ -4215,7 +4383,7 @@
         <v>45931</v>
       </c>
       <c r="C246" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.3">
@@ -4259,7 +4427,13 @@
         <v>45935</v>
       </c>
       <c r="C250" t="s">
-        <v>8</v>
+        <v>286</v>
+      </c>
+      <c r="D250" t="s">
+        <v>315</v>
+      </c>
+      <c r="E250" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.3">
@@ -4303,10 +4477,10 @@
         <v>45939</v>
       </c>
       <c r="C254" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F254" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
@@ -4537,7 +4711,7 @@
         <v>45960</v>
       </c>
       <c r="C275" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
@@ -4559,7 +4733,7 @@
         <v>45962</v>
       </c>
       <c r="C277" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
@@ -4746,10 +4920,10 @@
         <v>45979</v>
       </c>
       <c r="C294" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F294" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.3">
@@ -4881,7 +5055,7 @@
         <v>45991</v>
       </c>
       <c r="C306" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
@@ -4892,7 +5066,7 @@
         <v>45992</v>
       </c>
       <c r="C307" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
@@ -5211,7 +5385,7 @@
         <v>46021</v>
       </c>
       <c r="C336" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
@@ -5233,7 +5407,7 @@
         <v>46023</v>
       </c>
       <c r="C338" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
@@ -5553,7 +5727,7 @@
         <v>46052</v>
       </c>
       <c r="C367" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Nous videos, fotos i dies
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACD7D7F-7AF1-4A74-A52D-5A32F18FB1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ACAB37-DDAF-41D0-880A-51AEE68C75DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="363">
   <si>
     <t>Dia</t>
   </si>
@@ -1081,6 +1081,39 @@
   </si>
   <si>
     <t>./video/que_passa_aqui.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè ens estimem encara que fagi fred. Això ho pots veure en el vídeo </t>
+  </si>
+  <si>
+    <t>./video/peto_andorra.mp4</t>
+  </si>
+  <si>
+    <t>Perquè em graves fent cara de ratilla quan dormo, I TINC PROVES</t>
+  </si>
+  <si>
+    <t>./video/altre_dormint.mp4</t>
+  </si>
+  <si>
+    <t>Perquè ens ho passem molt bé fent trucades junts</t>
+  </si>
+  <si>
+    <t>Perquè encara que costi, sempre trobem algun moment per veure'ns</t>
+  </si>
+  <si>
+    <t>Perquè tot i que no tinguis el carnet (POTSER JA SI AIXÒ ESTÀ ESCRIT EL 18/02/2025) ets la millor copi del mon</t>
+  </si>
+  <si>
+    <t>Perquè dius que dormo amb els ulls oberts I NO ES VERITAT</t>
+  </si>
+  <si>
+    <t>./img/ulls_oberts.jpg</t>
+  </si>
+  <si>
+    <t>Bueno potser sí que tens raò (COM SEMPRE)</t>
+  </si>
+  <si>
+    <t>Perquè de tant en tant em deixes fer coses tot i que normalment vaig AMB LA CORREA!</t>
   </si>
 </sst>
 </file>
@@ -1461,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D68" zoomScale="80" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D220" sqref="D220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4062,7 +4095,10 @@
         <v>45892</v>
       </c>
       <c r="C207" t="s">
-        <v>8</v>
+        <v>354</v>
+      </c>
+      <c r="F207" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
@@ -4073,7 +4109,7 @@
         <v>45893</v>
       </c>
       <c r="C208" t="s">
-        <v>8</v>
+        <v>356</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
@@ -4084,7 +4120,7 @@
         <v>45894</v>
       </c>
       <c r="C209" t="s">
-        <v>8</v>
+        <v>357</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
@@ -4106,7 +4142,7 @@
         <v>45896</v>
       </c>
       <c r="C211" t="s">
-        <v>8</v>
+        <v>358</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
@@ -4117,7 +4153,13 @@
         <v>45897</v>
       </c>
       <c r="C212" t="s">
-        <v>8</v>
+        <v>359</v>
+      </c>
+      <c r="D212" t="s">
+        <v>360</v>
+      </c>
+      <c r="E212" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
@@ -4150,7 +4192,7 @@
         <v>45900</v>
       </c>
       <c r="C215" t="s">
-        <v>8</v>
+        <v>362</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
@@ -5124,7 +5166,10 @@
         <v>45985</v>
       </c>
       <c r="C300" t="s">
-        <v>8</v>
+        <v>352</v>
+      </c>
+      <c r="F300" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Noves fotos, vídeos, i dies
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ACAB37-DDAF-41D0-880A-51AEE68C75DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B4F800-50C2-45AD-966A-A8F93FCCE9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="413">
   <si>
     <t>Dia</t>
   </si>
@@ -474,12 +474,6 @@
     <t>Perquè fem viatges MOOOOLT guais (ANDORRAAA)</t>
   </si>
   <si>
-    <t>Perquè ets perfecte</t>
-  </si>
-  <si>
-    <t>Perquè juges als meus jocs de mòbil</t>
-  </si>
-  <si>
     <t>Perquè m'escoltes</t>
   </si>
   <si>
@@ -951,9 +945,6 @@
     <t>En aquesta Beral surts fent la teva activitat preferida</t>
   </si>
   <si>
-    <t>Perquè em deixies penjar ELS MILLORS BERALS amb tuu</t>
-  </si>
-  <si>
     <t>./img/bereal12.jpeg</t>
   </si>
   <si>
@@ -963,9 +954,6 @@
     <t>./img/bereal13.jpeg</t>
   </si>
   <si>
-    <t>En aquest Beral podem veure com, CLARISSIMAMENT, sóc moolt millor que tú a bolos (i no només a la Wii)</t>
-  </si>
-  <si>
     <t>Perquè quan rius jo també ric. PERCERT avui tinc metge visita i una radiografia (QUINA POR) per si em vols desitjar mooolta sort</t>
   </si>
   <si>
@@ -1114,6 +1102,168 @@
   </si>
   <si>
     <t>Perquè de tant en tant em deixes fer coses tot i que normalment vaig AMB LA CORREA!</t>
+  </si>
+  <si>
+    <t>Perquè fas regals HÍPER MEGA XULOS de manualitats (jo no en se fer PEROOO… mira quina web TAANT xula)</t>
+  </si>
+  <si>
+    <t>Perquè fas veure que T'ENCANTEN els meus regals (encara que no et mires MAI la web :( )</t>
+  </si>
+  <si>
+    <t>Perquè em graves MOOOLT mentre dormo (sí, un altre cop). En el vídeo pots veure un exemple</t>
+  </si>
+  <si>
+    <t>./video/dormint_2.mp4</t>
+  </si>
+  <si>
+    <t>Perquè jugues als meus jocs de mòbil</t>
+  </si>
+  <si>
+    <t>Perquè m'estimes encara que tingui MOOOLTA tos (o potser és perquè estàs amb la puça!). En tot cas, m'aguantes tot i tenir tos. Ho pots comprovar en el vídeo.</t>
+  </si>
+  <si>
+    <t>./video/pusa_i_tos.mp4</t>
+  </si>
+  <si>
+    <t>Perquè ets perfecte… O CASI tothom sap que només hi ha una persona perfecte en el món I SOC JO (el Marçal :) )</t>
+  </si>
+  <si>
+    <t>./img/no_be4.jpeg</t>
+  </si>
+  <si>
+    <t>En aquesta foto surts GUAPISSIMA mentres bevem un bubble tea a Sabadell.</t>
+  </si>
+  <si>
+    <t>Perquè encara que tu diguis que no surts PERFECTE a totes les fotos (part 6)</t>
+  </si>
+  <si>
+    <t>./img/no_be6.jpeg</t>
+  </si>
+  <si>
+    <t>En aquesta foto surts GUAPISSIMA quan estàvem mirant Chicago. Vam comprar una cosa per veure BASTANT rara!</t>
+  </si>
+  <si>
+    <t>Perquè encara que tu diguis que no surts PERFECTE a totes les fotos (part 5)</t>
+  </si>
+  <si>
+    <t>./img/no_be5.jpeg</t>
+  </si>
+  <si>
+    <t>Foto en la que surts GUAPISSIMA menjant al five guuuys</t>
+  </si>
+  <si>
+    <t>Perquè som LA PARELLA MÉS GUAPA DEL TEATRE.</t>
+  </si>
+  <si>
+    <t>./img/carnestoltes.jpeg</t>
+  </si>
+  <si>
+    <t>Perquè tenim cites junts MEGA GUAIS</t>
+  </si>
+  <si>
+    <t>./img/cita_friki.jpeg</t>
+  </si>
+  <si>
+    <t>Aquest és un CLARISSIM exemple, tú dius que va ser un lloc una mica friki, però ens ho vam passar molt bé!</t>
+  </si>
+  <si>
+    <t>Perquè m'estimes encara que dius que semblo UNA RATILLA</t>
+  </si>
+  <si>
+    <t>./img/jo_ratilla.jpeg</t>
+  </si>
+  <si>
+    <t>Sempre dius que faig cara molt de rata en aquesta foto PERÒ TOHOM SAP QUE TÚ ETS MÉS RATILLA QUE JO! (T'estimo!)</t>
+  </si>
+  <si>
+    <t>Perquè fem plans TAAANT xulos</t>
+  </si>
+  <si>
+    <t>./img/chicago.jpeg</t>
+  </si>
+  <si>
+    <t>Una foto de quan vam anar a veure CHICAGO al Tívoli, el Genís feia de tècnic!</t>
+  </si>
+  <si>
+    <t>Perquè em deixes penjar els MILLORS BEREALS amb tu</t>
+  </si>
+  <si>
+    <t>En aquest Bereal podem veure com, CLARISSIMAMENT, sóc moolt millor que tú a bolos (i no només a la Wii)</t>
+  </si>
+  <si>
+    <t>Perquè tens la expressió més maca del món mundial</t>
+  </si>
+  <si>
+    <t>./img/llengua.jpeg</t>
+  </si>
+  <si>
+    <t>Aquí tenim a la persona més guapa del món traient la llengua</t>
+  </si>
+  <si>
+    <t>Perquè em poses vermell quan amb mires</t>
+  </si>
+  <si>
+    <t>Perquè em deixes ser molt pesat amb tú</t>
+  </si>
+  <si>
+    <t>Perquè em deixes penjar ELS MILLORS BERALS amb tuu</t>
+  </si>
+  <si>
+    <t>Perquè deixes que t'acompanyi A TOOT ARREU amb cotxe. (Potser és perquè sóc el teu xòfer!)</t>
+  </si>
+  <si>
+    <t>Perquè ets una massatgista profesional. Fins i tot vam comprar un oli essencial per fer els nostres brutals massatges.</t>
+  </si>
+  <si>
+    <t>Perquè amb tu sóc molt feliç</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè t'enfades quan me'n enric de tu </t>
+  </si>
+  <si>
+    <t>Perquè saps com possar-me content ;)</t>
+  </si>
+  <si>
+    <t>Perquè rius encara què et digui que ets una ratilla.</t>
+  </si>
+  <si>
+    <t>Perquè m'expliques les teves històries amb un dramatisme IMPRESIONANT</t>
+  </si>
+  <si>
+    <t>Perquè encara que no ens fem mai fotos junts sempre tinc un record teu al cap</t>
+  </si>
+  <si>
+    <t>Perquè sabem superar els problemes quan ens en trobem</t>
+  </si>
+  <si>
+    <t>Perquè m'ajudes en moments difícils</t>
+  </si>
+  <si>
+    <t>Perquè acceptes els regals que et faig encara que no t'agradin gaire. Per exemple… LA MÀQUINA DE FER CRISPETES. Va ser pel teu Sant i no té vist fer-la servir MAI. Tot i així, t'estimoooo</t>
+  </si>
+  <si>
+    <t>Perquè encara que estiguem MOOOLT lluny ens seguim estimant</t>
+  </si>
+  <si>
+    <t>Perquè fem trucades moolt llargues i divertides on ens expliquem el que ens passa</t>
+  </si>
+  <si>
+    <t>Perquè ets una persona que em vas encantar només de coneixe't</t>
+  </si>
+  <si>
+    <t>Perquè cuides molt bé als del teu voltant. Això m'inclou a mi i a la Puçaaa</t>
+  </si>
+  <si>
+    <t>Perquè encara que vaig tardar a dir-te de que sortíssim junts, tu vas esperar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè em fiques la mà a la teva cama perquè et faci carícies quan estic conduint. </t>
+  </si>
+  <si>
+    <t>Perquè m'expliques històries molt boniques de quan eres petita</t>
+  </si>
+  <si>
+    <t>Perquè et queixes que rasco quan no m'he afaitat</t>
   </si>
 </sst>
 </file>
@@ -1494,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="80" workbookViewId="0">
-      <selection activeCell="D220" sqref="D220"/>
+    <sheetView tabSelected="1" topLeftCell="A239" zoomScale="80" workbookViewId="0">
+      <selection activeCell="C254" sqref="C254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1603,7 +1753,7 @@
         <v>45692</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1710,7 +1860,7 @@
         <v>45700</v>
       </c>
       <c r="C15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1739,7 +1889,7 @@
         <v>136</v>
       </c>
       <c r="E17" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1779,7 +1929,7 @@
         <v>45705</v>
       </c>
       <c r="C20" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1802,7 +1952,7 @@
         <v>45707</v>
       </c>
       <c r="C22" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1813,13 +1963,13 @@
         <v>45708</v>
       </c>
       <c r="C23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D23" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1841,10 +1991,10 @@
         <v>45710</v>
       </c>
       <c r="C25" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F25" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1891,7 +2041,7 @@
         <v>45714</v>
       </c>
       <c r="C29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1935,13 +2085,13 @@
         <v>45718</v>
       </c>
       <c r="C33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D33" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E33" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1974,13 +2124,13 @@
         <v>45721</v>
       </c>
       <c r="C36" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" t="s">
         <v>178</v>
-      </c>
-      <c r="D36" t="s">
-        <v>179</v>
-      </c>
-      <c r="E36" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2024,13 +2174,13 @@
         <v>45725</v>
       </c>
       <c r="C40" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D40" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E40" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2091,7 +2241,7 @@
         <v>45730</v>
       </c>
       <c r="C45" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F45" t="s">
         <v>60</v>
@@ -2127,13 +2277,13 @@
         <v>45733</v>
       </c>
       <c r="C48" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D48" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2177,7 +2327,7 @@
         <v>45737</v>
       </c>
       <c r="C52" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2199,13 +2349,13 @@
         <v>45739</v>
       </c>
       <c r="C54" t="s">
+        <v>293</v>
+      </c>
+      <c r="D54" t="s">
+        <v>294</v>
+      </c>
+      <c r="E54" t="s">
         <v>295</v>
-      </c>
-      <c r="D54" t="s">
-        <v>296</v>
-      </c>
-      <c r="E54" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2302,10 +2452,10 @@
         <v>45747</v>
       </c>
       <c r="C62" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F62" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2374,13 +2524,13 @@
         <v>45753</v>
       </c>
       <c r="C68" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D68" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E68" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2441,7 +2591,7 @@
         <v>45758</v>
       </c>
       <c r="C73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2463,10 +2613,10 @@
         <v>45760</v>
       </c>
       <c r="C75" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F75" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2488,13 +2638,13 @@
         <v>45762</v>
       </c>
       <c r="C77" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D77" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E77" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2652,10 +2802,10 @@
         <v>45775</v>
       </c>
       <c r="C90" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F90" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2755,7 +2905,7 @@
         <v>148</v>
       </c>
       <c r="D98" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2766,7 +2916,7 @@
         <v>45784</v>
       </c>
       <c r="C99" t="s">
-        <v>149</v>
+        <v>366</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2777,7 +2927,10 @@
         <v>45785</v>
       </c>
       <c r="C100" t="s">
-        <v>150</v>
+        <v>364</v>
+      </c>
+      <c r="F100" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2788,7 +2941,7 @@
         <v>45786</v>
       </c>
       <c r="C101" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2799,7 +2952,7 @@
         <v>45787</v>
       </c>
       <c r="C102" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2810,13 +2963,13 @@
         <v>45788</v>
       </c>
       <c r="C103" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D103" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E103" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2827,7 +2980,7 @@
         <v>45789</v>
       </c>
       <c r="C104" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2838,7 +2991,7 @@
         <v>45790</v>
       </c>
       <c r="C105" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2849,7 +3002,7 @@
         <v>45791</v>
       </c>
       <c r="C106" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2860,10 +3013,10 @@
         <v>45792</v>
       </c>
       <c r="C107" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D107" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2874,7 +3027,7 @@
         <v>45793</v>
       </c>
       <c r="C108" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2885,7 +3038,7 @@
         <v>45794</v>
       </c>
       <c r="C109" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2896,7 +3049,7 @@
         <v>45795</v>
       </c>
       <c r="C110" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2907,10 +3060,10 @@
         <v>45796</v>
       </c>
       <c r="C111" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F111" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -2921,7 +3074,7 @@
         <v>45797</v>
       </c>
       <c r="C112" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -2932,10 +3085,10 @@
         <v>45798</v>
       </c>
       <c r="C113" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D113" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -2946,7 +3099,7 @@
         <v>45799</v>
       </c>
       <c r="C114" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -2957,7 +3110,7 @@
         <v>45800</v>
       </c>
       <c r="C115" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -2968,7 +3121,7 @@
         <v>45801</v>
       </c>
       <c r="C116" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -2979,7 +3132,7 @@
         <v>45802</v>
       </c>
       <c r="C117" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3001,7 +3154,7 @@
         <v>45804</v>
       </c>
       <c r="C119" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3012,13 +3165,13 @@
         <v>45805</v>
       </c>
       <c r="C120" t="s">
+        <v>277</v>
+      </c>
+      <c r="D120" t="s">
+        <v>278</v>
+      </c>
+      <c r="E120" t="s">
         <v>279</v>
-      </c>
-      <c r="D120" t="s">
-        <v>280</v>
-      </c>
-      <c r="E120" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3029,7 +3182,7 @@
         <v>45806</v>
       </c>
       <c r="C121" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3051,10 +3204,10 @@
         <v>45808</v>
       </c>
       <c r="C123" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F123" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3076,7 +3229,7 @@
         <v>45810</v>
       </c>
       <c r="C125" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3087,7 +3240,7 @@
         <v>45811</v>
       </c>
       <c r="C126" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3109,13 +3262,13 @@
         <v>45813</v>
       </c>
       <c r="C128" t="s">
+        <v>181</v>
+      </c>
+      <c r="D128" t="s">
+        <v>182</v>
+      </c>
+      <c r="E128" t="s">
         <v>183</v>
-      </c>
-      <c r="D128" t="s">
-        <v>184</v>
-      </c>
-      <c r="E128" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3126,7 +3279,7 @@
         <v>45814</v>
       </c>
       <c r="C129" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3137,13 +3290,13 @@
         <v>45815</v>
       </c>
       <c r="C130" t="s">
+        <v>185</v>
+      </c>
+      <c r="D130" t="s">
+        <v>186</v>
+      </c>
+      <c r="E130" t="s">
         <v>187</v>
-      </c>
-      <c r="D130" t="s">
-        <v>188</v>
-      </c>
-      <c r="E130" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3154,7 +3307,7 @@
         <v>45816</v>
       </c>
       <c r="C131" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3165,7 +3318,7 @@
         <v>45817</v>
       </c>
       <c r="C132" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3176,7 +3329,7 @@
         <v>45818</v>
       </c>
       <c r="C133" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3187,7 +3340,7 @@
         <v>45819</v>
       </c>
       <c r="C134" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3198,7 +3351,7 @@
         <v>45820</v>
       </c>
       <c r="C135" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3209,7 +3362,7 @@
         <v>45821</v>
       </c>
       <c r="C136" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3220,13 +3373,13 @@
         <v>45822</v>
       </c>
       <c r="C137" t="s">
+        <v>208</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E137" t="s">
         <v>210</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E137" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3237,13 +3390,13 @@
         <v>45823</v>
       </c>
       <c r="C138" t="s">
+        <v>188</v>
+      </c>
+      <c r="D138" t="s">
+        <v>189</v>
+      </c>
+      <c r="E138" t="s">
         <v>190</v>
-      </c>
-      <c r="D138" t="s">
-        <v>191</v>
-      </c>
-      <c r="E138" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3254,7 +3407,7 @@
         <v>45824</v>
       </c>
       <c r="C139" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3265,7 +3418,7 @@
         <v>45825</v>
       </c>
       <c r="C140" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3276,7 +3429,7 @@
         <v>45826</v>
       </c>
       <c r="C141" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3287,10 +3440,10 @@
         <v>45827</v>
       </c>
       <c r="C142" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F142" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3301,7 +3454,7 @@
         <v>45828</v>
       </c>
       <c r="C143" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3312,7 +3465,7 @@
         <v>45829</v>
       </c>
       <c r="C144" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
@@ -3323,7 +3476,7 @@
         <v>45830</v>
       </c>
       <c r="C145" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -3334,13 +3487,13 @@
         <v>45831</v>
       </c>
       <c r="C146" t="s">
+        <v>218</v>
+      </c>
+      <c r="D146" t="s">
+        <v>219</v>
+      </c>
+      <c r="E146" t="s">
         <v>220</v>
-      </c>
-      <c r="D146" t="s">
-        <v>221</v>
-      </c>
-      <c r="E146" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
@@ -3351,7 +3504,7 @@
         <v>45832</v>
       </c>
       <c r="C147" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -3362,10 +3515,10 @@
         <v>45833</v>
       </c>
       <c r="C148" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D148" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
@@ -3387,7 +3540,7 @@
         <v>45835</v>
       </c>
       <c r="C150" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
@@ -3398,7 +3551,7 @@
         <v>45836</v>
       </c>
       <c r="C151" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
@@ -3409,7 +3562,13 @@
         <v>45837</v>
       </c>
       <c r="C152" t="s">
-        <v>228</v>
+        <v>377</v>
+      </c>
+      <c r="D152" t="s">
+        <v>378</v>
+      </c>
+      <c r="E152" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
@@ -3442,10 +3601,10 @@
         <v>45840</v>
       </c>
       <c r="C155" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F155" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
@@ -3467,10 +3626,10 @@
         <v>45842</v>
       </c>
       <c r="C157" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F157" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
@@ -3481,13 +3640,13 @@
         <v>45843</v>
       </c>
       <c r="C158" t="s">
+        <v>244</v>
+      </c>
+      <c r="D158" t="s">
+        <v>245</v>
+      </c>
+      <c r="E158" t="s">
         <v>246</v>
-      </c>
-      <c r="D158" t="s">
-        <v>247</v>
-      </c>
-      <c r="E158" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
@@ -3498,19 +3657,19 @@
         <v>45844</v>
       </c>
       <c r="C159" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E159" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F159" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G159" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H159" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
@@ -3521,7 +3680,7 @@
         <v>45845</v>
       </c>
       <c r="C160" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -3532,7 +3691,7 @@
         <v>45846</v>
       </c>
       <c r="C161" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
@@ -3543,7 +3702,7 @@
         <v>45847</v>
       </c>
       <c r="C162" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -3554,7 +3713,7 @@
         <v>45848</v>
       </c>
       <c r="C163" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
@@ -3565,7 +3724,7 @@
         <v>45849</v>
       </c>
       <c r="C164" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
@@ -3576,13 +3735,13 @@
         <v>45850</v>
       </c>
       <c r="C165" t="s">
+        <v>191</v>
+      </c>
+      <c r="D165" t="s">
+        <v>192</v>
+      </c>
+      <c r="E165" t="s">
         <v>193</v>
-      </c>
-      <c r="D165" t="s">
-        <v>194</v>
-      </c>
-      <c r="E165" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
@@ -3593,7 +3752,7 @@
         <v>45851</v>
       </c>
       <c r="C166" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
@@ -3604,13 +3763,13 @@
         <v>45852</v>
       </c>
       <c r="C167" t="s">
+        <v>253</v>
+      </c>
+      <c r="D167" t="s">
+        <v>254</v>
+      </c>
+      <c r="E167" t="s">
         <v>255</v>
-      </c>
-      <c r="D167" t="s">
-        <v>256</v>
-      </c>
-      <c r="E167" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
@@ -3621,7 +3780,7 @@
         <v>45853</v>
       </c>
       <c r="C168" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
@@ -3632,7 +3791,7 @@
         <v>45854</v>
       </c>
       <c r="C169" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
@@ -3643,7 +3802,7 @@
         <v>45855</v>
       </c>
       <c r="C170" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
@@ -3654,10 +3813,10 @@
         <v>45856</v>
       </c>
       <c r="C171" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F171" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
@@ -3668,7 +3827,7 @@
         <v>45857</v>
       </c>
       <c r="C172" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
@@ -3679,7 +3838,7 @@
         <v>45858</v>
       </c>
       <c r="C173" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
@@ -3690,13 +3849,13 @@
         <v>45859</v>
       </c>
       <c r="C174" t="s">
+        <v>264</v>
+      </c>
+      <c r="D174" t="s">
+        <v>265</v>
+      </c>
+      <c r="E174" t="s">
         <v>266</v>
-      </c>
-      <c r="D174" t="s">
-        <v>267</v>
-      </c>
-      <c r="E174" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
@@ -3707,7 +3866,7 @@
         <v>45860</v>
       </c>
       <c r="C175" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
@@ -3718,7 +3877,7 @@
         <v>45861</v>
       </c>
       <c r="C176" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
@@ -3729,7 +3888,7 @@
         <v>45862</v>
       </c>
       <c r="C177" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
@@ -3740,7 +3899,7 @@
         <v>45863</v>
       </c>
       <c r="C178" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
@@ -3762,13 +3921,13 @@
         <v>45865</v>
       </c>
       <c r="C180" t="s">
+        <v>274</v>
+      </c>
+      <c r="D180" t="s">
+        <v>275</v>
+      </c>
+      <c r="E180" t="s">
         <v>276</v>
-      </c>
-      <c r="D180" t="s">
-        <v>277</v>
-      </c>
-      <c r="E180" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
@@ -3779,7 +3938,7 @@
         <v>45866</v>
       </c>
       <c r="C181" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
@@ -3834,13 +3993,13 @@
         <v>45871</v>
       </c>
       <c r="C186" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D186" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E186" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
@@ -3851,7 +4010,7 @@
         <v>45872</v>
       </c>
       <c r="C187" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
@@ -3862,7 +4021,7 @@
         <v>45873</v>
       </c>
       <c r="C188" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
@@ -3884,10 +4043,10 @@
         <v>45875</v>
       </c>
       <c r="C190" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
@@ -3920,7 +4079,7 @@
         <v>45878</v>
       </c>
       <c r="C193" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
@@ -3931,13 +4090,13 @@
         <v>45879</v>
       </c>
       <c r="C194" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D194" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E194" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
@@ -3948,7 +4107,7 @@
         <v>45880</v>
       </c>
       <c r="C195" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
@@ -3959,13 +4118,13 @@
         <v>45881</v>
       </c>
       <c r="C196" t="s">
+        <v>194</v>
+      </c>
+      <c r="D196" t="s">
+        <v>195</v>
+      </c>
+      <c r="E196" t="s">
         <v>196</v>
-      </c>
-      <c r="D196" t="s">
-        <v>197</v>
-      </c>
-      <c r="E196" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
@@ -3976,7 +4135,7 @@
         <v>45882</v>
       </c>
       <c r="C197" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
@@ -3987,7 +4146,7 @@
         <v>45883</v>
       </c>
       <c r="C198" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
@@ -3998,10 +4157,10 @@
         <v>45884</v>
       </c>
       <c r="C199" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F199" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
@@ -4034,7 +4193,7 @@
         <v>45887</v>
       </c>
       <c r="C202" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
@@ -4045,7 +4204,7 @@
         <v>45888</v>
       </c>
       <c r="C203" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
@@ -4056,13 +4215,13 @@
         <v>45889</v>
       </c>
       <c r="C204" t="s">
+        <v>267</v>
+      </c>
+      <c r="D204" t="s">
+        <v>268</v>
+      </c>
+      <c r="E204" t="s">
         <v>269</v>
-      </c>
-      <c r="D204" t="s">
-        <v>270</v>
-      </c>
-      <c r="E204" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
@@ -4095,10 +4254,10 @@
         <v>45892</v>
       </c>
       <c r="C207" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F207" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
@@ -4109,10 +4268,10 @@
         <v>45893</v>
       </c>
       <c r="C208" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
@@ -4120,10 +4279,10 @@
         <v>45894</v>
       </c>
       <c r="C209" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
@@ -4134,7 +4293,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
@@ -4142,10 +4301,10 @@
         <v>45896</v>
       </c>
       <c r="C211" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
@@ -4153,16 +4312,16 @@
         <v>45897</v>
       </c>
       <c r="C212" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D212" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E212" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
@@ -4170,10 +4329,10 @@
         <v>45898</v>
       </c>
       <c r="C213" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
@@ -4184,7 +4343,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
@@ -4192,10 +4351,10 @@
         <v>45900</v>
       </c>
       <c r="C215" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
@@ -4206,7 +4365,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
@@ -4214,10 +4373,10 @@
         <v>45902</v>
       </c>
       <c r="C217" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
@@ -4225,10 +4384,10 @@
         <v>45903</v>
       </c>
       <c r="C218" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
@@ -4236,10 +4395,13 @@
         <v>45904</v>
       </c>
       <c r="C219" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+      <c r="F219" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
@@ -4247,10 +4409,10 @@
         <v>45905</v>
       </c>
       <c r="C220" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
@@ -4258,10 +4420,10 @@
         <v>45906</v>
       </c>
       <c r="C221" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
@@ -4269,10 +4431,10 @@
         <v>45907</v>
       </c>
       <c r="C222" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
@@ -4280,16 +4442,16 @@
         <v>45908</v>
       </c>
       <c r="C223" t="s">
-        <v>8</v>
+        <v>393</v>
       </c>
       <c r="D223" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E223" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
@@ -4297,7 +4459,7 @@
         <v>45909</v>
       </c>
       <c r="C224" t="s">
-        <v>8</v>
+        <v>392</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -4308,7 +4470,7 @@
         <v>45910</v>
       </c>
       <c r="C225" t="s">
-        <v>8</v>
+        <v>398</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
@@ -4319,7 +4481,7 @@
         <v>45911</v>
       </c>
       <c r="C226" t="s">
-        <v>8</v>
+        <v>394</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
@@ -4330,7 +4492,7 @@
         <v>45912</v>
       </c>
       <c r="C227" t="s">
-        <v>8</v>
+        <v>395</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
@@ -4341,13 +4503,13 @@
         <v>45913</v>
       </c>
       <c r="C228" t="s">
+        <v>197</v>
+      </c>
+      <c r="D228" t="s">
+        <v>198</v>
+      </c>
+      <c r="E228" t="s">
         <v>199</v>
-      </c>
-      <c r="D228" t="s">
-        <v>200</v>
-      </c>
-      <c r="E228" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
@@ -4358,7 +4520,7 @@
         <v>45914</v>
       </c>
       <c r="C229" t="s">
-        <v>8</v>
+        <v>397</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
@@ -4369,7 +4531,7 @@
         <v>45915</v>
       </c>
       <c r="C230" t="s">
-        <v>8</v>
+        <v>396</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
@@ -4380,7 +4542,7 @@
         <v>45916</v>
       </c>
       <c r="C231" t="s">
-        <v>8</v>
+        <v>399</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
@@ -4391,7 +4553,7 @@
         <v>45917</v>
       </c>
       <c r="C232" t="s">
-        <v>8</v>
+        <v>400</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
@@ -4402,7 +4564,7 @@
         <v>45918</v>
       </c>
       <c r="C233" t="s">
-        <v>8</v>
+        <v>401</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
@@ -4413,7 +4575,7 @@
         <v>45919</v>
       </c>
       <c r="C234" t="s">
-        <v>8</v>
+        <v>402</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.3">
@@ -4424,10 +4586,10 @@
         <v>45920</v>
       </c>
       <c r="C235" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.3">
@@ -4438,7 +4600,7 @@
         <v>45921</v>
       </c>
       <c r="C236" t="s">
-        <v>8</v>
+        <v>403</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.3">
@@ -4449,7 +4611,7 @@
         <v>45922</v>
       </c>
       <c r="C237" t="s">
-        <v>8</v>
+        <v>404</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
@@ -4460,7 +4622,13 @@
         <v>45923</v>
       </c>
       <c r="C238" t="s">
-        <v>8</v>
+        <v>197</v>
+      </c>
+      <c r="D238" t="s">
+        <v>367</v>
+      </c>
+      <c r="E238" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
@@ -4471,7 +4639,7 @@
         <v>45924</v>
       </c>
       <c r="C239" t="s">
-        <v>8</v>
+        <v>405</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
@@ -4482,7 +4650,7 @@
         <v>45925</v>
       </c>
       <c r="C240" t="s">
-        <v>8</v>
+        <v>406</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.3">
@@ -4504,7 +4672,7 @@
         <v>45927</v>
       </c>
       <c r="C242" t="s">
-        <v>8</v>
+        <v>407</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.3">
@@ -4515,7 +4683,7 @@
         <v>45928</v>
       </c>
       <c r="C243" t="s">
-        <v>8</v>
+        <v>408</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.3">
@@ -4526,7 +4694,7 @@
         <v>45929</v>
       </c>
       <c r="C244" t="s">
-        <v>8</v>
+        <v>409</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
@@ -4559,7 +4727,7 @@
         <v>45932</v>
       </c>
       <c r="C247" t="s">
-        <v>8</v>
+        <v>410</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.3">
@@ -4570,7 +4738,7 @@
         <v>45933</v>
       </c>
       <c r="C248" t="s">
-        <v>8</v>
+        <v>411</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.3">
@@ -4581,7 +4749,7 @@
         <v>45934</v>
       </c>
       <c r="C249" t="s">
-        <v>8</v>
+        <v>412</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.3">
@@ -4592,13 +4760,13 @@
         <v>45935</v>
       </c>
       <c r="C250" t="s">
-        <v>282</v>
+        <v>386</v>
       </c>
       <c r="D250" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E250" t="s">
-        <v>312</v>
+        <v>387</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.3">
@@ -4642,10 +4810,10 @@
         <v>45939</v>
       </c>
       <c r="C254" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F254" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
@@ -4722,10 +4890,10 @@
         <v>45946</v>
       </c>
       <c r="C261" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F261" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.3">
@@ -4780,7 +4948,13 @@
         <v>45951</v>
       </c>
       <c r="C266" t="s">
-        <v>8</v>
+        <v>380</v>
+      </c>
+      <c r="D266" t="s">
+        <v>381</v>
+      </c>
+      <c r="E266" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.3">
@@ -4868,7 +5042,13 @@
         <v>45959</v>
       </c>
       <c r="C274" t="s">
-        <v>8</v>
+        <v>388</v>
+      </c>
+      <c r="D274" t="s">
+        <v>389</v>
+      </c>
+      <c r="E274" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
@@ -4978,13 +5158,13 @@
         <v>45969</v>
       </c>
       <c r="C284" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D284" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E284" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
@@ -5039,10 +5219,10 @@
         <v>45974</v>
       </c>
       <c r="C289" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F289" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.3">
@@ -5097,10 +5277,10 @@
         <v>45979</v>
       </c>
       <c r="C294" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F294" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.3">
@@ -5166,10 +5346,10 @@
         <v>45985</v>
       </c>
       <c r="C300" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F300" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.3">
@@ -5290,7 +5470,10 @@
         <v>45996</v>
       </c>
       <c r="C311" t="s">
-        <v>8</v>
+        <v>375</v>
+      </c>
+      <c r="D311" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.3">
@@ -5345,13 +5528,13 @@
         <v>46001</v>
       </c>
       <c r="C316" t="s">
+        <v>310</v>
+      </c>
+      <c r="D316" t="s">
+        <v>313</v>
+      </c>
+      <c r="E316" t="s">
         <v>314</v>
-      </c>
-      <c r="D316" t="s">
-        <v>317</v>
-      </c>
-      <c r="E316" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.3">
@@ -5417,10 +5600,10 @@
         <v>46007</v>
       </c>
       <c r="C322" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F322" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.3">
@@ -5464,13 +5647,13 @@
         <v>46011</v>
       </c>
       <c r="C326" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D326" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E326" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.3">
@@ -5646,7 +5829,13 @@
         <v>46027</v>
       </c>
       <c r="C342" t="s">
-        <v>8</v>
+        <v>372</v>
+      </c>
+      <c r="D342" t="s">
+        <v>373</v>
+      </c>
+      <c r="E342" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.3">
@@ -5679,10 +5868,10 @@
         <v>46030</v>
       </c>
       <c r="C345" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F345" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.3">
@@ -5748,13 +5937,13 @@
         <v>46036</v>
       </c>
       <c r="C351" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D351" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E351" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.3">
@@ -5787,7 +5976,13 @@
         <v>46039</v>
       </c>
       <c r="C354" t="s">
-        <v>8</v>
+        <v>383</v>
+      </c>
+      <c r="D354" t="s">
+        <v>384</v>
+      </c>
+      <c r="E354" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.3">
@@ -5831,7 +6026,7 @@
         <v>46043</v>
       </c>
       <c r="C358" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.3">
@@ -5845,7 +6040,7 @@
         <v>8</v>
       </c>
       <c r="F359" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.3">
@@ -5867,7 +6062,13 @@
         <v>46046</v>
       </c>
       <c r="C361" t="s">
-        <v>8</v>
+        <v>369</v>
+      </c>
+      <c r="D361" t="s">
+        <v>370</v>
+      </c>
+      <c r="E361" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.3">
@@ -5934,7 +6135,7 @@
         <v>46052</v>
       </c>
       <c r="C367" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Nou progres, noves fotos
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2702AA2E-8130-4CFF-B6A0-387DD1B9E4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C34B2B5-1E7C-46EF-BE4E-FE15100ABEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="472">
   <si>
     <t>Dia</t>
   </si>
@@ -909,9 +909,6 @@
     <t>./img/bereal7.jpeg</t>
   </si>
   <si>
-    <t>En aquest Bereal surts ajudant me a netejar la limusina. No està malament perquè d'alguna manera s'ha de pagar el taxi.</t>
-  </si>
-  <si>
     <t>./img/bereal8.jpeg</t>
   </si>
   <si>
@@ -1423,6 +1420,27 @@
   </si>
   <si>
     <t>Perquè sempre dius que no faràs siesta pero després dorms 3 hores!</t>
+  </si>
+  <si>
+    <t>Perquè ajudes a que em cuidi les mans</t>
+  </si>
+  <si>
+    <t>./img/mans_mascara.jpg</t>
+  </si>
+  <si>
+    <t>Aquí vas acompanyar-me amb el meu cuidado de mans fent-ho tu també</t>
+  </si>
+  <si>
+    <t>Perquè T'ENCANTEN els regals que et fan els meus avis quan van de viatge</t>
+  </si>
+  <si>
+    <t>./img/regal_avis.jpg</t>
+  </si>
+  <si>
+    <t>Aquí estavem a un assaig de GERONIMO i vas provar la xocolata que et van portar els meus avis de Eslovàquia</t>
+  </si>
+  <si>
+    <t>En aquest Bereal surts ajudant-me a netejar la limusina. No està malament perquè d'alguna manera s'ha de pagar el taxi.</t>
   </si>
 </sst>
 </file>
@@ -1804,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A288" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C301" sqref="C301"/>
+    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D381" sqref="D381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2089,7 +2107,7 @@
         <v>45705</v>
       </c>
       <c r="C20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2112,7 +2130,7 @@
         <v>45707</v>
       </c>
       <c r="C22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2151,10 +2169,10 @@
         <v>45710</v>
       </c>
       <c r="C25" t="s">
+        <v>339</v>
+      </c>
+      <c r="F25" t="s">
         <v>340</v>
-      </c>
-      <c r="F25" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2284,7 +2302,7 @@
         <v>45721</v>
       </c>
       <c r="C36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D36" t="s">
         <v>174</v>
@@ -2301,7 +2319,7 @@
         <v>45722</v>
       </c>
       <c r="C37" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2579,7 +2597,7 @@
         <v>140</v>
       </c>
       <c r="F59" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2612,10 +2630,10 @@
         <v>45747</v>
       </c>
       <c r="C62" t="s">
+        <v>321</v>
+      </c>
+      <c r="F62" t="s">
         <v>322</v>
-      </c>
-      <c r="F62" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2637,7 +2655,7 @@
         <v>45749</v>
       </c>
       <c r="C64" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2689,8 +2707,8 @@
       <c r="D68" t="s">
         <v>293</v>
       </c>
-      <c r="E68" t="s">
-        <v>294</v>
+      <c r="E68" s="6" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2773,10 +2791,10 @@
         <v>45760</v>
       </c>
       <c r="C75" t="s">
+        <v>323</v>
+      </c>
+      <c r="F75" t="s">
         <v>324</v>
-      </c>
-      <c r="F75" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2801,10 +2819,10 @@
         <v>282</v>
       </c>
       <c r="D77" t="s">
+        <v>294</v>
+      </c>
+      <c r="E77" t="s">
         <v>295</v>
-      </c>
-      <c r="E77" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2962,10 +2980,10 @@
         <v>45775</v>
       </c>
       <c r="C90" t="s">
+        <v>342</v>
+      </c>
+      <c r="F90" t="s">
         <v>343</v>
-      </c>
-      <c r="F90" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -3076,7 +3094,7 @@
         <v>45784</v>
       </c>
       <c r="C99" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3087,10 +3105,10 @@
         <v>45785</v>
       </c>
       <c r="C100" t="s">
+        <v>360</v>
+      </c>
+      <c r="F100" t="s">
         <v>361</v>
-      </c>
-      <c r="F100" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3126,10 +3144,10 @@
         <v>282</v>
       </c>
       <c r="D103" t="s">
+        <v>298</v>
+      </c>
+      <c r="E103" t="s">
         <v>299</v>
-      </c>
-      <c r="E103" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3600,10 +3618,10 @@
         <v>45827</v>
       </c>
       <c r="C142" t="s">
+        <v>325</v>
+      </c>
+      <c r="F142" t="s">
         <v>326</v>
-      </c>
-      <c r="F142" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3722,13 +3740,13 @@
         <v>45837</v>
       </c>
       <c r="C152" t="s">
+        <v>373</v>
+      </c>
+      <c r="D152" t="s">
         <v>374</v>
       </c>
-      <c r="D152" t="s">
+      <c r="E152" t="s">
         <v>375</v>
-      </c>
-      <c r="E152" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
@@ -3862,7 +3880,7 @@
         <v>45847</v>
       </c>
       <c r="C162" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -4156,10 +4174,10 @@
         <v>282</v>
       </c>
       <c r="D186" t="s">
+        <v>296</v>
+      </c>
+      <c r="E186" t="s">
         <v>297</v>
-      </c>
-      <c r="E186" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
@@ -4253,10 +4271,10 @@
         <v>277</v>
       </c>
       <c r="D194" t="s">
+        <v>300</v>
+      </c>
+      <c r="E194" t="s">
         <v>301</v>
-      </c>
-      <c r="E194" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
@@ -4267,7 +4285,7 @@
         <v>45880</v>
       </c>
       <c r="C195" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
@@ -4295,7 +4313,7 @@
         <v>45882</v>
       </c>
       <c r="C197" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
@@ -4306,7 +4324,7 @@
         <v>45883</v>
       </c>
       <c r="C198" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
@@ -4317,10 +4335,10 @@
         <v>45884</v>
       </c>
       <c r="C199" t="s">
+        <v>318</v>
+      </c>
+      <c r="F199" t="s">
         <v>319</v>
-      </c>
-      <c r="F199" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
@@ -4364,7 +4382,7 @@
         <v>45888</v>
       </c>
       <c r="C203" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
@@ -4414,10 +4432,10 @@
         <v>45892</v>
       </c>
       <c r="C207" t="s">
+        <v>346</v>
+      </c>
+      <c r="F207" t="s">
         <v>347</v>
-      </c>
-      <c r="F207" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
@@ -4428,7 +4446,7 @@
         <v>45893</v>
       </c>
       <c r="C208" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
@@ -4439,7 +4457,7 @@
         <v>45894</v>
       </c>
       <c r="C209" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
@@ -4461,7 +4479,7 @@
         <v>45896</v>
       </c>
       <c r="C211" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
@@ -4472,13 +4490,13 @@
         <v>45897</v>
       </c>
       <c r="C212" t="s">
+        <v>351</v>
+      </c>
+      <c r="D212" t="s">
         <v>352</v>
       </c>
-      <c r="D212" t="s">
+      <c r="E212" t="s">
         <v>353</v>
-      </c>
-      <c r="E212" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
@@ -4511,7 +4529,7 @@
         <v>45900</v>
       </c>
       <c r="C215" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
@@ -4533,7 +4551,7 @@
         <v>45902</v>
       </c>
       <c r="C217" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
@@ -4544,7 +4562,7 @@
         <v>45903</v>
       </c>
       <c r="C218" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
@@ -4555,10 +4573,10 @@
         <v>45904</v>
       </c>
       <c r="C219" t="s">
+        <v>357</v>
+      </c>
+      <c r="F219" t="s">
         <v>358</v>
-      </c>
-      <c r="F219" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.3">
@@ -4569,7 +4587,7 @@
         <v>45905</v>
       </c>
       <c r="C220" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
@@ -4591,7 +4609,7 @@
         <v>45907</v>
       </c>
       <c r="C222" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
@@ -4602,13 +4620,13 @@
         <v>45908</v>
       </c>
       <c r="C223" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D223" t="s">
+        <v>302</v>
+      </c>
+      <c r="E223" t="s">
         <v>303</v>
-      </c>
-      <c r="E223" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.3">
@@ -4619,7 +4637,7 @@
         <v>45909</v>
       </c>
       <c r="C224" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -4630,7 +4648,7 @@
         <v>45910</v>
       </c>
       <c r="C225" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
@@ -4641,7 +4659,7 @@
         <v>45911</v>
       </c>
       <c r="C226" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
@@ -4652,7 +4670,7 @@
         <v>45912</v>
       </c>
       <c r="C227" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
@@ -4680,7 +4698,7 @@
         <v>45914</v>
       </c>
       <c r="C229" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
@@ -4691,7 +4709,7 @@
         <v>45915</v>
       </c>
       <c r="C230" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
@@ -4702,7 +4720,7 @@
         <v>45916</v>
       </c>
       <c r="C231" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
@@ -4713,13 +4731,13 @@
         <v>45917</v>
       </c>
       <c r="C232" t="s">
+        <v>427</v>
+      </c>
+      <c r="D232" t="s">
         <v>428</v>
       </c>
-      <c r="D232" t="s">
+      <c r="E232" t="s">
         <v>429</v>
-      </c>
-      <c r="E232" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
@@ -4730,7 +4748,7 @@
         <v>45918</v>
       </c>
       <c r="C233" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
@@ -4741,7 +4759,7 @@
         <v>45919</v>
       </c>
       <c r="C234" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.3">
@@ -4766,7 +4784,7 @@
         <v>45921</v>
       </c>
       <c r="C236" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.3">
@@ -4777,7 +4795,7 @@
         <v>45922</v>
       </c>
       <c r="C237" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
@@ -4791,10 +4809,10 @@
         <v>194</v>
       </c>
       <c r="D238" t="s">
+        <v>363</v>
+      </c>
+      <c r="E238" t="s">
         <v>364</v>
-      </c>
-      <c r="E238" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
@@ -4805,7 +4823,7 @@
         <v>45924</v>
       </c>
       <c r="C239" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
@@ -4816,7 +4834,7 @@
         <v>45925</v>
       </c>
       <c r="C240" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.3">
@@ -4838,7 +4856,7 @@
         <v>45927</v>
       </c>
       <c r="C242" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.3">
@@ -4849,7 +4867,7 @@
         <v>45928</v>
       </c>
       <c r="C243" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.3">
@@ -4860,13 +4878,13 @@
         <v>45929</v>
       </c>
       <c r="C244" t="s">
+        <v>414</v>
+      </c>
+      <c r="D244" t="s">
         <v>415</v>
       </c>
-      <c r="D244" t="s">
+      <c r="E244" t="s">
         <v>416</v>
-      </c>
-      <c r="E244" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
@@ -4899,7 +4917,7 @@
         <v>45932</v>
       </c>
       <c r="C247" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.3">
@@ -4910,7 +4928,7 @@
         <v>45933</v>
       </c>
       <c r="C248" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.3">
@@ -4921,7 +4939,7 @@
         <v>45934</v>
       </c>
       <c r="C249" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.3">
@@ -4932,13 +4950,13 @@
         <v>45935</v>
       </c>
       <c r="C250" t="s">
+        <v>382</v>
+      </c>
+      <c r="D250" t="s">
+        <v>304</v>
+      </c>
+      <c r="E250" t="s">
         <v>383</v>
-      </c>
-      <c r="D250" t="s">
-        <v>305</v>
-      </c>
-      <c r="E250" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.3">
@@ -4949,7 +4967,7 @@
         <v>45936</v>
       </c>
       <c r="C251" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.3">
@@ -4960,7 +4978,7 @@
         <v>45937</v>
       </c>
       <c r="C252" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.3">
@@ -4971,7 +4989,7 @@
         <v>45938</v>
       </c>
       <c r="C253" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.3">
@@ -4996,7 +5014,7 @@
         <v>45940</v>
       </c>
       <c r="C255" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
@@ -5007,13 +5025,13 @@
         <v>45941</v>
       </c>
       <c r="C256" t="s">
+        <v>417</v>
+      </c>
+      <c r="D256" t="s">
         <v>418</v>
       </c>
-      <c r="D256" t="s">
+      <c r="E256" t="s">
         <v>419</v>
-      </c>
-      <c r="E256" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.3">
@@ -5024,7 +5042,7 @@
         <v>45942</v>
       </c>
       <c r="C257" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.3">
@@ -5035,7 +5053,7 @@
         <v>45943</v>
       </c>
       <c r="C258" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.3">
@@ -5046,7 +5064,7 @@
         <v>45944</v>
       </c>
       <c r="C259" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.3">
@@ -5057,7 +5075,7 @@
         <v>45945</v>
       </c>
       <c r="C260" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.3">
@@ -5068,10 +5086,10 @@
         <v>45946</v>
       </c>
       <c r="C261" t="s">
+        <v>329</v>
+      </c>
+      <c r="F261" t="s">
         <v>330</v>
-      </c>
-      <c r="F261" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.3">
@@ -5082,7 +5100,7 @@
         <v>45947</v>
       </c>
       <c r="C262" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.3">
@@ -5093,7 +5111,7 @@
         <v>45948</v>
       </c>
       <c r="C263" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.3">
@@ -5115,7 +5133,7 @@
         <v>45950</v>
       </c>
       <c r="C265" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.3">
@@ -5126,13 +5144,13 @@
         <v>45951</v>
       </c>
       <c r="C266" t="s">
+        <v>376</v>
+      </c>
+      <c r="D266" t="s">
         <v>377</v>
       </c>
-      <c r="D266" t="s">
+      <c r="E266" t="s">
         <v>378</v>
-      </c>
-      <c r="E266" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.3">
@@ -5143,7 +5161,7 @@
         <v>45952</v>
       </c>
       <c r="C267" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.3">
@@ -5153,8 +5171,8 @@
       <c r="B268" s="4">
         <v>45953</v>
       </c>
-      <c r="C268" s="6" t="s">
-        <v>440</v>
+      <c r="C268" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.3">
@@ -5165,7 +5183,7 @@
         <v>45954</v>
       </c>
       <c r="C269" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.3">
@@ -5176,7 +5194,7 @@
         <v>45955</v>
       </c>
       <c r="C270" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.3">
@@ -5198,7 +5216,7 @@
         <v>45957</v>
       </c>
       <c r="C272" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
@@ -5209,7 +5227,7 @@
         <v>45958</v>
       </c>
       <c r="C273" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
@@ -5220,13 +5238,13 @@
         <v>45959</v>
       </c>
       <c r="C274" t="s">
+        <v>384</v>
+      </c>
+      <c r="D274" t="s">
         <v>385</v>
       </c>
-      <c r="D274" t="s">
+      <c r="E274" t="s">
         <v>386</v>
-      </c>
-      <c r="E274" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
@@ -5248,7 +5266,7 @@
         <v>45961</v>
       </c>
       <c r="C276" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
@@ -5270,7 +5288,7 @@
         <v>45963</v>
       </c>
       <c r="C278" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
@@ -5281,7 +5299,7 @@
         <v>45964</v>
       </c>
       <c r="C279" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
@@ -5292,13 +5310,13 @@
         <v>45965</v>
       </c>
       <c r="C280" t="s">
+        <v>420</v>
+      </c>
+      <c r="D280" t="s">
         <v>421</v>
       </c>
-      <c r="D280" t="s">
-        <v>422</v>
-      </c>
       <c r="E280" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
@@ -5309,7 +5327,7 @@
         <v>45966</v>
       </c>
       <c r="C281" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
@@ -5320,7 +5338,7 @@
         <v>45967</v>
       </c>
       <c r="C282" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
@@ -5331,7 +5349,7 @@
         <v>45968</v>
       </c>
       <c r="C283" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
@@ -5342,13 +5360,13 @@
         <v>45969</v>
       </c>
       <c r="C284" t="s">
+        <v>306</v>
+      </c>
+      <c r="D284" t="s">
         <v>307</v>
       </c>
-      <c r="D284" t="s">
+      <c r="E284" t="s">
         <v>308</v>
-      </c>
-      <c r="E284" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
@@ -5359,7 +5377,7 @@
         <v>45970</v>
       </c>
       <c r="C285" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
@@ -5370,7 +5388,7 @@
         <v>45971</v>
       </c>
       <c r="C286" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
@@ -5381,7 +5399,7 @@
         <v>45972</v>
       </c>
       <c r="C287" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
@@ -5392,7 +5410,7 @@
         <v>45973</v>
       </c>
       <c r="C288" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.3">
@@ -5403,10 +5421,10 @@
         <v>45974</v>
       </c>
       <c r="C289" t="s">
+        <v>331</v>
+      </c>
+      <c r="F289" t="s">
         <v>332</v>
-      </c>
-      <c r="F289" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.3">
@@ -5417,7 +5435,7 @@
         <v>45975</v>
       </c>
       <c r="C290" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.3">
@@ -5428,7 +5446,7 @@
         <v>45976</v>
       </c>
       <c r="C291" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.3">
@@ -5439,7 +5457,7 @@
         <v>45977</v>
       </c>
       <c r="C292" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.3">
@@ -5450,7 +5468,7 @@
         <v>45978</v>
       </c>
       <c r="C293" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.3">
@@ -5475,7 +5493,7 @@
         <v>45980</v>
       </c>
       <c r="C295" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.3">
@@ -5486,7 +5504,7 @@
         <v>45981</v>
       </c>
       <c r="C296" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.3">
@@ -5497,7 +5515,7 @@
         <v>45982</v>
       </c>
       <c r="C297" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.3">
@@ -5508,7 +5526,7 @@
         <v>45983</v>
       </c>
       <c r="C298" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.3">
@@ -5519,7 +5537,7 @@
         <v>45984</v>
       </c>
       <c r="C299" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.3">
@@ -5530,10 +5548,10 @@
         <v>45985</v>
       </c>
       <c r="C300" t="s">
+        <v>344</v>
+      </c>
+      <c r="F300" t="s">
         <v>345</v>
-      </c>
-      <c r="F300" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.3">
@@ -5544,7 +5562,7 @@
         <v>45986</v>
       </c>
       <c r="C301" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.3">
@@ -5566,7 +5584,13 @@
         <v>45988</v>
       </c>
       <c r="C303" t="s">
-        <v>8</v>
+        <v>465</v>
+      </c>
+      <c r="D303" t="s">
+        <v>466</v>
+      </c>
+      <c r="E303" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.3">
@@ -5654,10 +5678,10 @@
         <v>45996</v>
       </c>
       <c r="C311" t="s">
+        <v>371</v>
+      </c>
+      <c r="D311" t="s">
         <v>372</v>
-      </c>
-      <c r="D311" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.3">
@@ -5670,6 +5694,7 @@
       <c r="C312" t="s">
         <v>8</v>
       </c>
+      <c r="E312" s="6"/>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313">
@@ -5712,13 +5737,13 @@
         <v>46001</v>
       </c>
       <c r="C316" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D316" t="s">
+        <v>309</v>
+      </c>
+      <c r="E316" t="s">
         <v>310</v>
-      </c>
-      <c r="E316" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.3">
@@ -5751,7 +5776,13 @@
         <v>46004</v>
       </c>
       <c r="C319" t="s">
-        <v>8</v>
+        <v>468</v>
+      </c>
+      <c r="D319" t="s">
+        <v>469</v>
+      </c>
+      <c r="E319" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.3">
@@ -5784,10 +5815,10 @@
         <v>46007</v>
       </c>
       <c r="C322" t="s">
+        <v>333</v>
+      </c>
+      <c r="F322" t="s">
         <v>334</v>
-      </c>
-      <c r="F322" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.3">
@@ -5831,13 +5862,13 @@
         <v>46011</v>
       </c>
       <c r="C326" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D326" t="s">
+        <v>313</v>
+      </c>
+      <c r="E326" t="s">
         <v>314</v>
-      </c>
-      <c r="E326" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.3">
@@ -5870,13 +5901,13 @@
         <v>46014</v>
       </c>
       <c r="C329" t="s">
+        <v>422</v>
+      </c>
+      <c r="D329" t="s">
         <v>423</v>
       </c>
-      <c r="D329" t="s">
+      <c r="E329" t="s">
         <v>424</v>
-      </c>
-      <c r="E329" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.3">
@@ -5964,10 +5995,10 @@
         <v>46022</v>
       </c>
       <c r="C337" t="s">
+        <v>425</v>
+      </c>
+      <c r="D337" t="s">
         <v>426</v>
-      </c>
-      <c r="D337" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.3">
@@ -6022,13 +6053,13 @@
         <v>46027</v>
       </c>
       <c r="C342" t="s">
+        <v>368</v>
+      </c>
+      <c r="D342" t="s">
         <v>369</v>
       </c>
-      <c r="D342" t="s">
+      <c r="E342" t="s">
         <v>370</v>
-      </c>
-      <c r="E342" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.3">
@@ -6061,10 +6092,10 @@
         <v>46030</v>
       </c>
       <c r="C345" t="s">
+        <v>335</v>
+      </c>
+      <c r="F345" t="s">
         <v>336</v>
-      </c>
-      <c r="F345" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.3">
@@ -6130,13 +6161,13 @@
         <v>46036</v>
       </c>
       <c r="C351" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D351" t="s">
+        <v>311</v>
+      </c>
+      <c r="E351" t="s">
         <v>312</v>
-      </c>
-      <c r="E351" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.3">
@@ -6169,13 +6200,13 @@
         <v>46039</v>
       </c>
       <c r="C354" t="s">
+        <v>379</v>
+      </c>
+      <c r="D354" t="s">
         <v>380</v>
       </c>
-      <c r="D354" t="s">
+      <c r="E354" t="s">
         <v>381</v>
-      </c>
-      <c r="E354" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.3">
@@ -6219,7 +6250,7 @@
         <v>46043</v>
       </c>
       <c r="C358" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.3">
@@ -6233,7 +6264,7 @@
         <v>8</v>
       </c>
       <c r="F359" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.3">
@@ -6255,13 +6286,13 @@
         <v>46046</v>
       </c>
       <c r="C361" t="s">
+        <v>365</v>
+      </c>
+      <c r="D361" t="s">
         <v>366</v>
       </c>
-      <c r="D361" t="s">
+      <c r="E361" t="s">
         <v>367</v>
-      </c>
-      <c r="E361" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.3">
@@ -6328,7 +6359,7 @@
         <v>46052</v>
       </c>
       <c r="C367" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Afegit foto tornada Egipte
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E7316A-BEED-4CAA-8B30-435753E078C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F451C1-E3C8-4CBC-86D6-043E2898EDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="476">
   <si>
     <t>Dia</t>
   </si>
@@ -1441,6 +1441,18 @@
   </si>
   <si>
     <t>En aquest Bereal surts ajudant-me a netejar la limusina. No està malament perquè d'alguna manera s'ha de pagar el taxi.</t>
+  </si>
+  <si>
+    <t>Perquè et trobo MOOOOLT a faltar quan marxes de viatje</t>
+  </si>
+  <si>
+    <t>./img/jo_ram.jpeg</t>
+  </si>
+  <si>
+    <t>Em sap greu no poder ser-hi ara que tornes de Egitpe amb un ram. Espero que la foto et serveixi! T'estimo mooolt i aviat ens veiem</t>
+  </si>
+  <si>
+    <t>Perquè m'expliques tots els cotillos de DOMINGAS (ets la meva espia secreta)</t>
   </si>
 </sst>
 </file>
@@ -1497,14 +1509,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1822,8 +1833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C301" sqref="C301"/>
+    <sheetView tabSelected="1" topLeftCell="A281" zoomScale="80" workbookViewId="0">
+      <selection activeCell="C294" sqref="C294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2891,13 +2902,13 @@
         <v>45768</v>
       </c>
       <c r="C83" t="s">
-        <v>102</v>
+        <v>472</v>
       </c>
       <c r="D83" t="s">
-        <v>104</v>
+        <v>473</v>
       </c>
       <c r="E83" t="s">
-        <v>105</v>
+        <v>474</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -5601,7 +5612,7 @@
         <v>45989</v>
       </c>
       <c r="C304" t="s">
-        <v>8</v>
+        <v>475</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.3">
@@ -5612,7 +5623,13 @@
         <v>45990</v>
       </c>
       <c r="C305" t="s">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="D305" t="s">
+        <v>104</v>
+      </c>
+      <c r="E305" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
@@ -6364,53 +6381,52 @@
     <row r="368" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B368" s="1"/>
     </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="369" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B369" s="1"/>
     </row>
-    <row r="370" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="370" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B370" s="1"/>
     </row>
-    <row r="371" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="371" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B371" s="1"/>
     </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="372" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B372" s="1"/>
     </row>
-    <row r="373" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="373" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B373" s="1"/>
     </row>
-    <row r="374" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="374" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B374" s="1"/>
     </row>
-    <row r="375" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="375" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B375" s="1"/>
-      <c r="C375" s="6"/>
-    </row>
-    <row r="376" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="376" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B376" s="1"/>
     </row>
-    <row r="377" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="377" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B377" s="1"/>
     </row>
-    <row r="378" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="378" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B378" s="1"/>
     </row>
-    <row r="379" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="379" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B379" s="1"/>
     </row>
-    <row r="380" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="380" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B380" s="1"/>
     </row>
-    <row r="381" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="381" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B381" s="1"/>
     </row>
-    <row r="382" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="382" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B382" s="1"/>
     </row>
-    <row r="383" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="383" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B383" s="1"/>
     </row>
-    <row r="384" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="384" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B384" s="1"/>
     </row>
     <row r="385" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Videos afegits i dies
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F451C1-E3C8-4CBC-86D6-043E2898EDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAB29B2-F878-4314-9B59-3F67B8A80B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="485">
   <si>
     <t>Dia</t>
   </si>
@@ -1453,6 +1453,33 @@
   </si>
   <si>
     <t>Perquè m'expliques tots els cotillos de DOMINGAS (ets la meva espia secreta)</t>
+  </si>
+  <si>
+    <t>Perquè aguantes les meves MEGA tonteries com quan vaig intentar cassar a la SIRENITAA</t>
+  </si>
+  <si>
+    <t>./video/sirenita.mp4</t>
+  </si>
+  <si>
+    <t>Perquè m'acompanyes a Manlleu a veure la meva àvia i a fer activitats SUPER XULES (com donar menjar a les gallines)</t>
+  </si>
+  <si>
+    <t>./video/manlleu.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè encara que no tinguis gana menjes MOOOLT perquè el meu avi no et critiqui </t>
+  </si>
+  <si>
+    <t>En aquesta foto podem veure com som els més guapos que han passat MAI com a monitors.</t>
+  </si>
+  <si>
+    <t>Perquè m'intentes fer una mica de cas quan et dic que no et mosseguis els llabis</t>
+  </si>
+  <si>
+    <t>Perquè quan estic MOOOOLT malalt (sempre) em cuides.</t>
+  </si>
+  <si>
+    <t>Perquè quan estàs malalta (quasi mai) deixes que et cuidi</t>
   </si>
 </sst>
 </file>
@@ -1833,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A281" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C294" sqref="C294"/>
+    <sheetView tabSelected="1" topLeftCell="A297" zoomScale="80" workbookViewId="0">
+      <selection activeCell="C313" sqref="C313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5615,7 +5642,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>304</v>
       </c>
@@ -5632,7 +5659,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>305</v>
       </c>
@@ -5643,7 +5670,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>306</v>
       </c>
@@ -5654,7 +5681,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>307</v>
       </c>
@@ -5662,10 +5689,13 @@
         <v>45993</v>
       </c>
       <c r="C308" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+        <v>476</v>
+      </c>
+      <c r="F308" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>308</v>
       </c>
@@ -5673,10 +5703,10 @@
         <v>45994</v>
       </c>
       <c r="C309" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>309</v>
       </c>
@@ -5684,10 +5714,10 @@
         <v>45995</v>
       </c>
       <c r="C310" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>310</v>
       </c>
@@ -5700,8 +5730,11 @@
       <c r="D311" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E311" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>311</v>
       </c>
@@ -5709,10 +5742,10 @@
         <v>45997</v>
       </c>
       <c r="C312" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>312</v>
       </c>
@@ -5720,10 +5753,10 @@
         <v>45998</v>
       </c>
       <c r="C313" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>313</v>
       </c>
@@ -5734,7 +5767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>314</v>
       </c>
@@ -5745,7 +5778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>315</v>
       </c>
@@ -5762,7 +5795,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>316</v>
       </c>
@@ -5773,7 +5806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>317</v>
       </c>
@@ -5784,7 +5817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>318</v>
       </c>
@@ -5801,7 +5834,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>319</v>
       </c>
@@ -5967,7 +6000,10 @@
         <v>46018</v>
       </c>
       <c r="C333" t="s">
-        <v>8</v>
+        <v>478</v>
+      </c>
+      <c r="F333" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
DIES FINAL. TOT ESCRIT
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAB29B2-F878-4314-9B59-3F67B8A80B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE880A1-92B1-4CDE-BBA1-D0C00F945557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="520">
   <si>
     <t>Dia</t>
   </si>
@@ -51,9 +51,6 @@
     <t>./img/lola_flores.jpg</t>
   </si>
   <si>
-    <t>Hola</t>
-  </si>
-  <si>
     <t>Aquesta foto és de quan portàvem 6 mesos. Pero segur que el somirure no l'has perdut</t>
   </si>
   <si>
@@ -1480,6 +1477,114 @@
   </si>
   <si>
     <t>Perquè quan estàs malalta (quasi mai) deixes que et cuidi</t>
+  </si>
+  <si>
+    <t>Perquè et mous a dormir (algun cop) a la meva habitació quan hi ha colònies infants!</t>
+  </si>
+  <si>
+    <t>Perquè ajudes a tothom de la teva família sempre que pots</t>
+  </si>
+  <si>
+    <t>Perquè sempre em preguntes "un iogurt?" quan arribem tard a casa</t>
+  </si>
+  <si>
+    <t>Perquè fas stickers de mi SUPER EXTRA xulos</t>
+  </si>
+  <si>
+    <t>Perquè m'acompanyes a fer plans MOOOLT guais amb els meus amics (per exemple veure l'Edgar i la Judit participar a soc i sere)</t>
+  </si>
+  <si>
+    <t>Perquè quan et faig el dinar dius que esta molt bo encara que sempre siguin raviolis de formatge</t>
+  </si>
+  <si>
+    <t>Perquè em recordes els aniversaris de la gent que he de felicitar</t>
+  </si>
+  <si>
+    <t>Perquè aguantes les meves bromes de "personatges" que et venen a veure. El meu preferit és el MAGÇAL</t>
+  </si>
+  <si>
+    <t>Perquè proves el menjar que fa la meva germana (NORMALMENT MOOOLT DOLENT) i fas veure que esta bo</t>
+  </si>
+  <si>
+    <t>Perquè m'acompanyes a fer plans XULISSIMS encara que només m'agradin a mi (BUNQUEER)</t>
+  </si>
+  <si>
+    <t>Perquè escoltes els audios super guais que et faig de tant en tant explican-te com em va el dia</t>
+  </si>
+  <si>
+    <t>Perquè m'expliques anècdotes molt divertides que et passen a les pràctiques de la universitat</t>
+  </si>
+  <si>
+    <t>Perquè em fas regals NINJAS però moolt guais (em vas regalar anar a fer un sushi amb tu a Altafulla pel meu cumple. Quan escric això: 19/05/2025 encara NO ho hem fet. Espero que quan llegeixis això sii jijiji)</t>
+  </si>
+  <si>
+    <t>Perquè quan em convides a dinar a casa teva el teu pare fa UN ARROS MOOOOLT BO</t>
+  </si>
+  <si>
+    <t>Perquè em dius que em talli el cavell SEMPRE encara que just me'l acabi de tallar</t>
+  </si>
+  <si>
+    <t>Perquè m'encanta que (ara que ja portem més de dos anys coneixent-nos) poguem fer plans en dies especials PER SEGON COP</t>
+  </si>
+  <si>
+    <t>Perquè SEMPRE estaves preguntant-me si seguiria al taller o no!</t>
+  </si>
+  <si>
+    <t>Perquè quan estem els dos junts ens ho passem MOOOLT be</t>
+  </si>
+  <si>
+    <t>Perquè sempre intentes buscar un temps per mi encara que estiguem MOOLT ocupats</t>
+  </si>
+  <si>
+    <t>Perquè tens una figureta meva de Lego sempre aprop teu a l'habitació</t>
+  </si>
+  <si>
+    <t>Perquè em vas regalar un braçelet verd per remplaçar el que se'm va trencar (que l'havies fet tuuu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè t'adones de les actualtizacions MEGA GUAIS que faig a la web </t>
+  </si>
+  <si>
+    <t>Perquè et vas copiar de la app de la meva agenda MEGA XULA</t>
+  </si>
+  <si>
+    <t>Perquè cada dia (o casi cada dia) tens un moment per llegir-te el missatge diari</t>
+  </si>
+  <si>
+    <t>Perquè dediques el teu temps en fer regals macos per mi (el mes guai) i els altres</t>
+  </si>
+  <si>
+    <t>Perquè em passes algunes fotos de la puça</t>
+  </si>
+  <si>
+    <t>Perquè aguantes que li digui MONSTRE a la puça (no és un monstres però es porta BASTANT malament)</t>
+  </si>
+  <si>
+    <t>Perquè et preocupes per les meves mans quan estan tallades</t>
+  </si>
+  <si>
+    <t>Perquè ets LA MARGARITA més guapa del món (a colònies monis ho vas demostrar)</t>
+  </si>
+  <si>
+    <t>Perquè em robes TOTS els mitjons que tinc</t>
+  </si>
+  <si>
+    <t>Perquè et preocupes perquè no tingui molta alèrgia quan vinc a casa teva</t>
+  </si>
+  <si>
+    <t>Perquè em preguntes sobre com em va la carrera</t>
+  </si>
+  <si>
+    <t>Perquè t'has convertit en 2 anys en una persona molt important per mi</t>
+  </si>
+  <si>
+    <t>Perquè SEMPRE vols que anem a menjar sushi</t>
+  </si>
+  <si>
+    <t>Perquè ets una gran massatgista i vam comprar uns oli de massatges a Altafulla perquè ho poguessis demostrar</t>
+  </si>
+  <si>
+    <t>Perquè sempre estàs molt atenta a mi i al que necessito. PREPARA'T QUE DEMÀ ES L'ÚLTIM DIA DE LA WEB. Tot i això, et seguirè estimant sempre.</t>
   </si>
 </sst>
 </file>
@@ -1860,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C313" sqref="C313"/>
+    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1901,16 +2006,16 @@
         <v>45687</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1921,7 +2026,7 @@
         <v>45688</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -1935,7 +2040,7 @@
         <v>45689</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1947,7 +2052,7 @@
         <v>45690</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1958,7 +2063,7 @@
         <v>45691</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1969,7 +2074,7 @@
         <v>45692</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1980,13 +2085,13 @@
         <v>45693</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
         <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
@@ -1999,7 +2104,7 @@
         <v>45694</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -2011,7 +2116,7 @@
         <v>45695</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -2023,7 +2128,7 @@
         <v>45696</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -2035,13 +2140,13 @@
         <v>45697</v>
       </c>
       <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
         <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2052,7 +2157,7 @@
         <v>45698</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2063,7 +2168,7 @@
         <v>45699</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2076,7 +2181,7 @@
         <v>45700</v>
       </c>
       <c r="C15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2087,7 +2192,7 @@
         <v>45701</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -2099,13 +2204,13 @@
         <v>45702</v>
       </c>
       <c r="C17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" t="s">
         <v>134</v>
       </c>
-      <c r="D17" t="s">
-        <v>135</v>
-      </c>
       <c r="E17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2116,7 +2221,7 @@
         <v>45703</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2127,13 +2232,13 @@
         <v>45704</v>
       </c>
       <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
         <v>22</v>
       </c>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -2145,7 +2250,7 @@
         <v>45705</v>
       </c>
       <c r="C20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2156,7 +2261,7 @@
         <v>45706</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="2"/>
     </row>
@@ -2168,7 +2273,7 @@
         <v>45707</v>
       </c>
       <c r="C22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2179,13 +2284,13 @@
         <v>45708</v>
       </c>
       <c r="C23" t="s">
+        <v>276</v>
+      </c>
+      <c r="D23" t="s">
         <v>277</v>
       </c>
-      <c r="D23" t="s">
-        <v>278</v>
-      </c>
       <c r="E23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2196,7 +2301,7 @@
         <v>45709</v>
       </c>
       <c r="C24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2207,10 +2312,10 @@
         <v>45710</v>
       </c>
       <c r="C25" t="s">
+        <v>338</v>
+      </c>
+      <c r="F25" t="s">
         <v>339</v>
-      </c>
-      <c r="F25" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2221,7 +2326,7 @@
         <v>45711</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -2232,7 +2337,7 @@
         <v>45712</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2243,10 +2348,10 @@
         <v>45713</v>
       </c>
       <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
         <v>31</v>
-      </c>
-      <c r="F28" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2257,7 +2362,7 @@
         <v>45714</v>
       </c>
       <c r="C29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2268,7 +2373,7 @@
         <v>45715</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2279,7 +2384,7 @@
         <v>45716</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2290,7 +2395,7 @@
         <v>45717</v>
       </c>
       <c r="C32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2301,13 +2406,13 @@
         <v>45718</v>
       </c>
       <c r="C33" t="s">
+        <v>281</v>
+      </c>
+      <c r="D33" t="s">
+        <v>278</v>
+      </c>
+      <c r="E33" t="s">
         <v>282</v>
-      </c>
-      <c r="D33" t="s">
-        <v>279</v>
-      </c>
-      <c r="E33" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -2318,7 +2423,7 @@
         <v>45719</v>
       </c>
       <c r="C34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2329,7 +2434,7 @@
         <v>45720</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2340,13 +2445,13 @@
         <v>45721</v>
       </c>
       <c r="C36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D36" t="s">
+        <v>173</v>
+      </c>
+      <c r="E36" t="s">
         <v>174</v>
-      </c>
-      <c r="E36" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2357,7 +2462,7 @@
         <v>45722</v>
       </c>
       <c r="C37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2368,7 +2473,7 @@
         <v>45723</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2379,7 +2484,7 @@
         <v>45724</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2390,13 +2495,13 @@
         <v>45725</v>
       </c>
       <c r="C40" t="s">
+        <v>283</v>
+      </c>
+      <c r="D40" t="s">
+        <v>279</v>
+      </c>
+      <c r="E40" t="s">
         <v>284</v>
-      </c>
-      <c r="D40" t="s">
-        <v>280</v>
-      </c>
-      <c r="E40" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2407,7 +2512,7 @@
         <v>45726</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2418,7 +2523,7 @@
         <v>45727</v>
       </c>
       <c r="C42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2429,13 +2534,13 @@
         <v>45728</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" t="s">
         <v>138</v>
-      </c>
-      <c r="E43" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2446,7 +2551,7 @@
         <v>45729</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2457,10 +2562,10 @@
         <v>45730</v>
       </c>
       <c r="C45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2471,7 +2576,7 @@
         <v>45731</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2482,7 +2587,7 @@
         <v>45732</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2493,13 +2598,13 @@
         <v>45733</v>
       </c>
       <c r="C48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D48" t="s">
+        <v>286</v>
+      </c>
+      <c r="E48" t="s">
         <v>287</v>
-      </c>
-      <c r="E48" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2510,7 +2615,7 @@
         <v>45734</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2521,7 +2626,7 @@
         <v>45735</v>
       </c>
       <c r="C50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2532,7 +2637,7 @@
         <v>45736</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2543,7 +2648,7 @@
         <v>45737</v>
       </c>
       <c r="C52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2554,7 +2659,7 @@
         <v>45738</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2565,13 +2670,13 @@
         <v>45739</v>
       </c>
       <c r="C54" t="s">
+        <v>289</v>
+      </c>
+      <c r="D54" t="s">
         <v>290</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>291</v>
-      </c>
-      <c r="E54" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2582,7 +2687,7 @@
         <v>45740</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2593,7 +2698,7 @@
         <v>45741</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2604,7 +2709,7 @@
         <v>45742</v>
       </c>
       <c r="C57" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2615,13 +2720,13 @@
         <v>45743</v>
       </c>
       <c r="C58" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" t="s">
         <v>69</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>70</v>
-      </c>
-      <c r="E58" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2632,10 +2737,10 @@
         <v>45744</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F59" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2646,7 +2751,7 @@
         <v>45745</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2657,7 +2762,7 @@
         <v>45746</v>
       </c>
       <c r="C61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2668,10 +2773,10 @@
         <v>45747</v>
       </c>
       <c r="C62" t="s">
+        <v>320</v>
+      </c>
+      <c r="F62" t="s">
         <v>321</v>
-      </c>
-      <c r="F62" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2682,7 +2787,7 @@
         <v>45748</v>
       </c>
       <c r="C63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2693,7 +2798,7 @@
         <v>45749</v>
       </c>
       <c r="C64" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2704,10 +2809,10 @@
         <v>45750</v>
       </c>
       <c r="C65" t="s">
+        <v>84</v>
+      </c>
+      <c r="F65" t="s">
         <v>85</v>
-      </c>
-      <c r="F65" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2718,7 +2823,7 @@
         <v>45751</v>
       </c>
       <c r="C66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2729,7 +2834,7 @@
         <v>45752</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2740,13 +2845,13 @@
         <v>45753</v>
       </c>
       <c r="C68" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E68" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2757,7 +2862,7 @@
         <v>45754</v>
       </c>
       <c r="C69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2768,7 +2873,7 @@
         <v>45755</v>
       </c>
       <c r="C70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2779,13 +2884,13 @@
         <v>45756</v>
       </c>
       <c r="C71" t="s">
+        <v>91</v>
+      </c>
+      <c r="D71" t="s">
         <v>92</v>
       </c>
-      <c r="D71" t="s">
-        <v>93</v>
-      </c>
       <c r="E71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2796,7 +2901,7 @@
         <v>45757</v>
       </c>
       <c r="C72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2807,7 +2912,7 @@
         <v>45758</v>
       </c>
       <c r="C73" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2818,7 +2923,7 @@
         <v>45759</v>
       </c>
       <c r="C74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2829,10 +2934,10 @@
         <v>45760</v>
       </c>
       <c r="C75" t="s">
+        <v>322</v>
+      </c>
+      <c r="F75" t="s">
         <v>323</v>
-      </c>
-      <c r="F75" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2843,7 +2948,7 @@
         <v>45761</v>
       </c>
       <c r="C76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2854,13 +2959,13 @@
         <v>45762</v>
       </c>
       <c r="C77" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D77" t="s">
+        <v>293</v>
+      </c>
+      <c r="E77" t="s">
         <v>294</v>
-      </c>
-      <c r="E77" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2871,7 +2976,7 @@
         <v>45763</v>
       </c>
       <c r="C78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2882,7 +2987,7 @@
         <v>45764</v>
       </c>
       <c r="C79" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2893,10 +2998,10 @@
         <v>45765</v>
       </c>
       <c r="C80" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F80" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2907,7 +3012,7 @@
         <v>45766</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2918,7 +3023,7 @@
         <v>45767</v>
       </c>
       <c r="C82" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2929,13 +3034,13 @@
         <v>45768</v>
       </c>
       <c r="C83" t="s">
+        <v>471</v>
+      </c>
+      <c r="D83" t="s">
         <v>472</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>473</v>
-      </c>
-      <c r="E83" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2946,7 +3051,7 @@
         <v>45769</v>
       </c>
       <c r="C84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2957,13 +3062,13 @@
         <v>45770</v>
       </c>
       <c r="C85" t="s">
+        <v>106</v>
+      </c>
+      <c r="D85" t="s">
         <v>107</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>108</v>
-      </c>
-      <c r="E85" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2974,7 +3079,7 @@
         <v>45771</v>
       </c>
       <c r="C86" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2985,7 +3090,7 @@
         <v>45772</v>
       </c>
       <c r="C87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2996,7 +3101,7 @@
         <v>45773</v>
       </c>
       <c r="C88" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -3007,7 +3112,7 @@
         <v>45774</v>
       </c>
       <c r="C89" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -3018,10 +3123,10 @@
         <v>45775</v>
       </c>
       <c r="C90" t="s">
+        <v>341</v>
+      </c>
+      <c r="F90" t="s">
         <v>342</v>
-      </c>
-      <c r="F90" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -3032,7 +3137,7 @@
         <v>45776</v>
       </c>
       <c r="C91" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -3043,7 +3148,7 @@
         <v>45777</v>
       </c>
       <c r="C92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -3054,7 +3159,7 @@
         <v>45778</v>
       </c>
       <c r="C93" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -3065,10 +3170,10 @@
         <v>45779</v>
       </c>
       <c r="C94" t="s">
+        <v>114</v>
+      </c>
+      <c r="F94" t="s">
         <v>115</v>
-      </c>
-      <c r="F94" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -3079,13 +3184,13 @@
         <v>45780</v>
       </c>
       <c r="C95" t="s">
+        <v>45</v>
+      </c>
+      <c r="D95" t="s">
         <v>46</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>47</v>
-      </c>
-      <c r="E95" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -3096,7 +3201,7 @@
         <v>45781</v>
       </c>
       <c r="C96" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -3107,7 +3212,7 @@
         <v>45782</v>
       </c>
       <c r="C97" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -3118,10 +3223,10 @@
         <v>45783</v>
       </c>
       <c r="C98" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D98" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -3132,7 +3237,7 @@
         <v>45784</v>
       </c>
       <c r="C99" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3143,10 +3248,10 @@
         <v>45785</v>
       </c>
       <c r="C100" t="s">
+        <v>359</v>
+      </c>
+      <c r="F100" t="s">
         <v>360</v>
-      </c>
-      <c r="F100" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3157,7 +3262,7 @@
         <v>45786</v>
       </c>
       <c r="C101" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3168,7 +3273,7 @@
         <v>45787</v>
       </c>
       <c r="C102" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3179,13 +3284,13 @@
         <v>45788</v>
       </c>
       <c r="C103" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D103" t="s">
+        <v>297</v>
+      </c>
+      <c r="E103" t="s">
         <v>298</v>
-      </c>
-      <c r="E103" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3196,7 +3301,7 @@
         <v>45789</v>
       </c>
       <c r="C104" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3207,7 +3312,7 @@
         <v>45790</v>
       </c>
       <c r="C105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3218,7 +3323,7 @@
         <v>45791</v>
       </c>
       <c r="C106" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3229,10 +3334,10 @@
         <v>45792</v>
       </c>
       <c r="C107" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D107" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3243,7 +3348,7 @@
         <v>45793</v>
       </c>
       <c r="C108" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3254,7 +3359,7 @@
         <v>45794</v>
       </c>
       <c r="C109" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3265,7 +3370,7 @@
         <v>45795</v>
       </c>
       <c r="C110" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3276,10 +3381,10 @@
         <v>45796</v>
       </c>
       <c r="C111" t="s">
+        <v>159</v>
+      </c>
+      <c r="F111" t="s">
         <v>160</v>
-      </c>
-      <c r="F111" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3290,7 +3395,7 @@
         <v>45797</v>
       </c>
       <c r="C112" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3301,10 +3406,10 @@
         <v>45798</v>
       </c>
       <c r="C113" t="s">
+        <v>162</v>
+      </c>
+      <c r="D113" t="s">
         <v>163</v>
-      </c>
-      <c r="D113" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3315,7 +3420,7 @@
         <v>45799</v>
       </c>
       <c r="C114" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3326,7 +3431,7 @@
         <v>45800</v>
       </c>
       <c r="C115" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3337,7 +3442,7 @@
         <v>45801</v>
       </c>
       <c r="C116" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3348,7 +3453,7 @@
         <v>45802</v>
       </c>
       <c r="C117" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3359,7 +3464,7 @@
         <v>45803</v>
       </c>
       <c r="C118" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3370,7 +3475,7 @@
         <v>45804</v>
       </c>
       <c r="C119" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3381,13 +3486,13 @@
         <v>45805</v>
       </c>
       <c r="C120" t="s">
+        <v>273</v>
+      </c>
+      <c r="D120" t="s">
         <v>274</v>
       </c>
-      <c r="D120" t="s">
+      <c r="E120" t="s">
         <v>275</v>
-      </c>
-      <c r="E120" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3398,7 +3503,7 @@
         <v>45806</v>
       </c>
       <c r="C121" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3409,7 +3514,7 @@
         <v>45807</v>
       </c>
       <c r="C122" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3420,10 +3525,10 @@
         <v>45808</v>
       </c>
       <c r="C123" t="s">
+        <v>175</v>
+      </c>
+      <c r="F123" t="s">
         <v>176</v>
-      </c>
-      <c r="F123" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3434,7 +3539,7 @@
         <v>45809</v>
       </c>
       <c r="C124" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3445,7 +3550,7 @@
         <v>45810</v>
       </c>
       <c r="C125" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3456,7 +3561,7 @@
         <v>45811</v>
       </c>
       <c r="C126" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3467,7 +3572,7 @@
         <v>45812</v>
       </c>
       <c r="C127" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3478,13 +3583,13 @@
         <v>45813</v>
       </c>
       <c r="C128" t="s">
+        <v>177</v>
+      </c>
+      <c r="D128" t="s">
         <v>178</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" t="s">
         <v>179</v>
-      </c>
-      <c r="E128" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3495,7 +3600,7 @@
         <v>45814</v>
       </c>
       <c r="C129" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3506,13 +3611,13 @@
         <v>45815</v>
       </c>
       <c r="C130" t="s">
+        <v>181</v>
+      </c>
+      <c r="D130" t="s">
         <v>182</v>
       </c>
-      <c r="D130" t="s">
+      <c r="E130" t="s">
         <v>183</v>
-      </c>
-      <c r="E130" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3523,7 +3628,7 @@
         <v>45816</v>
       </c>
       <c r="C131" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3534,7 +3639,7 @@
         <v>45817</v>
       </c>
       <c r="C132" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3545,7 +3650,7 @@
         <v>45818</v>
       </c>
       <c r="C133" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3556,7 +3661,7 @@
         <v>45819</v>
       </c>
       <c r="C134" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3567,7 +3672,7 @@
         <v>45820</v>
       </c>
       <c r="C135" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3578,7 +3683,7 @@
         <v>45821</v>
       </c>
       <c r="C136" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3589,13 +3694,13 @@
         <v>45822</v>
       </c>
       <c r="C137" t="s">
+        <v>204</v>
+      </c>
+      <c r="D137" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D137" s="2" t="s">
+      <c r="E137" t="s">
         <v>206</v>
-      </c>
-      <c r="E137" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3606,13 +3711,13 @@
         <v>45823</v>
       </c>
       <c r="C138" t="s">
+        <v>184</v>
+      </c>
+      <c r="D138" t="s">
         <v>185</v>
       </c>
-      <c r="D138" t="s">
+      <c r="E138" t="s">
         <v>186</v>
-      </c>
-      <c r="E138" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3623,7 +3728,7 @@
         <v>45824</v>
       </c>
       <c r="C139" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3634,7 +3739,7 @@
         <v>45825</v>
       </c>
       <c r="C140" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3645,7 +3750,7 @@
         <v>45826</v>
       </c>
       <c r="C141" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3656,10 +3761,10 @@
         <v>45827</v>
       </c>
       <c r="C142" t="s">
+        <v>324</v>
+      </c>
+      <c r="F142" t="s">
         <v>325</v>
-      </c>
-      <c r="F142" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3670,7 +3775,7 @@
         <v>45828</v>
       </c>
       <c r="C143" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3681,7 +3786,7 @@
         <v>45829</v>
       </c>
       <c r="C144" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
@@ -3692,7 +3797,7 @@
         <v>45830</v>
       </c>
       <c r="C145" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -3703,13 +3808,13 @@
         <v>45831</v>
       </c>
       <c r="C146" t="s">
+        <v>214</v>
+      </c>
+      <c r="D146" t="s">
         <v>215</v>
       </c>
-      <c r="D146" t="s">
+      <c r="E146" t="s">
         <v>216</v>
-      </c>
-      <c r="E146" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
@@ -3720,7 +3825,7 @@
         <v>45832</v>
       </c>
       <c r="C147" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -3731,10 +3836,10 @@
         <v>45833</v>
       </c>
       <c r="C148" t="s">
+        <v>218</v>
+      </c>
+      <c r="D148" t="s">
         <v>219</v>
-      </c>
-      <c r="D148" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
@@ -3745,7 +3850,7 @@
         <v>45834</v>
       </c>
       <c r="C149" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
@@ -3756,7 +3861,7 @@
         <v>45835</v>
       </c>
       <c r="C150" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
@@ -3767,7 +3872,7 @@
         <v>45836</v>
       </c>
       <c r="C151" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
@@ -3778,13 +3883,13 @@
         <v>45837</v>
       </c>
       <c r="C152" t="s">
+        <v>372</v>
+      </c>
+      <c r="D152" t="s">
         <v>373</v>
       </c>
-      <c r="D152" t="s">
+      <c r="E152" t="s">
         <v>374</v>
-      </c>
-      <c r="E152" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
@@ -3795,7 +3900,7 @@
         <v>45838</v>
       </c>
       <c r="C153" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
@@ -3806,7 +3911,7 @@
         <v>45839</v>
       </c>
       <c r="C154" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
@@ -3817,10 +3922,10 @@
         <v>45840</v>
       </c>
       <c r="C155" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F155" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
@@ -3831,7 +3936,7 @@
         <v>45841</v>
       </c>
       <c r="C156" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
@@ -3842,10 +3947,10 @@
         <v>45842</v>
       </c>
       <c r="C157" t="s">
+        <v>228</v>
+      </c>
+      <c r="F157" t="s">
         <v>229</v>
-      </c>
-      <c r="F157" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
@@ -3856,13 +3961,13 @@
         <v>45843</v>
       </c>
       <c r="C158" t="s">
+        <v>240</v>
+      </c>
+      <c r="D158" t="s">
         <v>241</v>
       </c>
-      <c r="D158" t="s">
+      <c r="E158" t="s">
         <v>242</v>
-      </c>
-      <c r="E158" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
@@ -3873,19 +3978,19 @@
         <v>45844</v>
       </c>
       <c r="C159" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E159" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F159" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G159" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H159" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
@@ -3896,7 +4001,7 @@
         <v>45845</v>
       </c>
       <c r="C160" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -3907,7 +4012,7 @@
         <v>45846</v>
       </c>
       <c r="C161" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
@@ -3918,7 +4023,7 @@
         <v>45847</v>
       </c>
       <c r="C162" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -3929,7 +4034,7 @@
         <v>45848</v>
       </c>
       <c r="C163" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
@@ -3940,7 +4045,7 @@
         <v>45849</v>
       </c>
       <c r="C164" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
@@ -3951,13 +4056,13 @@
         <v>45850</v>
       </c>
       <c r="C165" t="s">
+        <v>187</v>
+      </c>
+      <c r="D165" t="s">
         <v>188</v>
       </c>
-      <c r="D165" t="s">
+      <c r="E165" t="s">
         <v>189</v>
-      </c>
-      <c r="E165" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
@@ -3968,7 +4073,7 @@
         <v>45851</v>
       </c>
       <c r="C166" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
@@ -3979,13 +4084,13 @@
         <v>45852</v>
       </c>
       <c r="C167" t="s">
+        <v>249</v>
+      </c>
+      <c r="D167" t="s">
         <v>250</v>
       </c>
-      <c r="D167" t="s">
+      <c r="E167" t="s">
         <v>251</v>
-      </c>
-      <c r="E167" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
@@ -3996,7 +4101,7 @@
         <v>45853</v>
       </c>
       <c r="C168" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
@@ -4007,7 +4112,7 @@
         <v>45854</v>
       </c>
       <c r="C169" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
@@ -4018,7 +4123,7 @@
         <v>45855</v>
       </c>
       <c r="C170" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
@@ -4029,10 +4134,10 @@
         <v>45856</v>
       </c>
       <c r="C171" t="s">
+        <v>230</v>
+      </c>
+      <c r="F171" t="s">
         <v>231</v>
-      </c>
-      <c r="F171" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
@@ -4043,7 +4148,7 @@
         <v>45857</v>
       </c>
       <c r="C172" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
@@ -4054,7 +4159,7 @@
         <v>45858</v>
       </c>
       <c r="C173" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
@@ -4065,13 +4170,13 @@
         <v>45859</v>
       </c>
       <c r="C174" t="s">
+        <v>260</v>
+      </c>
+      <c r="D174" t="s">
         <v>261</v>
       </c>
-      <c r="D174" t="s">
+      <c r="E174" t="s">
         <v>262</v>
-      </c>
-      <c r="E174" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
@@ -4082,7 +4187,7 @@
         <v>45860</v>
       </c>
       <c r="C175" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
@@ -4093,7 +4198,7 @@
         <v>45861</v>
       </c>
       <c r="C176" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
@@ -4104,7 +4209,7 @@
         <v>45862</v>
       </c>
       <c r="C177" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
@@ -4115,7 +4220,7 @@
         <v>45863</v>
       </c>
       <c r="C178" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
@@ -4126,7 +4231,7 @@
         <v>45864</v>
       </c>
       <c r="C179" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
@@ -4137,13 +4242,13 @@
         <v>45865</v>
       </c>
       <c r="C180" t="s">
+        <v>270</v>
+      </c>
+      <c r="D180" t="s">
         <v>271</v>
       </c>
-      <c r="D180" t="s">
+      <c r="E180" t="s">
         <v>272</v>
-      </c>
-      <c r="E180" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
@@ -4154,7 +4259,7 @@
         <v>45866</v>
       </c>
       <c r="C181" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
@@ -4165,7 +4270,7 @@
         <v>45867</v>
       </c>
       <c r="C182" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
@@ -4176,7 +4281,7 @@
         <v>45868</v>
       </c>
       <c r="C183" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
@@ -4187,7 +4292,7 @@
         <v>45869</v>
       </c>
       <c r="C184" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
@@ -4198,7 +4303,7 @@
         <v>45870</v>
       </c>
       <c r="C185" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
@@ -4209,13 +4314,13 @@
         <v>45871</v>
       </c>
       <c r="C186" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D186" t="s">
+        <v>295</v>
+      </c>
+      <c r="E186" t="s">
         <v>296</v>
-      </c>
-      <c r="E186" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
@@ -4226,7 +4331,7 @@
         <v>45872</v>
       </c>
       <c r="C187" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
@@ -4237,7 +4342,7 @@
         <v>45873</v>
       </c>
       <c r="C188" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
@@ -4248,7 +4353,7 @@
         <v>45874</v>
       </c>
       <c r="C189" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
@@ -4259,10 +4364,10 @@
         <v>45875</v>
       </c>
       <c r="C190" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
@@ -4273,7 +4378,7 @@
         <v>45876</v>
       </c>
       <c r="C191" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
@@ -4284,7 +4389,7 @@
         <v>45877</v>
       </c>
       <c r="C192" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
@@ -4295,7 +4400,7 @@
         <v>45878</v>
       </c>
       <c r="C193" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
@@ -4306,13 +4411,13 @@
         <v>45879</v>
       </c>
       <c r="C194" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D194" t="s">
+        <v>299</v>
+      </c>
+      <c r="E194" t="s">
         <v>300</v>
-      </c>
-      <c r="E194" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
@@ -4323,7 +4428,7 @@
         <v>45880</v>
       </c>
       <c r="C195" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
@@ -4334,13 +4439,13 @@
         <v>45881</v>
       </c>
       <c r="C196" t="s">
+        <v>190</v>
+      </c>
+      <c r="D196" t="s">
         <v>191</v>
       </c>
-      <c r="D196" t="s">
+      <c r="E196" t="s">
         <v>192</v>
-      </c>
-      <c r="E196" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
@@ -4351,7 +4456,7 @@
         <v>45882</v>
       </c>
       <c r="C197" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
@@ -4362,7 +4467,7 @@
         <v>45883</v>
       </c>
       <c r="C198" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
@@ -4373,10 +4478,10 @@
         <v>45884</v>
       </c>
       <c r="C199" t="s">
+        <v>317</v>
+      </c>
+      <c r="F199" t="s">
         <v>318</v>
-      </c>
-      <c r="F199" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
@@ -4387,7 +4492,7 @@
         <v>45885</v>
       </c>
       <c r="C200" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
@@ -4398,7 +4503,7 @@
         <v>45886</v>
       </c>
       <c r="C201" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
@@ -4409,7 +4514,7 @@
         <v>45887</v>
       </c>
       <c r="C202" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
@@ -4420,7 +4525,7 @@
         <v>45888</v>
       </c>
       <c r="C203" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
@@ -4431,13 +4536,13 @@
         <v>45889</v>
       </c>
       <c r="C204" t="s">
+        <v>263</v>
+      </c>
+      <c r="D204" t="s">
         <v>264</v>
       </c>
-      <c r="D204" t="s">
+      <c r="E204" t="s">
         <v>265</v>
-      </c>
-      <c r="E204" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
@@ -4448,7 +4553,7 @@
         <v>45890</v>
       </c>
       <c r="C205" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
@@ -4459,7 +4564,7 @@
         <v>45891</v>
       </c>
       <c r="C206" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
@@ -4470,10 +4575,10 @@
         <v>45892</v>
       </c>
       <c r="C207" t="s">
+        <v>345</v>
+      </c>
+      <c r="F207" t="s">
         <v>346</v>
-      </c>
-      <c r="F207" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
@@ -4484,7 +4589,7 @@
         <v>45893</v>
       </c>
       <c r="C208" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
@@ -4495,7 +4600,7 @@
         <v>45894</v>
       </c>
       <c r="C209" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
@@ -4506,7 +4611,7 @@
         <v>45895</v>
       </c>
       <c r="C210" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
@@ -4517,7 +4622,7 @@
         <v>45896</v>
       </c>
       <c r="C211" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
@@ -4528,13 +4633,13 @@
         <v>45897</v>
       </c>
       <c r="C212" t="s">
+        <v>350</v>
+      </c>
+      <c r="D212" t="s">
         <v>351</v>
       </c>
-      <c r="D212" t="s">
+      <c r="E212" t="s">
         <v>352</v>
-      </c>
-      <c r="E212" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
@@ -4545,7 +4650,7 @@
         <v>45898</v>
       </c>
       <c r="C213" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.3">
@@ -4556,7 +4661,7 @@
         <v>45899</v>
       </c>
       <c r="C214" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
@@ -4567,7 +4672,7 @@
         <v>45900</v>
       </c>
       <c r="C215" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
@@ -4578,7 +4683,7 @@
         <v>45901</v>
       </c>
       <c r="C216" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
@@ -4589,7 +4694,7 @@
         <v>45902</v>
       </c>
       <c r="C217" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
@@ -4600,7 +4705,7 @@
         <v>45903</v>
       </c>
       <c r="C218" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
@@ -4611,10 +4716,10 @@
         <v>45904</v>
       </c>
       <c r="C219" t="s">
+        <v>356</v>
+      </c>
+      <c r="F219" t="s">
         <v>357</v>
-      </c>
-      <c r="F219" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.3">
@@ -4625,7 +4730,7 @@
         <v>45905</v>
       </c>
       <c r="C220" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
@@ -4636,7 +4741,7 @@
         <v>45906</v>
       </c>
       <c r="C221" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.3">
@@ -4647,7 +4752,7 @@
         <v>45907</v>
       </c>
       <c r="C222" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
@@ -4658,13 +4763,13 @@
         <v>45908</v>
       </c>
       <c r="C223" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D223" t="s">
+        <v>301</v>
+      </c>
+      <c r="E223" t="s">
         <v>302</v>
-      </c>
-      <c r="E223" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.3">
@@ -4675,7 +4780,7 @@
         <v>45909</v>
       </c>
       <c r="C224" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -4686,7 +4791,7 @@
         <v>45910</v>
       </c>
       <c r="C225" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
@@ -4697,7 +4802,7 @@
         <v>45911</v>
       </c>
       <c r="C226" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
@@ -4708,7 +4813,7 @@
         <v>45912</v>
       </c>
       <c r="C227" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
@@ -4719,13 +4824,13 @@
         <v>45913</v>
       </c>
       <c r="C228" t="s">
+        <v>193</v>
+      </c>
+      <c r="D228" t="s">
         <v>194</v>
       </c>
-      <c r="D228" t="s">
+      <c r="E228" t="s">
         <v>195</v>
-      </c>
-      <c r="E228" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
@@ -4736,7 +4841,7 @@
         <v>45914</v>
       </c>
       <c r="C229" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
@@ -4747,7 +4852,7 @@
         <v>45915</v>
       </c>
       <c r="C230" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
@@ -4758,7 +4863,7 @@
         <v>45916</v>
       </c>
       <c r="C231" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
@@ -4769,13 +4874,13 @@
         <v>45917</v>
       </c>
       <c r="C232" t="s">
+        <v>426</v>
+      </c>
+      <c r="D232" t="s">
         <v>427</v>
       </c>
-      <c r="D232" t="s">
+      <c r="E232" t="s">
         <v>428</v>
-      </c>
-      <c r="E232" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
@@ -4786,7 +4891,7 @@
         <v>45918</v>
       </c>
       <c r="C233" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
@@ -4797,7 +4902,7 @@
         <v>45919</v>
       </c>
       <c r="C234" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.3">
@@ -4808,10 +4913,10 @@
         <v>45920</v>
       </c>
       <c r="C235" t="s">
+        <v>234</v>
+      </c>
+      <c r="F235" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="F235" s="5" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.3">
@@ -4822,7 +4927,7 @@
         <v>45921</v>
       </c>
       <c r="C236" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.3">
@@ -4833,7 +4938,7 @@
         <v>45922</v>
       </c>
       <c r="C237" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
@@ -4844,13 +4949,13 @@
         <v>45923</v>
       </c>
       <c r="C238" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D238" t="s">
+        <v>362</v>
+      </c>
+      <c r="E238" t="s">
         <v>363</v>
-      </c>
-      <c r="E238" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
@@ -4861,7 +4966,7 @@
         <v>45924</v>
       </c>
       <c r="C239" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
@@ -4872,7 +4977,7 @@
         <v>45925</v>
       </c>
       <c r="C240" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.3">
@@ -4883,7 +4988,7 @@
         <v>45926</v>
       </c>
       <c r="C241" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.3">
@@ -4894,7 +4999,7 @@
         <v>45927</v>
       </c>
       <c r="C242" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.3">
@@ -4905,7 +5010,7 @@
         <v>45928</v>
       </c>
       <c r="C243" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.3">
@@ -4916,13 +5021,13 @@
         <v>45929</v>
       </c>
       <c r="C244" t="s">
+        <v>413</v>
+      </c>
+      <c r="D244" t="s">
         <v>414</v>
       </c>
-      <c r="D244" t="s">
+      <c r="E244" t="s">
         <v>415</v>
-      </c>
-      <c r="E244" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
@@ -4933,7 +5038,7 @@
         <v>45930</v>
       </c>
       <c r="C245" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.3">
@@ -4944,7 +5049,7 @@
         <v>45931</v>
       </c>
       <c r="C246" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.3">
@@ -4955,7 +5060,7 @@
         <v>45932</v>
       </c>
       <c r="C247" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.3">
@@ -4966,7 +5071,7 @@
         <v>45933</v>
       </c>
       <c r="C248" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.3">
@@ -4977,7 +5082,7 @@
         <v>45934</v>
       </c>
       <c r="C249" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.3">
@@ -4988,13 +5093,13 @@
         <v>45935</v>
       </c>
       <c r="C250" t="s">
+        <v>381</v>
+      </c>
+      <c r="D250" t="s">
+        <v>303</v>
+      </c>
+      <c r="E250" t="s">
         <v>382</v>
-      </c>
-      <c r="D250" t="s">
-        <v>304</v>
-      </c>
-      <c r="E250" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.3">
@@ -5005,7 +5110,7 @@
         <v>45936</v>
       </c>
       <c r="C251" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.3">
@@ -5016,7 +5121,7 @@
         <v>45937</v>
       </c>
       <c r="C252" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.3">
@@ -5027,7 +5132,7 @@
         <v>45938</v>
       </c>
       <c r="C253" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.3">
@@ -5038,10 +5143,10 @@
         <v>45939</v>
       </c>
       <c r="C254" t="s">
+        <v>236</v>
+      </c>
+      <c r="F254" s="5" t="s">
         <v>237</v>
-      </c>
-      <c r="F254" s="5" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
@@ -5052,7 +5157,7 @@
         <v>45940</v>
       </c>
       <c r="C255" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
@@ -5063,13 +5168,13 @@
         <v>45941</v>
       </c>
       <c r="C256" t="s">
+        <v>416</v>
+      </c>
+      <c r="D256" t="s">
         <v>417</v>
       </c>
-      <c r="D256" t="s">
+      <c r="E256" t="s">
         <v>418</v>
-      </c>
-      <c r="E256" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.3">
@@ -5080,7 +5185,7 @@
         <v>45942</v>
       </c>
       <c r="C257" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.3">
@@ -5091,7 +5196,7 @@
         <v>45943</v>
       </c>
       <c r="C258" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.3">
@@ -5102,7 +5207,7 @@
         <v>45944</v>
       </c>
       <c r="C259" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.3">
@@ -5113,7 +5218,7 @@
         <v>45945</v>
       </c>
       <c r="C260" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.3">
@@ -5124,10 +5229,10 @@
         <v>45946</v>
       </c>
       <c r="C261" t="s">
+        <v>328</v>
+      </c>
+      <c r="F261" t="s">
         <v>329</v>
-      </c>
-      <c r="F261" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.3">
@@ -5138,7 +5243,7 @@
         <v>45947</v>
       </c>
       <c r="C262" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.3">
@@ -5149,7 +5254,7 @@
         <v>45948</v>
       </c>
       <c r="C263" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.3">
@@ -5160,7 +5265,7 @@
         <v>45949</v>
       </c>
       <c r="C264" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.3">
@@ -5171,7 +5276,7 @@
         <v>45950</v>
       </c>
       <c r="C265" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.3">
@@ -5182,13 +5287,13 @@
         <v>45951</v>
       </c>
       <c r="C266" t="s">
+        <v>375</v>
+      </c>
+      <c r="D266" t="s">
         <v>376</v>
       </c>
-      <c r="D266" t="s">
+      <c r="E266" t="s">
         <v>377</v>
-      </c>
-      <c r="E266" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.3">
@@ -5199,7 +5304,7 @@
         <v>45952</v>
       </c>
       <c r="C267" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.3">
@@ -5210,7 +5315,7 @@
         <v>45953</v>
       </c>
       <c r="C268" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.3">
@@ -5221,7 +5326,7 @@
         <v>45954</v>
       </c>
       <c r="C269" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.3">
@@ -5232,7 +5337,7 @@
         <v>45955</v>
       </c>
       <c r="C270" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.3">
@@ -5243,7 +5348,7 @@
         <v>45956</v>
       </c>
       <c r="C271" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.3">
@@ -5254,7 +5359,7 @@
         <v>45957</v>
       </c>
       <c r="C272" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
@@ -5265,7 +5370,7 @@
         <v>45958</v>
       </c>
       <c r="C273" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
@@ -5276,13 +5381,13 @@
         <v>45959</v>
       </c>
       <c r="C274" t="s">
+        <v>383</v>
+      </c>
+      <c r="D274" t="s">
         <v>384</v>
       </c>
-      <c r="D274" t="s">
+      <c r="E274" t="s">
         <v>385</v>
-      </c>
-      <c r="E274" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
@@ -5293,7 +5398,7 @@
         <v>45960</v>
       </c>
       <c r="C275" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
@@ -5304,7 +5409,7 @@
         <v>45961</v>
       </c>
       <c r="C276" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
@@ -5315,7 +5420,7 @@
         <v>45962</v>
       </c>
       <c r="C277" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.3">
@@ -5326,7 +5431,7 @@
         <v>45963</v>
       </c>
       <c r="C278" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
@@ -5337,7 +5442,7 @@
         <v>45964</v>
       </c>
       <c r="C279" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
@@ -5348,13 +5453,13 @@
         <v>45965</v>
       </c>
       <c r="C280" t="s">
+        <v>419</v>
+      </c>
+      <c r="D280" t="s">
         <v>420</v>
       </c>
-      <c r="D280" t="s">
-        <v>421</v>
-      </c>
       <c r="E280" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
@@ -5365,7 +5470,7 @@
         <v>45966</v>
       </c>
       <c r="C281" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
@@ -5376,7 +5481,7 @@
         <v>45967</v>
       </c>
       <c r="C282" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
@@ -5387,7 +5492,7 @@
         <v>45968</v>
       </c>
       <c r="C283" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
@@ -5398,13 +5503,13 @@
         <v>45969</v>
       </c>
       <c r="C284" t="s">
+        <v>305</v>
+      </c>
+      <c r="D284" t="s">
         <v>306</v>
       </c>
-      <c r="D284" t="s">
+      <c r="E284" t="s">
         <v>307</v>
-      </c>
-      <c r="E284" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
@@ -5415,7 +5520,7 @@
         <v>45970</v>
       </c>
       <c r="C285" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
@@ -5426,7 +5531,7 @@
         <v>45971</v>
       </c>
       <c r="C286" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
@@ -5437,7 +5542,7 @@
         <v>45972</v>
       </c>
       <c r="C287" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
@@ -5448,7 +5553,7 @@
         <v>45973</v>
       </c>
       <c r="C288" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.3">
@@ -5459,10 +5564,10 @@
         <v>45974</v>
       </c>
       <c r="C289" t="s">
+        <v>330</v>
+      </c>
+      <c r="F289" t="s">
         <v>331</v>
-      </c>
-      <c r="F289" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.3">
@@ -5473,7 +5578,7 @@
         <v>45975</v>
       </c>
       <c r="C290" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.3">
@@ -5484,7 +5589,7 @@
         <v>45976</v>
       </c>
       <c r="C291" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.3">
@@ -5495,7 +5600,7 @@
         <v>45977</v>
       </c>
       <c r="C292" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.3">
@@ -5506,7 +5611,7 @@
         <v>45978</v>
       </c>
       <c r="C293" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.3">
@@ -5517,10 +5622,10 @@
         <v>45979</v>
       </c>
       <c r="C294" t="s">
+        <v>238</v>
+      </c>
+      <c r="F294" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="F294" s="5" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.3">
@@ -5531,7 +5636,7 @@
         <v>45980</v>
       </c>
       <c r="C295" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.3">
@@ -5542,7 +5647,7 @@
         <v>45981</v>
       </c>
       <c r="C296" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.3">
@@ -5553,7 +5658,7 @@
         <v>45982</v>
       </c>
       <c r="C297" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.3">
@@ -5564,7 +5669,7 @@
         <v>45983</v>
       </c>
       <c r="C298" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.3">
@@ -5575,7 +5680,7 @@
         <v>45984</v>
       </c>
       <c r="C299" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.3">
@@ -5586,10 +5691,10 @@
         <v>45985</v>
       </c>
       <c r="C300" t="s">
+        <v>343</v>
+      </c>
+      <c r="F300" t="s">
         <v>344</v>
-      </c>
-      <c r="F300" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.3">
@@ -5600,7 +5705,7 @@
         <v>45986</v>
       </c>
       <c r="C301" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.3">
@@ -5611,7 +5716,7 @@
         <v>45987</v>
       </c>
       <c r="C302" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.3">
@@ -5622,13 +5727,13 @@
         <v>45988</v>
       </c>
       <c r="C303" t="s">
+        <v>464</v>
+      </c>
+      <c r="D303" t="s">
         <v>465</v>
       </c>
-      <c r="D303" t="s">
+      <c r="E303" t="s">
         <v>466</v>
-      </c>
-      <c r="E303" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.3">
@@ -5639,7 +5744,7 @@
         <v>45989</v>
       </c>
       <c r="C304" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.3">
@@ -5650,13 +5755,13 @@
         <v>45990</v>
       </c>
       <c r="C305" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D305" t="s">
+        <v>103</v>
+      </c>
+      <c r="E305" t="s">
         <v>104</v>
-      </c>
-      <c r="E305" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.3">
@@ -5667,7 +5772,7 @@
         <v>45991</v>
       </c>
       <c r="C306" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.3">
@@ -5678,7 +5783,7 @@
         <v>45992</v>
       </c>
       <c r="C307" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.3">
@@ -5689,10 +5794,10 @@
         <v>45993</v>
       </c>
       <c r="C308" t="s">
+        <v>475</v>
+      </c>
+      <c r="F308" t="s">
         <v>476</v>
-      </c>
-      <c r="F308" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.3">
@@ -5703,7 +5808,7 @@
         <v>45994</v>
       </c>
       <c r="C309" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.3">
@@ -5714,7 +5819,7 @@
         <v>45995</v>
       </c>
       <c r="C310" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.3">
@@ -5725,13 +5830,13 @@
         <v>45996</v>
       </c>
       <c r="C311" t="s">
+        <v>370</v>
+      </c>
+      <c r="D311" t="s">
         <v>371</v>
       </c>
-      <c r="D311" t="s">
-        <v>372</v>
-      </c>
       <c r="E311" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.3">
@@ -5742,7 +5847,7 @@
         <v>45997</v>
       </c>
       <c r="C312" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.3">
@@ -5753,7 +5858,7 @@
         <v>45998</v>
       </c>
       <c r="C313" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.3">
@@ -5764,7 +5869,7 @@
         <v>45999</v>
       </c>
       <c r="C314" t="s">
-        <v>8</v>
+        <v>484</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.3">
@@ -5775,7 +5880,7 @@
         <v>46000</v>
       </c>
       <c r="C315" t="s">
-        <v>8</v>
+        <v>485</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.3">
@@ -5786,13 +5891,13 @@
         <v>46001</v>
       </c>
       <c r="C316" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D316" t="s">
+        <v>308</v>
+      </c>
+      <c r="E316" t="s">
         <v>309</v>
-      </c>
-      <c r="E316" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.3">
@@ -5803,7 +5908,7 @@
         <v>46002</v>
       </c>
       <c r="C317" t="s">
-        <v>8</v>
+        <v>486</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.3">
@@ -5814,7 +5919,7 @@
         <v>46003</v>
       </c>
       <c r="C318" t="s">
-        <v>8</v>
+        <v>487</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.3">
@@ -5825,13 +5930,13 @@
         <v>46004</v>
       </c>
       <c r="C319" t="s">
+        <v>467</v>
+      </c>
+      <c r="D319" t="s">
         <v>468</v>
       </c>
-      <c r="D319" t="s">
+      <c r="E319" t="s">
         <v>469</v>
-      </c>
-      <c r="E319" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.3">
@@ -5842,7 +5947,7 @@
         <v>46005</v>
       </c>
       <c r="C320" t="s">
-        <v>8</v>
+        <v>488</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.3">
@@ -5853,7 +5958,7 @@
         <v>46006</v>
       </c>
       <c r="C321" t="s">
-        <v>8</v>
+        <v>489</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.3">
@@ -5864,10 +5969,10 @@
         <v>46007</v>
       </c>
       <c r="C322" t="s">
+        <v>332</v>
+      </c>
+      <c r="F322" t="s">
         <v>333</v>
-      </c>
-      <c r="F322" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.3">
@@ -5878,7 +5983,7 @@
         <v>46008</v>
       </c>
       <c r="C323" t="s">
-        <v>8</v>
+        <v>490</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.3">
@@ -5889,7 +5994,7 @@
         <v>46009</v>
       </c>
       <c r="C324" t="s">
-        <v>8</v>
+        <v>491</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.3">
@@ -5900,7 +6005,7 @@
         <v>46010</v>
       </c>
       <c r="C325" t="s">
-        <v>8</v>
+        <v>492</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.3">
@@ -5911,13 +6016,13 @@
         <v>46011</v>
       </c>
       <c r="C326" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D326" t="s">
+        <v>312</v>
+      </c>
+      <c r="E326" t="s">
         <v>313</v>
-      </c>
-      <c r="E326" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.3">
@@ -5928,7 +6033,7 @@
         <v>46012</v>
       </c>
       <c r="C327" t="s">
-        <v>8</v>
+        <v>493</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.3">
@@ -5939,7 +6044,7 @@
         <v>46013</v>
       </c>
       <c r="C328" t="s">
-        <v>8</v>
+        <v>494</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.3">
@@ -5950,13 +6055,13 @@
         <v>46014</v>
       </c>
       <c r="C329" t="s">
+        <v>421</v>
+      </c>
+      <c r="D329" t="s">
         <v>422</v>
       </c>
-      <c r="D329" t="s">
+      <c r="E329" t="s">
         <v>423</v>
-      </c>
-      <c r="E329" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.3">
@@ -5967,7 +6072,7 @@
         <v>46015</v>
       </c>
       <c r="C330" t="s">
-        <v>8</v>
+        <v>495</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.3">
@@ -5978,7 +6083,7 @@
         <v>46016</v>
       </c>
       <c r="C331" t="s">
-        <v>8</v>
+        <v>496</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.3">
@@ -5989,7 +6094,7 @@
         <v>46017</v>
       </c>
       <c r="C332" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.3">
@@ -6000,10 +6105,10 @@
         <v>46018</v>
       </c>
       <c r="C333" t="s">
+        <v>477</v>
+      </c>
+      <c r="F333" t="s">
         <v>478</v>
-      </c>
-      <c r="F333" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.3">
@@ -6014,7 +6119,7 @@
         <v>46019</v>
       </c>
       <c r="C334" t="s">
-        <v>8</v>
+        <v>497</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.3">
@@ -6025,7 +6130,7 @@
         <v>46020</v>
       </c>
       <c r="C335" t="s">
-        <v>8</v>
+        <v>498</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.3">
@@ -6036,7 +6141,7 @@
         <v>46021</v>
       </c>
       <c r="C336" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.3">
@@ -6047,10 +6152,10 @@
         <v>46022</v>
       </c>
       <c r="C337" t="s">
+        <v>424</v>
+      </c>
+      <c r="D337" t="s">
         <v>425</v>
-      </c>
-      <c r="D337" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.3">
@@ -6061,7 +6166,7 @@
         <v>46023</v>
       </c>
       <c r="C338" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.3">
@@ -6072,7 +6177,7 @@
         <v>46024</v>
       </c>
       <c r="C339" t="s">
-        <v>8</v>
+        <v>499</v>
       </c>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.3">
@@ -6083,7 +6188,7 @@
         <v>46025</v>
       </c>
       <c r="C340" t="s">
-        <v>8</v>
+        <v>500</v>
       </c>
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.3">
@@ -6094,7 +6199,7 @@
         <v>46026</v>
       </c>
       <c r="C341" t="s">
-        <v>8</v>
+        <v>501</v>
       </c>
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.3">
@@ -6105,13 +6210,13 @@
         <v>46027</v>
       </c>
       <c r="C342" t="s">
+        <v>367</v>
+      </c>
+      <c r="D342" t="s">
         <v>368</v>
       </c>
-      <c r="D342" t="s">
+      <c r="E342" t="s">
         <v>369</v>
-      </c>
-      <c r="E342" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.3">
@@ -6122,7 +6227,7 @@
         <v>46028</v>
       </c>
       <c r="C343" t="s">
-        <v>8</v>
+        <v>502</v>
       </c>
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.3">
@@ -6133,7 +6238,7 @@
         <v>46029</v>
       </c>
       <c r="C344" t="s">
-        <v>8</v>
+        <v>503</v>
       </c>
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.3">
@@ -6144,10 +6249,10 @@
         <v>46030</v>
       </c>
       <c r="C345" t="s">
+        <v>334</v>
+      </c>
+      <c r="F345" t="s">
         <v>335</v>
-      </c>
-      <c r="F345" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.3">
@@ -6158,7 +6263,7 @@
         <v>46031</v>
       </c>
       <c r="C346" t="s">
-        <v>8</v>
+        <v>504</v>
       </c>
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.3">
@@ -6169,7 +6274,7 @@
         <v>46032</v>
       </c>
       <c r="C347" t="s">
-        <v>8</v>
+        <v>505</v>
       </c>
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.3">
@@ -6180,7 +6285,7 @@
         <v>46033</v>
       </c>
       <c r="C348" t="s">
-        <v>8</v>
+        <v>506</v>
       </c>
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.3">
@@ -6191,7 +6296,7 @@
         <v>46034</v>
       </c>
       <c r="C349" t="s">
-        <v>8</v>
+        <v>507</v>
       </c>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.3">
@@ -6202,7 +6307,7 @@
         <v>46035</v>
       </c>
       <c r="C350" t="s">
-        <v>8</v>
+        <v>508</v>
       </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.3">
@@ -6213,13 +6318,13 @@
         <v>46036</v>
       </c>
       <c r="C351" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D351" t="s">
+        <v>310</v>
+      </c>
+      <c r="E351" t="s">
         <v>311</v>
-      </c>
-      <c r="E351" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.3">
@@ -6230,7 +6335,7 @@
         <v>46037</v>
       </c>
       <c r="C352" t="s">
-        <v>8</v>
+        <v>509</v>
       </c>
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.3">
@@ -6241,7 +6346,7 @@
         <v>46038</v>
       </c>
       <c r="C353" t="s">
-        <v>8</v>
+        <v>510</v>
       </c>
     </row>
     <row r="354" spans="1:6" x14ac:dyDescent="0.3">
@@ -6252,13 +6357,13 @@
         <v>46039</v>
       </c>
       <c r="C354" t="s">
+        <v>378</v>
+      </c>
+      <c r="D354" t="s">
         <v>379</v>
       </c>
-      <c r="D354" t="s">
+      <c r="E354" t="s">
         <v>380</v>
-      </c>
-      <c r="E354" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.3">
@@ -6269,7 +6374,7 @@
         <v>46040</v>
       </c>
       <c r="C355" t="s">
-        <v>8</v>
+        <v>511</v>
       </c>
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.3">
@@ -6280,7 +6385,7 @@
         <v>46041</v>
       </c>
       <c r="C356" t="s">
-        <v>8</v>
+        <v>512</v>
       </c>
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.3">
@@ -6291,7 +6396,7 @@
         <v>46042</v>
       </c>
       <c r="C357" t="s">
-        <v>8</v>
+        <v>513</v>
       </c>
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.3">
@@ -6302,7 +6407,7 @@
         <v>46043</v>
       </c>
       <c r="C358" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.3">
@@ -6313,10 +6418,10 @@
         <v>46044</v>
       </c>
       <c r="C359" t="s">
-        <v>8</v>
+        <v>514</v>
       </c>
       <c r="F359" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.3">
@@ -6327,7 +6432,7 @@
         <v>46045</v>
       </c>
       <c r="C360" t="s">
-        <v>8</v>
+        <v>515</v>
       </c>
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.3">
@@ -6338,13 +6443,13 @@
         <v>46046</v>
       </c>
       <c r="C361" t="s">
+        <v>364</v>
+      </c>
+      <c r="D361" t="s">
         <v>365</v>
       </c>
-      <c r="D361" t="s">
+      <c r="E361" t="s">
         <v>366</v>
-      </c>
-      <c r="E361" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.3">
@@ -6355,7 +6460,7 @@
         <v>46047</v>
       </c>
       <c r="C362" t="s">
-        <v>8</v>
+        <v>516</v>
       </c>
       <c r="D362" s="2"/>
     </row>
@@ -6367,7 +6472,7 @@
         <v>46048</v>
       </c>
       <c r="C363" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.3">
@@ -6378,7 +6483,7 @@
         <v>46049</v>
       </c>
       <c r="C364" t="s">
-        <v>8</v>
+        <v>517</v>
       </c>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.3">
@@ -6389,7 +6494,7 @@
         <v>46050</v>
       </c>
       <c r="C365" t="s">
-        <v>8</v>
+        <v>518</v>
       </c>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.3">
@@ -6400,7 +6505,7 @@
         <v>46051</v>
       </c>
       <c r="C366" t="s">
-        <v>8</v>
+        <v>519</v>
       </c>
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.3">
@@ -6411,7 +6516,7 @@
         <v>46052</v>
       </c>
       <c r="C367" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Afegit colonies i bug fixed
</commit_message>
<xml_diff>
--- a/projecte/missatges.xlsx
+++ b/projecte/missatges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marçal\Desktop\appp\lolaa\projecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE880A1-92B1-4CDE-BBA1-D0C00F945557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4105F2-DEE8-4BC4-BFF5-F178888E84D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD45C792-848E-477D-81CD-048F598EDCC3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="531">
   <si>
     <t>Dia</t>
   </si>
@@ -771,9 +771,6 @@
     <t>Perquè tot i que no coincidim molt en gustos musicals, sempre ets LA MILLOR DJ quan et porto en cotxe. (Per cert, espero que ja tinguis el carnet!)</t>
   </si>
   <si>
-    <t>Perquè no t'enfades amb mi tot i que alguns cops faig molt el tonto (siusplau no t'enfadis per posar la foto d'ahir)</t>
-  </si>
-  <si>
     <t>Perquè som una parella SUPER GUAPA</t>
   </si>
   <si>
@@ -783,15 +780,6 @@
     <t>Una foto que vaig fer jo encara que no tinc una gran habilitat amb el mòbil</t>
   </si>
   <si>
-    <t>Perquè m'encanta quan poguem anem agafats de la mà tot i que al principi no ho feiem</t>
-  </si>
-  <si>
-    <t>Perquè m'has fet descobrir-te i descorir-me més a mi mateix</t>
-  </si>
-  <si>
-    <t>Perquè et poses MOLT vermella quan et poses nerviosa</t>
-  </si>
-  <si>
     <t>Perquè t'encanta queixar-te</t>
   </si>
   <si>
@@ -834,9 +822,6 @@
     <t>Perquè la meva roba et queda millor que a mi</t>
   </si>
   <si>
-    <t>Perquè em fas regals MOLT XULOS (alguns cops robats de l'Eloi)</t>
-  </si>
-  <si>
     <t>Perquè m'ajudes a netejar</t>
   </si>
   <si>
@@ -1068,9 +1053,6 @@
     <t>./video/altre_dormint.mp4</t>
   </si>
   <si>
-    <t>Perquè ens ho passem molt bé fent trucades junts</t>
-  </si>
-  <si>
     <t>Perquè encara que costi, sempre trobem algun moment per veure'ns</t>
   </si>
   <si>
@@ -1585,6 +1567,57 @@
   </si>
   <si>
     <t>Perquè sempre estàs molt atenta a mi i al que necessito. PREPARA'T QUE DEMÀ ES L'ÚLTIM DIA DE LA WEB. Tot i això, et seguirè estimant sempre.</t>
+  </si>
+  <si>
+    <t>Perquè no t'enfades amb mi tot i que no et pugui explcar gaire com van les colònies de Falcons. Aquesta tanda et farè un petit resum de que faig cada dia! DIA 1: Avui els nens arriben a la cassa i allà coneixen als guies que hi haurà duran les colònies. El Xamàn, la Constructora i l'Agricultora. Fan una activitat on apareix el Mercader Make (jo!!) i per la nit fan un encanteri per intentar protegir l'illa, que s'està destruïnt.</t>
+  </si>
+  <si>
+    <t>./img/col_1.jpeg</t>
+  </si>
+  <si>
+    <t>A la primera tanda va ploure i per això estàvem dins de la carpa :)</t>
+  </si>
+  <si>
+    <t>Perquè no t'enfades amb mi tot i que no et pugui explcar gaire com van les colònies de Falcons.  DIA 2: Avui els infants conèixen a la Vaiana i fan una activitat perquè pugi crear una barca per poder anar a buscar el cor de l'illa. Una part important de la illa per poder-la salvar. En aquesta activitat surt un dels personatges mes guapos, interpretat pel fantàstic Marçal Armengol. El personatger és diu Bonko-Banko i et deixo un video de com va vestit!</t>
+  </si>
+  <si>
+    <t>./video/col_2.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè no t'enfades amb mi tot i que no et pugui explcar gaire com van les colònies de Falcons. DIA 3: Els caps es barallen perquè creuen que els infants els han perdut la confiança. És fa la guerra guarra per poder resoldra-ho. Després de la guerra guarra, s'ha d'equilibrar fent una activitat la magnífica balança de la confiança per poder recuperar la connexió amb els líders de l'illa. A la nit, per descansar, es mira una peli: VAIANA 2. </t>
+  </si>
+  <si>
+    <t>./img/col_3.jpeg</t>
+  </si>
+  <si>
+    <t>Tot i que els infants si que descansen, jo no gaire, en la foto pots veure com m'estàn molestant intenant-me fer cuetes.</t>
+  </si>
+  <si>
+    <t>Perquè no t'enfades amb mi tot i que no et pugui explcar gaire com van les colònies de Falcons. DIA 4: Torna la Vaiana del seu viatge amb barco que va començar el dia 2 però no torna sola. S'ha trobat al Maui pel camí! Els infants hauràn de fer una excursió per poder recuperar el bàcul màgic del Maui, i així ell els podrà ajudar a recuperar l'illa. A més, el Maui els dona unes pedres protectores que els podràn ajudar contra els cremats. Uns dolents molt dolents creats a partir de Te Kà, una entitat que te com a únic objectiu destrossar el món.</t>
+  </si>
+  <si>
+    <t>./img/col_4.jpeg</t>
+  </si>
+  <si>
+    <t>Et deixo una foto del Maui amb el seu bàcul màgic, preparant-se per derrotar TOOOTS els malvats.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perquè no t'enfades amb mi tot i que no et pugui explcar gaire com van les colònies de Falcons. DIA 5: Avui els infants descobreixen que Te Kà ha arribat a la illa de Moto Nui, on és troben, i l'han de derrotar. Fent una activitat per ajuntar els 3 cors de la illa i gràcies a l'ajuda del fabulós Maui, ho poden aconseguir. Per celebrar-ho, a la nit fan un ball de gala on han d'anar vestits de blanc amb alguns detalls blaus o platejats. </t>
+  </si>
+  <si>
+    <t>./img/col_5.jpeg</t>
+  </si>
+  <si>
+    <t>Aquí podem veure com anem vestits pel photocall del ball de gala. GUAPISSIMS</t>
+  </si>
+  <si>
+    <t>Perquè no t'enfades amb mi tot i que no et pugui explcar gaire com van les colònies de Falcons. DIA 6: Avui es l'últim dia. Els infants és despedeixen de l'illa i conèixen a la Te Fiti. Aquest personatge és l'essència del Té Ka que ara s'ha convertit en bona. Per la tarda reben una nova visita. Son les seves famílies! Aquest també és una dia molt important pels monitors (i per mi!). És quan torno a Sabadell i puc veure la meva fantàstica novia! (Ets tu, la més guapa!)</t>
+  </si>
+  <si>
+    <t>./img/col_6.jpeg</t>
+  </si>
+  <si>
+    <t>En la foto ja veiem com el Maui es comença a treure la perruca per poder-se retrovar amb la seva magnífica parella!!</t>
   </si>
 </sst>
 </file>
@@ -1965,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC97EF-2C97-4372-89FB-A6AC9B4A4377}">
   <dimension ref="A1:H441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="80" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" topLeftCell="B152" zoomScale="80" workbookViewId="0">
+      <selection activeCell="C173" sqref="C173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2210,7 +2243,7 @@
         <v>134</v>
       </c>
       <c r="E17" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2250,7 +2283,7 @@
         <v>45705</v>
       </c>
       <c r="C20" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2273,7 +2306,7 @@
         <v>45707</v>
       </c>
       <c r="C22" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2284,13 +2317,13 @@
         <v>45708</v>
       </c>
       <c r="C23" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D23" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E23" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2312,10 +2345,10 @@
         <v>45710</v>
       </c>
       <c r="C25" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F25" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2362,7 +2395,7 @@
         <v>45714</v>
       </c>
       <c r="C29" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2406,13 +2439,13 @@
         <v>45718</v>
       </c>
       <c r="C33" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D33" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E33" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -2445,7 +2478,7 @@
         <v>45721</v>
       </c>
       <c r="C36" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="D36" t="s">
         <v>173</v>
@@ -2462,7 +2495,7 @@
         <v>45722</v>
       </c>
       <c r="C37" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2495,13 +2528,13 @@
         <v>45725</v>
       </c>
       <c r="C40" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D40" t="s">
+        <v>274</v>
+      </c>
+      <c r="E40" t="s">
         <v>279</v>
-      </c>
-      <c r="E40" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2562,7 +2595,7 @@
         <v>45730</v>
       </c>
       <c r="C45" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F45" t="s">
         <v>58</v>
@@ -2598,13 +2631,13 @@
         <v>45733</v>
       </c>
       <c r="C48" t="s">
+        <v>276</v>
+      </c>
+      <c r="D48" t="s">
         <v>281</v>
       </c>
-      <c r="D48" t="s">
-        <v>286</v>
-      </c>
       <c r="E48" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2670,13 +2703,13 @@
         <v>45739</v>
       </c>
       <c r="C54" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D54" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E54" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2740,7 +2773,7 @@
         <v>139</v>
       </c>
       <c r="F59" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2773,10 +2806,10 @@
         <v>45747</v>
       </c>
       <c r="C62" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F62" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2798,7 +2831,7 @@
         <v>45749</v>
       </c>
       <c r="C64" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2845,13 +2878,13 @@
         <v>45753</v>
       </c>
       <c r="C68" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D68" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E68" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2934,10 +2967,10 @@
         <v>45760</v>
       </c>
       <c r="C75" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F75" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2959,13 +2992,13 @@
         <v>45762</v>
       </c>
       <c r="C77" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D77" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E77" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -3034,13 +3067,13 @@
         <v>45768</v>
       </c>
       <c r="C83" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D83" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="E83" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -3123,10 +3156,10 @@
         <v>45775</v>
       </c>
       <c r="C90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="F90" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -3237,7 +3270,7 @@
         <v>45784</v>
       </c>
       <c r="C99" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3248,10 +3281,10 @@
         <v>45785</v>
       </c>
       <c r="C100" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="F100" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3284,13 +3317,13 @@
         <v>45788</v>
       </c>
       <c r="C103" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D103" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E103" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3486,13 +3519,13 @@
         <v>45805</v>
       </c>
       <c r="C120" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D120" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E120" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3761,10 +3794,10 @@
         <v>45827</v>
       </c>
       <c r="C142" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F142" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3883,13 +3916,13 @@
         <v>45837</v>
       </c>
       <c r="C152" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D152" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="E152" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
@@ -3983,9 +4016,6 @@
       <c r="E159" t="s">
         <v>225</v>
       </c>
-      <c r="F159" t="s">
-        <v>225</v>
-      </c>
       <c r="G159" t="s">
         <v>225</v>
       </c>
@@ -4023,7 +4053,7 @@
         <v>45847</v>
       </c>
       <c r="C162" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -4073,7 +4103,13 @@
         <v>45851</v>
       </c>
       <c r="C166" t="s">
-        <v>248</v>
+        <v>514</v>
+      </c>
+      <c r="D166" t="s">
+        <v>515</v>
+      </c>
+      <c r="E166" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
@@ -4084,13 +4120,10 @@
         <v>45852</v>
       </c>
       <c r="C167" t="s">
-        <v>249</v>
-      </c>
-      <c r="D167" t="s">
-        <v>250</v>
-      </c>
-      <c r="E167" t="s">
-        <v>251</v>
+        <v>517</v>
+      </c>
+      <c r="F167" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
@@ -4101,7 +4134,13 @@
         <v>45853</v>
       </c>
       <c r="C168" t="s">
-        <v>252</v>
+        <v>519</v>
+      </c>
+      <c r="D168" t="s">
+        <v>520</v>
+      </c>
+      <c r="E168" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
@@ -4112,7 +4151,13 @@
         <v>45854</v>
       </c>
       <c r="C169" t="s">
-        <v>253</v>
+        <v>522</v>
+      </c>
+      <c r="D169" t="s">
+        <v>523</v>
+      </c>
+      <c r="E169" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
@@ -4123,7 +4168,13 @@
         <v>45855</v>
       </c>
       <c r="C170" t="s">
-        <v>254</v>
+        <v>525</v>
+      </c>
+      <c r="D170" t="s">
+        <v>526</v>
+      </c>
+      <c r="E170" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
@@ -4134,10 +4185,13 @@
         <v>45856</v>
       </c>
       <c r="C171" t="s">
-        <v>230</v>
-      </c>
-      <c r="F171" t="s">
-        <v>231</v>
+        <v>528</v>
+      </c>
+      <c r="D171" t="s">
+        <v>529</v>
+      </c>
+      <c r="E171" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
@@ -4148,7 +4202,7 @@
         <v>45857</v>
       </c>
       <c r="C172" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
@@ -4159,7 +4213,7 @@
         <v>45858</v>
       </c>
       <c r="C173" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
@@ -4170,13 +4224,13 @@
         <v>45859</v>
       </c>
       <c r="C174" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D174" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E174" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
@@ -4187,7 +4241,7 @@
         <v>45860</v>
       </c>
       <c r="C175" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
@@ -4198,7 +4252,7 @@
         <v>45861</v>
       </c>
       <c r="C176" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
@@ -4209,7 +4263,7 @@
         <v>45862</v>
       </c>
       <c r="C177" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
@@ -4220,7 +4274,10 @@
         <v>45863</v>
       </c>
       <c r="C178" t="s">
-        <v>269</v>
+        <v>230</v>
+      </c>
+      <c r="F178" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
@@ -4242,13 +4299,13 @@
         <v>45865</v>
       </c>
       <c r="C180" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D180" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E180" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
@@ -4314,13 +4371,13 @@
         <v>45871</v>
       </c>
       <c r="C186" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D186" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E186" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
@@ -4331,7 +4388,7 @@
         <v>45872</v>
       </c>
       <c r="C187" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
@@ -4342,7 +4399,7 @@
         <v>45873</v>
       </c>
       <c r="C188" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
@@ -4411,13 +4468,13 @@
         <v>45879</v>
       </c>
       <c r="C194" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D194" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E194" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
@@ -4428,7 +4485,7 @@
         <v>45880</v>
       </c>
       <c r="C195" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
@@ -4456,7 +4513,7 @@
         <v>45882</v>
       </c>
       <c r="C197" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
@@ -4467,7 +4524,7 @@
         <v>45883</v>
       </c>
       <c r="C198" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
@@ -4478,10 +4535,10 @@
         <v>45884</v>
       </c>
       <c r="C199" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F199" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
@@ -4525,7 +4582,7 @@
         <v>45888</v>
       </c>
       <c r="C203" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
@@ -4536,13 +4593,13 @@
         <v>45889</v>
       </c>
       <c r="C204" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D204" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E204" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
@@ -4575,10 +4632,10 @@
         <v>45892</v>
       </c>
       <c r="C207" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F207" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
@@ -4589,7 +4646,13 @@
         <v>45893</v>
       </c>
       <c r="C208" t="s">
-        <v>347</v>
+        <v>248</v>
+      </c>
+      <c r="D208" t="s">
+        <v>249</v>
+      </c>
+      <c r="E208" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
@@ -4600,7 +4663,7 @@
         <v>45894</v>
       </c>
       <c r="C209" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
@@ -4622,7 +4685,7 @@
         <v>45896</v>
       </c>
       <c r="C211" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
@@ -4633,13 +4696,13 @@
         <v>45897</v>
       </c>
       <c r="C212" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D212" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E212" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
@@ -4672,7 +4735,7 @@
         <v>45900</v>
       </c>
       <c r="C215" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
@@ -4694,7 +4757,7 @@
         <v>45902</v>
       </c>
       <c r="C217" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
@@ -4705,7 +4768,7 @@
         <v>45903</v>
       </c>
       <c r="C218" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
@@ -4716,10 +4779,10 @@
         <v>45904</v>
       </c>
       <c r="C219" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F219" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.3">
@@ -4730,7 +4793,7 @@
         <v>45905</v>
       </c>
       <c r="C220" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
@@ -4752,7 +4815,7 @@
         <v>45907</v>
       </c>
       <c r="C222" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
@@ -4763,13 +4826,13 @@
         <v>45908</v>
       </c>
       <c r="C223" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D223" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E223" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.3">
@@ -4780,7 +4843,7 @@
         <v>45909</v>
       </c>
       <c r="C224" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -4791,7 +4854,7 @@
         <v>45910</v>
       </c>
       <c r="C225" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
@@ -4802,7 +4865,7 @@
         <v>45911</v>
       </c>
       <c r="C226" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
@@ -4813,7 +4876,7 @@
         <v>45912</v>
       </c>
       <c r="C227" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
@@ -4841,7 +4904,7 @@
         <v>45914</v>
       </c>
       <c r="C229" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
@@ -4852,7 +4915,7 @@
         <v>45915</v>
       </c>
       <c r="C230" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
@@ -4863,7 +4926,7 @@
         <v>45916</v>
       </c>
       <c r="C231" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
@@ -4874,13 +4937,13 @@
         <v>45917</v>
       </c>
       <c r="C232" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D232" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="E232" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
@@ -4891,7 +4954,7 @@
         <v>45918</v>
       </c>
       <c r="C233" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
@@ -4902,7 +4965,7 @@
         <v>45919</v>
       </c>
       <c r="C234" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.3">
@@ -4927,7 +4990,7 @@
         <v>45921</v>
       </c>
       <c r="C236" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.3">
@@ -4938,7 +5001,7 @@
         <v>45922</v>
       </c>
       <c r="C237" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
@@ -4952,10 +5015,10 @@
         <v>193</v>
       </c>
       <c r="D238" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E238" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
@@ -4966,7 +5029,7 @@
         <v>45924</v>
       </c>
       <c r="C239" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
@@ -4977,7 +5040,7 @@
         <v>45925</v>
       </c>
       <c r="C240" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.3">
@@ -4999,7 +5062,7 @@
         <v>45927</v>
       </c>
       <c r="C242" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.3">
@@ -5010,7 +5073,7 @@
         <v>45928</v>
       </c>
       <c r="C243" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.3">
@@ -5021,13 +5084,13 @@
         <v>45929</v>
       </c>
       <c r="C244" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D244" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="E244" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
@@ -5060,7 +5123,7 @@
         <v>45932</v>
       </c>
       <c r="C247" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.3">
@@ -5071,7 +5134,7 @@
         <v>45933</v>
       </c>
       <c r="C248" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.3">
@@ -5082,7 +5145,7 @@
         <v>45934</v>
       </c>
       <c r="C249" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.3">
@@ -5093,13 +5156,13 @@
         <v>45935</v>
       </c>
       <c r="C250" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D250" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E250" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.3">
@@ -5110,7 +5173,7 @@
         <v>45936</v>
       </c>
       <c r="C251" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.3">
@@ -5121,7 +5184,7 @@
         <v>45937</v>
       </c>
       <c r="C252" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.3">
@@ -5132,7 +5195,7 @@
         <v>45938</v>
       </c>
       <c r="C253" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.3">
@@ -5157,7 +5220,7 @@
         <v>45940</v>
       </c>
       <c r="C255" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
@@ -5168,13 +5231,13 @@
         <v>45941</v>
       </c>
       <c r="C256" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D256" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="E256" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.3">
@@ -5185,7 +5248,7 @@
         <v>45942</v>
       </c>
       <c r="C257" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.3">
@@ -5196,7 +5259,7 @@
         <v>45943</v>
       </c>
       <c r="C258" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.3">
@@ -5207,7 +5270,7 @@
         <v>45944</v>
       </c>
       <c r="C259" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.3">
@@ -5218,7 +5281,7 @@
         <v>45945</v>
       </c>
       <c r="C260" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.3">
@@ -5229,10 +5292,10 @@
         <v>45946</v>
       </c>
       <c r="C261" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F261" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.3">
@@ -5243,7 +5306,7 @@
         <v>45947</v>
       </c>
       <c r="C262" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.3">
@@ -5254,7 +5317,7 @@
         <v>45948</v>
       </c>
       <c r="C263" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.3">
@@ -5276,7 +5339,7 @@
         <v>45950</v>
       </c>
       <c r="C265" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.3">
@@ -5287,13 +5350,13 @@
         <v>45951</v>
       </c>
       <c r="C266" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D266" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E266" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.3">
@@ -5304,7 +5367,7 @@
         <v>45952</v>
       </c>
       <c r="C267" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.3">
@@ -5315,7 +5378,7 @@
         <v>45953</v>
       </c>
       <c r="C268" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.3">
@@ -5326,7 +5389,7 @@
         <v>45954</v>
       </c>
       <c r="C269" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.3">
@@ -5337,7 +5400,7 @@
         <v>45955</v>
       </c>
       <c r="C270" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.3">
@@ -5359,7 +5422,7 @@
         <v>45957</v>
       </c>
       <c r="C272" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
@@ -5370,7 +5433,7 @@
         <v>45958</v>
       </c>
       <c r="C273" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
@@ -5381,13 +5444,13 @@
         <v>45959</v>
       </c>
       <c r="C274" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D274" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="E274" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
@@ -5409,7 +5472,7 @@
         <v>45961</v>
       </c>
       <c r="C276" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
@@ -5431,7 +5494,7 @@
         <v>45963</v>
       </c>
       <c r="C278" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
@@ -5442,7 +5505,7 @@
         <v>45964</v>
       </c>
       <c r="C279" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
@@ -5453,13 +5516,13 @@
         <v>45965</v>
       </c>
       <c r="C280" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D280" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="E280" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
@@ -5470,7 +5533,7 @@
         <v>45966</v>
       </c>
       <c r="C281" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
@@ -5481,7 +5544,7 @@
         <v>45967</v>
       </c>
       <c r="C282" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
@@ -5492,7 +5555,7 @@
         <v>45968</v>
       </c>
       <c r="C283" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
@@ -5503,13 +5566,13 @@
         <v>45969</v>
       </c>
       <c r="C284" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D284" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E284" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
@@ -5520,7 +5583,7 @@
         <v>45970</v>
       </c>
       <c r="C285" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
@@ -5531,7 +5594,7 @@
         <v>45971</v>
       </c>
       <c r="C286" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
@@ -5542,7 +5605,7 @@
         <v>45972</v>
       </c>
       <c r="C287" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
@@ -5553,7 +5616,7 @@
         <v>45973</v>
       </c>
       <c r="C288" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.3">
@@ -5564,10 +5627,10 @@
         <v>45974</v>
       </c>
       <c r="C289" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F289" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.3">
@@ -5578,7 +5641,7 @@
         <v>45975</v>
       </c>
       <c r="C290" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.3">
@@ -5589,7 +5652,7 @@
         <v>45976</v>
       </c>
       <c r="C291" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.3">
@@ -5600,7 +5663,7 @@
         <v>45977</v>
       </c>
       <c r="C292" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.3">
@@ -5611,7 +5674,7 @@
         <v>45978</v>
       </c>
       <c r="C293" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.3">
@@ -5636,7 +5699,7 @@
         <v>45980</v>
       </c>
       <c r="C295" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.3">
@@ -5647,7 +5710,7 @@
         <v>45981</v>
       </c>
       <c r="C296" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.3">
@@ -5658,7 +5721,7 @@
         <v>45982</v>
       </c>
       <c r="C297" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.3">
@@ -5669,7 +5732,7 @@
         <v>45983</v>
       </c>
       <c r="C298" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.3">
@@ -5680,7 +5743,7 @@
         <v>45984</v>
       </c>
       <c r="C299" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.3">
@@ -5691,10 +5754,10 @@
         <v>45985</v>
       </c>
       <c r="C300" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F300" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.3">
@@ -5705,7 +5768,7 @@
         <v>45986</v>
       </c>
       <c r="C301" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.3">
@@ -5727,13 +5790,13 @@
         <v>45988</v>
       </c>
       <c r="C303" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="D303" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="E303" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.3">
@@ -5744,7 +5807,7 @@
         <v>45989</v>
       </c>
       <c r="C304" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.3">
@@ -5794,10 +5857,10 @@
         <v>45993</v>
       </c>
       <c r="C308" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="F308" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.3">
@@ -5808,7 +5871,7 @@
         <v>45994</v>
       </c>
       <c r="C309" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.3">
@@ -5819,7 +5882,7 @@
         <v>45995</v>
       </c>
       <c r="C310" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.3">
@@ -5830,13 +5893,13 @@
         <v>45996</v>
       </c>
       <c r="C311" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D311" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="E311" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.3">
@@ -5847,7 +5910,7 @@
         <v>45997</v>
       </c>
       <c r="C312" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.3">
@@ -5858,7 +5921,7 @@
         <v>45998</v>
       </c>
       <c r="C313" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.3">
@@ -5869,7 +5932,7 @@
         <v>45999</v>
       </c>
       <c r="C314" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.3">
@@ -5880,7 +5943,7 @@
         <v>46000</v>
       </c>
       <c r="C315" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.3">
@@ -5891,13 +5954,13 @@
         <v>46001</v>
       </c>
       <c r="C316" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D316" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E316" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.3">
@@ -5908,7 +5971,7 @@
         <v>46002</v>
       </c>
       <c r="C317" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.3">
@@ -5919,7 +5982,7 @@
         <v>46003</v>
       </c>
       <c r="C318" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.3">
@@ -5930,13 +5993,13 @@
         <v>46004</v>
       </c>
       <c r="C319" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="D319" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="E319" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.3">
@@ -5947,7 +6010,7 @@
         <v>46005</v>
       </c>
       <c r="C320" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.3">
@@ -5958,7 +6021,7 @@
         <v>46006</v>
       </c>
       <c r="C321" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.3">
@@ -5969,10 +6032,10 @@
         <v>46007</v>
       </c>
       <c r="C322" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F322" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.3">
@@ -5983,7 +6046,7 @@
         <v>46008</v>
       </c>
       <c r="C323" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.3">
@@ -5994,7 +6057,7 @@
         <v>46009</v>
       </c>
       <c r="C324" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.3">
@@ -6005,7 +6068,7 @@
         <v>46010</v>
       </c>
       <c r="C325" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.3">
@@ -6016,13 +6079,13 @@
         <v>46011</v>
       </c>
       <c r="C326" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D326" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E326" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.3">
@@ -6033,7 +6096,7 @@
         <v>46012</v>
       </c>
       <c r="C327" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.3">
@@ -6044,7 +6107,7 @@
         <v>46013</v>
       </c>
       <c r="C328" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.3">
@@ -6055,13 +6118,13 @@
         <v>46014</v>
       </c>
       <c r="C329" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="D329" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="E329" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.3">
@@ -6072,7 +6135,7 @@
         <v>46015</v>
       </c>
       <c r="C330" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.3">
@@ -6083,7 +6146,7 @@
         <v>46016</v>
       </c>
       <c r="C331" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.3">
@@ -6105,10 +6168,10 @@
         <v>46018</v>
       </c>
       <c r="C333" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="F333" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.3">
@@ -6119,7 +6182,7 @@
         <v>46019</v>
       </c>
       <c r="C334" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.3">
@@ -6130,7 +6193,7 @@
         <v>46020</v>
       </c>
       <c r="C335" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.3">
@@ -6152,10 +6215,10 @@
         <v>46022</v>
       </c>
       <c r="C337" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="D337" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.3">
@@ -6177,7 +6240,7 @@
         <v>46024</v>
       </c>
       <c r="C339" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.3">
@@ -6188,7 +6251,7 @@
         <v>46025</v>
       </c>
       <c r="C340" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.3">
@@ -6199,7 +6262,7 @@
         <v>46026</v>
       </c>
       <c r="C341" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.3">
@@ -6210,13 +6273,13 @@
         <v>46027</v>
       </c>
       <c r="C342" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D342" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E342" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.3">
@@ -6227,7 +6290,7 @@
         <v>46028</v>
       </c>
       <c r="C343" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.3">
@@ -6238,7 +6301,7 @@
         <v>46029</v>
       </c>
       <c r="C344" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.3">
@@ -6249,10 +6312,10 @@
         <v>46030</v>
       </c>
       <c r="C345" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F345" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.3">
@@ -6263,7 +6326,7 @@
         <v>46031</v>
       </c>
       <c r="C346" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.3">
@@ -6274,7 +6337,7 @@
         <v>46032</v>
       </c>
       <c r="C347" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.3">
@@ -6285,7 +6348,7 @@
         <v>46033</v>
       </c>
       <c r="C348" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.3">
@@ -6296,7 +6359,7 @@
         <v>46034</v>
       </c>
       <c r="C349" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.3">
@@ -6307,7 +6370,7 @@
         <v>46035</v>
       </c>
       <c r="C350" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.3">
@@ -6318,13 +6381,13 @@
         <v>46036</v>
       </c>
       <c r="C351" t="s">
+        <v>300</v>
+      </c>
+      <c r="D351" t="s">
         <v>305</v>
       </c>
-      <c r="D351" t="s">
-        <v>310</v>
-      </c>
       <c r="E351" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.3">
@@ -6335,7 +6398,7 @@
         <v>46037</v>
       </c>
       <c r="C352" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.3">
@@ -6346,7 +6409,7 @@
         <v>46038</v>
       </c>
       <c r="C353" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="354" spans="1:6" x14ac:dyDescent="0.3">
@@ -6357,13 +6420,13 @@
         <v>46039</v>
       </c>
       <c r="C354" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D354" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="E354" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.3">
@@ -6374,7 +6437,7 @@
         <v>46040</v>
       </c>
       <c r="C355" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.3">
@@ -6385,7 +6448,7 @@
         <v>46041</v>
       </c>
       <c r="C356" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.3">
@@ -6396,7 +6459,7 @@
         <v>46042</v>
       </c>
       <c r="C357" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.3">
@@ -6407,7 +6470,7 @@
         <v>46043</v>
       </c>
       <c r="C358" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.3">
@@ -6418,10 +6481,10 @@
         <v>46044</v>
       </c>
       <c r="C359" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="F359" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.3">
@@ -6432,7 +6495,7 @@
         <v>46045</v>
       </c>
       <c r="C360" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.3">
@@ -6443,13 +6506,13 @@
         <v>46046</v>
       </c>
       <c r="C361" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D361" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="E361" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.3">
@@ -6460,7 +6523,7 @@
         <v>46047</v>
       </c>
       <c r="C362" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="D362" s="2"/>
     </row>
@@ -6483,7 +6546,7 @@
         <v>46049</v>
       </c>
       <c r="C364" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.3">
@@ -6494,7 +6557,7 @@
         <v>46050</v>
       </c>
       <c r="C365" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.3">
@@ -6505,7 +6568,7 @@
         <v>46051</v>
       </c>
       <c r="C366" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.3">
@@ -6516,7 +6579,7 @@
         <v>46052</v>
       </c>
       <c r="C367" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>